<commit_message>
Commiting changes for Ruchika(MT2012119)
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20055" windowHeight="9210"/>
+    <workbookView visibility="veryHidden" xWindow="4005" yWindow="3390" windowWidth="11940" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -165,7 +166,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -392,7 +393,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="G23" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1436,9 +1437,15 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
       <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="M28" s="19">
+        <v>2</v>
+      </c>
+      <c r="N28" s="19">
+        <v>0</v>
+      </c>
+      <c r="O28" s="19">
+        <v>0</v>
+      </c>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
       <c r="R28" s="19"/>
@@ -1475,9 +1482,15 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
+      <c r="M29" s="19">
+        <v>7</v>
+      </c>
+      <c r="N29" s="19">
+        <v>2</v>
+      </c>
+      <c r="O29" s="19">
+        <v>2</v>
+      </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
       <c r="R29" s="19"/>
@@ -1514,9 +1527,15 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="M30" s="19">
+        <v>0</v>
+      </c>
+      <c r="N30" s="19">
+        <v>3</v>
+      </c>
+      <c r="O30" s="19">
+        <v>0</v>
+      </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
       <c r="R30" s="19"/>
@@ -1553,9 +1572,15 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="M31" s="19">
+        <v>0</v>
+      </c>
+      <c r="N31" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="O31" s="19">
+        <v>1</v>
+      </c>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
       <c r="R31" s="19"/>

</xml_diff>

<commit_message>
updated by sravani date:9/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="4005" yWindow="3390" windowWidth="11940" windowHeight="4590"/>
+    <workbookView xWindow="4005" yWindow="3390" windowWidth="11940" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -709,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G23" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1621,7 +1620,9 @@
       <c r="N32" s="19">
         <v>0</v>
       </c>
-      <c r="O32" s="19"/>
+      <c r="O32" s="19">
+        <v>0</v>
+      </c>
       <c r="P32" s="19"/>
       <c r="Q32" s="19"/>
       <c r="R32" s="19"/>
@@ -1662,7 +1663,9 @@
       <c r="N33" s="19">
         <v>2</v>
       </c>
-      <c r="O33" s="19"/>
+      <c r="O33" s="19">
+        <v>8</v>
+      </c>
       <c r="P33" s="19"/>
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
@@ -1703,7 +1706,9 @@
       <c r="N34" s="19">
         <v>4</v>
       </c>
-      <c r="O34" s="19"/>
+      <c r="O34" s="19">
+        <v>0</v>
+      </c>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
       <c r="R34" s="19"/>
@@ -1744,7 +1749,9 @@
       <c r="N35" s="19">
         <v>0.25</v>
       </c>
-      <c r="O35" s="19"/>
+      <c r="O35" s="19">
+        <v>1</v>
+      </c>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="19"/>
@@ -1787,7 +1794,9 @@
       <c r="N36" s="19">
         <v>0</v>
       </c>
-      <c r="O36" s="19"/>
+      <c r="O36" s="19">
+        <v>0</v>
+      </c>
       <c r="P36" s="19"/>
       <c r="Q36" s="19"/>
       <c r="R36" s="19"/>
@@ -1830,7 +1839,9 @@
       <c r="N37" s="19">
         <v>0.5</v>
       </c>
-      <c r="O37" s="19"/>
+      <c r="O37" s="19">
+        <v>8</v>
+      </c>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
       <c r="R37" s="19"/>
@@ -1873,7 +1884,9 @@
       <c r="N38" s="19">
         <v>4</v>
       </c>
-      <c r="O38" s="19"/>
+      <c r="O38" s="19">
+        <v>0</v>
+      </c>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
       <c r="R38" s="19"/>
@@ -1916,7 +1929,9 @@
       <c r="N39" s="19">
         <v>0.25</v>
       </c>
-      <c r="O39" s="19"/>
+      <c r="O39" s="19">
+        <v>1</v>
+      </c>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
       <c r="R39" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date:09-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -709,7 +709,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1840,7 +1840,7 @@
         <v>0.5</v>
       </c>
       <c r="O37" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Done By: 10-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -163,11 +163,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,7 +501,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -536,7 +535,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -712,14 +710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -728,7 +726,7 @@
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -740,7 +738,7 @@
       </c>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -754,7 +752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -768,7 +766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -780,7 +778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -792,7 +790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -804,7 +802,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -816,7 +814,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -828,7 +826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -840,7 +838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -848,7 +846,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -856,7 +854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -864,7 +862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -959,7 +957,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -998,7 +996,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1041,7 +1039,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1078,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1119,7 +1117,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1158,7 +1156,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1197,7 +1195,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1236,7 +1234,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1275,7 +1273,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1314,7 +1312,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1353,7 +1351,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1392,7 +1390,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1431,7 +1429,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1476,7 +1474,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1521,7 +1519,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1566,7 +1564,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -1611,7 +1609,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -1654,7 +1652,7 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -1697,7 +1695,7 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -1740,7 +1738,7 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -1783,7 +1781,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -1808,7 +1806,9 @@
       <c r="O36" s="19">
         <v>0</v>
       </c>
-      <c r="P36" s="19"/>
+      <c r="P36" s="19">
+        <v>0</v>
+      </c>
       <c r="Q36" s="19"/>
       <c r="R36" s="19"/>
       <c r="S36" s="19"/>
@@ -1828,7 +1828,7 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -1853,7 +1853,9 @@
       <c r="O37" s="19">
         <v>9</v>
       </c>
-      <c r="P37" s="19"/>
+      <c r="P37" s="19">
+        <v>7</v>
+      </c>
       <c r="Q37" s="19"/>
       <c r="R37" s="19"/>
       <c r="S37" s="19"/>
@@ -1873,7 +1875,7 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -1898,7 +1900,9 @@
       <c r="O38" s="19">
         <v>0</v>
       </c>
-      <c r="P38" s="19"/>
+      <c r="P38" s="19">
+        <v>0</v>
+      </c>
       <c r="Q38" s="19"/>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
@@ -1918,7 +1922,7 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -1943,7 +1947,9 @@
       <c r="O39" s="19">
         <v>1</v>
       </c>
-      <c r="P39" s="19"/>
+      <c r="P39" s="19">
+        <v>1</v>
+      </c>
       <c r="Q39" s="19"/>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
@@ -1963,7 +1969,7 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2006,7 +2012,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2049,7 +2055,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2092,7 +2098,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2145,24 +2151,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravani date:10/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1632,7 +1632,9 @@
       <c r="O32" s="19">
         <v>0</v>
       </c>
-      <c r="P32" s="19"/>
+      <c r="P32" s="19">
+        <v>0</v>
+      </c>
       <c r="Q32" s="19"/>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
@@ -1675,7 +1677,9 @@
       <c r="O33" s="19">
         <v>8</v>
       </c>
-      <c r="P33" s="19"/>
+      <c r="P33" s="19">
+        <v>8</v>
+      </c>
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
       <c r="S33" s="19"/>
@@ -1718,7 +1722,9 @@
       <c r="O34" s="19">
         <v>0</v>
       </c>
-      <c r="P34" s="19"/>
+      <c r="P34" s="19">
+        <v>0</v>
+      </c>
       <c r="Q34" s="19"/>
       <c r="R34" s="19"/>
       <c r="S34" s="19"/>
@@ -1761,7 +1767,9 @@
       <c r="O35" s="19">
         <v>1</v>
       </c>
-      <c r="P35" s="19"/>
+      <c r="P35" s="19">
+        <v>1</v>
+      </c>
       <c r="Q35" s="19"/>
       <c r="R35" s="19"/>
       <c r="S35" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 12-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -163,11 +163,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,7 +504,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -539,7 +538,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -715,14 +713,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N10" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -731,7 +729,7 @@
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -743,7 +741,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -757,7 +755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -771,7 +769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -783,7 +781,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -795,7 +793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -807,7 +805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -819,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -831,7 +829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -843,7 +841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -851,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -859,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -867,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -962,7 +960,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1009,7 +1007,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1056,7 +1054,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1103,7 +1101,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1150,7 +1148,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1189,7 +1187,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1228,7 +1226,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1267,7 +1265,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1306,7 +1304,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1347,7 +1345,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1388,7 +1386,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1431,7 +1429,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1474,7 +1472,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1519,7 +1517,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1564,7 +1562,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1609,7 +1607,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -1654,7 +1652,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -1699,7 +1697,7 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -1744,7 +1742,7 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -1789,7 +1787,7 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -1834,7 +1832,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -1863,7 +1861,9 @@
         <v>0</v>
       </c>
       <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
+      <c r="R36" s="19">
+        <v>0</v>
+      </c>
       <c r="S36" s="19"/>
       <c r="T36" s="19"/>
       <c r="U36" s="19"/>
@@ -1881,7 +1881,7 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -1910,7 +1910,9 @@
         <v>7</v>
       </c>
       <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
+      <c r="R37" s="19">
+        <v>0</v>
+      </c>
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
       <c r="U37" s="19"/>
@@ -1928,7 +1930,7 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -1957,7 +1959,9 @@
         <v>0</v>
       </c>
       <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
+      <c r="R38" s="19">
+        <v>2</v>
+      </c>
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
       <c r="U38" s="19"/>
@@ -1975,7 +1979,7 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2004,7 +2008,9 @@
         <v>1</v>
       </c>
       <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
+      <c r="R39" s="19">
+        <v>1.5</v>
+      </c>
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
       <c r="U39" s="19"/>
@@ -2022,7 +2028,7 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2069,7 +2075,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2116,7 +2122,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2163,7 +2169,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2220,24 +2226,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date :  14-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="46">
   <si>
     <t>Activity Code</t>
   </si>
@@ -717,17 +716,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M43" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -742,7 +741,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="18">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -756,7 +755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -770,7 +769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="27.6">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -782,7 +781,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="69">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -794,7 +793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="18">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -806,7 +805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -818,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="18">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -830,7 +829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -858,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="27.6">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -866,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="28.2">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -961,7 +960,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="18">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1010,7 +1009,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="18">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1059,7 +1058,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="18">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1108,7 +1107,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="18">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1157,7 +1156,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="18">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1196,7 +1195,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="18">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1235,7 +1234,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="18">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1274,7 +1273,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="18">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1313,7 +1312,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="18">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1354,7 +1353,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="18">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1395,7 +1394,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="18">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1438,7 +1437,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="18">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1481,7 +1480,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="18">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1526,7 +1525,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="18">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1571,7 +1570,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="18">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1616,7 +1615,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="18">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -1661,7 +1660,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="18">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -1706,7 +1705,7 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="18">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -1751,7 +1750,7 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="18">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -1796,7 +1795,7 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="18">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -1841,7 +1840,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="18">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -1869,12 +1868,18 @@
       <c r="P36" s="19">
         <v>0</v>
       </c>
-      <c r="Q36" s="19"/>
+      <c r="Q36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="R36" s="19">
         <v>0</v>
       </c>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
+      <c r="S36" s="19">
+        <v>0</v>
+      </c>
+      <c r="T36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="U36" s="19"/>
       <c r="V36" s="19"/>
       <c r="W36" s="19"/>
@@ -1890,7 +1895,7 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="18">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -1918,12 +1923,18 @@
       <c r="P37" s="19">
         <v>7</v>
       </c>
-      <c r="Q37" s="19"/>
+      <c r="Q37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="R37" s="19">
         <v>0</v>
       </c>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
+      <c r="S37" s="19">
+        <v>0</v>
+      </c>
+      <c r="T37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="U37" s="19"/>
       <c r="V37" s="19"/>
       <c r="W37" s="19"/>
@@ -1939,7 +1950,7 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="18">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -1967,12 +1978,18 @@
       <c r="P38" s="19">
         <v>0</v>
       </c>
-      <c r="Q38" s="19"/>
+      <c r="Q38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="R38" s="19">
         <v>2</v>
       </c>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
+      <c r="S38" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="T38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="U38" s="19"/>
       <c r="V38" s="19"/>
       <c r="W38" s="19"/>
@@ -1988,7 +2005,7 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="18">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2016,12 +2033,18 @@
       <c r="P39" s="19">
         <v>1</v>
       </c>
-      <c r="Q39" s="19"/>
+      <c r="Q39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="R39" s="19">
         <v>1.5</v>
       </c>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
+      <c r="S39" s="19">
+        <v>0</v>
+      </c>
+      <c r="T39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="U39" s="19"/>
       <c r="V39" s="19"/>
       <c r="W39" s="19"/>
@@ -2037,7 +2060,7 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="18">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2088,7 +2111,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="18">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2139,7 +2162,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2190,7 +2213,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2256,7 +2279,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2268,7 +2291,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 15-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="19470" windowHeight="6390"/>
@@ -11,8 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -717,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S14" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1921,7 +1920,9 @@
       <c r="T36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U36" s="19"/>
+      <c r="U36" s="19">
+        <v>0</v>
+      </c>
       <c r="V36" s="19"/>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
@@ -1976,7 +1977,9 @@
       <c r="T37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U37" s="19"/>
+      <c r="U37" s="19">
+        <v>0</v>
+      </c>
       <c r="V37" s="19"/>
       <c r="W37" s="19"/>
       <c r="X37" s="19"/>
@@ -2031,7 +2034,9 @@
       <c r="T38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U38" s="19"/>
+      <c r="U38" s="19">
+        <v>5</v>
+      </c>
       <c r="V38" s="19"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
@@ -2086,7 +2091,9 @@
       <c r="T39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U39" s="19"/>
+      <c r="U39" s="19">
+        <v>0</v>
+      </c>
       <c r="V39" s="19"/>
       <c r="W39" s="19"/>
       <c r="X39" s="19"/>

</xml_diff>

<commit_message>
Timesheet Changes by Ruchika
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19470" windowHeight="6390"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="46">
   <si>
     <t>Activity Code</t>
   </si>
@@ -716,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView tabSelected="1" topLeftCell="O22" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1545,13 +1546,25 @@
       <c r="O28" s="19">
         <v>0</v>
       </c>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
+      <c r="P28" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R28" s="19">
+        <v>0</v>
+      </c>
+      <c r="S28" s="19">
+        <v>0</v>
+      </c>
+      <c r="T28" s="19">
+        <v>0</v>
+      </c>
+      <c r="U28" s="19">
+        <v>0</v>
+      </c>
+      <c r="V28" s="22"/>
       <c r="W28" s="19"/>
       <c r="X28" s="19"/>
       <c r="Y28" s="19"/>
@@ -1590,13 +1603,25 @@
       <c r="O29" s="19">
         <v>2</v>
       </c>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
+      <c r="P29" s="19">
+        <v>6</v>
+      </c>
+      <c r="Q29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R29" s="19">
+        <v>0</v>
+      </c>
+      <c r="S29" s="19">
+        <v>2</v>
+      </c>
+      <c r="T29" s="19">
+        <v>0</v>
+      </c>
+      <c r="U29" s="19">
+        <v>0</v>
+      </c>
+      <c r="V29" s="22"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19"/>
       <c r="Y29" s="19"/>
@@ -1635,13 +1660,25 @@
       <c r="O30" s="19">
         <v>0</v>
       </c>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
+      <c r="P30" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R30" s="19">
+        <v>2</v>
+      </c>
+      <c r="S30" s="19">
+        <v>0</v>
+      </c>
+      <c r="T30" s="19">
+        <v>3</v>
+      </c>
+      <c r="U30" s="19">
+        <v>3</v>
+      </c>
+      <c r="V30" s="22"/>
       <c r="W30" s="19"/>
       <c r="X30" s="19"/>
       <c r="Y30" s="19"/>
@@ -1680,13 +1717,25 @@
       <c r="O31" s="19">
         <v>1</v>
       </c>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
+      <c r="P31" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="S31" s="19">
+        <v>0</v>
+      </c>
+      <c r="T31" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="U31" s="19">
+        <v>2</v>
+      </c>
+      <c r="V31" s="22"/>
       <c r="W31" s="19"/>
       <c r="X31" s="19"/>
       <c r="Y31" s="19"/>

</xml_diff>

<commit_message>
Done by: B S Deepthi Date: 16-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -163,11 +163,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,7 +504,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -539,7 +538,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -715,14 +713,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M14" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="I23" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -731,7 +729,7 @@
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -743,7 +741,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -757,7 +755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -771,7 +769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -783,7 +781,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -795,7 +793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -807,7 +805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -819,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -831,7 +829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -843,7 +841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -851,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -859,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -867,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -962,7 +960,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1017,7 +1015,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1072,7 +1070,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1127,7 +1125,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1182,7 +1180,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1221,7 +1219,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1260,7 +1258,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1299,7 +1297,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1338,7 +1336,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1385,7 +1383,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1432,7 +1430,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1481,7 +1479,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1530,7 +1528,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1587,7 +1585,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1644,7 +1642,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1701,7 +1699,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -1758,7 +1756,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -1803,7 +1801,7 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -1848,7 +1846,7 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -1893,7 +1891,7 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -1938,7 +1936,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -1981,7 +1979,9 @@
       <c r="U36" s="19">
         <v>0</v>
       </c>
-      <c r="V36" s="19"/>
+      <c r="V36" s="19">
+        <v>0</v>
+      </c>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
       <c r="Y36" s="19"/>
@@ -1995,7 +1995,7 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2038,7 +2038,9 @@
       <c r="U37" s="19">
         <v>0</v>
       </c>
-      <c r="V37" s="19"/>
+      <c r="V37" s="19">
+        <v>0</v>
+      </c>
       <c r="W37" s="19"/>
       <c r="X37" s="19"/>
       <c r="Y37" s="19"/>
@@ -2052,7 +2054,7 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2095,7 +2097,9 @@
       <c r="U38" s="19">
         <v>5</v>
       </c>
-      <c r="V38" s="19"/>
+      <c r="V38" s="19">
+        <v>2</v>
+      </c>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
       <c r="Y38" s="19"/>
@@ -2109,7 +2113,7 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2152,7 +2156,9 @@
       <c r="U39" s="19">
         <v>0</v>
       </c>
-      <c r="V39" s="19"/>
+      <c r="V39" s="19">
+        <v>0</v>
+      </c>
       <c r="W39" s="19"/>
       <c r="X39" s="19"/>
       <c r="Y39" s="19"/>
@@ -2166,7 +2172,7 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2223,7 +2229,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2280,7 +2286,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2337,7 +2343,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2404,24 +2410,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravani date:17/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Time Sheet for th month of February</t>
+  </si>
+  <si>
+    <t>LEAVE</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I23" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1782,13 +1785,27 @@
       <c r="P32" s="19">
         <v>0</v>
       </c>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
+      <c r="Q32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R32" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S32" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T32" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U32" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="V32" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="W32" s="19">
+        <v>0</v>
+      </c>
       <c r="X32" s="19"/>
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
@@ -1827,13 +1844,27 @@
       <c r="P33" s="19">
         <v>8</v>
       </c>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
+      <c r="Q33" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="V33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="W33" s="19">
+        <v>0</v>
+      </c>
       <c r="X33" s="19"/>
       <c r="Y33" s="19"/>
       <c r="Z33" s="19"/>
@@ -1872,13 +1903,27 @@
       <c r="P34" s="19">
         <v>0</v>
       </c>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
+      <c r="Q34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="V34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="W34" s="19">
+        <v>7</v>
+      </c>
       <c r="X34" s="19"/>
       <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
@@ -1917,13 +1962,27 @@
       <c r="P35" s="19">
         <v>1</v>
       </c>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
+      <c r="Q35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="V35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="W35" s="19">
+        <v>0</v>
+      </c>
       <c r="X35" s="19"/>
       <c r="Y35" s="19"/>
       <c r="Z35" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 17-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="K27" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2041,7 +2041,9 @@
       <c r="V36" s="19">
         <v>0</v>
       </c>
-      <c r="W36" s="19"/>
+      <c r="W36" s="19">
+        <v>0</v>
+      </c>
       <c r="X36" s="19"/>
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
@@ -2100,7 +2102,9 @@
       <c r="V37" s="19">
         <v>0</v>
       </c>
-      <c r="W37" s="19"/>
+      <c r="W37" s="19">
+        <v>0</v>
+      </c>
       <c r="X37" s="19"/>
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
@@ -2159,7 +2163,9 @@
       <c r="V38" s="19">
         <v>2</v>
       </c>
-      <c r="W38" s="19"/>
+      <c r="W38" s="19">
+        <v>0.5</v>
+      </c>
       <c r="X38" s="19"/>
       <c r="Y38" s="19"/>
       <c r="Z38" s="19"/>
@@ -2218,7 +2224,9 @@
       <c r="V39" s="19">
         <v>0</v>
       </c>
-      <c r="W39" s="19"/>
+      <c r="W39" s="19">
+        <v>0.5</v>
+      </c>
       <c r="X39" s="19"/>
       <c r="Y39" s="19"/>
       <c r="Z39" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date:19-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -720,17 +719,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P35" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" topLeftCell="L31" workbookViewId="0">
+      <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -745,7 +744,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="18">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -759,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -773,7 +772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="27.6">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -785,7 +784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="69">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -797,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="18">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -809,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -821,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="18">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -833,7 +832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -861,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="27.6">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -869,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="28.2">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -964,7 +963,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="18">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1025,7 +1024,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="18">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1086,7 +1085,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="18">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1147,7 +1146,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="18">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1208,7 +1207,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="18">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1247,7 +1246,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="18">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1286,7 +1285,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="18">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1325,7 +1324,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="18">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1364,7 +1363,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="18">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1414,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="18">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1466,7 +1465,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="18">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1519,7 +1518,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="18">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1571,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="18">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1629,7 +1628,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="18">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1686,7 +1685,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="18">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1743,7 +1742,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="18">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -1800,7 +1799,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="18">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -1861,7 +1860,7 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="18">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -1922,7 +1921,7 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="18">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -1983,7 +1982,7 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="18">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2044,7 +2043,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="18">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2093,8 +2092,12 @@
       <c r="W36" s="19">
         <v>0</v>
       </c>
-      <c r="X36" s="19"/>
-      <c r="Y36" s="19"/>
+      <c r="X36" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="19">
+        <v>0</v>
+      </c>
       <c r="Z36" s="19"/>
       <c r="AA36" s="19"/>
       <c r="AB36" s="19"/>
@@ -2105,7 +2108,7 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="18">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2154,8 +2157,12 @@
       <c r="W37" s="19">
         <v>0</v>
       </c>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
+      <c r="X37" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="19">
+        <v>0</v>
+      </c>
       <c r="Z37" s="19"/>
       <c r="AA37" s="19"/>
       <c r="AB37" s="19"/>
@@ -2166,7 +2173,7 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="18">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2215,8 +2222,12 @@
       <c r="W38" s="19">
         <v>0.5</v>
       </c>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
+      <c r="X38" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="19">
+        <v>0</v>
+      </c>
       <c r="Z38" s="19"/>
       <c r="AA38" s="19"/>
       <c r="AB38" s="19"/>
@@ -2227,7 +2238,7 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="18">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2276,8 +2287,12 @@
       <c r="W39" s="19">
         <v>0.5</v>
       </c>
-      <c r="X39" s="19"/>
-      <c r="Y39" s="19"/>
+      <c r="X39" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="19">
+        <v>1</v>
+      </c>
       <c r="Z39" s="19"/>
       <c r="AA39" s="19"/>
       <c r="AB39" s="19"/>
@@ -2288,7 +2303,7 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="18">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2351,7 +2366,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="18">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2414,7 +2429,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2477,7 +2492,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2555,7 +2570,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2567,7 +2582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravani date: 19/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -721,7 +720,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R23" workbookViewId="0">
-      <selection activeCell="Z34" sqref="Z34"/>
+      <selection activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1882,7 +1881,9 @@
       <c r="X32" s="19">
         <v>0</v>
       </c>
-      <c r="Y32" s="19"/>
+      <c r="Y32" s="19">
+        <v>0</v>
+      </c>
       <c r="Z32" s="19"/>
       <c r="AA32" s="19"/>
       <c r="AB32" s="19"/>
@@ -1943,7 +1944,9 @@
       <c r="X33" s="19">
         <v>0</v>
       </c>
-      <c r="Y33" s="19"/>
+      <c r="Y33" s="19">
+        <v>0</v>
+      </c>
       <c r="Z33" s="19"/>
       <c r="AA33" s="19"/>
       <c r="AB33" s="19"/>
@@ -2004,7 +2007,9 @@
       <c r="X34" s="19">
         <v>0</v>
       </c>
-      <c r="Y34" s="19"/>
+      <c r="Y34" s="19">
+        <v>0</v>
+      </c>
       <c r="Z34" s="19"/>
       <c r="AA34" s="19"/>
       <c r="AB34" s="19"/>
@@ -2065,7 +2070,9 @@
       <c r="X35" s="19">
         <v>0</v>
       </c>
-      <c r="Y35" s="19"/>
+      <c r="Y35" s="19">
+        <v>2</v>
+      </c>
       <c r="Z35" s="19"/>
       <c r="AA35" s="19"/>
       <c r="AB35" s="19"/>

</xml_diff>

<commit_message>
updated by sravani date:20/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="19470" windowHeight="6390"/>
@@ -11,8 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -720,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView tabSelected="1" topLeftCell="M25" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33:Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1893,7 +1892,9 @@
       <c r="Y32" s="19">
         <v>0</v>
       </c>
-      <c r="Z32" s="19"/>
+      <c r="Z32" s="19">
+        <v>0</v>
+      </c>
       <c r="AA32" s="19"/>
       <c r="AB32" s="19"/>
       <c r="AC32" s="19"/>
@@ -1956,7 +1957,9 @@
       <c r="Y33" s="19">
         <v>0</v>
       </c>
-      <c r="Z33" s="19"/>
+      <c r="Z33" s="19">
+        <v>0</v>
+      </c>
       <c r="AA33" s="19"/>
       <c r="AB33" s="19"/>
       <c r="AC33" s="19"/>
@@ -2019,7 +2022,9 @@
       <c r="Y34" s="19">
         <v>0</v>
       </c>
-      <c r="Z34" s="19"/>
+      <c r="Z34" s="19">
+        <v>0</v>
+      </c>
       <c r="AA34" s="19"/>
       <c r="AB34" s="19"/>
       <c r="AC34" s="19"/>
@@ -2082,7 +2087,9 @@
       <c r="Y35" s="19">
         <v>2</v>
       </c>
-      <c r="Z35" s="19"/>
+      <c r="Z35" s="19">
+        <v>0</v>
+      </c>
       <c r="AA35" s="19"/>
       <c r="AB35" s="19"/>
       <c r="AC35" s="19"/>

</xml_diff>

<commit_message>
updated by alpna date:20/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M25" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33:Z35"/>
+    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1014,7 +1014,9 @@
       <c r="Y16" s="19">
         <v>0</v>
       </c>
-      <c r="Z16" s="19"/>
+      <c r="Z16" s="19">
+        <v>0</v>
+      </c>
       <c r="AA16" s="19"/>
       <c r="AB16" s="19"/>
       <c r="AC16" s="19"/>
@@ -1075,7 +1077,9 @@
       <c r="Y17" s="19">
         <v>2</v>
       </c>
-      <c r="Z17" s="19"/>
+      <c r="Z17" s="19">
+        <v>0</v>
+      </c>
       <c r="AA17" s="19"/>
       <c r="AB17" s="19"/>
       <c r="AC17" s="19"/>
@@ -1136,7 +1140,9 @@
       <c r="Y18" s="19">
         <v>0</v>
       </c>
-      <c r="Z18" s="19"/>
+      <c r="Z18" s="19">
+        <v>0</v>
+      </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="19"/>
       <c r="AC18" s="19"/>
@@ -1197,7 +1203,9 @@
       <c r="Y19" s="19">
         <v>0</v>
       </c>
-      <c r="Z19" s="19"/>
+      <c r="Z19" s="19">
+        <v>0</v>
+      </c>
       <c r="AA19" s="19"/>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>

</xml_diff>

<commit_message>
updated by Deepthi Bhagi date: 20/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16:Z19"/>
+    <sheetView tabSelected="1" topLeftCell="L22" workbookViewId="0">
+      <selection activeCell="Z36" sqref="Z36:Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2162,7 +2162,9 @@
       <c r="Y36" s="19">
         <v>0</v>
       </c>
-      <c r="Z36" s="19"/>
+      <c r="Z36" s="19">
+        <v>0</v>
+      </c>
       <c r="AA36" s="19"/>
       <c r="AB36" s="19"/>
       <c r="AC36" s="19"/>
@@ -2227,7 +2229,9 @@
       <c r="Y37" s="19">
         <v>0</v>
       </c>
-      <c r="Z37" s="19"/>
+      <c r="Z37" s="19">
+        <v>0</v>
+      </c>
       <c r="AA37" s="19"/>
       <c r="AB37" s="19"/>
       <c r="AC37" s="19"/>
@@ -2292,7 +2296,9 @@
       <c r="Y38" s="19">
         <v>0</v>
       </c>
-      <c r="Z38" s="19"/>
+      <c r="Z38" s="19">
+        <v>0</v>
+      </c>
       <c r="AA38" s="19"/>
       <c r="AB38" s="19"/>
       <c r="AC38" s="19"/>
@@ -2357,7 +2363,9 @@
       <c r="Y39" s="19">
         <v>1</v>
       </c>
-      <c r="Z39" s="19"/>
+      <c r="Z39" s="19">
+        <v>0</v>
+      </c>
       <c r="AA39" s="19"/>
       <c r="AB39" s="19"/>
       <c r="AC39" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 21-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L22" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36:Z39"/>
+    <sheetView tabSelected="1" topLeftCell="M22" workbookViewId="0">
+      <selection activeCell="AA40" sqref="AA40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2156,16 +2156,18 @@
       <c r="W36" s="19">
         <v>0</v>
       </c>
-      <c r="X36" s="19">
-        <v>0</v>
+      <c r="X36" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y36" s="19">
         <v>0</v>
       </c>
-      <c r="Z36" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="19"/>
+      <c r="Z36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB36" s="19"/>
       <c r="AC36" s="19"/>
       <c r="AD36" s="19"/>
@@ -2223,16 +2225,18 @@
       <c r="W37" s="19">
         <v>0</v>
       </c>
-      <c r="X37" s="19">
-        <v>0</v>
+      <c r="X37" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y37" s="19">
         <v>0</v>
       </c>
-      <c r="Z37" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="19"/>
+      <c r="Z37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB37" s="19"/>
       <c r="AC37" s="19"/>
       <c r="AD37" s="19"/>
@@ -2290,16 +2294,18 @@
       <c r="W38" s="19">
         <v>0.5</v>
       </c>
-      <c r="X38" s="19">
-        <v>0</v>
+      <c r="X38" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y38" s="19">
         <v>0</v>
       </c>
-      <c r="Z38" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="19"/>
+      <c r="Z38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB38" s="19"/>
       <c r="AC38" s="19"/>
       <c r="AD38" s="19"/>
@@ -2357,16 +2363,18 @@
       <c r="W39" s="19">
         <v>0.5</v>
       </c>
-      <c r="X39" s="19">
-        <v>0</v>
+      <c r="X39" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y39" s="19">
         <v>1</v>
       </c>
-      <c r="Z39" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA39" s="19"/>
+      <c r="Z39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB39" s="19"/>
       <c r="AC39" s="19"/>
       <c r="AD39" s="19"/>

</xml_diff>

<commit_message>
updated by sravani date:21/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M22" workbookViewId="0">
-      <selection activeCell="AA40" sqref="AA40"/>
+    <sheetView tabSelected="1" topLeftCell="N16" workbookViewId="0">
+      <selection activeCell="AC35" sqref="AC35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1900,10 +1900,12 @@
       <c r="Y32" s="19">
         <v>0</v>
       </c>
-      <c r="Z32" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="19"/>
+      <c r="Z32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB32" s="19"/>
       <c r="AC32" s="19"/>
       <c r="AD32" s="19"/>
@@ -1965,10 +1967,12 @@
       <c r="Y33" s="19">
         <v>0</v>
       </c>
-      <c r="Z33" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA33" s="19"/>
+      <c r="Z33" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB33" s="19"/>
       <c r="AC33" s="19"/>
       <c r="AD33" s="19"/>
@@ -2025,15 +2029,17 @@
         <v>7</v>
       </c>
       <c r="X34" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y34" s="19">
         <v>0</v>
       </c>
-      <c r="Z34" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA34" s="19"/>
+      <c r="Z34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA34" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB34" s="19"/>
       <c r="AC34" s="19"/>
       <c r="AD34" s="19"/>
@@ -2087,7 +2093,7 @@
         <v>46</v>
       </c>
       <c r="W35" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X35" s="19">
         <v>0</v>
@@ -2095,10 +2101,12 @@
       <c r="Y35" s="19">
         <v>2</v>
       </c>
-      <c r="Z35" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA35" s="19"/>
+      <c r="Z35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA35" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB35" s="19"/>
       <c r="AC35" s="19"/>
       <c r="AD35" s="19"/>

</xml_diff>

<commit_message>
updated by alpna date:21/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N16" workbookViewId="0">
-      <selection activeCell="AC35" sqref="AC35"/>
+    <sheetView tabSelected="1" topLeftCell="N7" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1014,10 +1014,12 @@
       <c r="Y16" s="19">
         <v>0</v>
       </c>
-      <c r="Z16" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="19"/>
+      <c r="Z16" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA16" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB16" s="19"/>
       <c r="AC16" s="19"/>
       <c r="AD16" s="19"/>
@@ -1077,10 +1079,12 @@
       <c r="Y17" s="19">
         <v>2</v>
       </c>
-      <c r="Z17" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="19"/>
+      <c r="Z17" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA17" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB17" s="19"/>
       <c r="AC17" s="19"/>
       <c r="AD17" s="19"/>
@@ -1140,10 +1144,12 @@
       <c r="Y18" s="19">
         <v>0</v>
       </c>
-      <c r="Z18" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="19"/>
+      <c r="Z18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA18" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB18" s="19"/>
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
@@ -1203,10 +1209,12 @@
       <c r="Y19" s="19">
         <v>0</v>
       </c>
-      <c r="Z19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="19"/>
+      <c r="Z19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA19" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>

</xml_diff>

<commit_message>
updated by sravani date:23/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -720,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R24" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" topLeftCell="Q24" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2072,11 +2071,15 @@
       <c r="Z32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA32" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
+      <c r="AA32" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD32" s="19"/>
       <c r="AE32" s="19"/>
       <c r="AF32" s="19"/>
@@ -2139,11 +2142,15 @@
       <c r="Z33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA33" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="19"/>
+      <c r="AA33" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD33" s="19"/>
       <c r="AE33" s="19"/>
       <c r="AF33" s="19"/>
@@ -2206,11 +2213,15 @@
       <c r="Z34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA34" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB34" s="19"/>
-      <c r="AC34" s="19"/>
+      <c r="AA34" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD34" s="19"/>
       <c r="AE34" s="19"/>
       <c r="AF34" s="19"/>
@@ -2273,11 +2284,15 @@
       <c r="Z35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA35" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="19"/>
+      <c r="AA35" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="AB35" s="19">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD35" s="19"/>
       <c r="AE35" s="19"/>
       <c r="AF35" s="19"/>
@@ -2342,11 +2357,15 @@
       <c r="Z36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="19"/>
+      <c r="AA36" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD36" s="19"/>
       <c r="AE36" s="19"/>
       <c r="AF36" s="19"/>
@@ -2411,11 +2430,15 @@
       <c r="Z37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
+      <c r="AA37" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD37" s="19"/>
       <c r="AE37" s="19"/>
       <c r="AF37" s="19"/>
@@ -2480,11 +2503,15 @@
       <c r="Z38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
+      <c r="AA38" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD38" s="19"/>
       <c r="AE38" s="19"/>
       <c r="AF38" s="19"/>
@@ -2549,11 +2576,15 @@
       <c r="Z39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
+      <c r="AA39" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="AB39" s="19">
+        <v>1</v>
+      </c>
+      <c r="AC39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AD39" s="19"/>
       <c r="AE39" s="19"/>
       <c r="AF39" s="19"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 23-02-2012
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q24" workbookViewId="0">
-      <selection activeCell="AA35" sqref="AA35"/>
+    <sheetView tabSelected="1" topLeftCell="Q22" workbookViewId="0">
+      <selection activeCell="AB39" sqref="AB39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2580,7 +2580,7 @@
         <v>1.5</v>
       </c>
       <c r="AB39" s="19">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AC39" s="20" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
updated by sravani date: 24/2/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -166,11 +166,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,7 +507,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -542,7 +541,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -718,14 +716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W13" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView tabSelected="1" topLeftCell="W24" workbookViewId="0">
+      <selection activeCell="AE35" sqref="AE35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -734,7 +732,7 @@
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,7 +744,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -760,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -774,7 +772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -786,7 +784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -798,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -810,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -822,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -834,7 +832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -846,7 +844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -854,7 +852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -862,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -870,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -965,7 +963,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1036,7 +1034,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1107,7 +1105,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1178,7 +1176,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1249,7 +1247,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1316,7 +1314,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1383,7 +1381,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1450,7 +1448,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1517,7 +1515,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1578,7 +1576,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1639,7 +1637,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1702,7 +1700,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1765,7 +1763,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1836,7 +1834,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1907,7 +1905,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1978,7 +1976,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2049,7 +2047,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2114,13 +2112,15 @@
       <c r="AC32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD32" s="19"/>
+      <c r="AD32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE32" s="19"/>
       <c r="AF32" s="19"/>
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2185,13 +2185,15 @@
       <c r="AC33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD33" s="19"/>
+      <c r="AD33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE33" s="19"/>
       <c r="AF33" s="19"/>
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2256,13 +2258,15 @@
       <c r="AC34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD34" s="19"/>
+      <c r="AD34" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE34" s="19"/>
       <c r="AF34" s="19"/>
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2327,13 +2331,15 @@
       <c r="AC35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD35" s="19"/>
+      <c r="AD35" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE35" s="19"/>
       <c r="AF35" s="19"/>
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2400,13 +2406,13 @@
       <c r="AC36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD36" s="19"/>
+      <c r="AD36" s="20"/>
       <c r="AE36" s="19"/>
       <c r="AF36" s="19"/>
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2473,13 +2479,13 @@
       <c r="AC37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD37" s="19"/>
+      <c r="AD37" s="20"/>
       <c r="AE37" s="19"/>
       <c r="AF37" s="19"/>
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2546,13 +2552,13 @@
       <c r="AC38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD38" s="19"/>
+      <c r="AD38" s="20"/>
       <c r="AE38" s="19"/>
       <c r="AF38" s="19"/>
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2619,13 +2625,13 @@
       <c r="AC39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD39" s="19"/>
+      <c r="AD39" s="20"/>
       <c r="AE39" s="19"/>
       <c r="AF39" s="19"/>
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2698,7 +2704,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2771,7 +2777,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2844,7 +2850,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2927,24 +2933,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
done by B.S. Deepthi date:24/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -720,7 +720,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W24" workbookViewId="0">
-      <selection activeCell="AE35" sqref="AE35"/>
+      <selection activeCell="AD36" sqref="AD36:AD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2406,7 +2406,9 @@
       <c r="AC36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD36" s="20"/>
+      <c r="AD36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE36" s="19"/>
       <c r="AF36" s="19"/>
       <c r="AG36" s="19"/>
@@ -2479,7 +2481,9 @@
       <c r="AC37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD37" s="20"/>
+      <c r="AD37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE37" s="19"/>
       <c r="AF37" s="19"/>
       <c r="AG37" s="19"/>
@@ -2552,7 +2556,9 @@
       <c r="AC38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD38" s="20"/>
+      <c r="AD38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE38" s="19"/>
       <c r="AF38" s="19"/>
       <c r="AG38" s="19"/>
@@ -2625,7 +2631,9 @@
       <c r="AC39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AD39" s="20"/>
+      <c r="AD39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AE39" s="19"/>
       <c r="AF39" s="19"/>
       <c r="AG39" s="19"/>

</xml_diff>

<commit_message>
DoneBy: B S Deepthi Date: 25-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -166,11 +166,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,7 +507,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -542,7 +541,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -718,14 +716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W8" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+    <sheetView tabSelected="1" topLeftCell="W26" workbookViewId="0">
+      <selection activeCell="AE36" sqref="AE36:AE39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -734,7 +732,7 @@
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,7 +744,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -760,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -774,7 +772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -786,7 +784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -798,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -810,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -822,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -834,7 +832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -846,7 +844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -854,7 +852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -862,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -870,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -965,7 +963,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1038,7 +1036,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1111,7 +1109,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1184,7 +1182,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1257,7 +1255,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1324,7 +1322,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1391,7 +1389,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1458,7 +1456,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1525,7 +1523,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1586,7 +1584,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1647,7 +1645,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1710,7 +1708,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1773,7 +1771,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1844,7 +1842,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1915,7 +1913,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -1986,7 +1984,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2057,7 +2055,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2130,7 +2128,7 @@
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2203,7 +2201,7 @@
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2276,7 +2274,7 @@
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2349,7 +2347,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2419,12 +2417,14 @@
       <c r="AD36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE36" s="19"/>
+      <c r="AE36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF36" s="19"/>
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2494,12 +2494,14 @@
       <c r="AD37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE37" s="19"/>
+      <c r="AE37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF37" s="19"/>
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2569,12 +2571,14 @@
       <c r="AD38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE38" s="19"/>
+      <c r="AE38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF38" s="19"/>
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2644,12 +2648,14 @@
       <c r="AD39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE39" s="19"/>
+      <c r="AE39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF39" s="19"/>
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2724,7 +2730,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2799,7 +2805,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2874,7 +2880,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -2959,24 +2965,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by: sravani date: 25/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -720,7 +720,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W26" workbookViewId="0">
-      <selection activeCell="AE36" sqref="AE36:AE39"/>
+      <selection activeCell="AE32" sqref="AE32:AE35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2123,7 +2123,9 @@
       <c r="AD32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE32" s="19"/>
+      <c r="AE32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF32" s="19"/>
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
@@ -2196,7 +2198,9 @@
       <c r="AD33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE33" s="19"/>
+      <c r="AE33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF33" s="19"/>
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
@@ -2269,7 +2273,9 @@
       <c r="AD34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE34" s="19"/>
+      <c r="AE34" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF34" s="19"/>
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
@@ -2342,7 +2348,9 @@
       <c r="AD35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AE35" s="19"/>
+      <c r="AE35" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AF35" s="19"/>
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>

</xml_diff>

<commit_message>
updated by sravani date:26/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W26" workbookViewId="0">
-      <selection activeCell="AE32" sqref="AE32:AE35"/>
+    <sheetView tabSelected="1" topLeftCell="W16" workbookViewId="0">
+      <selection activeCell="AF32" sqref="AF32:AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2126,7 +2126,9 @@
       <c r="AE32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF32" s="19"/>
+      <c r="AF32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG32" s="19"/>
       <c r="AH32" s="19"/>
     </row>
@@ -2201,7 +2203,9 @@
       <c r="AE33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF33" s="19"/>
+      <c r="AF33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG33" s="19"/>
       <c r="AH33" s="19"/>
     </row>
@@ -2276,7 +2280,9 @@
       <c r="AE34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF34" s="19"/>
+      <c r="AF34" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG34" s="19"/>
       <c r="AH34" s="19"/>
     </row>
@@ -2351,7 +2357,9 @@
       <c r="AE35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF35" s="19"/>
+      <c r="AF35" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
     </row>

</xml_diff>

<commit_message>
done by B.S.Deepthi date:26/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W16" workbookViewId="0">
-      <selection activeCell="AF32" sqref="AF32:AF35"/>
+    <sheetView tabSelected="1" topLeftCell="W25" workbookViewId="0">
+      <selection activeCell="AF36" sqref="AF36:AF39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2436,7 +2436,9 @@
       <c r="AE36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF36" s="19"/>
+      <c r="AF36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
@@ -2513,7 +2515,9 @@
       <c r="AE37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF37" s="19"/>
+      <c r="AF37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
@@ -2590,7 +2594,9 @@
       <c r="AE38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF38" s="19"/>
+      <c r="AF38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
@@ -2667,7 +2673,9 @@
       <c r="AE39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AF39" s="19"/>
+      <c r="AF39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>

</xml_diff>

<commit_message>
updated by sravani date:27/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -166,11 +166,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,7 +507,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -542,7 +541,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -718,14 +716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W9" workbookViewId="0">
-      <selection activeCell="AF24" sqref="AF24"/>
+    <sheetView tabSelected="1" topLeftCell="W27" workbookViewId="0">
+      <selection activeCell="AF35" sqref="AF35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -734,7 +732,7 @@
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,7 +744,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -760,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -774,7 +772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -786,7 +784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -798,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -810,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -822,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -834,7 +832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -846,7 +844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -854,7 +852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -862,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -870,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -965,7 +963,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1040,7 +1038,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1115,7 +1113,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1190,7 +1188,7 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1265,7 +1263,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1332,7 +1330,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1399,7 +1397,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1466,7 +1464,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1533,7 +1531,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1598,7 +1596,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1663,7 +1661,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1730,7 +1728,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1797,7 +1795,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1868,7 +1866,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1939,7 +1937,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2010,7 +2008,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2081,7 +2079,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2155,10 +2153,12 @@
       <c r="AF32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG32" s="19"/>
+      <c r="AG32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH32" s="19"/>
     </row>
-    <row r="33" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2232,10 +2232,12 @@
       <c r="AF33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG33" s="19"/>
+      <c r="AG33" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH33" s="19"/>
     </row>
-    <row r="34" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2309,10 +2311,12 @@
       <c r="AF34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG34" s="19"/>
+      <c r="AG34" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH34" s="19"/>
     </row>
-    <row r="35" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2386,10 +2390,12 @@
       <c r="AF35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG35" s="19"/>
+      <c r="AG35" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH35" s="19"/>
     </row>
-    <row r="36" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2468,7 +2474,7 @@
       <c r="AG36" s="19"/>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2547,7 +2553,7 @@
       <c r="AG37" s="19"/>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2626,7 +2632,7 @@
       <c r="AG38" s="19"/>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2705,7 +2711,7 @@
       <c r="AG39" s="19"/>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2782,7 +2788,7 @@
       <c r="AG40" s="19"/>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2859,7 +2865,7 @@
       <c r="AG41" s="19"/>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2936,7 +2942,7 @@
       <c r="AG42" s="19"/>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -3023,24 +3029,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
done by B.S.Deepthi date:27/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -720,7 +720,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W27" workbookViewId="0">
-      <selection activeCell="AF35" sqref="AF35"/>
+      <selection activeCell="AG36" sqref="AG36:AG39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2471,7 +2471,9 @@
       <c r="AF36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG36" s="19"/>
+      <c r="AG36" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH36" s="19"/>
     </row>
     <row r="37" spans="4:34" ht="17.25">
@@ -2550,7 +2552,9 @@
       <c r="AF37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG37" s="19"/>
+      <c r="AG37" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH37" s="19"/>
     </row>
     <row r="38" spans="4:34" ht="17.25">
@@ -2629,7 +2633,9 @@
       <c r="AF38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG38" s="19"/>
+      <c r="AG38" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH38" s="19"/>
     </row>
     <row r="39" spans="4:34" ht="17.25">
@@ -2708,7 +2714,9 @@
       <c r="AF39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AG39" s="19"/>
+      <c r="AG39" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AH39" s="19"/>
     </row>
     <row r="40" spans="4:34" ht="17.25">

</xml_diff>

<commit_message>
updated by alpna date: 27/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W27" workbookViewId="0">
-      <selection activeCell="AG36" sqref="AG36:AG39"/>
+    <sheetView tabSelected="1" topLeftCell="W6" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16:AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,7 +1035,9 @@
       <c r="AF16" s="19">
         <v>0</v>
       </c>
-      <c r="AG16" s="19"/>
+      <c r="AG16" s="19">
+        <v>0</v>
+      </c>
       <c r="AH16" s="19"/>
     </row>
     <row r="17" spans="4:34" ht="17.25">
@@ -1110,7 +1112,9 @@
       <c r="AF17" s="19">
         <v>0</v>
       </c>
-      <c r="AG17" s="19"/>
+      <c r="AG17" s="19">
+        <v>0</v>
+      </c>
       <c r="AH17" s="19"/>
     </row>
     <row r="18" spans="4:34" ht="17.25">
@@ -1185,7 +1189,9 @@
       <c r="AF18" s="19">
         <v>0</v>
       </c>
-      <c r="AG18" s="19"/>
+      <c r="AG18" s="19">
+        <v>0</v>
+      </c>
       <c r="AH18" s="19"/>
     </row>
     <row r="19" spans="4:34" ht="17.25">
@@ -1260,7 +1266,9 @@
       <c r="AF19" s="19">
         <v>0</v>
       </c>
-      <c r="AG19" s="19"/>
+      <c r="AG19" s="19">
+        <v>0</v>
+      </c>
       <c r="AH19" s="19"/>
     </row>
     <row r="20" spans="4:34" ht="17.25">

</xml_diff>

<commit_message>
updated by sravani date:28/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -720,17 +719,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W34" workbookViewId="0">
-      <selection activeCell="AG43" sqref="AG43"/>
+    <sheetView tabSelected="1" topLeftCell="W25" workbookViewId="0">
+      <selection activeCell="AH32" sqref="AH32:AH35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -745,7 +744,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="18">
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -759,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -773,7 +772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="27.6">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -785,7 +784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="69">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -797,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="18">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -809,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -821,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="18">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -833,7 +832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -861,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="27.6">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -869,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="28.2">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -964,7 +963,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="18">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1041,7 +1040,7 @@
       </c>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="4:34" ht="18">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1118,7 +1117,7 @@
       </c>
       <c r="AH17" s="19"/>
     </row>
-    <row r="18" spans="4:34" ht="18">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1195,7 +1194,7 @@
       </c>
       <c r="AH18" s="19"/>
     </row>
-    <row r="19" spans="4:34" ht="18">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1272,7 +1271,7 @@
       </c>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="18">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1339,7 +1338,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="18">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1406,7 +1405,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="18">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1472,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="18">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1540,7 +1539,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="18">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1605,7 +1604,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="18">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1670,7 +1669,7 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="19"/>
     </row>
-    <row r="26" spans="4:34" ht="18">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1737,7 +1736,7 @@
       <c r="AG26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="4:34" ht="18">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1804,7 +1803,7 @@
       <c r="AG27" s="19"/>
       <c r="AH27" s="19"/>
     </row>
-    <row r="28" spans="4:34" ht="18">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1875,7 +1874,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="18">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +1945,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="18">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2017,7 +2016,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="18">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2088,7 +2087,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="18">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2165,9 +2164,11 @@
       <c r="AG32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH32" s="19"/>
-    </row>
-    <row r="33" spans="4:34" ht="18">
+      <c r="AH32" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2244,9 +2245,11 @@
       <c r="AG33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH33" s="19"/>
-    </row>
-    <row r="34" spans="4:34" ht="18">
+      <c r="AH33" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2323,9 +2326,11 @@
       <c r="AG34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH34" s="19"/>
-    </row>
-    <row r="35" spans="4:34" ht="18">
+      <c r="AH34" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2402,9 +2407,11 @@
       <c r="AG35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH35" s="19"/>
-    </row>
-    <row r="36" spans="4:34" ht="18">
+      <c r="AH35" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2485,7 +2492,7 @@
       </c>
       <c r="AH36" s="19"/>
     </row>
-    <row r="37" spans="4:34" ht="18">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2566,7 +2573,7 @@
       </c>
       <c r="AH37" s="19"/>
     </row>
-    <row r="38" spans="4:34" ht="18">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2647,7 +2654,7 @@
       </c>
       <c r="AH38" s="19"/>
     </row>
-    <row r="39" spans="4:34" ht="18">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2728,7 +2735,7 @@
       </c>
       <c r="AH39" s="19"/>
     </row>
-    <row r="40" spans="4:34" ht="18">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2807,7 +2814,7 @@
       </c>
       <c r="AH40" s="19"/>
     </row>
-    <row r="41" spans="4:34" ht="18">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2886,7 +2893,7 @@
       </c>
       <c r="AH41" s="19"/>
     </row>
-    <row r="42" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="42" spans="4:34" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -2965,7 +2972,7 @@
       </c>
       <c r="AH42" s="19"/>
     </row>
-    <row r="43" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="43" spans="4:34" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -3059,7 +3066,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3071,7 +3078,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
done by B.S.Deepthi date:28-02-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -720,7 +720,7 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W25" workbookViewId="0">
-      <selection activeCell="AH32" sqref="AH32:AH35"/>
+      <selection activeCell="AH36" sqref="AH36:AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2490,7 +2490,9 @@
       <c r="AG36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH36" s="19"/>
+      <c r="AH36" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
@@ -2571,7 +2573,9 @@
       <c r="AG37" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH37" s="19"/>
+      <c r="AH37" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
@@ -2652,7 +2656,9 @@
       <c r="AG38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH38" s="19"/>
+      <c r="AH38" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
@@ -2733,7 +2739,9 @@
       <c r="AG39" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AH39" s="19"/>
+      <c r="AH39" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">

</xml_diff>

<commit_message>
updated by alpna date:28/02/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W25" workbookViewId="0">
-      <selection activeCell="AH36" sqref="AH36:AH39"/>
+    <sheetView tabSelected="1" topLeftCell="W10" workbookViewId="0">
+      <selection activeCell="AH16" sqref="AH16:AH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1038,7 +1038,9 @@
       <c r="AG16" s="19">
         <v>0</v>
       </c>
-      <c r="AH16" s="19"/>
+      <c r="AH16" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
@@ -1115,7 +1117,9 @@
       <c r="AG17" s="19">
         <v>0</v>
       </c>
-      <c r="AH17" s="19"/>
+      <c r="AH17" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
@@ -1192,7 +1196,9 @@
       <c r="AG18" s="19">
         <v>0</v>
       </c>
-      <c r="AH18" s="19"/>
+      <c r="AH18" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
@@ -1269,7 +1275,9 @@
       <c r="AG19" s="19">
         <v>0</v>
       </c>
-      <c r="AH19" s="19"/>
+      <c r="AH19" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">

</xml_diff>

<commit_message>
updated by sravani date: 1/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="14745" windowHeight="4005"/>
@@ -11,13 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -231,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -339,6 +338,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -352,7 +371,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -416,6 +435,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="3" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="3" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH43"/>
+  <dimension ref="A1:AI43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z19" workbookViewId="0">
-      <selection activeCell="AH27" sqref="AH27"/>
+    <sheetView tabSelected="1" topLeftCell="V25" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1043,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:34" ht="17.25">
+    <row r="17" spans="4:35" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1122,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:34" ht="17.25">
+    <row r="18" spans="4:35" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1201,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:34" ht="17.25">
+    <row r="19" spans="4:35" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1280,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:34" ht="17.25">
+    <row r="20" spans="4:35" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1347,7 +1372,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:34" ht="17.25">
+    <row r="21" spans="4:35" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1414,7 +1439,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="17.25">
+    <row r="22" spans="4:35" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1481,7 +1506,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="17.25">
+    <row r="23" spans="4:35" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1573,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="17.25">
+    <row r="24" spans="4:35" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1615,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:34" ht="17.25">
+    <row r="25" spans="4:35" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1682,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:34" ht="17.25">
+    <row r="26" spans="4:35" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1751,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:34" ht="17.25">
+    <row r="27" spans="4:35" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1820,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:34" ht="17.25">
+    <row r="28" spans="4:35" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1891,7 +1916,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:34" ht="17.25">
+    <row r="29" spans="4:35" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1962,7 +1987,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:34" ht="17.25">
+    <row r="30" spans="4:35" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2033,7 +2058,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:34" ht="17.25">
+    <row r="31" spans="4:35" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2104,7 +2129,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:34" ht="17.25">
+    <row r="32" spans="4:35" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2184,8 +2209,11 @@
       <c r="AH32" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="4:34" ht="17.25">
+      <c r="AI32" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="4:35" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2265,8 +2293,11 @@
       <c r="AH33" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="4:34" ht="17.25">
+      <c r="AI33" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="4:35" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2346,8 +2377,11 @@
       <c r="AH34" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="4:34" ht="17.25">
+      <c r="AI34" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="4:35" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2427,8 +2461,11 @@
       <c r="AH35" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="4:34" ht="17.25">
+      <c r="AI35" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="4:35" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2511,7 +2548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="4:34" ht="17.25">
+    <row r="37" spans="4:35" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2594,7 +2631,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="4:34" ht="17.25">
+    <row r="38" spans="4:35" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2677,7 +2714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="4:34" ht="17.25">
+    <row r="39" spans="4:35" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2760,7 +2797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:34" ht="17.25">
+    <row r="40" spans="4:35" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2841,7 +2878,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="4:34" ht="17.25">
+    <row r="41" spans="4:35" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -2922,7 +2959,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="4:34" ht="18" thickBot="1">
+    <row r="42" spans="4:35" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -3003,7 +3040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:34" ht="18" thickBot="1">
+    <row r="43" spans="4:35" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
done by B.S.Deepthi date:01-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -230,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -338,26 +338,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -371,7 +351,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -435,12 +415,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="3" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="3" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V25" workbookViewId="0">
-      <selection activeCell="AJ36" sqref="AJ36"/>
+    <sheetView tabSelected="1" topLeftCell="V13" workbookViewId="0">
+      <selection activeCell="AI17" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,9 +730,10 @@
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -770,7 +745,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25">
+    <row r="2" spans="1:35" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -784,7 +759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25">
+    <row r="3" spans="1:35" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -798,7 +773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5">
+    <row r="4" spans="1:35" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -810,7 +785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25">
+    <row r="5" spans="1:35" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -822,7 +797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25">
+    <row r="6" spans="1:35" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -834,7 +809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25">
+    <row r="7" spans="1:35" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -846,7 +821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25">
+    <row r="8" spans="1:35" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -858,7 +833,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25">
+    <row r="9" spans="1:35" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -870,7 +845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -878,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -886,7 +861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75">
+    <row r="12" spans="1:35" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -894,7 +869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30">
+    <row r="15" spans="1:35" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -988,8 +963,11 @@
       <c r="AH15" s="17">
         <v>40967</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" ht="17.25">
+      <c r="AI15" s="17">
+        <v>40969</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -2209,7 +2187,7 @@
       <c r="AH32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AI32" s="25" t="s">
+      <c r="AI32" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2293,7 +2271,7 @@
       <c r="AH33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AI33" s="25" t="s">
+      <c r="AI33" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2377,7 +2355,7 @@
       <c r="AH34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AI34" s="25" t="s">
+      <c r="AI34" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2461,7 +2439,7 @@
       <c r="AH35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AI35" s="26" t="s">
+      <c r="AI35" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2547,6 +2525,9 @@
       <c r="AH36" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="AI36" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="4:35" ht="17.25">
       <c r="D37" s="18" t="s">
@@ -2630,6 +2611,9 @@
       <c r="AH37" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="AI37" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="38" spans="4:35" ht="17.25">
       <c r="D38" s="18" t="s">
@@ -2713,6 +2697,9 @@
       <c r="AH38" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="AI38" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="39" spans="4:35" ht="17.25">
       <c r="D39" s="18" t="s">
@@ -2794,6 +2781,9 @@
         <v>43</v>
       </c>
       <c r="AH39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI39" s="20" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated by alpna date: 01/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -720,7 +720,7 @@
   <dimension ref="A1:AI43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V13" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+      <selection activeCell="AI16" sqref="AI16:AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1045,6 +1045,9 @@
       <c r="AH16" s="19">
         <v>0</v>
       </c>
+      <c r="AI16" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="4:35" ht="17.25">
       <c r="D17" s="18" t="s">
@@ -1124,6 +1127,9 @@
       <c r="AH17" s="19">
         <v>0</v>
       </c>
+      <c r="AI17" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="4:35" ht="17.25">
       <c r="D18" s="18" t="s">
@@ -1201,6 +1207,9 @@
         <v>0</v>
       </c>
       <c r="AH18" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1280,6 +1289,9 @@
         <v>0</v>
       </c>
       <c r="AH19" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="19">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated by sravani date:2/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -166,11 +166,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,13 +434,13 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="3" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +533,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -568,7 +567,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -744,14 +742,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X13" workbookViewId="0">
-      <selection activeCell="AJ23" sqref="AJ23"/>
+    <sheetView tabSelected="1" topLeftCell="X28" workbookViewId="0">
+      <selection activeCell="AJ32" sqref="AJ32:AJ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -759,21 +757,22 @@
     <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="24"/>
-    </row>
-    <row r="2" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -787,7 +786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -801,7 +800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -813,7 +812,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -825,7 +824,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -837,7 +836,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -849,7 +848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -861,7 +860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -873,7 +872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -881,7 +880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -889,7 +888,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -897,7 +896,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -994,8 +993,11 @@
       <c r="AI15" s="17">
         <v>40969</v>
       </c>
-    </row>
-    <row r="16" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ15" s="17">
+        <v>40970</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1077,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:36" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:36" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1241,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:36" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:36" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1390,7 +1392,7 @@
       <c r="AG20" s="19"/>
       <c r="AH20" s="19"/>
     </row>
-    <row r="21" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:36" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1457,7 +1459,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:36" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1524,7 +1526,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:36" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1591,7 +1593,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:36" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1657,11 +1659,11 @@
       <c r="AH24" s="19">
         <v>0</v>
       </c>
-      <c r="AI24" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AI24" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:36" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1727,11 +1729,11 @@
       <c r="AH25" s="19">
         <v>0</v>
       </c>
-      <c r="AI25" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AI25" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:36" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -1799,11 +1801,11 @@
       <c r="AH26" s="19">
         <v>0</v>
       </c>
-      <c r="AI26" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AI26" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:36" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -1871,11 +1873,11 @@
       <c r="AH27" s="19">
         <v>0</v>
       </c>
-      <c r="AI27" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AI27" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:36" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +1948,7 @@
       <c r="AG28" s="19"/>
       <c r="AH28" s="19"/>
     </row>
-    <row r="29" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:36" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2017,7 +2019,7 @@
       <c r="AG29" s="19"/>
       <c r="AH29" s="19"/>
     </row>
-    <row r="30" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:36" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2088,7 +2090,7 @@
       <c r="AG30" s="19"/>
       <c r="AH30" s="19"/>
     </row>
-    <row r="31" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:36" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2159,7 +2161,7 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="19"/>
     </row>
-    <row r="32" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:36" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2242,8 +2244,11 @@
       <c r="AI32" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ32" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="4:36" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2326,8 +2331,11 @@
       <c r="AI33" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ33" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="4:36" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2410,8 +2418,11 @@
       <c r="AI34" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ34" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="4:36" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2494,8 +2505,11 @@
       <c r="AI35" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ35" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="4:36" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2580,8 +2594,11 @@
       <c r="AI36" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ36" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="4:36" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2667,7 +2684,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:36" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2753,7 +2770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:36" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2839,7 +2856,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:36" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -2923,7 +2940,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:36" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -3007,7 +3024,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="4:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:36" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -3091,7 +3108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:36" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -3185,24 +3202,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
done by B.S.Deepthi date:2-3-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -746,7 +746,7 @@
   <dimension ref="A1:AJ43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X28" workbookViewId="0">
-      <selection activeCell="AJ32" sqref="AJ32:AJ36"/>
+      <selection activeCell="AJ37" sqref="AJ37:AJ39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2683,6 +2683,9 @@
       <c r="AI37" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="AJ37" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="38" spans="4:36" ht="17.25">
       <c r="D38" s="18" t="s">
@@ -2769,6 +2772,9 @@
       <c r="AI38" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="AJ38" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="39" spans="4:36" ht="17.25">
       <c r="D39" s="18" t="s">
@@ -2853,6 +2859,9 @@
         <v>43</v>
       </c>
       <c r="AI39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ39" s="20" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated by alpna date:2/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X28" workbookViewId="0">
-      <selection activeCell="AJ37" sqref="AJ37:AJ39"/>
+    <sheetView tabSelected="1" topLeftCell="X13" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16:AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1078,6 +1078,9 @@
       <c r="AI16" s="19">
         <v>0</v>
       </c>
+      <c r="AJ16" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="4:36" ht="17.25">
       <c r="D17" s="18" t="s">
@@ -1160,6 +1163,9 @@
       <c r="AI17" s="19">
         <v>0</v>
       </c>
+      <c r="AJ17" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="4:36" ht="17.25">
       <c r="D18" s="18" t="s">
@@ -1240,6 +1246,9 @@
         <v>0</v>
       </c>
       <c r="AI18" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1322,6 +1331,9 @@
         <v>0</v>
       </c>
       <c r="AI19" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="19">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Timesheet changes by Ruchika(MT2012119)
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="FebruaryMarch 2013" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -732,25 +732,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI13" workbookViewId="0">
-      <selection activeCell="AP17" sqref="AP17"/>
+    <sheetView tabSelected="1" topLeftCell="AG16" workbookViewId="0">
+      <selection activeCell="AQ27" sqref="AQ27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="43" width="11.21875" customWidth="1"/>
-    <col min="44" max="45" width="11.33203125" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45">
@@ -765,7 +764,7 @@
       </c>
       <c r="E1" s="28"/>
     </row>
-    <row r="2" spans="1:45" ht="18">
+    <row r="2" spans="1:45" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -779,7 +778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="18">
+    <row r="3" spans="1:45" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -793,7 +792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="27.6">
+    <row r="4" spans="1:45" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -805,7 +804,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="69">
+    <row r="5" spans="1:45" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -817,7 +816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="18">
+    <row r="6" spans="1:45" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -829,7 +828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="18">
+    <row r="7" spans="1:45" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -841,7 +840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="18">
+    <row r="8" spans="1:45" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -853,7 +852,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="18">
+    <row r="9" spans="1:45" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -881,7 +880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:45" ht="27.6">
+    <row r="12" spans="1:45" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -903,7 +902,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:45" ht="28.2">
+    <row r="15" spans="1:45" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1031,7 +1030,7 @@
         <v>40979</v>
       </c>
     </row>
-    <row r="16" spans="1:45" ht="18">
+    <row r="16" spans="1:45" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1135,7 +1134,7 @@
       <c r="AR16" s="26"/>
       <c r="AS16" s="26"/>
     </row>
-    <row r="17" spans="4:45" ht="18">
+    <row r="17" spans="4:45" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1239,7 +1238,7 @@
       <c r="AR17" s="26"/>
       <c r="AS17" s="26"/>
     </row>
-    <row r="18" spans="4:45" ht="18">
+    <row r="18" spans="4:45" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1343,7 +1342,7 @@
       <c r="AR18" s="26"/>
       <c r="AS18" s="26"/>
     </row>
-    <row r="19" spans="4:45" ht="18">
+    <row r="19" spans="4:45" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1446,7 @@
       <c r="AR19" s="26"/>
       <c r="AS19" s="26"/>
     </row>
-    <row r="20" spans="4:45" ht="18">
+    <row r="20" spans="4:45" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1525,7 +1524,7 @@
       <c r="AR20" s="26"/>
       <c r="AS20" s="26"/>
     </row>
-    <row r="21" spans="4:45" ht="18">
+    <row r="21" spans="4:45" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1603,7 +1602,7 @@
       <c r="AR21" s="26"/>
       <c r="AS21" s="26"/>
     </row>
-    <row r="22" spans="4:45" ht="18">
+    <row r="22" spans="4:45" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1680,7 @@
       <c r="AR22" s="26"/>
       <c r="AS22" s="26"/>
     </row>
-    <row r="23" spans="4:45" ht="18">
+    <row r="23" spans="4:45" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1759,7 +1758,7 @@
       <c r="AR23" s="26"/>
       <c r="AS23" s="26"/>
     </row>
-    <row r="24" spans="4:45" ht="18">
+    <row r="24" spans="4:45" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1849,7 +1848,7 @@
       <c r="AR24" s="26"/>
       <c r="AS24" s="26"/>
     </row>
-    <row r="25" spans="4:45" ht="18">
+    <row r="25" spans="4:45" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1939,7 +1938,7 @@
       <c r="AR25" s="26"/>
       <c r="AS25" s="26"/>
     </row>
-    <row r="26" spans="4:45" ht="18">
+    <row r="26" spans="4:45" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2031,7 +2030,7 @@
       <c r="AR26" s="26"/>
       <c r="AS26" s="26"/>
     </row>
-    <row r="27" spans="4:45" ht="18">
+    <row r="27" spans="4:45" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2123,7 +2122,7 @@
       <c r="AR27" s="26"/>
       <c r="AS27" s="26"/>
     </row>
-    <row r="28" spans="4:45" ht="18">
+    <row r="28" spans="4:45" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -2187,25 +2186,51 @@
       <c r="AB28" s="19">
         <v>0</v>
       </c>
-      <c r="AC28" s="19"/>
-      <c r="AD28" s="19"/>
-      <c r="AE28" s="19"/>
-      <c r="AF28" s="19"/>
-      <c r="AG28" s="19"/>
-      <c r="AH28" s="19"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="26"/>
-      <c r="AL28" s="26"/>
-      <c r="AM28" s="26"/>
-      <c r="AN28" s="26"/>
-      <c r="AO28" s="26"/>
+      <c r="AC28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AN28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO28" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AP28" s="26"/>
       <c r="AQ28" s="26"/>
       <c r="AR28" s="26"/>
       <c r="AS28" s="26"/>
     </row>
-    <row r="29" spans="4:45" ht="18">
+    <row r="29" spans="4:45" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2269,25 +2294,51 @@
       <c r="AB29" s="19">
         <v>0</v>
       </c>
-      <c r="AC29" s="19"/>
-      <c r="AD29" s="19"/>
-      <c r="AE29" s="19"/>
-      <c r="AF29" s="19"/>
-      <c r="AG29" s="19"/>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="26"/>
-      <c r="AL29" s="26"/>
-      <c r="AM29" s="26"/>
-      <c r="AN29" s="26"/>
-      <c r="AO29" s="26"/>
+      <c r="AC29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL29" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM29" s="26">
+        <v>1</v>
+      </c>
+      <c r="AN29" s="26">
+        <v>1</v>
+      </c>
+      <c r="AO29" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AP29" s="26"/>
       <c r="AQ29" s="26"/>
       <c r="AR29" s="26"/>
       <c r="AS29" s="26"/>
     </row>
-    <row r="30" spans="4:45" ht="18">
+    <row r="30" spans="4:45" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2351,25 +2402,51 @@
       <c r="AB30" s="19">
         <v>0</v>
       </c>
-      <c r="AC30" s="19"/>
-      <c r="AD30" s="19"/>
-      <c r="AE30" s="19"/>
-      <c r="AF30" s="19"/>
-      <c r="AG30" s="19"/>
-      <c r="AH30" s="19"/>
-      <c r="AI30" s="22"/>
-      <c r="AJ30" s="22"/>
-      <c r="AK30" s="26"/>
-      <c r="AL30" s="26"/>
-      <c r="AM30" s="26"/>
-      <c r="AN30" s="26"/>
-      <c r="AO30" s="26"/>
+      <c r="AC30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM30" s="26">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO30" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AP30" s="26"/>
       <c r="AQ30" s="26"/>
       <c r="AR30" s="26"/>
       <c r="AS30" s="26"/>
     </row>
-    <row r="31" spans="4:45" ht="18">
+    <row r="31" spans="4:45" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2433,25 +2510,51 @@
       <c r="AB31" s="19">
         <v>1</v>
       </c>
-      <c r="AC31" s="19"/>
-      <c r="AD31" s="19"/>
-      <c r="AE31" s="19"/>
-      <c r="AF31" s="19"/>
-      <c r="AG31" s="19"/>
-      <c r="AH31" s="19"/>
-      <c r="AI31" s="22"/>
-      <c r="AJ31" s="22"/>
-      <c r="AK31" s="26"/>
-      <c r="AL31" s="26"/>
-      <c r="AM31" s="26"/>
-      <c r="AN31" s="26"/>
-      <c r="AO31" s="26"/>
+      <c r="AC31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO31" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="AP31" s="26"/>
       <c r="AQ31" s="26"/>
       <c r="AR31" s="26"/>
       <c r="AS31" s="26"/>
     </row>
-    <row r="32" spans="4:45" ht="18">
+    <row r="32" spans="4:45" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2557,7 +2660,7 @@
       <c r="AR32" s="26"/>
       <c r="AS32" s="26"/>
     </row>
-    <row r="33" spans="4:45" ht="18">
+    <row r="33" spans="4:45" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2663,7 +2766,7 @@
       <c r="AR33" s="26"/>
       <c r="AS33" s="26"/>
     </row>
-    <row r="34" spans="4:45" ht="18">
+    <row r="34" spans="4:45" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -2769,7 +2872,7 @@
       <c r="AR34" s="26"/>
       <c r="AS34" s="26"/>
     </row>
-    <row r="35" spans="4:45" ht="18">
+    <row r="35" spans="4:45" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2875,7 +2978,7 @@
       <c r="AR35" s="26"/>
       <c r="AS35" s="26"/>
     </row>
-    <row r="36" spans="4:45" ht="18">
+    <row r="36" spans="4:45" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2983,7 +3086,7 @@
       <c r="AR36" s="26"/>
       <c r="AS36" s="26"/>
     </row>
-    <row r="37" spans="4:45" ht="18">
+    <row r="37" spans="4:45" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -3091,7 +3194,7 @@
       <c r="AR37" s="26"/>
       <c r="AS37" s="26"/>
     </row>
-    <row r="38" spans="4:45" ht="18">
+    <row r="38" spans="4:45" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3199,7 +3302,7 @@
       <c r="AR38" s="26"/>
       <c r="AS38" s="26"/>
     </row>
-    <row r="39" spans="4:45" ht="18">
+    <row r="39" spans="4:45" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3307,7 +3410,7 @@
       <c r="AR39" s="26"/>
       <c r="AS39" s="26"/>
     </row>
-    <row r="40" spans="4:45" ht="18">
+    <row r="40" spans="4:45" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -3415,7 +3518,7 @@
       <c r="AR40" s="26"/>
       <c r="AS40" s="26"/>
     </row>
-    <row r="41" spans="4:45" ht="18">
+    <row r="41" spans="4:45" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -3523,7 +3626,7 @@
       <c r="AR41" s="26"/>
       <c r="AS41" s="26"/>
     </row>
-    <row r="42" spans="4:45" ht="18.600000000000001" thickBot="1">
+    <row r="42" spans="4:45" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -3631,7 +3734,7 @@
       <c r="AR42" s="26"/>
       <c r="AS42" s="26"/>
     </row>
-    <row r="43" spans="4:45" ht="18.600000000000001" thickBot="1">
+    <row r="43" spans="4:45" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -3761,7 +3864,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3773,7 +3876,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravani date:11/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="FebruaryMarch 2013" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -732,30 +731,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI38" workbookViewId="0">
-      <selection activeCell="AR44" sqref="AR44"/>
+    <sheetView tabSelected="1" topLeftCell="AI20" workbookViewId="0">
+      <selection activeCell="AS32" sqref="AS32:AS35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -770,7 +769,7 @@
       </c>
       <c r="E1" s="28"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -784,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -798,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -810,7 +809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -822,7 +821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -834,7 +833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -846,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -858,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -886,7 +885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -908,7 +907,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1168,7 +1167,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1279,7 +1278,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1390,7 +1389,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1501,7 +1500,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1586,7 +1585,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1671,7 +1670,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1756,7 +1755,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1841,7 +1840,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1938,7 +1937,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2035,7 +2034,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2134,7 +2133,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2233,7 +2232,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -2348,7 +2347,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2463,7 +2462,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2578,7 +2577,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2693,7 +2692,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2794,10 +2793,18 @@
       <c r="AO32" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP32" s="26"/>
-      <c r="AQ32" s="26"/>
-      <c r="AR32" s="26"/>
-      <c r="AS32" s="26"/>
+      <c r="AP32" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ32" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR32" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS32" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT32" s="26"/>
       <c r="AU32" s="26"/>
       <c r="AV32" s="26"/>
@@ -2806,7 +2813,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2907,10 +2914,18 @@
       <c r="AO33" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP33" s="26"/>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="26"/>
+      <c r="AP33" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ33" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR33" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS33" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT33" s="26"/>
       <c r="AU33" s="26"/>
       <c r="AV33" s="26"/>
@@ -2919,7 +2934,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3020,10 +3035,18 @@
       <c r="AO34" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP34" s="26"/>
-      <c r="AQ34" s="26"/>
-      <c r="AR34" s="26"/>
-      <c r="AS34" s="26"/>
+      <c r="AP34" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ34" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR34" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS34" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT34" s="26"/>
       <c r="AU34" s="26"/>
       <c r="AV34" s="26"/>
@@ -3032,7 +3055,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3133,10 +3156,18 @@
       <c r="AO35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP35" s="26"/>
-      <c r="AQ35" s="26"/>
-      <c r="AR35" s="26"/>
-      <c r="AS35" s="26"/>
+      <c r="AP35" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ35" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR35" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS35" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT35" s="26"/>
       <c r="AU35" s="26"/>
       <c r="AV35" s="26"/>
@@ -3145,7 +3176,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -3248,9 +3279,15 @@
       <c r="AO36" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP36" s="26"/>
-      <c r="AQ36" s="26"/>
-      <c r="AR36" s="26"/>
+      <c r="AP36" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ36" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR36" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AS36" s="26"/>
       <c r="AT36" s="26"/>
       <c r="AU36" s="26"/>
@@ -3260,7 +3297,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -3363,9 +3400,15 @@
       <c r="AO37" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP37" s="26"/>
-      <c r="AQ37" s="26"/>
-      <c r="AR37" s="26"/>
+      <c r="AP37" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ37" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR37" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AS37" s="26"/>
       <c r="AT37" s="26"/>
       <c r="AU37" s="26"/>
@@ -3375,7 +3418,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3478,9 +3521,15 @@
       <c r="AO38" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP38" s="26"/>
-      <c r="AQ38" s="26"/>
-      <c r="AR38" s="26"/>
+      <c r="AP38" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ38" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR38" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AS38" s="26"/>
       <c r="AT38" s="26"/>
       <c r="AU38" s="26"/>
@@ -3490,7 +3539,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3593,9 +3642,15 @@
       <c r="AO39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AP39" s="26"/>
-      <c r="AQ39" s="26"/>
-      <c r="AR39" s="26"/>
+      <c r="AP39" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ39" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR39" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AS39" s="26"/>
       <c r="AT39" s="26"/>
       <c r="AU39" s="26"/>
@@ -3605,7 +3660,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -3724,7 +3779,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -3843,7 +3898,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="42" spans="4:52" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -3962,7 +4017,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="43" spans="4:52" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -4103,7 +4158,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4115,7 +4170,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:11-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -732,7 +732,7 @@
   <dimension ref="A1:AZ44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AI20" workbookViewId="0">
-      <selection activeCell="AS32" sqref="AS32:AS35"/>
+      <selection activeCell="AS36" sqref="AS36:AS39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3288,7 +3288,9 @@
       <c r="AR36" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AS36" s="26"/>
+      <c r="AS36" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT36" s="26"/>
       <c r="AU36" s="26"/>
       <c r="AV36" s="26"/>
@@ -3409,7 +3411,9 @@
       <c r="AR37" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AS37" s="26"/>
+      <c r="AS37" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT37" s="26"/>
       <c r="AU37" s="26"/>
       <c r="AV37" s="26"/>
@@ -3530,7 +3534,9 @@
       <c r="AR38" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AS38" s="26"/>
+      <c r="AS38" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT38" s="26"/>
       <c r="AU38" s="26"/>
       <c r="AV38" s="26"/>
@@ -3651,7 +3657,9 @@
       <c r="AR39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AS39" s="26"/>
+      <c r="AS39" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AT39" s="26"/>
       <c r="AU39" s="26"/>
       <c r="AV39" s="26"/>

</xml_diff>

<commit_message>
updated by Alpna Date:11-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI20" workbookViewId="0">
-      <selection activeCell="AS36" sqref="AS36:AS39"/>
+    <sheetView tabSelected="1" topLeftCell="AI11" workbookViewId="0">
+      <selection activeCell="AS16" sqref="AS16:AS19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1155,10 +1155,18 @@
       <c r="AO16" s="26">
         <v>0</v>
       </c>
-      <c r="AP16" s="26"/>
-      <c r="AQ16" s="26"/>
-      <c r="AR16" s="26"/>
-      <c r="AS16" s="26"/>
+      <c r="AP16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="26">
+        <v>0</v>
+      </c>
       <c r="AT16" s="26"/>
       <c r="AU16" s="26"/>
       <c r="AV16" s="26"/>
@@ -1266,10 +1274,18 @@
       <c r="AO17" s="26">
         <v>0</v>
       </c>
-      <c r="AP17" s="26"/>
-      <c r="AQ17" s="26"/>
-      <c r="AR17" s="26"/>
-      <c r="AS17" s="26"/>
+      <c r="AP17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="26">
+        <v>0</v>
+      </c>
       <c r="AT17" s="26"/>
       <c r="AU17" s="26"/>
       <c r="AV17" s="26"/>
@@ -1377,10 +1393,18 @@
       <c r="AO18" s="26">
         <v>0</v>
       </c>
-      <c r="AP18" s="26"/>
-      <c r="AQ18" s="26"/>
-      <c r="AR18" s="26"/>
-      <c r="AS18" s="26"/>
+      <c r="AP18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="26">
+        <v>0</v>
+      </c>
       <c r="AT18" s="26"/>
       <c r="AU18" s="26"/>
       <c r="AV18" s="26"/>
@@ -1488,10 +1512,18 @@
       <c r="AO19" s="26">
         <v>0</v>
       </c>
-      <c r="AP19" s="26"/>
-      <c r="AQ19" s="26"/>
-      <c r="AR19" s="26"/>
-      <c r="AS19" s="26"/>
+      <c r="AP19" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="26">
+        <v>0</v>
+      </c>
       <c r="AT19" s="26"/>
       <c r="AU19" s="26"/>
       <c r="AV19" s="26"/>

</xml_diff>

<commit_message>
updated by sravani date:12-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -166,11 +166,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,7 +519,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -554,7 +553,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -730,14 +728,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI11" workbookViewId="0">
-      <selection activeCell="AT19" sqref="AT19"/>
+    <sheetView tabSelected="1" topLeftCell="AI17" workbookViewId="0">
+      <selection activeCell="AT32" sqref="AT32:AT35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -759,7 +757,7 @@
     <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -771,7 +769,7 @@
       </c>
       <c r="E1" s="28"/>
     </row>
-    <row r="2" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -785,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -799,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -811,7 +809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -823,7 +821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -835,7 +833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -847,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -859,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -871,7 +869,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -879,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -887,7 +885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -895,21 +893,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52">
       <c r="AN13" s="27"/>
       <c r="AO13" s="27"/>
       <c r="AP13" s="27"/>
       <c r="AQ13" s="27"/>
       <c r="AR13" s="27"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52">
       <c r="AN14" s="27"/>
       <c r="AO14" s="27"/>
       <c r="AP14" s="27"/>
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1058,7 +1056,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1179,7 +1177,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1300,7 +1298,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1421,7 +1419,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1542,7 +1540,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1627,7 +1625,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1712,7 +1710,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1797,7 +1795,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1882,7 +1880,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1979,7 +1977,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2076,7 +2074,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2175,7 +2173,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2274,7 +2272,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -2389,7 +2387,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2504,7 +2502,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2619,7 +2617,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2734,7 +2732,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2847,7 +2845,9 @@
       <c r="AS32" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT32" s="26"/>
+      <c r="AT32" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU32" s="26"/>
       <c r="AV32" s="26"/>
       <c r="AW32" s="26"/>
@@ -2855,7 +2855,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2968,7 +2968,9 @@
       <c r="AS33" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT33" s="26"/>
+      <c r="AT33" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU33" s="26"/>
       <c r="AV33" s="26"/>
       <c r="AW33" s="26"/>
@@ -2976,7 +2978,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3089,7 +3091,9 @@
       <c r="AS34" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT34" s="26"/>
+      <c r="AT34" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU34" s="26"/>
       <c r="AV34" s="26"/>
       <c r="AW34" s="26"/>
@@ -3097,7 +3101,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3210,7 +3214,9 @@
       <c r="AS35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT35" s="26"/>
+      <c r="AT35" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU35" s="26"/>
       <c r="AV35" s="26"/>
       <c r="AW35" s="26"/>
@@ -3218,7 +3224,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -3341,7 +3347,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -3464,7 +3470,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3587,7 +3593,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3710,7 +3716,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -3829,7 +3835,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -3948,7 +3954,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:52" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -4067,7 +4073,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:52" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -4186,7 +4192,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:52">
       <c r="AN44" s="27"/>
       <c r="AO44" s="27"/>
       <c r="AP44" s="27"/>
@@ -4203,24 +4209,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:12-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI17" workbookViewId="0">
-      <selection activeCell="AT32" sqref="AT32:AT35"/>
+    <sheetView tabSelected="1" topLeftCell="AI21" workbookViewId="0">
+      <selection activeCell="AT36" sqref="AT36:AT39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3339,7 +3339,9 @@
       <c r="AS36" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT36" s="26"/>
+      <c r="AT36" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU36" s="26"/>
       <c r="AV36" s="26"/>
       <c r="AW36" s="26"/>
@@ -3462,7 +3464,9 @@
       <c r="AS37" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT37" s="26"/>
+      <c r="AT37" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU37" s="26"/>
       <c r="AV37" s="26"/>
       <c r="AW37" s="26"/>
@@ -3585,7 +3589,9 @@
       <c r="AS38" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT38" s="26"/>
+      <c r="AT38" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU38" s="26"/>
       <c r="AV38" s="26"/>
       <c r="AW38" s="26"/>
@@ -3708,7 +3714,9 @@
       <c r="AS39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AT39" s="26"/>
+      <c r="AT39" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AU39" s="26"/>
       <c r="AV39" s="26"/>
       <c r="AW39" s="26"/>

</xml_diff>

<commit_message>
updated by sravani date:13/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="FebruaryMarch 2013" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -732,30 +731,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO35" workbookViewId="0">
-      <selection activeCell="AU44" sqref="AU44"/>
+    <sheetView tabSelected="1" topLeftCell="AO26" workbookViewId="0">
+      <selection activeCell="AU32" sqref="AU32:AU35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -770,7 +769,7 @@
       </c>
       <c r="E1" s="28"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -784,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -798,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -810,7 +809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -822,7 +821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -834,7 +833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -846,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -858,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -886,7 +885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -908,7 +907,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1178,7 +1177,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1299,7 +1298,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1420,7 +1419,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1541,7 +1540,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>38</v>
       </c>
@@ -1626,7 +1625,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1711,7 +1710,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1796,7 +1795,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1881,7 +1880,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>39</v>
       </c>
@@ -1988,7 +1987,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2095,7 +2094,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2204,7 +2203,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2313,7 +2312,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>40</v>
       </c>
@@ -2428,7 +2427,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2543,7 +2542,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2658,7 +2657,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2773,7 +2772,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2889,14 +2888,16 @@
       <c r="AT32" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU32" s="26"/>
+      <c r="AU32" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV32" s="26"/>
       <c r="AW32" s="26"/>
       <c r="AX32" s="26"/>
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3012,14 +3013,16 @@
       <c r="AT33" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU33" s="26"/>
+      <c r="AU33" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV33" s="26"/>
       <c r="AW33" s="26"/>
       <c r="AX33" s="26"/>
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3135,14 +3138,16 @@
       <c r="AT34" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU34" s="26"/>
+      <c r="AU34" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV34" s="26"/>
       <c r="AW34" s="26"/>
       <c r="AX34" s="26"/>
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3258,14 +3263,16 @@
       <c r="AT35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU35" s="26"/>
+      <c r="AU35" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV35" s="26"/>
       <c r="AW35" s="26"/>
       <c r="AX35" s="26"/>
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
@@ -3390,7 +3397,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
@@ -3515,7 +3522,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3640,7 +3647,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3765,7 +3772,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>44</v>
       </c>
@@ -3890,7 +3897,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>44</v>
       </c>
@@ -4015,7 +4022,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="42" spans="4:52" ht="18" thickBot="1">
       <c r="D42" s="12" t="s">
         <v>44</v>
       </c>
@@ -4140,7 +4147,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="43" spans="4:52" ht="18" thickBot="1">
       <c r="D43" s="12" t="s">
         <v>44</v>
       </c>
@@ -4287,7 +4294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4299,7 +4306,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by alpna date:13-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO26" workbookViewId="0">
-      <selection activeCell="AU32" sqref="AU32:AU35"/>
+    <sheetView tabSelected="1" topLeftCell="AO8" workbookViewId="0">
+      <selection activeCell="AU16" sqref="AU16:AU19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1170,7 +1170,9 @@
       <c r="AT16" s="26">
         <v>0</v>
       </c>
-      <c r="AU16" s="26"/>
+      <c r="AU16" s="26">
+        <v>0</v>
+      </c>
       <c r="AV16" s="26"/>
       <c r="AW16" s="26"/>
       <c r="AX16" s="26"/>
@@ -1291,7 +1293,9 @@
       <c r="AT17" s="26">
         <v>0</v>
       </c>
-      <c r="AU17" s="26"/>
+      <c r="AU17" s="26">
+        <v>0</v>
+      </c>
       <c r="AV17" s="26"/>
       <c r="AW17" s="26"/>
       <c r="AX17" s="26"/>
@@ -1412,7 +1416,9 @@
       <c r="AT18" s="26">
         <v>0</v>
       </c>
-      <c r="AU18" s="26"/>
+      <c r="AU18" s="26">
+        <v>0</v>
+      </c>
       <c r="AV18" s="26"/>
       <c r="AW18" s="26"/>
       <c r="AX18" s="26"/>
@@ -1533,7 +1539,9 @@
       <c r="AT19" s="26">
         <v>0</v>
       </c>
-      <c r="AU19" s="26"/>
+      <c r="AU19" s="26">
+        <v>0</v>
+      </c>
       <c r="AV19" s="26"/>
       <c r="AW19" s="26"/>
       <c r="AX19" s="26"/>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:13-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO8" workbookViewId="0">
-      <selection activeCell="AU16" sqref="AU16:AU19"/>
+    <sheetView tabSelected="1" topLeftCell="AO20" workbookViewId="0">
+      <selection activeCell="AU36" sqref="AU36:AU39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3398,7 +3398,9 @@
       <c r="AT36" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU36" s="26"/>
+      <c r="AU36" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV36" s="26"/>
       <c r="AW36" s="26"/>
       <c r="AX36" s="26"/>
@@ -3523,7 +3525,9 @@
       <c r="AT37" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU37" s="26"/>
+      <c r="AU37" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV37" s="26"/>
       <c r="AW37" s="26"/>
       <c r="AX37" s="26"/>
@@ -3648,7 +3652,9 @@
       <c r="AT38" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU38" s="26"/>
+      <c r="AU38" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV38" s="26"/>
       <c r="AW38" s="26"/>
       <c r="AX38" s="26"/>
@@ -3773,7 +3779,9 @@
       <c r="AT39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU39" s="26"/>
+      <c r="AU39" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AV39" s="26"/>
       <c r="AW39" s="26"/>
       <c r="AX39" s="26"/>

</xml_diff>

<commit_message>
updated by sravani date:14/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="FebruaryMarch 2013" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -730,32 +729,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ44"/>
+  <dimension ref="A1:AZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO35" workbookViewId="0">
-      <selection activeCell="AV44" sqref="AV44"/>
+    <sheetView tabSelected="1" topLeftCell="AK16" workbookViewId="0">
+      <selection activeCell="AV33" sqref="AV33:AV35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -770,7 +769,7 @@
       </c>
       <c r="E1" s="28"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -784,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -798,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -810,7 +809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -822,7 +821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -834,7 +833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -846,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -858,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -886,7 +885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -908,7 +907,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1174,13 +1173,15 @@
       <c r="AU16" s="26">
         <v>0</v>
       </c>
-      <c r="AV16" s="26"/>
+      <c r="AV16" s="26">
+        <v>0</v>
+      </c>
       <c r="AW16" s="26"/>
       <c r="AX16" s="26"/>
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1297,13 +1298,15 @@
       <c r="AU17" s="26">
         <v>0</v>
       </c>
-      <c r="AV17" s="26"/>
+      <c r="AV17" s="26">
+        <v>0</v>
+      </c>
       <c r="AW17" s="26"/>
       <c r="AX17" s="26"/>
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1420,13 +1423,15 @@
       <c r="AU18" s="26">
         <v>0</v>
       </c>
-      <c r="AV18" s="26"/>
+      <c r="AV18" s="26">
+        <v>0</v>
+      </c>
       <c r="AW18" s="26"/>
       <c r="AX18" s="26"/>
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1434,7 +1439,7 @@
         <v>27</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
@@ -1444,120 +1449,58 @@
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
-      <c r="O19" s="19">
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+      <c r="AG19" s="19"/>
+      <c r="AH19" s="19"/>
+      <c r="AI19" s="19"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="26"/>
+      <c r="AM19" s="26"/>
+      <c r="AN19" s="26"/>
+      <c r="AO19" s="26"/>
+      <c r="AP19" s="26"/>
+      <c r="AQ19" s="26"/>
+      <c r="AR19" s="26"/>
+      <c r="AS19" s="26"/>
+      <c r="AT19" s="26"/>
+      <c r="AU19" s="26">
         <v>1</v>
       </c>
-      <c r="P19" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="19">
-        <v>0</v>
-      </c>
-      <c r="R19" s="23">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S19" s="19">
-        <v>0</v>
-      </c>
-      <c r="T19" s="19">
-        <v>0</v>
-      </c>
-      <c r="U19" s="19">
+      <c r="AV19" s="26">
         <v>2</v>
       </c>
-      <c r="V19" s="19">
-        <v>0</v>
-      </c>
-      <c r="W19" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="X19" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="19">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AL19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AN19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AP19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AU19" s="26">
-        <v>0</v>
-      </c>
-      <c r="AV19" s="26"/>
       <c r="AW19" s="26"/>
       <c r="AX19" s="26"/>
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
@@ -1568,16 +1511,16 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="19">
         <v>0</v>
       </c>
-      <c r="R20" s="19">
-        <v>0</v>
+      <c r="R20" s="23">
+        <v>6.25E-2</v>
       </c>
       <c r="S20" s="19">
         <v>0</v>
@@ -1585,14 +1528,14 @@
       <c r="T20" s="19">
         <v>0</v>
       </c>
-      <c r="U20" s="20" t="s">
-        <v>43</v>
+      <c r="U20" s="19">
+        <v>2</v>
       </c>
       <c r="V20" s="19">
         <v>0</v>
       </c>
       <c r="W20" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X20" s="19">
         <v>0</v>
@@ -1600,41 +1543,81 @@
       <c r="Y20" s="19">
         <v>0</v>
       </c>
-      <c r="Z20" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="19">
+      <c r="Z20" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="20">
         <v>0</v>
       </c>
       <c r="AB20" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AF20" s="19"/>
-      <c r="AG20" s="19"/>
-      <c r="AH20" s="19"/>
-      <c r="AI20" s="22"/>
-      <c r="AJ20" s="22"/>
-      <c r="AK20" s="26"/>
-      <c r="AL20" s="26"/>
-      <c r="AM20" s="26"/>
-      <c r="AN20" s="26"/>
-      <c r="AO20" s="26"/>
-      <c r="AP20" s="26"/>
-      <c r="AQ20" s="26"/>
-      <c r="AR20" s="26"/>
-      <c r="AS20" s="26"/>
-      <c r="AT20" s="26"/>
-      <c r="AU20" s="26"/>
-      <c r="AV20" s="26"/>
+        <v>1</v>
+      </c>
+      <c r="AC20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="26">
+        <v>1</v>
+      </c>
       <c r="AW20" s="26"/>
       <c r="AX20" s="26"/>
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1642,7 +1625,7 @@
         <v>28</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
@@ -1653,13 +1636,13 @@
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P21" s="19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="R21" s="19">
         <v>0</v>
@@ -1683,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="19">
         <v>0</v>
@@ -1719,7 +1702,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1727,7 +1710,7 @@
         <v>28</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -1738,13 +1721,13 @@
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P22" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q22" s="19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R22" s="19">
         <v>0</v>
@@ -1759,16 +1742,16 @@
         <v>43</v>
       </c>
       <c r="V22" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" s="19">
+        <v>0</v>
+      </c>
+      <c r="X22" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="19">
         <v>2</v>
-      </c>
-      <c r="X22" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="19">
-        <v>0</v>
       </c>
       <c r="Z22" s="19">
         <v>0</v>
@@ -1804,7 +1787,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1812,7 +1795,7 @@
         <v>28</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -1822,32 +1805,32 @@
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="22">
+      <c r="O23" s="19">
+        <v>0</v>
+      </c>
+      <c r="P23" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="19">
+        <v>0</v>
+      </c>
+      <c r="R23" s="19">
+        <v>0</v>
+      </c>
+      <c r="S23" s="19">
+        <v>0</v>
+      </c>
+      <c r="T23" s="19">
+        <v>0</v>
+      </c>
+      <c r="U23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="V23" s="19">
         <v>1</v>
       </c>
-      <c r="P23" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="22">
-        <v>1</v>
-      </c>
-      <c r="R23" s="22">
-        <v>0</v>
-      </c>
-      <c r="S23" s="22">
-        <v>3</v>
-      </c>
-      <c r="T23" s="22">
-        <v>0</v>
-      </c>
-      <c r="U23" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="V23" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="W23" s="22">
-        <v>1</v>
+      <c r="W23" s="19">
+        <v>2</v>
       </c>
       <c r="X23" s="19">
         <v>0</v>
@@ -1859,10 +1842,10 @@
         <v>0</v>
       </c>
       <c r="AA23" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AB23" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC23" s="19"/>
       <c r="AD23" s="19"/>
@@ -1889,15 +1872,15 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
@@ -1907,24 +1890,32 @@
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19">
-        <v>0</v>
-      </c>
-      <c r="T24" s="19">
-        <v>0</v>
-      </c>
-      <c r="U24" s="19">
-        <v>0</v>
-      </c>
-      <c r="V24" s="19"/>
-      <c r="W24" s="19">
-        <v>0</v>
+      <c r="O24" s="22">
+        <v>1</v>
+      </c>
+      <c r="P24" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="22">
+        <v>1</v>
+      </c>
+      <c r="R24" s="22">
+        <v>0</v>
+      </c>
+      <c r="S24" s="22">
+        <v>3</v>
+      </c>
+      <c r="T24" s="22">
+        <v>0</v>
+      </c>
+      <c r="U24" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="V24" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="W24" s="22">
+        <v>1</v>
       </c>
       <c r="X24" s="19">
         <v>0</v>
@@ -1936,59 +1927,29 @@
         <v>0</v>
       </c>
       <c r="AA24" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="19">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="19">
-        <v>0</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="AB24" s="19">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
       <c r="AG24" s="19"/>
-      <c r="AH24" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="24">
-        <v>0</v>
-      </c>
+      <c r="AH24" s="19"/>
+      <c r="AI24" s="22"/>
       <c r="AJ24" s="22"/>
-      <c r="AK24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AN24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AO24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AP24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AQ24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AR24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS24" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT24" s="26">
-        <v>0</v>
-      </c>
+      <c r="AK24" s="26"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="26"/>
+      <c r="AN24" s="26"/>
+      <c r="AO24" s="26"/>
+      <c r="AP24" s="26"/>
+      <c r="AQ24" s="26"/>
+      <c r="AR24" s="26"/>
+      <c r="AS24" s="26"/>
+      <c r="AT24" s="26"/>
       <c r="AU24" s="26"/>
       <c r="AV24" s="26"/>
       <c r="AW24" s="26"/>
@@ -1996,7 +1957,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2004,7 +1965,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
@@ -2016,15 +1977,15 @@
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
       <c r="P25" s="19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="19"/>
       <c r="S25" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T25" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U25" s="19">
         <v>0</v>
@@ -2103,7 +2064,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2111,7 +2072,7 @@
         <v>29</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
@@ -2123,30 +2084,28 @@
       <c r="N26" s="19"/>
       <c r="O26" s="19"/>
       <c r="P26" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q26" s="19"/>
-      <c r="R26" s="19">
+      <c r="R26" s="19"/>
+      <c r="S26" s="19">
         <v>2</v>
       </c>
-      <c r="S26" s="19">
-        <v>0</v>
-      </c>
       <c r="T26" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26" s="19"/>
       <c r="W26" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="19">
         <v>0</v>
@@ -2212,7 +2171,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2220,7 +2179,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -2232,36 +2191,36 @@
       <c r="N27" s="19"/>
       <c r="O27" s="19"/>
       <c r="P27" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19">
+        <v>2</v>
+      </c>
+      <c r="S27" s="19">
+        <v>0</v>
+      </c>
+      <c r="T27" s="19">
+        <v>0</v>
+      </c>
+      <c r="U27" s="19">
         <v>1</v>
-      </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="23">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S27" s="19">
-        <v>0</v>
-      </c>
-      <c r="T27" s="19">
-        <v>0</v>
-      </c>
-      <c r="U27" s="19">
-        <v>2</v>
       </c>
       <c r="V27" s="19"/>
       <c r="W27" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X27" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y27" s="19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z27" s="19">
         <v>0</v>
       </c>
-      <c r="AA27" s="23">
-        <v>4.8611111111111112E-2</v>
+      <c r="AA27" s="19">
+        <v>0</v>
       </c>
       <c r="AB27" s="19"/>
       <c r="AC27" s="19">
@@ -2321,15 +2280,15 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
@@ -2337,83 +2296,67 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
       <c r="L28" s="19"/>
-      <c r="M28" s="19">
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="23">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S28" s="19">
+        <v>0</v>
+      </c>
+      <c r="T28" s="19">
+        <v>0</v>
+      </c>
+      <c r="U28" s="19">
         <v>2</v>
       </c>
-      <c r="N28" s="19">
-        <v>0</v>
-      </c>
-      <c r="O28" s="19">
-        <v>0</v>
-      </c>
-      <c r="P28" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R28" s="19">
-        <v>0</v>
-      </c>
-      <c r="S28" s="19">
-        <v>0</v>
-      </c>
-      <c r="T28" s="19">
-        <v>0</v>
-      </c>
-      <c r="U28" s="19">
-        <v>0</v>
-      </c>
-      <c r="V28" s="22">
-        <v>0</v>
-      </c>
+      <c r="V28" s="19"/>
       <c r="W28" s="19">
-        <v>0</v>
-      </c>
-      <c r="X28" s="20" t="s">
-        <v>43</v>
+        <v>0.5</v>
+      </c>
+      <c r="X28" s="19">
+        <v>0</v>
       </c>
       <c r="Y28" s="19">
         <v>0</v>
       </c>
-      <c r="Z28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA28" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL28" s="20" t="s">
-        <v>43</v>
+      <c r="Z28" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="23">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="24">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="26">
+        <v>0</v>
       </c>
       <c r="AM28" s="26">
         <v>0</v>
@@ -2421,34 +2364,32 @@
       <c r="AN28" s="26">
         <v>0</v>
       </c>
-      <c r="AO28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU28" s="20" t="s">
-        <v>43</v>
-      </c>
+      <c r="AO28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AP28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AU28" s="26"/>
       <c r="AV28" s="26"/>
       <c r="AW28" s="26"/>
       <c r="AX28" s="26"/>
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2456,7 +2397,7 @@
         <v>30</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
@@ -2465,16 +2406,16 @@
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
       <c r="M29" s="19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N29" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O29" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P29" s="19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="20" t="s">
         <v>43</v>
@@ -2483,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T29" s="19">
         <v>0</v>
@@ -2543,10 +2484,10 @@
         <v>43</v>
       </c>
       <c r="AM29" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN29" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO29" s="20" t="s">
         <v>43</v>
@@ -2575,7 +2516,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2583,7 +2524,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
@@ -2592,88 +2533,88 @@
       <c r="K30" s="19"/>
       <c r="L30" s="19"/>
       <c r="M30" s="19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N30" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O30" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P30" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q30" s="20" t="s">
         <v>43</v>
       </c>
       <c r="R30" s="19">
+        <v>0</v>
+      </c>
+      <c r="S30" s="19">
         <v>2</v>
       </c>
-      <c r="S30" s="19">
-        <v>0</v>
-      </c>
       <c r="T30" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U30" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V30" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W30" s="19">
+        <v>0</v>
+      </c>
+      <c r="X30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y30" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA30" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL30" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM30" s="26">
         <v>1</v>
       </c>
-      <c r="X30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y30" s="19">
-        <v>2</v>
-      </c>
-      <c r="Z30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA30" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB30" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM30" s="26">
-        <v>0</v>
-      </c>
       <c r="AN30" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO30" s="20" t="s">
         <v>43</v>
@@ -2702,7 +2643,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2710,7 +2651,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -2722,34 +2663,34 @@
         <v>0</v>
       </c>
       <c r="N31" s="19">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="O31" s="19">
+        <v>0</v>
+      </c>
+      <c r="P31" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="19">
+        <v>2</v>
+      </c>
+      <c r="S31" s="19">
+        <v>0</v>
+      </c>
+      <c r="T31" s="19">
+        <v>3</v>
+      </c>
+      <c r="U31" s="19">
+        <v>3</v>
+      </c>
+      <c r="V31" s="22">
+        <v>2</v>
+      </c>
+      <c r="W31" s="19">
         <v>1</v>
-      </c>
-      <c r="P31" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R31" s="19">
-        <v>1.3</v>
-      </c>
-      <c r="S31" s="19">
-        <v>0</v>
-      </c>
-      <c r="T31" s="19">
-        <v>1.4</v>
-      </c>
-      <c r="U31" s="19">
-        <v>2</v>
-      </c>
-      <c r="V31" s="22">
-        <v>0</v>
-      </c>
-      <c r="W31" s="19">
-        <v>0.5</v>
       </c>
       <c r="X31" s="20" t="s">
         <v>43</v>
@@ -2761,10 +2702,10 @@
         <v>43</v>
       </c>
       <c r="AA31" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AB31" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="20" t="s">
         <v>43</v>
@@ -2829,15 +2770,15 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
@@ -2845,51 +2786,53 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
+      <c r="M32" s="19">
+        <v>0</v>
+      </c>
       <c r="N32" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O32" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="R32" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="S32" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T32" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="U32" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="V32" s="20" t="s">
-        <v>46</v>
+      <c r="R32" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="S32" s="19">
+        <v>0</v>
+      </c>
+      <c r="T32" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="U32" s="19">
+        <v>2</v>
+      </c>
+      <c r="V32" s="22">
+        <v>0</v>
       </c>
       <c r="W32" s="19">
-        <v>0</v>
-      </c>
-      <c r="X32" s="19">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="X32" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y32" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z32" s="20" t="s">
         <v>43</v>
       </c>
       <c r="AA32" s="19">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AB32" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC32" s="20" t="s">
         <v>43</v>
@@ -2915,37 +2858,37 @@
       <c r="AJ32" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AK32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU32" s="26" t="s">
+      <c r="AK32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM32" s="26">
+        <v>0</v>
+      </c>
+      <c r="AN32" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU32" s="20" t="s">
         <v>43</v>
       </c>
       <c r="AV32" s="26"/>
@@ -2954,7 +2897,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -2962,7 +2905,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
@@ -2972,13 +2915,13 @@
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O33" s="19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P33" s="19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="20" t="s">
         <v>43</v>
@@ -3073,13 +3016,15 @@
       <c r="AU33" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV33" s="26"/>
+      <c r="AV33" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AW33" s="26"/>
       <c r="AX33" s="26"/>
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3087,7 +3032,7 @@
         <v>31</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
@@ -3097,13 +3042,13 @@
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
       <c r="N34" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O34" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P34" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q34" s="20" t="s">
         <v>43</v>
@@ -3124,10 +3069,10 @@
         <v>46</v>
       </c>
       <c r="W34" s="19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="X34" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y34" s="19">
         <v>0</v>
@@ -3198,13 +3143,15 @@
       <c r="AU34" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV34" s="26"/>
+      <c r="AV34" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AW34" s="26"/>
       <c r="AX34" s="26"/>
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3212,7 +3159,7 @@
         <v>31</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -3222,13 +3169,13 @@
       <c r="L35" s="19"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="O35" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="20" t="s">
         <v>43</v>
@@ -3249,22 +3196,22 @@
         <v>46</v>
       </c>
       <c r="W35" s="19">
-        <v>0.5</v>
+        <v>7</v>
       </c>
       <c r="X35" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y35" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="20" t="s">
         <v>43</v>
       </c>
       <c r="AA35" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AB35" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC35" s="20" t="s">
         <v>43</v>
@@ -3323,21 +3270,23 @@
       <c r="AU35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV35" s="26"/>
+      <c r="AV35" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AW35" s="26"/>
       <c r="AX35" s="26"/>
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
@@ -3345,126 +3294,60 @@
       <c r="J36" s="19"/>
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
-      <c r="M36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N36" s="19">
-        <v>0</v>
-      </c>
-      <c r="O36" s="19">
-        <v>0</v>
-      </c>
-      <c r="P36" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R36" s="19">
-        <v>0</v>
-      </c>
-      <c r="S36" s="19">
-        <v>0</v>
-      </c>
-      <c r="T36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U36" s="19">
-        <v>0</v>
-      </c>
-      <c r="V36" s="19">
-        <v>0</v>
-      </c>
-      <c r="W36" s="19">
-        <v>0</v>
-      </c>
-      <c r="X36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y36" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA36" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ36" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU36" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV36" s="26"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="19"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="19"/>
+      <c r="AB36" s="19"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="20"/>
+      <c r="AH36" s="20"/>
+      <c r="AI36" s="20"/>
+      <c r="AJ36" s="20"/>
+      <c r="AK36" s="26"/>
+      <c r="AL36" s="26"/>
+      <c r="AM36" s="26"/>
+      <c r="AN36" s="26"/>
+      <c r="AO36" s="26"/>
+      <c r="AP36" s="26"/>
+      <c r="AQ36" s="26"/>
+      <c r="AR36" s="26"/>
+      <c r="AS36" s="26"/>
+      <c r="AT36" s="26"/>
+      <c r="AU36" s="26">
+        <v>1</v>
+      </c>
+      <c r="AV36" s="26">
+        <v>2</v>
+      </c>
       <c r="AW36" s="26"/>
       <c r="AX36" s="26"/>
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
@@ -3472,53 +3355,51 @@
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
-      <c r="M37" s="20" t="s">
-        <v>43</v>
-      </c>
+      <c r="M37" s="19"/>
       <c r="N37" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="O37" s="19">
+        <v>1</v>
+      </c>
+      <c r="P37" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R37" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S37" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T37" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U37" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="V37" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="W37" s="19">
         <v>0.5</v>
       </c>
-      <c r="O37" s="19">
-        <v>9</v>
-      </c>
-      <c r="P37" s="19">
-        <v>7</v>
-      </c>
-      <c r="Q37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R37" s="19">
-        <v>0</v>
-      </c>
-      <c r="S37" s="19">
-        <v>0</v>
-      </c>
-      <c r="T37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U37" s="19">
-        <v>0</v>
-      </c>
-      <c r="V37" s="19">
-        <v>0</v>
-      </c>
-      <c r="W37" s="19">
-        <v>0</v>
-      </c>
-      <c r="X37" s="20" t="s">
-        <v>43</v>
+      <c r="X37" s="19">
+        <v>0</v>
       </c>
       <c r="Y37" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z37" s="20" t="s">
         <v>43</v>
       </c>
       <c r="AA37" s="19">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AB37" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC37" s="20" t="s">
         <v>43</v>
@@ -3577,13 +3458,15 @@
       <c r="AU37" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV37" s="26"/>
+      <c r="AV37" s="26">
+        <v>1</v>
+      </c>
       <c r="AW37" s="26"/>
       <c r="AX37" s="26"/>
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3591,7 +3474,7 @@
         <v>32</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
@@ -3603,7 +3486,7 @@
         <v>43</v>
       </c>
       <c r="N38" s="19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O38" s="19">
         <v>0</v>
@@ -3615,22 +3498,22 @@
         <v>43</v>
       </c>
       <c r="R38" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S38" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T38" s="20" t="s">
         <v>43</v>
       </c>
       <c r="U38" s="19">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V38" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W38" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X38" s="20" t="s">
         <v>43</v>
@@ -3710,7 +3593,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3718,7 +3601,7 @@
         <v>32</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
@@ -3730,19 +3613,19 @@
         <v>43</v>
       </c>
       <c r="N39" s="19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="O39" s="19">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="P39" s="19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q39" s="20" t="s">
         <v>43</v>
       </c>
       <c r="R39" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="S39" s="19">
         <v>0</v>
@@ -3757,22 +3640,22 @@
         <v>0</v>
       </c>
       <c r="W39" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X39" s="20" t="s">
         <v>43</v>
       </c>
       <c r="Y39" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z39" s="20" t="s">
         <v>43</v>
       </c>
       <c r="AA39" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AB39" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AC39" s="20" t="s">
         <v>43</v>
@@ -3837,15 +3720,15 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
@@ -3853,9 +3736,11 @@
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
+      <c r="M40" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="N40" s="19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O40" s="19">
         <v>0</v>
@@ -3863,29 +3748,29 @@
       <c r="P40" s="19">
         <v>0</v>
       </c>
-      <c r="Q40" s="19">
-        <v>0</v>
+      <c r="Q40" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="R40" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S40" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T40" s="20" t="s">
         <v>43</v>
       </c>
       <c r="U40" s="19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V40" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W40" s="19">
-        <v>0</v>
-      </c>
-      <c r="X40" s="19">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="X40" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y40" s="19">
         <v>0</v>
@@ -3893,8 +3778,8 @@
       <c r="Z40" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA40" s="20" t="s">
-        <v>43</v>
+      <c r="AA40" s="19">
+        <v>0</v>
       </c>
       <c r="AB40" s="19">
         <v>0</v>
@@ -3923,56 +3808,54 @@
       <c r="AJ40" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AK40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AO40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AP40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AQ40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AR40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AU40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AV40" s="26">
-        <v>0</v>
-      </c>
+      <c r="AK40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV40" s="26"/>
       <c r="AW40" s="26"/>
       <c r="AX40" s="26"/>
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
@@ -3980,126 +3863,60 @@
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
       <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19">
-        <v>10</v>
-      </c>
-      <c r="O41" s="19">
-        <v>6</v>
-      </c>
-      <c r="P41" s="19">
-        <v>7</v>
-      </c>
-      <c r="Q41" s="19">
-        <v>0</v>
-      </c>
-      <c r="R41" s="19">
-        <v>0</v>
-      </c>
-      <c r="S41" s="19">
-        <v>0</v>
-      </c>
-      <c r="T41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U41" s="19">
-        <v>0</v>
-      </c>
-      <c r="V41" s="19">
-        <v>0</v>
-      </c>
-      <c r="W41" s="19">
-        <v>0</v>
-      </c>
-      <c r="X41" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB41" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AO41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AP41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AQ41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AR41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT41" s="26">
-        <v>0</v>
-      </c>
+      <c r="M41" s="20"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="20"/>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="20"/>
+      <c r="AA41" s="19"/>
+      <c r="AB41" s="19"/>
+      <c r="AC41" s="20"/>
+      <c r="AD41" s="20"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="20"/>
+      <c r="AG41" s="20"/>
+      <c r="AH41" s="20"/>
+      <c r="AI41" s="20"/>
+      <c r="AJ41" s="20"/>
+      <c r="AK41" s="26"/>
+      <c r="AL41" s="26"/>
+      <c r="AM41" s="26"/>
+      <c r="AN41" s="26"/>
+      <c r="AO41" s="26"/>
+      <c r="AP41" s="26"/>
+      <c r="AQ41" s="26"/>
+      <c r="AR41" s="26"/>
+      <c r="AS41" s="26"/>
+      <c r="AT41" s="26"/>
       <c r="AU41" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV41" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW41" s="26"/>
       <c r="AX41" s="26"/>
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18.600000000000001" thickBot="1">
-      <c r="D42" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>33</v>
+    <row r="42" spans="4:52" ht="17.25">
+      <c r="D42" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
@@ -4107,21 +3924,23 @@
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
+      <c r="M42" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="N42" s="19">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="O42" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P42" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q42" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="R42" s="19">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S42" s="19">
         <v>0</v>
@@ -4130,28 +3949,28 @@
         <v>43</v>
       </c>
       <c r="U42" s="19">
+        <v>0</v>
+      </c>
+      <c r="V42" s="19">
+        <v>0</v>
+      </c>
+      <c r="W42" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="X42" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y42" s="19">
         <v>1</v>
       </c>
-      <c r="V42" s="19">
-        <v>2</v>
-      </c>
-      <c r="W42" s="19">
-        <v>7</v>
-      </c>
-      <c r="X42" s="19">
-        <v>7</v>
-      </c>
-      <c r="Y42" s="19">
-        <v>3</v>
-      </c>
       <c r="Z42" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AA42" s="20" t="s">
-        <v>43</v>
+      <c r="AA42" s="19">
+        <v>1.5</v>
       </c>
       <c r="AB42" s="19">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AC42" s="20" t="s">
         <v>43</v>
@@ -4177,99 +3996,99 @@
       <c r="AJ42" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AK42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AO42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AP42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AQ42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AR42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AU42" s="26">
-        <v>0</v>
+      <c r="AK42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU42" s="26" t="s">
+        <v>43</v>
       </c>
       <c r="AV42" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW42" s="26"/>
       <c r="AX42" s="26"/>
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18.600000000000001" thickBot="1">
-      <c r="D43" s="12" t="s">
+    <row r="43" spans="4:52" ht="17.25">
+      <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="18" t="s">
         <v>33</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22">
-        <v>1</v>
-      </c>
-      <c r="O43" s="22">
-        <v>1</v>
-      </c>
-      <c r="P43" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="22">
-        <v>0</v>
-      </c>
-      <c r="R43" s="22">
-        <v>3</v>
-      </c>
-      <c r="S43" s="22">
+        <v>4</v>
+      </c>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19">
+        <v>0</v>
+      </c>
+      <c r="O43" s="19">
+        <v>0</v>
+      </c>
+      <c r="P43" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="19">
+        <v>0</v>
+      </c>
+      <c r="R43" s="19">
+        <v>0</v>
+      </c>
+      <c r="S43" s="19">
         <v>0</v>
       </c>
       <c r="T43" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U43" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="V43" s="22">
-        <v>1</v>
-      </c>
-      <c r="W43" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="X43" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="22">
-        <v>1</v>
+      <c r="U43" s="19">
+        <v>0</v>
+      </c>
+      <c r="V43" s="19">
+        <v>0</v>
+      </c>
+      <c r="W43" s="19">
+        <v>0</v>
+      </c>
+      <c r="X43" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="19">
+        <v>0</v>
       </c>
       <c r="Z43" s="20" t="s">
         <v>43</v>
@@ -4277,8 +4096,8 @@
       <c r="AA43" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="AB43" s="22">
-        <v>2</v>
+      <c r="AB43" s="19">
+        <v>0</v>
       </c>
       <c r="AC43" s="20" t="s">
         <v>43</v>
@@ -4345,12 +4164,393 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52">
-      <c r="AN44" s="27"/>
-      <c r="AO44" s="27"/>
-      <c r="AP44" s="27"/>
-      <c r="AQ44" s="27"/>
-      <c r="AR44" s="27"/>
+    <row r="44" spans="4:52" ht="17.25">
+      <c r="D44" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19">
+        <v>10</v>
+      </c>
+      <c r="O44" s="19">
+        <v>6</v>
+      </c>
+      <c r="P44" s="19">
+        <v>7</v>
+      </c>
+      <c r="Q44" s="19">
+        <v>0</v>
+      </c>
+      <c r="R44" s="19">
+        <v>0</v>
+      </c>
+      <c r="S44" s="19">
+        <v>0</v>
+      </c>
+      <c r="T44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U44" s="19">
+        <v>0</v>
+      </c>
+      <c r="V44" s="19">
+        <v>0</v>
+      </c>
+      <c r="W44" s="19">
+        <v>0</v>
+      </c>
+      <c r="X44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB44" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AP44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AU44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AV44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AW44" s="26"/>
+      <c r="AX44" s="26"/>
+      <c r="AY44" s="26"/>
+      <c r="AZ44" s="26"/>
+    </row>
+    <row r="45" spans="4:52" ht="18" thickBot="1">
+      <c r="D45" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19">
+        <v>0</v>
+      </c>
+      <c r="O45" s="19">
+        <v>0</v>
+      </c>
+      <c r="P45" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="19">
+        <v>0</v>
+      </c>
+      <c r="R45" s="19">
+        <v>0</v>
+      </c>
+      <c r="S45" s="19">
+        <v>0</v>
+      </c>
+      <c r="T45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U45" s="19">
+        <v>1</v>
+      </c>
+      <c r="V45" s="19">
+        <v>2</v>
+      </c>
+      <c r="W45" s="19">
+        <v>7</v>
+      </c>
+      <c r="X45" s="19">
+        <v>7</v>
+      </c>
+      <c r="Y45" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB45" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AP45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AU45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AV45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AW45" s="26"/>
+      <c r="AX45" s="26"/>
+      <c r="AY45" s="26"/>
+      <c r="AZ45" s="26"/>
+    </row>
+    <row r="46" spans="4:52" ht="18" thickBot="1">
+      <c r="D46" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22">
+        <v>1</v>
+      </c>
+      <c r="O46" s="22">
+        <v>1</v>
+      </c>
+      <c r="P46" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="22">
+        <v>0</v>
+      </c>
+      <c r="R46" s="22">
+        <v>3</v>
+      </c>
+      <c r="S46" s="22">
+        <v>0</v>
+      </c>
+      <c r="T46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U46" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="V46" s="22">
+        <v>1</v>
+      </c>
+      <c r="W46" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="X46" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB46" s="22">
+        <v>2</v>
+      </c>
+      <c r="AC46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AO46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AP46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AQ46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AR46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AU46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AV46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AW46" s="26"/>
+      <c r="AX46" s="26"/>
+      <c r="AY46" s="26"/>
+      <c r="AZ46" s="26"/>
+    </row>
+    <row r="47" spans="4:52">
+      <c r="AN47" s="27"/>
+      <c r="AO47" s="27"/>
+      <c r="AP47" s="27"/>
+      <c r="AQ47" s="27"/>
+      <c r="AR47" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4367,7 +4567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4379,7 +4579,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:14-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK16" workbookViewId="0">
-      <selection activeCell="AV33" sqref="AV33:AV35"/>
+    <sheetView tabSelected="1" topLeftCell="AK25" workbookViewId="0">
+      <selection activeCell="AV38" sqref="AV38:AV40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3587,7 +3587,9 @@
       <c r="AU38" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV38" s="26"/>
+      <c r="AV38" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AW38" s="26"/>
       <c r="AX38" s="26"/>
       <c r="AY38" s="26"/>
@@ -3714,7 +3716,9 @@
       <c r="AU39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV39" s="26"/>
+      <c r="AV39" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AW39" s="26"/>
       <c r="AX39" s="26"/>
       <c r="AY39" s="26"/>
@@ -3841,7 +3845,9 @@
       <c r="AU40" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AV40" s="26"/>
+      <c r="AV40" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="AW40" s="26"/>
       <c r="AX40" s="26"/>
       <c r="AY40" s="26"/>

</xml_diff>

<commit_message>
updated by alpna date:14-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK25" workbookViewId="0">
-      <selection activeCell="AV38" sqref="AV38:AV40"/>
+    <sheetView tabSelected="1" topLeftCell="AK13" workbookViewId="0">
+      <selection activeCell="AV21" sqref="AV21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date:15-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FebruaryMarch 2013" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="February 2013" sheetId="1" r:id="rId1"/>
+    <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="47">
   <si>
     <t>Activity Code</t>
   </si>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK13" workbookViewId="0">
-      <selection activeCell="AV21" sqref="AV21"/>
+    <sheetView topLeftCell="AJ27" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4569,12 +4569,2401 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I40" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="28"/>
+    </row>
+    <row r="2" spans="1:24" ht="17.25">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="17.25">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="28.5">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="71.25">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="17.25">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="17.25">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="17.25">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="17.25">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="42.75">
+      <c r="A12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+    </row>
+    <row r="15" spans="1:24" ht="30">
+      <c r="D15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="17">
+        <v>40969</v>
+      </c>
+      <c r="H15" s="17">
+        <v>40970</v>
+      </c>
+      <c r="I15" s="25">
+        <v>40971</v>
+      </c>
+      <c r="J15" s="25">
+        <v>40972</v>
+      </c>
+      <c r="K15" s="25">
+        <v>40973</v>
+      </c>
+      <c r="L15" s="25">
+        <v>40974</v>
+      </c>
+      <c r="M15" s="25">
+        <v>40975</v>
+      </c>
+      <c r="N15" s="25">
+        <v>40976</v>
+      </c>
+      <c r="O15" s="25">
+        <v>40977</v>
+      </c>
+      <c r="P15" s="25">
+        <v>40978</v>
+      </c>
+      <c r="Q15" s="25">
+        <v>40979</v>
+      </c>
+      <c r="R15" s="25">
+        <v>40980</v>
+      </c>
+      <c r="S15" s="25">
+        <v>40981</v>
+      </c>
+      <c r="T15" s="25">
+        <v>40982</v>
+      </c>
+      <c r="U15" s="25">
+        <v>40983</v>
+      </c>
+      <c r="V15" s="25">
+        <v>40984</v>
+      </c>
+      <c r="W15" s="25">
+        <v>40985</v>
+      </c>
+      <c r="X15" s="25">
+        <v>40986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="17.25">
+      <c r="D16" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0</v>
+      </c>
+      <c r="I16" s="26">
+        <v>0</v>
+      </c>
+      <c r="J16" s="26">
+        <v>0</v>
+      </c>
+      <c r="K16" s="26">
+        <v>0</v>
+      </c>
+      <c r="L16" s="26">
+        <v>0</v>
+      </c>
+      <c r="M16" s="26">
+        <v>0</v>
+      </c>
+      <c r="N16" s="26">
+        <v>0</v>
+      </c>
+      <c r="O16" s="26">
+        <v>0</v>
+      </c>
+      <c r="P16" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="26">
+        <v>0</v>
+      </c>
+      <c r="R16" s="26">
+        <v>0</v>
+      </c>
+      <c r="S16" s="26">
+        <v>0</v>
+      </c>
+      <c r="T16" s="26">
+        <v>0</v>
+      </c>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+    </row>
+    <row r="17" spans="4:24" ht="17.25">
+      <c r="D17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+      <c r="H17" s="19">
+        <v>0</v>
+      </c>
+      <c r="I17" s="26">
+        <v>0</v>
+      </c>
+      <c r="J17" s="26">
+        <v>0</v>
+      </c>
+      <c r="K17" s="26">
+        <v>0</v>
+      </c>
+      <c r="L17" s="26">
+        <v>0</v>
+      </c>
+      <c r="M17" s="26">
+        <v>0</v>
+      </c>
+      <c r="N17" s="26">
+        <v>0</v>
+      </c>
+      <c r="O17" s="26">
+        <v>0</v>
+      </c>
+      <c r="P17" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="26">
+        <v>0</v>
+      </c>
+      <c r="R17" s="26">
+        <v>0</v>
+      </c>
+      <c r="S17" s="26">
+        <v>0</v>
+      </c>
+      <c r="T17" s="26">
+        <v>0</v>
+      </c>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+    </row>
+    <row r="18" spans="4:24" ht="17.25">
+      <c r="D18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="19">
+        <v>0</v>
+      </c>
+      <c r="H18" s="19">
+        <v>0</v>
+      </c>
+      <c r="I18" s="26">
+        <v>0</v>
+      </c>
+      <c r="J18" s="26">
+        <v>0</v>
+      </c>
+      <c r="K18" s="26">
+        <v>2</v>
+      </c>
+      <c r="L18" s="26">
+        <v>2</v>
+      </c>
+      <c r="M18" s="26">
+        <v>0</v>
+      </c>
+      <c r="N18" s="26">
+        <v>0</v>
+      </c>
+      <c r="O18" s="26">
+        <v>0</v>
+      </c>
+      <c r="P18" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>0</v>
+      </c>
+      <c r="R18" s="26">
+        <v>0</v>
+      </c>
+      <c r="S18" s="26">
+        <v>0</v>
+      </c>
+      <c r="T18" s="26">
+        <v>0</v>
+      </c>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+    </row>
+    <row r="19" spans="4:24" ht="17.25">
+      <c r="D19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26">
+        <v>1</v>
+      </c>
+      <c r="T19" s="26">
+        <v>2</v>
+      </c>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+    </row>
+    <row r="20" spans="4:24" ht="17.25">
+      <c r="D20" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26">
+        <v>0</v>
+      </c>
+      <c r="T20" s="26">
+        <v>0</v>
+      </c>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+    </row>
+    <row r="21" spans="4:24" ht="17.25">
+      <c r="D21" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="19">
+        <v>0</v>
+      </c>
+      <c r="H21" s="19">
+        <v>0</v>
+      </c>
+      <c r="I21" s="26">
+        <v>0</v>
+      </c>
+      <c r="J21" s="26">
+        <v>0</v>
+      </c>
+      <c r="K21" s="26">
+        <v>0</v>
+      </c>
+      <c r="L21" s="26">
+        <v>0</v>
+      </c>
+      <c r="M21" s="26">
+        <v>0</v>
+      </c>
+      <c r="N21" s="26">
+        <v>0</v>
+      </c>
+      <c r="O21" s="26">
+        <v>0</v>
+      </c>
+      <c r="P21" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>0</v>
+      </c>
+      <c r="R21" s="26">
+        <v>0</v>
+      </c>
+      <c r="S21" s="26">
+        <v>0</v>
+      </c>
+      <c r="T21" s="26">
+        <v>1</v>
+      </c>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+    </row>
+    <row r="22" spans="4:24" ht="17.25">
+      <c r="D22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+    </row>
+    <row r="23" spans="4:24" ht="17.25">
+      <c r="D23" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+    </row>
+    <row r="24" spans="4:24" ht="17.25">
+      <c r="D24" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+    </row>
+    <row r="25" spans="4:24" ht="17.25">
+      <c r="D25" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+    </row>
+    <row r="26" spans="4:24" ht="17.25">
+      <c r="D26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+    </row>
+    <row r="27" spans="4:24" ht="17.25">
+      <c r="D27" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+    </row>
+    <row r="28" spans="4:24" ht="17.25">
+      <c r="D28" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0</v>
+      </c>
+      <c r="H28" s="22"/>
+      <c r="I28" s="26">
+        <v>0</v>
+      </c>
+      <c r="J28" s="26">
+        <v>0</v>
+      </c>
+      <c r="K28" s="26">
+        <v>0</v>
+      </c>
+      <c r="L28" s="26">
+        <v>0</v>
+      </c>
+      <c r="M28" s="26">
+        <v>0</v>
+      </c>
+      <c r="N28" s="26">
+        <v>0</v>
+      </c>
+      <c r="O28" s="26">
+        <v>0</v>
+      </c>
+      <c r="P28" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="26">
+        <v>0</v>
+      </c>
+      <c r="R28" s="26">
+        <v>0</v>
+      </c>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+    </row>
+    <row r="29" spans="4:24" ht="17.25">
+      <c r="D29" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="24">
+        <v>0</v>
+      </c>
+      <c r="H29" s="22"/>
+      <c r="I29" s="26">
+        <v>0</v>
+      </c>
+      <c r="J29" s="26">
+        <v>0</v>
+      </c>
+      <c r="K29" s="26">
+        <v>0</v>
+      </c>
+      <c r="L29" s="26">
+        <v>0</v>
+      </c>
+      <c r="M29" s="26">
+        <v>0</v>
+      </c>
+      <c r="N29" s="26">
+        <v>0</v>
+      </c>
+      <c r="O29" s="26">
+        <v>0</v>
+      </c>
+      <c r="P29" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="26">
+        <v>0</v>
+      </c>
+      <c r="R29" s="26">
+        <v>0</v>
+      </c>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+    </row>
+    <row r="30" spans="4:24" ht="17.25">
+      <c r="D30" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="24">
+        <v>0</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="26">
+        <v>0</v>
+      </c>
+      <c r="J30" s="26">
+        <v>0</v>
+      </c>
+      <c r="K30" s="26">
+        <v>0</v>
+      </c>
+      <c r="L30" s="26">
+        <v>0</v>
+      </c>
+      <c r="M30" s="26">
+        <v>0</v>
+      </c>
+      <c r="N30" s="26">
+        <v>0</v>
+      </c>
+      <c r="O30" s="26">
+        <v>0</v>
+      </c>
+      <c r="P30" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="26">
+        <v>0</v>
+      </c>
+      <c r="R30" s="26">
+        <v>0</v>
+      </c>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+    </row>
+    <row r="31" spans="4:24" ht="17.25">
+      <c r="D31" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="24">
+        <v>0</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="26">
+        <v>0</v>
+      </c>
+      <c r="J31" s="26">
+        <v>0</v>
+      </c>
+      <c r="K31" s="26">
+        <v>0</v>
+      </c>
+      <c r="L31" s="26">
+        <v>0</v>
+      </c>
+      <c r="M31" s="26">
+        <v>0</v>
+      </c>
+      <c r="N31" s="26">
+        <v>0</v>
+      </c>
+      <c r="O31" s="26">
+        <v>0</v>
+      </c>
+      <c r="P31" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="26">
+        <v>0</v>
+      </c>
+      <c r="R31" s="26">
+        <v>0</v>
+      </c>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+    </row>
+    <row r="32" spans="4:24" ht="17.25">
+      <c r="D32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="I32" s="26">
+        <v>0</v>
+      </c>
+      <c r="J32" s="26">
+        <v>0</v>
+      </c>
+      <c r="K32" s="26">
+        <v>0</v>
+      </c>
+      <c r="L32" s="26">
+        <v>0</v>
+      </c>
+      <c r="M32" s="26">
+        <v>0</v>
+      </c>
+      <c r="N32" s="26">
+        <v>0</v>
+      </c>
+      <c r="O32" s="26">
+        <v>0</v>
+      </c>
+      <c r="P32" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="26">
+        <v>0</v>
+      </c>
+      <c r="R32" s="26">
+        <v>0</v>
+      </c>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+    </row>
+    <row r="33" spans="4:24" ht="17.25">
+      <c r="D33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="24">
+        <v>0</v>
+      </c>
+      <c r="H33" s="22"/>
+      <c r="I33" s="26">
+        <v>0</v>
+      </c>
+      <c r="J33" s="26">
+        <v>0</v>
+      </c>
+      <c r="K33" s="26">
+        <v>0</v>
+      </c>
+      <c r="L33" s="26">
+        <v>0</v>
+      </c>
+      <c r="M33" s="26">
+        <v>0</v>
+      </c>
+      <c r="N33" s="26">
+        <v>0</v>
+      </c>
+      <c r="O33" s="26">
+        <v>0</v>
+      </c>
+      <c r="P33" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="26">
+        <v>0</v>
+      </c>
+      <c r="R33" s="26">
+        <v>0</v>
+      </c>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+    </row>
+    <row r="34" spans="4:24" ht="17.25">
+      <c r="D34" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K34" s="26">
+        <v>0</v>
+      </c>
+      <c r="L34" s="26">
+        <v>0</v>
+      </c>
+      <c r="M34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="S34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+    </row>
+    <row r="35" spans="4:24" ht="17.25">
+      <c r="D35" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="26">
+        <v>1</v>
+      </c>
+      <c r="L35" s="26">
+        <v>1</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="S35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
+    </row>
+    <row r="36" spans="4:24" ht="17.25">
+      <c r="D36" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" s="26">
+        <v>0</v>
+      </c>
+      <c r="L36" s="26">
+        <v>0</v>
+      </c>
+      <c r="M36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="S36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
+    </row>
+    <row r="37" spans="4:24" ht="17.25">
+      <c r="D37" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" s="26">
+        <v>1</v>
+      </c>
+      <c r="L37" s="26">
+        <v>1</v>
+      </c>
+      <c r="M37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="S37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+    </row>
+    <row r="38" spans="4:24" ht="17.25">
+      <c r="D38" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K38" s="26">
+        <v>0</v>
+      </c>
+      <c r="L38" s="26">
+        <v>0</v>
+      </c>
+      <c r="M38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="S38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+    </row>
+    <row r="39" spans="4:24" ht="17.25">
+      <c r="D39" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" s="26">
+        <v>0</v>
+      </c>
+      <c r="L39" s="26">
+        <v>0</v>
+      </c>
+      <c r="M39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="O39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="S39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+    </row>
+    <row r="40" spans="4:24" ht="17.25">
+      <c r="D40" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T40" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+    </row>
+    <row r="41" spans="4:24" ht="17.25">
+      <c r="D41" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T41" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+    </row>
+    <row r="42" spans="4:24" ht="17.25">
+      <c r="D42" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T42" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U42" s="26"/>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+    </row>
+    <row r="43" spans="4:24" ht="17.25">
+      <c r="D43" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R43" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S43" s="26">
+        <v>1</v>
+      </c>
+      <c r="T43" s="26">
+        <v>2</v>
+      </c>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+    </row>
+    <row r="44" spans="4:24" ht="17.25">
+      <c r="D44" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R44" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S44" s="26">
+        <v>0</v>
+      </c>
+      <c r="T44" s="26">
+        <v>0</v>
+      </c>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
+    </row>
+    <row r="45" spans="4:24" ht="17.25">
+      <c r="D45" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H45" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S45" s="26">
+        <v>0</v>
+      </c>
+      <c r="T45" s="26">
+        <v>1</v>
+      </c>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
+    </row>
+    <row r="46" spans="4:24" ht="17.25">
+      <c r="D46" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R46" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S46" s="26">
+        <v>0</v>
+      </c>
+      <c r="T46" s="26">
+        <v>0</v>
+      </c>
+      <c r="U46" s="26">
+        <v>0</v>
+      </c>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
+    </row>
+    <row r="47" spans="4:24" ht="17.25">
+      <c r="D47" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S47" s="26">
+        <v>0</v>
+      </c>
+      <c r="T47" s="26">
+        <v>0</v>
+      </c>
+      <c r="U47" s="26">
+        <v>0</v>
+      </c>
+      <c r="V47" s="26"/>
+      <c r="W47" s="26"/>
+      <c r="X47" s="26"/>
+    </row>
+    <row r="48" spans="4:24" ht="17.25">
+      <c r="D48" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R48" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S48" s="26">
+        <v>0</v>
+      </c>
+      <c r="T48" s="26">
+        <v>0</v>
+      </c>
+      <c r="U48" s="26">
+        <v>0</v>
+      </c>
+      <c r="V48" s="26"/>
+      <c r="W48" s="26"/>
+      <c r="X48" s="26"/>
+    </row>
+    <row r="49" spans="4:24" ht="17.25">
+      <c r="D49" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S49" s="26">
+        <v>1</v>
+      </c>
+      <c r="T49" s="26">
+        <v>2</v>
+      </c>
+      <c r="U49" s="26">
+        <v>2</v>
+      </c>
+      <c r="V49" s="26"/>
+      <c r="W49" s="26"/>
+      <c r="X49" s="26"/>
+    </row>
+    <row r="50" spans="4:24" ht="17.25">
+      <c r="D50" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R50" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S50" s="26">
+        <v>0</v>
+      </c>
+      <c r="T50" s="26">
+        <v>0</v>
+      </c>
+      <c r="U50" s="26">
+        <v>0</v>
+      </c>
+      <c r="V50" s="26"/>
+      <c r="W50" s="26"/>
+      <c r="X50" s="26"/>
+    </row>
+    <row r="51" spans="4:24" ht="17.25">
+      <c r="D51" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="R51" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S51" s="26">
+        <v>0</v>
+      </c>
+      <c r="T51" s="26">
+        <v>1</v>
+      </c>
+      <c r="U51" s="26">
+        <v>0</v>
+      </c>
+      <c r="V51" s="26"/>
+      <c r="W51" s="26"/>
+      <c r="X51" s="26"/>
+    </row>
+    <row r="52" spans="4:24" ht="17.25">
+      <c r="D52" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H52" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I52" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K52" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L52" s="26">
+        <v>0</v>
+      </c>
+      <c r="M52" s="26">
+        <v>0</v>
+      </c>
+      <c r="N52" s="26">
+        <v>0</v>
+      </c>
+      <c r="O52" s="26">
+        <v>0</v>
+      </c>
+      <c r="P52" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="26">
+        <v>0</v>
+      </c>
+      <c r="R52" s="26">
+        <v>0</v>
+      </c>
+      <c r="S52" s="26">
+        <v>0</v>
+      </c>
+      <c r="T52" s="26">
+        <v>0</v>
+      </c>
+      <c r="U52" s="26"/>
+      <c r="V52" s="26"/>
+      <c r="W52" s="26"/>
+      <c r="X52" s="26"/>
+    </row>
+    <row r="53" spans="4:24" ht="17.25">
+      <c r="D53" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H53" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I53" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J53" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L53" s="26">
+        <v>0</v>
+      </c>
+      <c r="M53" s="26">
+        <v>0</v>
+      </c>
+      <c r="N53" s="26">
+        <v>0</v>
+      </c>
+      <c r="O53" s="26">
+        <v>0</v>
+      </c>
+      <c r="P53" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="26">
+        <v>0</v>
+      </c>
+      <c r="R53" s="26">
+        <v>0</v>
+      </c>
+      <c r="S53" s="26">
+        <v>0</v>
+      </c>
+      <c r="T53" s="26">
+        <v>0</v>
+      </c>
+      <c r="U53" s="26"/>
+      <c r="V53" s="26"/>
+      <c r="W53" s="26"/>
+      <c r="X53" s="26"/>
+    </row>
+    <row r="54" spans="4:24" ht="18" thickBot="1">
+      <c r="D54" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H54" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I54" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J54" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K54" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L54" s="26">
+        <v>0</v>
+      </c>
+      <c r="M54" s="26">
+        <v>0</v>
+      </c>
+      <c r="N54" s="26">
+        <v>0</v>
+      </c>
+      <c r="O54" s="26">
+        <v>0</v>
+      </c>
+      <c r="P54" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="26">
+        <v>0</v>
+      </c>
+      <c r="R54" s="26">
+        <v>0</v>
+      </c>
+      <c r="S54" s="26">
+        <v>0</v>
+      </c>
+      <c r="T54" s="26">
+        <v>0</v>
+      </c>
+      <c r="U54" s="26"/>
+      <c r="V54" s="26"/>
+      <c r="W54" s="26"/>
+      <c r="X54" s="26"/>
+    </row>
+    <row r="55" spans="4:24" ht="17.25">
+      <c r="D55" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I55" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K55" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L55" s="26">
+        <v>0</v>
+      </c>
+      <c r="M55" s="26">
+        <v>0</v>
+      </c>
+      <c r="N55" s="26">
+        <v>0</v>
+      </c>
+      <c r="O55" s="26">
+        <v>0</v>
+      </c>
+      <c r="P55" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="26">
+        <v>0</v>
+      </c>
+      <c r="R55" s="26">
+        <v>0</v>
+      </c>
+      <c r="S55" s="26">
+        <v>0</v>
+      </c>
+      <c r="T55" s="26">
+        <v>0</v>
+      </c>
+      <c r="U55" s="26"/>
+      <c r="V55" s="26"/>
+      <c r="W55" s="26"/>
+      <c r="X55" s="26"/>
+    </row>
+    <row r="56" spans="4:24" ht="18" thickBot="1">
+      <c r="D56" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H56" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I56" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J56" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K56" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L56" s="26">
+        <v>0</v>
+      </c>
+      <c r="M56" s="26">
+        <v>0</v>
+      </c>
+      <c r="N56" s="26">
+        <v>0</v>
+      </c>
+      <c r="O56" s="26">
+        <v>0</v>
+      </c>
+      <c r="P56" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="26">
+        <v>0</v>
+      </c>
+      <c r="R56" s="26">
+        <v>0</v>
+      </c>
+      <c r="S56" s="26">
+        <v>0</v>
+      </c>
+      <c r="T56" s="26">
+        <v>0</v>
+      </c>
+      <c r="U56" s="26"/>
+      <c r="V56" s="26"/>
+      <c r="W56" s="26"/>
+      <c r="X56" s="26"/>
+    </row>
+    <row r="57" spans="4:24" ht="18" thickBot="1">
+      <c r="D57" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J57" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K57" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L57" s="26">
+        <v>0</v>
+      </c>
+      <c r="M57" s="26">
+        <v>0</v>
+      </c>
+      <c r="N57" s="26">
+        <v>0</v>
+      </c>
+      <c r="O57" s="26">
+        <v>0</v>
+      </c>
+      <c r="P57" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="26">
+        <v>0</v>
+      </c>
+      <c r="R57" s="26">
+        <v>0</v>
+      </c>
+      <c r="S57" s="26">
+        <v>0</v>
+      </c>
+      <c r="T57" s="26">
+        <v>0</v>
+      </c>
+      <c r="U57" s="26"/>
+      <c r="V57" s="26"/>
+      <c r="W57" s="26"/>
+      <c r="X57" s="26"/>
+    </row>
+    <row r="58" spans="4:24">
+      <c r="L58" s="27"/>
+      <c r="M58" s="27"/>
+      <c r="N58" s="27"/>
+      <c r="O58" s="27"/>
+      <c r="P58" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 16-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -4581,8 +4580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N32" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+    <sheetView tabSelected="1" topLeftCell="H38" workbookViewId="0">
+      <selection activeCell="V59" sqref="V59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6846,7 +6845,7 @@
         <v>0</v>
       </c>
       <c r="V50" s="26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W50" s="26"/>
       <c r="X50" s="26"/>

</xml_diff>

<commit_message>
Updated by sravani date:17/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G7"/>
 </workbook>
 </file>
 
@@ -4581,8 +4580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M13" workbookViewId="0">
-      <selection activeCell="W27" sqref="D15:X57"/>
+    <sheetView tabSelected="1" topLeftCell="J39" workbookViewId="0">
+      <selection activeCell="X42" sqref="X42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4878,7 +4877,9 @@
       <c r="V16" s="26">
         <v>0</v>
       </c>
-      <c r="W16" s="26"/>
+      <c r="W16" s="26">
+        <v>0</v>
+      </c>
       <c r="X16" s="26"/>
     </row>
     <row r="17" spans="4:24" ht="17.25">
@@ -4939,7 +4940,9 @@
       <c r="V17" s="26">
         <v>0</v>
       </c>
-      <c r="W17" s="26"/>
+      <c r="W17" s="26">
+        <v>2</v>
+      </c>
       <c r="X17" s="26"/>
     </row>
     <row r="18" spans="4:24" ht="17.25">
@@ -5000,7 +5003,9 @@
       <c r="V18" s="26">
         <v>0</v>
       </c>
-      <c r="W18" s="26"/>
+      <c r="W18" s="26">
+        <v>0</v>
+      </c>
       <c r="X18" s="26"/>
     </row>
     <row r="19" spans="4:24" ht="17.25">
@@ -5061,7 +5066,9 @@
       <c r="V19" s="26">
         <v>1</v>
       </c>
-      <c r="W19" s="26"/>
+      <c r="W19" s="26">
+        <v>0</v>
+      </c>
       <c r="X19" s="26"/>
     </row>
     <row r="20" spans="4:24" ht="17.25">
@@ -5118,7 +5125,9 @@
       </c>
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
+      <c r="W20" s="26">
+        <v>0</v>
+      </c>
       <c r="X20" s="26"/>
     </row>
     <row r="21" spans="4:24" ht="17.25">
@@ -5175,7 +5184,9 @@
       </c>
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
+      <c r="W21" s="26">
+        <v>0</v>
+      </c>
       <c r="X21" s="26"/>
     </row>
     <row r="22" spans="4:24" ht="17.25">
@@ -6382,9 +6393,11 @@
         <v>0</v>
       </c>
       <c r="V42" s="26">
-        <v>0</v>
-      </c>
-      <c r="W42" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="W42" s="26">
+        <v>5</v>
+      </c>
       <c r="X42" s="26"/>
     </row>
     <row r="43" spans="4:24" ht="17.25">
@@ -6872,7 +6885,9 @@
       <c r="V50" s="26">
         <v>4</v>
       </c>
-      <c r="W50" s="26"/>
+      <c r="W50" s="26">
+        <v>4</v>
+      </c>
       <c r="X50" s="26"/>
     </row>
     <row r="51" spans="4:24" ht="17.25">

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:17-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4581,7 +4581,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J39" workbookViewId="0">
-      <selection activeCell="X42" sqref="X42"/>
+      <selection activeCell="W51" sqref="W51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6458,7 +6458,9 @@
       <c r="V43" s="26">
         <v>0</v>
       </c>
-      <c r="W43" s="26"/>
+      <c r="W43" s="26">
+        <v>0</v>
+      </c>
       <c r="X43" s="26"/>
     </row>
     <row r="44" spans="4:24" ht="17.25">
@@ -6519,7 +6521,9 @@
       <c r="V44" s="26">
         <v>0</v>
       </c>
-      <c r="W44" s="26"/>
+      <c r="W44" s="26">
+        <v>0</v>
+      </c>
       <c r="X44" s="26"/>
     </row>
     <row r="45" spans="4:24" ht="17.25">
@@ -6580,7 +6584,9 @@
       <c r="V45" s="26">
         <v>0</v>
       </c>
-      <c r="W45" s="26"/>
+      <c r="W45" s="26">
+        <v>0</v>
+      </c>
       <c r="X45" s="26"/>
     </row>
     <row r="46" spans="4:24" ht="17.25">
@@ -6641,7 +6647,9 @@
       <c r="V46" s="26">
         <v>0</v>
       </c>
-      <c r="W46" s="26"/>
+      <c r="W46" s="26">
+        <v>0</v>
+      </c>
       <c r="X46" s="26"/>
     </row>
     <row r="47" spans="4:24" ht="17.25">
@@ -6702,7 +6710,9 @@
       <c r="V47" s="26">
         <v>0</v>
       </c>
-      <c r="W47" s="26"/>
+      <c r="W47" s="26">
+        <v>0</v>
+      </c>
       <c r="X47" s="26"/>
     </row>
     <row r="48" spans="4:24" ht="17.25">
@@ -6763,7 +6773,9 @@
       <c r="V48" s="26">
         <v>0</v>
       </c>
-      <c r="W48" s="26"/>
+      <c r="W48" s="26">
+        <v>0</v>
+      </c>
       <c r="X48" s="26"/>
     </row>
     <row r="49" spans="4:24" ht="17.25">
@@ -6824,7 +6836,9 @@
       <c r="V49" s="26">
         <v>0</v>
       </c>
-      <c r="W49" s="26"/>
+      <c r="W49" s="26">
+        <v>0</v>
+      </c>
       <c r="X49" s="26"/>
     </row>
     <row r="50" spans="4:24" ht="17.25">
@@ -6948,7 +6962,9 @@
       <c r="V51" s="26">
         <v>0</v>
       </c>
-      <c r="W51" s="26"/>
+      <c r="W51" s="26">
+        <v>0</v>
+      </c>
       <c r="X51" s="26"/>
     </row>
     <row r="52" spans="4:24" ht="17.25">

</xml_diff>

<commit_message>
Updated by Alpna date:17-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4580,8 +4580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J39" workbookViewId="0">
-      <selection activeCell="W51" sqref="W51"/>
+    <sheetView tabSelected="1" topLeftCell="I9" workbookViewId="0">
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6273,7 +6273,9 @@
       <c r="V40" s="26">
         <v>0</v>
       </c>
-      <c r="W40" s="26"/>
+      <c r="W40" s="26">
+        <v>0</v>
+      </c>
       <c r="X40" s="26"/>
     </row>
     <row r="41" spans="4:24" ht="17.25">
@@ -6334,7 +6336,9 @@
       <c r="V41" s="26">
         <v>0</v>
       </c>
-      <c r="W41" s="26"/>
+      <c r="W41" s="26">
+        <v>0</v>
+      </c>
       <c r="X41" s="26"/>
     </row>
     <row r="42" spans="4:24" ht="17.25">

</xml_diff>

<commit_message>
Updated by Sravani date:18/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -745,26 +744,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -779,7 +778,7 @@
       </c>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -793,7 +792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -807,7 +806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -819,7 +818,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -831,7 +830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -843,7 +842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -855,7 +854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -867,7 +866,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -895,7 +894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -917,7 +916,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1191,7 +1190,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1316,7 +1315,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1441,7 +1440,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1502,7 +1501,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1627,7 +1626,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1712,7 +1711,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1797,7 +1796,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1882,7 +1881,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -1967,7 +1966,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2074,7 +2073,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2181,7 +2180,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2290,7 +2289,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2399,7 +2398,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2526,7 +2525,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2653,7 +2652,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2780,7 +2779,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -2907,7 +2906,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3034,7 +3033,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3161,7 +3160,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3288,7 +3287,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3349,7 +3348,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3476,7 +3475,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3605,7 +3604,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3734,7 +3733,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3863,7 +3862,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3924,7 +3923,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4053,7 +4052,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4180,7 +4179,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4307,7 +4306,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4434,7 +4433,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4581,28 +4580,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N9" workbookViewId="0">
-      <selection activeCell="X58" sqref="X58"/>
+    <sheetView tabSelected="1" topLeftCell="J33" workbookViewId="0">
+      <selection activeCell="X46" sqref="X46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -4617,7 +4616,7 @@
       </c>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:24" ht="18">
+    <row r="2" spans="1:24" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="18">
+    <row r="3" spans="1:24" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4645,7 +4644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="27.6">
+    <row r="4" spans="1:24" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4657,7 +4656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="69">
+    <row r="5" spans="1:24" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4669,7 +4668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="18">
+    <row r="6" spans="1:24" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="18">
+    <row r="7" spans="1:24" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="18">
+    <row r="8" spans="1:24" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4705,7 +4704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="18">
+    <row r="9" spans="1:24" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4733,7 +4732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="27.6">
+    <row r="12" spans="1:24" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4755,7 +4754,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:24" ht="28.2">
+    <row r="15" spans="1:24" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4820,7 +4819,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="18">
+    <row r="16" spans="1:24" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -4881,9 +4880,11 @@
       <c r="W16" s="26">
         <v>0</v>
       </c>
-      <c r="X16" s="26"/>
-    </row>
-    <row r="17" spans="4:24" ht="18">
+      <c r="X16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:24" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -4944,9 +4945,11 @@
       <c r="W17" s="26">
         <v>2</v>
       </c>
-      <c r="X17" s="26"/>
-    </row>
-    <row r="18" spans="4:24" ht="18">
+      <c r="X17" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:24" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5009,7 +5012,7 @@
       </c>
       <c r="X18" s="26"/>
     </row>
-    <row r="19" spans="4:24" ht="18">
+    <row r="19" spans="4:24" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5072,7 +5075,7 @@
       </c>
       <c r="X19" s="26"/>
     </row>
-    <row r="20" spans="4:24" ht="18">
+    <row r="20" spans="4:24" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5131,7 +5134,7 @@
       </c>
       <c r="X20" s="26"/>
     </row>
-    <row r="21" spans="4:24" ht="18">
+    <row r="21" spans="4:24" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5190,7 +5193,7 @@
       </c>
       <c r="X21" s="26"/>
     </row>
-    <row r="22" spans="4:24" ht="18">
+    <row r="22" spans="4:24" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5251,7 +5254,7 @@
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
     </row>
-    <row r="23" spans="4:24" ht="18">
+    <row r="23" spans="4:24" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5312,7 +5315,7 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
     </row>
-    <row r="24" spans="4:24" ht="18">
+    <row r="24" spans="4:24" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5373,7 +5376,7 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
     </row>
-    <row r="25" spans="4:24" ht="18">
+    <row r="25" spans="4:24" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5434,7 +5437,7 @@
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
     </row>
-    <row r="26" spans="4:24" ht="18">
+    <row r="26" spans="4:24" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5495,7 +5498,7 @@
       <c r="W26" s="26"/>
       <c r="X26" s="26"/>
     </row>
-    <row r="27" spans="4:24" ht="18">
+    <row r="27" spans="4:24" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -5556,7 +5559,7 @@
       <c r="W27" s="26"/>
       <c r="X27" s="26"/>
     </row>
-    <row r="28" spans="4:24" ht="18">
+    <row r="28" spans="4:24" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -5607,7 +5610,7 @@
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
     </row>
-    <row r="29" spans="4:24" ht="18">
+    <row r="29" spans="4:24" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -5658,7 +5661,7 @@
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
     </row>
-    <row r="30" spans="4:24" ht="18">
+    <row r="30" spans="4:24" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -5709,7 +5712,7 @@
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
     </row>
-    <row r="31" spans="4:24" ht="18">
+    <row r="31" spans="4:24" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -5760,7 +5763,7 @@
       <c r="W31" s="26"/>
       <c r="X31" s="26"/>
     </row>
-    <row r="32" spans="4:24" ht="18">
+    <row r="32" spans="4:24" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -5811,7 +5814,7 @@
       <c r="W32" s="26"/>
       <c r="X32" s="26"/>
     </row>
-    <row r="33" spans="4:24" ht="18">
+    <row r="33" spans="4:24" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -5862,7 +5865,7 @@
       <c r="W33" s="26"/>
       <c r="X33" s="26"/>
     </row>
-    <row r="34" spans="4:24" ht="18">
+    <row r="34" spans="4:24" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -5921,7 +5924,7 @@
       <c r="W34" s="26"/>
       <c r="X34" s="26"/>
     </row>
-    <row r="35" spans="4:24" ht="18">
+    <row r="35" spans="4:24" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -5980,7 +5983,7 @@
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
     </row>
-    <row r="36" spans="4:24" ht="18">
+    <row r="36" spans="4:24" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6039,7 +6042,7 @@
       <c r="W36" s="26"/>
       <c r="X36" s="26"/>
     </row>
-    <row r="37" spans="4:24" ht="18">
+    <row r="37" spans="4:24" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6098,7 +6101,7 @@
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
     </row>
-    <row r="38" spans="4:24" ht="18">
+    <row r="38" spans="4:24" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6157,7 +6160,7 @@
       <c r="W38" s="26"/>
       <c r="X38" s="26"/>
     </row>
-    <row r="39" spans="4:24" ht="18">
+    <row r="39" spans="4:24" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6216,7 +6219,7 @@
       <c r="W39" s="26"/>
       <c r="X39" s="26"/>
     </row>
-    <row r="40" spans="4:24" ht="18">
+    <row r="40" spans="4:24" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6277,9 +6280,11 @@
       <c r="W40" s="26">
         <v>0</v>
       </c>
-      <c r="X40" s="26"/>
-    </row>
-    <row r="41" spans="4:24" ht="18">
+      <c r="X40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:24" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6340,9 +6345,11 @@
       <c r="W41" s="26">
         <v>0</v>
       </c>
-      <c r="X41" s="26"/>
-    </row>
-    <row r="42" spans="4:24" ht="18">
+      <c r="X41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:24" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -6398,14 +6405,16 @@
         <v>0</v>
       </c>
       <c r="V42" s="26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W42" s="26">
-        <v>5</v>
-      </c>
-      <c r="X42" s="26"/>
-    </row>
-    <row r="43" spans="4:24" ht="18">
+        <v>0</v>
+      </c>
+      <c r="X42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:24" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -6466,9 +6475,11 @@
       <c r="W43" s="26">
         <v>0</v>
       </c>
-      <c r="X43" s="26"/>
-    </row>
-    <row r="44" spans="4:24" ht="18">
+      <c r="X43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:24" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -6524,14 +6535,16 @@
         <v>0</v>
       </c>
       <c r="V44" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W44" s="26">
-        <v>0</v>
-      </c>
-      <c r="X44" s="26"/>
-    </row>
-    <row r="45" spans="4:24" ht="18">
+        <v>5</v>
+      </c>
+      <c r="X44" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:24" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -6592,9 +6605,11 @@
       <c r="W45" s="26">
         <v>0</v>
       </c>
-      <c r="X45" s="26"/>
-    </row>
-    <row r="46" spans="4:24" ht="18">
+      <c r="X45" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:24" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -6657,7 +6672,7 @@
       </c>
       <c r="X46" s="26"/>
     </row>
-    <row r="47" spans="4:24" ht="18">
+    <row r="47" spans="4:24" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -6720,7 +6735,7 @@
       </c>
       <c r="X47" s="26"/>
     </row>
-    <row r="48" spans="4:24" ht="18">
+    <row r="48" spans="4:24" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -6783,7 +6798,7 @@
       </c>
       <c r="X48" s="26"/>
     </row>
-    <row r="49" spans="4:24" ht="18">
+    <row r="49" spans="4:24" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -6846,7 +6861,7 @@
       </c>
       <c r="X49" s="26"/>
     </row>
-    <row r="50" spans="4:24" ht="18">
+    <row r="50" spans="4:24" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -6907,9 +6922,11 @@
       <c r="W50" s="26">
         <v>4</v>
       </c>
-      <c r="X50" s="26"/>
-    </row>
-    <row r="51" spans="4:24" ht="18">
+      <c r="X50" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="4:24" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -6972,7 +6989,7 @@
       </c>
       <c r="X51" s="26"/>
     </row>
-    <row r="52" spans="4:24" ht="18">
+    <row r="52" spans="4:24" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7037,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:24" ht="18">
+    <row r="53" spans="4:24" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -7102,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:24" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:24" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -7167,7 +7184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:24" ht="18">
+    <row r="55" spans="4:24" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -7232,7 +7249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:24" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:24" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -7297,7 +7314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:24" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:24" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -7383,7 +7400,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done by B.S.Deepthi Date:18-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4581,7 +4581,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J33" workbookViewId="0">
-      <selection activeCell="X46" sqref="X46"/>
+      <selection activeCell="X51" sqref="X51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6670,7 +6670,9 @@
       <c r="W46" s="26">
         <v>0</v>
       </c>
-      <c r="X46" s="26"/>
+      <c r="X46" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="4:24" ht="17.25">
       <c r="D47" s="18" t="s">
@@ -6733,7 +6735,9 @@
       <c r="W47" s="26">
         <v>0</v>
       </c>
-      <c r="X47" s="26"/>
+      <c r="X47" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="4:24" ht="17.25">
       <c r="D48" s="18" t="s">
@@ -6796,7 +6800,9 @@
       <c r="W48" s="26">
         <v>0</v>
       </c>
-      <c r="X48" s="26"/>
+      <c r="X48" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="4:24" ht="17.25">
       <c r="D49" s="18" t="s">
@@ -6859,7 +6865,9 @@
       <c r="W49" s="26">
         <v>0</v>
       </c>
-      <c r="X49" s="26"/>
+      <c r="X49" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="4:24" ht="17.25">
       <c r="D50" s="18" t="s">
@@ -6987,7 +6995,9 @@
       <c r="W51" s="26">
         <v>0</v>
       </c>
-      <c r="X51" s="26"/>
+      <c r="X51" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="4:24" ht="17.25">
       <c r="D52" s="18" t="s">

</xml_diff>

<commit_message>
updated by Alpna date:18-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4580,8 +4580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J33" workbookViewId="0">
-      <selection activeCell="X51" sqref="X51"/>
+    <sheetView tabSelected="1" topLeftCell="J15" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18:X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5010,7 +5010,9 @@
       <c r="W18" s="26">
         <v>0</v>
       </c>
-      <c r="X18" s="26"/>
+      <c r="X18" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="4:24" ht="17.25">
       <c r="D19" s="18" t="s">
@@ -5073,7 +5075,9 @@
       <c r="W19" s="26">
         <v>0</v>
       </c>
-      <c r="X19" s="26"/>
+      <c r="X19" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="4:24" ht="17.25">
       <c r="D20" s="18" t="s">
@@ -5132,7 +5136,9 @@
       <c r="W20" s="26">
         <v>0</v>
       </c>
-      <c r="X20" s="26"/>
+      <c r="X20" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="4:24" ht="17.25">
       <c r="D21" s="18" t="s">
@@ -5191,7 +5197,9 @@
       <c r="W21" s="26">
         <v>0</v>
       </c>
-      <c r="X21" s="26"/>
+      <c r="X21" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="4:24" ht="17.25">
       <c r="D22" s="18" t="s">

</xml_diff>

<commit_message>
updated by sravani date:19/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -242,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -350,6 +350,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -363,7 +374,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -436,6 +447,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4578,10 +4590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X58"/>
+  <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J15" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18:X21"/>
+    <sheetView tabSelected="1" topLeftCell="K38" workbookViewId="0">
+      <selection activeCell="Y51" sqref="Y51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4601,10 +4613,10 @@
     <col min="19" max="20" width="11.28515625" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" customWidth="1"/>
     <col min="22" max="23" width="13.140625" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4616,7 +4628,7 @@
       </c>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:24" ht="17.25">
+    <row r="2" spans="1:25" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4630,7 +4642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="17.25">
+    <row r="3" spans="1:25" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4644,7 +4656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="28.5">
+    <row r="4" spans="1:25" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4656,7 +4668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="71.25">
+    <row r="5" spans="1:25" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4668,7 +4680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="17.25">
+    <row r="6" spans="1:25" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4680,7 +4692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="17.25">
+    <row r="7" spans="1:25" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4692,7 +4704,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="17.25">
+    <row r="8" spans="1:25" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4704,7 +4716,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="17.25">
+    <row r="9" spans="1:25" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4716,7 +4728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4724,7 +4736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -4732,7 +4744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="42.75">
+    <row r="12" spans="1:25" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4740,21 +4752,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:25">
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:25">
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:24" ht="30">
+    <row r="15" spans="1:25" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4818,8 +4830,11 @@
       <c r="X15" s="25">
         <v>40986</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" ht="17.25">
+      <c r="Y15" s="25">
+        <v>40986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5822,7 +5837,7 @@
       <c r="W32" s="26"/>
       <c r="X32" s="26"/>
     </row>
-    <row r="33" spans="4:24" ht="17.25">
+    <row r="33" spans="4:25" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -5873,7 +5888,7 @@
       <c r="W33" s="26"/>
       <c r="X33" s="26"/>
     </row>
-    <row r="34" spans="4:24" ht="17.25">
+    <row r="34" spans="4:25" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -5932,7 +5947,7 @@
       <c r="W34" s="26"/>
       <c r="X34" s="26"/>
     </row>
-    <row r="35" spans="4:24" ht="17.25">
+    <row r="35" spans="4:25" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -5991,7 +6006,7 @@
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
     </row>
-    <row r="36" spans="4:24" ht="17.25">
+    <row r="36" spans="4:25" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6050,7 +6065,7 @@
       <c r="W36" s="26"/>
       <c r="X36" s="26"/>
     </row>
-    <row r="37" spans="4:24" ht="17.25">
+    <row r="37" spans="4:25" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6109,7 +6124,7 @@
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
     </row>
-    <row r="38" spans="4:24" ht="17.25">
+    <row r="38" spans="4:25" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6168,7 +6183,7 @@
       <c r="W38" s="26"/>
       <c r="X38" s="26"/>
     </row>
-    <row r="39" spans="4:24" ht="17.25">
+    <row r="39" spans="4:25" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6227,7 +6242,7 @@
       <c r="W39" s="26"/>
       <c r="X39" s="26"/>
     </row>
-    <row r="40" spans="4:24" ht="17.25">
+    <row r="40" spans="4:25" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6291,8 +6306,11 @@
       <c r="X40" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="4:24" ht="17.25">
+      <c r="Y40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:25" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6356,8 +6374,11 @@
       <c r="X41" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="4:24" ht="17.25">
+      <c r="Y41" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="4:25" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -6421,8 +6442,11 @@
       <c r="X42" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="4:24" ht="17.25">
+      <c r="Y42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:25" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -6486,8 +6510,11 @@
       <c r="X43" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="4:24" ht="17.25">
+      <c r="Y43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:25" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -6551,8 +6578,11 @@
       <c r="X44" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="4:24" ht="17.25">
+      <c r="Y44" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="4:25" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -6616,8 +6646,11 @@
       <c r="X45" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="4:24" ht="17.25">
+      <c r="Y45" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:25" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -6681,8 +6714,11 @@
       <c r="X46" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="4:24" ht="17.25">
+      <c r="Y46" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:25" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -6746,8 +6782,11 @@
       <c r="X47" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="4:24" ht="17.25">
+      <c r="Y47" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="4:25" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -6811,8 +6850,11 @@
       <c r="X48" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:24" ht="17.25">
+      <c r="Y48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:25" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -6876,8 +6918,11 @@
       <c r="X49" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="4:24" ht="17.25">
+      <c r="Y49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:25" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -6941,8 +6986,11 @@
       <c r="X50" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="4:24" ht="17.25">
+      <c r="Y50" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:25" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -7006,8 +7054,11 @@
       <c r="X51" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="4:24" ht="17.25">
+      <c r="Y51" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:25" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7072,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:24" ht="17.25">
+    <row r="53" spans="4:25" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -7137,7 +7188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:24" ht="18" thickBot="1">
+    <row r="54" spans="4:25" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -7202,7 +7253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:24" ht="17.25">
+    <row r="55" spans="4:25" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -7267,7 +7318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:24" ht="18" thickBot="1">
+    <row r="56" spans="4:25" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -7332,7 +7383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:24" ht="18" thickBot="1">
+    <row r="57" spans="4:25" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -7397,7 +7448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:24">
+    <row r="58" spans="4:25">
       <c r="L58" s="27"/>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:19-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -446,8 +446,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="3" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,10 +785,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="29"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
@@ -4592,8 +4592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K38" workbookViewId="0">
-      <selection activeCell="Y51" sqref="Y51"/>
+    <sheetView tabSelected="1" topLeftCell="K11" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16:Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4623,10 +4623,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="29"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:25" ht="17.25">
       <c r="A2" s="4" t="s">
@@ -4898,8 +4898,11 @@
       <c r="X16" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="4:24" ht="17.25">
+      <c r="Y16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:25" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -4963,8 +4966,11 @@
       <c r="X17" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="4:24" ht="17.25">
+      <c r="Y17" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:25" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5028,8 +5034,11 @@
       <c r="X18" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="4:24" ht="17.25">
+      <c r="Y18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:25" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5093,8 +5102,11 @@
       <c r="X19" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="4:24" ht="17.25">
+      <c r="Y19" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:25" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5154,8 +5166,11 @@
       <c r="X20" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="4:24" ht="17.25">
+      <c r="Y20" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:25" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5215,8 +5230,11 @@
       <c r="X21" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="4:24" ht="17.25">
+      <c r="Y21" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:25" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5277,7 +5295,7 @@
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
     </row>
-    <row r="23" spans="4:24" ht="17.25">
+    <row r="23" spans="4:25" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5338,7 +5356,7 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
     </row>
-    <row r="24" spans="4:24" ht="17.25">
+    <row r="24" spans="4:25" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5399,7 +5417,7 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
     </row>
-    <row r="25" spans="4:24" ht="17.25">
+    <row r="25" spans="4:25" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5460,7 +5478,7 @@
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
     </row>
-    <row r="26" spans="4:24" ht="17.25">
+    <row r="26" spans="4:25" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5521,7 +5539,7 @@
       <c r="W26" s="26"/>
       <c r="X26" s="26"/>
     </row>
-    <row r="27" spans="4:24" ht="17.25">
+    <row r="27" spans="4:25" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -5582,7 +5600,7 @@
       <c r="W27" s="26"/>
       <c r="X27" s="26"/>
     </row>
-    <row r="28" spans="4:24" ht="17.25">
+    <row r="28" spans="4:25" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -5633,7 +5651,7 @@
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
     </row>
-    <row r="29" spans="4:24" ht="17.25">
+    <row r="29" spans="4:25" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -5684,7 +5702,7 @@
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
     </row>
-    <row r="30" spans="4:24" ht="17.25">
+    <row r="30" spans="4:25" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -5735,7 +5753,7 @@
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
     </row>
-    <row r="31" spans="4:24" ht="17.25">
+    <row r="31" spans="4:25" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -5786,7 +5804,7 @@
       <c r="W31" s="26"/>
       <c r="X31" s="26"/>
     </row>
-    <row r="32" spans="4:24" ht="17.25">
+    <row r="32" spans="4:25" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6374,7 +6392,7 @@
       <c r="X41" s="26">
         <v>0</v>
       </c>
-      <c r="Y41" s="30">
+      <c r="Y41" s="29">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated by sravvani date:20/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -243,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -351,6 +350,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -364,7 +374,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -438,6 +448,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4580,10 +4591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y58"/>
+  <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O32" workbookViewId="0">
-      <selection activeCell="Y34" sqref="Y34"/>
+    <sheetView tabSelected="1" topLeftCell="M37" workbookViewId="0">
+      <selection activeCell="Z52" sqref="Z52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4604,9 +4615,10 @@
     <col min="21" max="21" width="14.28515625" customWidth="1"/>
     <col min="22" max="23" width="13.140625" customWidth="1"/>
     <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4618,7 +4630,7 @@
       </c>
       <c r="E1" s="30"/>
     </row>
-    <row r="2" spans="1:25" ht="17.25">
+    <row r="2" spans="1:26" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4632,7 +4644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="17.25">
+    <row r="3" spans="1:26" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4646,7 +4658,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="28.5">
+    <row r="4" spans="1:26" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4658,7 +4670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="71.25">
+    <row r="5" spans="1:26" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4670,7 +4682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="17.25">
+    <row r="6" spans="1:26" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4682,7 +4694,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="17.25">
+    <row r="7" spans="1:26" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4694,7 +4706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="17.25">
+    <row r="8" spans="1:26" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4706,7 +4718,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="17.25">
+    <row r="9" spans="1:26" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4718,7 +4730,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:26">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4726,7 +4738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:26">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -4734,7 +4746,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="42.75">
+    <row r="12" spans="1:26" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4742,21 +4754,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:26">
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:26">
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:25" ht="30">
+    <row r="15" spans="1:26" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4823,8 +4835,11 @@
       <c r="Y15" s="25">
         <v>40987</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" ht="17.25">
+      <c r="Z15" s="25">
+        <v>40988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -4892,7 +4907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:25" ht="17.25">
+    <row r="17" spans="4:26" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -4960,7 +4975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="4:25" ht="17.25">
+    <row r="18" spans="4:26" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5028,7 +5043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:25" ht="17.25">
+    <row r="19" spans="4:26" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5096,7 +5111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:25" ht="17.25">
+    <row r="20" spans="4:26" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5159,8 +5174,11 @@
       <c r="Y20" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="4:25" ht="17.25">
+      <c r="Z20" s="31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:26" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5224,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:25" ht="17.25">
+    <row r="22" spans="4:26" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5286,7 +5304,7 @@
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
     </row>
-    <row r="23" spans="4:25" ht="17.25">
+    <row r="23" spans="4:26" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5348,7 +5366,7 @@
       <c r="X23" s="26"/>
       <c r="Y23" s="22"/>
     </row>
-    <row r="24" spans="4:25" ht="17.25">
+    <row r="24" spans="4:26" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5410,7 +5428,7 @@
       <c r="X24" s="26"/>
       <c r="Y24" s="22"/>
     </row>
-    <row r="25" spans="4:25" ht="17.25">
+    <row r="25" spans="4:26" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5472,7 +5490,7 @@
       <c r="X25" s="26"/>
       <c r="Y25" s="22"/>
     </row>
-    <row r="26" spans="4:25" ht="17.25">
+    <row r="26" spans="4:26" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5534,7 +5552,7 @@
       <c r="X26" s="26"/>
       <c r="Y26" s="22"/>
     </row>
-    <row r="27" spans="4:25" ht="17.25">
+    <row r="27" spans="4:26" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -5596,7 +5614,7 @@
       <c r="X27" s="26"/>
       <c r="Y27" s="22"/>
     </row>
-    <row r="28" spans="4:25" ht="17.25">
+    <row r="28" spans="4:26" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -5648,7 +5666,7 @@
       <c r="X28" s="26"/>
       <c r="Y28" s="22"/>
     </row>
-    <row r="29" spans="4:25" ht="17.25">
+    <row r="29" spans="4:26" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -5700,7 +5718,7 @@
       <c r="X29" s="26"/>
       <c r="Y29" s="22"/>
     </row>
-    <row r="30" spans="4:25" ht="17.25">
+    <row r="30" spans="4:26" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -5752,7 +5770,7 @@
       <c r="X30" s="26"/>
       <c r="Y30" s="22"/>
     </row>
-    <row r="31" spans="4:25" ht="17.25">
+    <row r="31" spans="4:26" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -5804,7 +5822,7 @@
       <c r="X31" s="26"/>
       <c r="Y31" s="22"/>
     </row>
-    <row r="32" spans="4:25" ht="17.25">
+    <row r="32" spans="4:26" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -5856,7 +5874,7 @@
       <c r="X32" s="26"/>
       <c r="Y32" s="22"/>
     </row>
-    <row r="33" spans="4:25" ht="17.25">
+    <row r="33" spans="4:26" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -5908,7 +5926,7 @@
       <c r="X33" s="26"/>
       <c r="Y33" s="22"/>
     </row>
-    <row r="34" spans="4:25" ht="17.25">
+    <row r="34" spans="4:26" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -5976,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:25" ht="17.25">
+    <row r="35" spans="4:26" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6044,7 +6062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="4:25" ht="17.25">
+    <row r="36" spans="4:26" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6112,7 +6130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:25" ht="17.25">
+    <row r="37" spans="4:26" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6180,7 +6198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:25" ht="17.25">
+    <row r="38" spans="4:26" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6248,7 +6266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:25" ht="17.25">
+    <row r="39" spans="4:26" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6316,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:25" ht="17.25">
+    <row r="40" spans="4:26" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6383,8 +6401,11 @@
       <c r="Y40" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="4:25" ht="17.25">
+      <c r="Z40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:26" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6451,8 +6472,11 @@
       <c r="Y41" s="29">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="4:25" ht="17.25">
+      <c r="Z41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:26" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -6519,8 +6543,11 @@
       <c r="Y42" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="4:25" ht="17.25">
+      <c r="Z42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:26" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -6587,8 +6614,11 @@
       <c r="Y43" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="4:25" ht="17.25">
+      <c r="Z43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:26" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -6655,8 +6685,11 @@
       <c r="Y44" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="4:25" ht="17.25">
+      <c r="Z44" s="31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="4:26" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -6723,8 +6756,11 @@
       <c r="Y45" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="4:25" ht="17.25">
+      <c r="Z45" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:26" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -6791,8 +6827,11 @@
       <c r="Y46" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="4:25" ht="17.25">
+      <c r="Z46" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:26" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -6859,8 +6898,11 @@
       <c r="Y47" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="4:25" ht="17.25">
+      <c r="Z47" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:26" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -6927,8 +6969,11 @@
       <c r="Y48" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:25" ht="17.25">
+      <c r="Z48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:26" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -6995,8 +7040,11 @@
       <c r="Y49" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="4:25" ht="17.25">
+      <c r="Z49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:26" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -7063,8 +7111,11 @@
       <c r="Y50" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="4:25" ht="17.25">
+      <c r="Z50" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="4:26" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -7131,8 +7182,11 @@
       <c r="Y51" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="4:25" ht="17.25">
+      <c r="Z51" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:26" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7199,8 +7253,9 @@
       <c r="Y52" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="4:25" ht="17.25">
+      <c r="Z52" s="26"/>
+    </row>
+    <row r="53" spans="4:26" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -7268,7 +7323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="4:25" ht="18" thickBot="1">
+    <row r="54" spans="4:26" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -7336,7 +7391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:25" ht="17.25">
+    <row r="55" spans="4:26" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -7404,7 +7459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:25" ht="18" thickBot="1">
+    <row r="56" spans="4:26" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -7472,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:25" ht="18" thickBot="1">
+    <row r="57" spans="4:26" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -7540,7 +7595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:25">
+    <row r="58" spans="4:26">
       <c r="L58" s="27"/>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:20-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -447,8 +447,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +786,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
@@ -4593,8 +4593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M37" workbookViewId="0">
-      <selection activeCell="Z52" sqref="Z52"/>
+    <sheetView tabSelected="1" topLeftCell="M7" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4625,10 +4625,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:26" ht="17.25">
       <c r="A2" s="4" t="s">
@@ -4906,6 +4906,9 @@
       <c r="Y16" s="26">
         <v>0</v>
       </c>
+      <c r="Z16" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="4:26" ht="17.25">
       <c r="D17" s="18" t="s">
@@ -4974,6 +4977,9 @@
       <c r="Y17" s="26">
         <v>4</v>
       </c>
+      <c r="Z17" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="4:26" ht="17.25">
       <c r="D18" s="18" t="s">
@@ -5042,6 +5048,9 @@
       <c r="Y18" s="26">
         <v>0</v>
       </c>
+      <c r="Z18" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="4:26" ht="17.25">
       <c r="D19" s="18" t="s">
@@ -5110,6 +5119,9 @@
       <c r="Y19" s="26">
         <v>0</v>
       </c>
+      <c r="Z19" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="4:26" ht="17.25">
       <c r="D20" s="18" t="s">
@@ -5174,7 +5186,7 @@
       <c r="Y20" s="26">
         <v>0</v>
       </c>
-      <c r="Z20" s="31">
+      <c r="Z20" s="30">
         <v>5</v>
       </c>
     </row>
@@ -5239,6 +5251,9 @@
         <v>0</v>
       </c>
       <c r="Y21" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="26">
         <v>0</v>
       </c>
     </row>
@@ -6685,7 +6700,7 @@
       <c r="Y44" s="26">
         <v>0</v>
       </c>
-      <c r="Z44" s="31">
+      <c r="Z44" s="30">
         <v>5</v>
       </c>
     </row>
@@ -7111,7 +7126,7 @@
       <c r="Y50" s="26">
         <v>0</v>
       </c>
-      <c r="Z50" s="31">
+      <c r="Z50" s="30">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated by alpna date:20-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4593,8 +4593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5318,6 +5318,7 @@
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
     </row>
     <row r="23" spans="4:26" ht="17.25">
       <c r="D23" s="18" t="s">

</xml_diff>

<commit_message>
updated by sravvani date 21/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4308" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4305" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -758,26 +757,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -792,7 +791,7 @@
       </c>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -806,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -820,7 +819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -832,7 +831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -844,7 +843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -856,7 +855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -868,7 +867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -880,7 +879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -908,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -930,7 +929,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1204,7 +1203,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1329,7 +1328,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1454,7 +1453,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1515,7 +1514,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1639,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1725,7 +1724,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1810,7 +1809,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1895,7 +1894,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -1980,7 +1979,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2087,7 +2086,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2194,7 +2193,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2303,7 +2302,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2412,7 +2411,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2539,7 +2538,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2665,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2793,7 +2792,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -2920,7 +2919,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3047,7 +3046,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3174,7 +3173,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3301,7 +3300,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3362,7 +3361,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3489,7 +3488,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3618,7 +3617,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3747,7 +3746,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3876,7 +3875,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3937,7 +3936,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4066,7 +4065,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4193,7 +4192,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4320,7 +4319,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4447,7 +4446,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4592,34 +4591,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z58"/>
+  <dimension ref="A1:AA58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="Z57" sqref="Z57"/>
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
+    <col min="27" max="27" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:26" ht="18">
+    <row r="2" spans="1:27" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="18">
+    <row r="3" spans="1:27" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="27.6">
+    <row r="4" spans="1:27" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="69">
+    <row r="5" spans="1:27" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="18">
+    <row r="6" spans="1:27" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="18">
+    <row r="7" spans="1:27" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="18">
+    <row r="8" spans="1:27" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="18">
+    <row r="9" spans="1:27" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:27">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:27">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="27.6">
+    <row r="12" spans="1:27" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4755,21 +4755,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:27">
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:27">
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:26" ht="28.2">
+    <row r="15" spans="1:27" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4839,8 +4839,11 @@
       <c r="Z15" s="25">
         <v>40988</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="18">
+      <c r="AA15" s="25">
+        <v>40989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -4910,8 +4913,11 @@
       <c r="Z16" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="4:26" ht="18">
+      <c r="AA16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:27" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -4981,8 +4987,11 @@
       <c r="Z17" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="4:26" ht="18">
+      <c r="AA17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5052,8 +5061,11 @@
       <c r="Z18" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="4:26" ht="18">
+      <c r="AA18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5123,8 +5135,11 @@
       <c r="Z19" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="4:26" ht="18">
+      <c r="AA19" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5190,8 +5205,11 @@
       <c r="Z20" s="30">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="4:26" ht="18">
+      <c r="AA20" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:27" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5257,8 +5275,11 @@
       <c r="Z21" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="4:26" ht="18">
+      <c r="AA21" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:27" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5321,7 +5342,7 @@
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
     </row>
-    <row r="23" spans="4:26" ht="18">
+    <row r="23" spans="4:27" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5383,7 +5404,7 @@
       <c r="X23" s="26"/>
       <c r="Y23" s="22"/>
     </row>
-    <row r="24" spans="4:26" ht="18">
+    <row r="24" spans="4:27" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5445,7 +5466,7 @@
       <c r="X24" s="26"/>
       <c r="Y24" s="22"/>
     </row>
-    <row r="25" spans="4:26" ht="18">
+    <row r="25" spans="4:27" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5507,7 +5528,7 @@
       <c r="X25" s="26"/>
       <c r="Y25" s="22"/>
     </row>
-    <row r="26" spans="4:26" ht="18">
+    <row r="26" spans="4:27" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5569,7 +5590,7 @@
       <c r="X26" s="26"/>
       <c r="Y26" s="22"/>
     </row>
-    <row r="27" spans="4:26" ht="18">
+    <row r="27" spans="4:27" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -5631,7 +5652,7 @@
       <c r="X27" s="26"/>
       <c r="Y27" s="22"/>
     </row>
-    <row r="28" spans="4:26" ht="18">
+    <row r="28" spans="4:27" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -5683,7 +5704,7 @@
       <c r="X28" s="26"/>
       <c r="Y28" s="22"/>
     </row>
-    <row r="29" spans="4:26" ht="18">
+    <row r="29" spans="4:27" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -5735,7 +5756,7 @@
       <c r="X29" s="26"/>
       <c r="Y29" s="22"/>
     </row>
-    <row r="30" spans="4:26" ht="18">
+    <row r="30" spans="4:27" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -5787,7 +5808,7 @@
       <c r="X30" s="26"/>
       <c r="Y30" s="22"/>
     </row>
-    <row r="31" spans="4:26" ht="18">
+    <row r="31" spans="4:27" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -5839,7 +5860,7 @@
       <c r="X31" s="26"/>
       <c r="Y31" s="22"/>
     </row>
-    <row r="32" spans="4:26" ht="18">
+    <row r="32" spans="4:27" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -5891,7 +5912,7 @@
       <c r="X32" s="26"/>
       <c r="Y32" s="22"/>
     </row>
-    <row r="33" spans="4:26" ht="18">
+    <row r="33" spans="4:26" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -5943,7 +5964,7 @@
       <c r="X33" s="26"/>
       <c r="Y33" s="22"/>
     </row>
-    <row r="34" spans="4:26" ht="18">
+    <row r="34" spans="4:26" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6011,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:26" ht="18">
+    <row r="35" spans="4:26" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6079,7 +6100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="4:26" ht="18">
+    <row r="36" spans="4:26" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6147,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:26" ht="18">
+    <row r="37" spans="4:26" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6215,7 +6236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:26" ht="18">
+    <row r="38" spans="4:26" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6283,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:26" ht="18">
+    <row r="39" spans="4:26" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6351,7 +6372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:26" ht="18">
+    <row r="40" spans="4:26" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6422,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:26" ht="18">
+    <row r="41" spans="4:26" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6493,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:26" ht="18">
+    <row r="42" spans="4:26" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -6564,7 +6585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:26" ht="18">
+    <row r="43" spans="4:26" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -6635,7 +6656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:26" ht="18">
+    <row r="44" spans="4:26" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -6706,7 +6727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="4:26" ht="18">
+    <row r="45" spans="4:26" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -6777,7 +6798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:26" ht="18">
+    <row r="46" spans="4:26" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -6848,7 +6869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:26" ht="18">
+    <row r="47" spans="4:26" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -6919,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:26" ht="18">
+    <row r="48" spans="4:26" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -6990,7 +7011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:26" ht="18">
+    <row r="49" spans="4:26" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -7061,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:26" ht="18">
+    <row r="50" spans="4:26" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -7132,7 +7153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="4:26" ht="18">
+    <row r="51" spans="4:26" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -7203,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:26" ht="18">
+    <row r="52" spans="4:26" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7274,7 +7295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:26" ht="18">
+    <row r="53" spans="4:26" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -7345,7 +7366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:26" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:26" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -7416,7 +7437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:26" ht="18">
+    <row r="55" spans="4:26" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -7487,7 +7508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:26" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:26" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -7558,7 +7579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="4:26" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:26" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -7651,7 +7672,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date 21-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4593,8 +4593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+    <sheetView tabSelected="1" topLeftCell="M31" workbookViewId="0">
+      <selection activeCell="AA46" sqref="AA46:AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5276,7 +5276,7 @@
         <v>0</v>
       </c>
       <c r="AA21" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="4:27" ht="17.25">
@@ -5912,7 +5912,7 @@
       <c r="X32" s="26"/>
       <c r="Y32" s="22"/>
     </row>
-    <row r="33" spans="4:26" ht="17.25">
+    <row r="33" spans="4:27" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -5964,7 +5964,7 @@
       <c r="X33" s="26"/>
       <c r="Y33" s="22"/>
     </row>
-    <row r="34" spans="4:26" ht="17.25">
+    <row r="34" spans="4:27" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:26" ht="17.25">
+    <row r="35" spans="4:27" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="4:26" ht="17.25">
+    <row r="36" spans="4:27" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:26" ht="17.25">
+    <row r="37" spans="4:27" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:26" ht="17.25">
+    <row r="38" spans="4:27" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:26" ht="17.25">
+    <row r="39" spans="4:27" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:26" ht="17.25">
+    <row r="40" spans="4:27" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6442,8 +6442,11 @@
       <c r="Z40" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="4:26" ht="17.25">
+      <c r="AA40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:27" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6513,8 +6516,11 @@
       <c r="Z41" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="4:26" ht="17.25">
+      <c r="AA41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:27" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -6584,8 +6590,11 @@
       <c r="Z42" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="4:26" ht="17.25">
+      <c r="AA42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:27" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -6655,8 +6664,11 @@
       <c r="Z43" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="4:26" ht="17.25">
+      <c r="AA43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:27" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -6726,8 +6738,11 @@
       <c r="Z44" s="30">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="4:26" ht="17.25">
+      <c r="AA44" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="4:27" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -6797,8 +6812,11 @@
       <c r="Z45" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="4:26" ht="17.25">
+      <c r="AA45" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:27" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -6868,8 +6886,11 @@
       <c r="Z46" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="4:26" ht="17.25">
+      <c r="AA46" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:27" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -6939,8 +6960,11 @@
       <c r="Z47" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="4:26" ht="17.25">
+      <c r="AA47" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:27" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -7010,8 +7034,11 @@
       <c r="Z48" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:26" ht="17.25">
+      <c r="AA48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:27" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -7081,8 +7108,11 @@
       <c r="Z49" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="4:26" ht="17.25">
+      <c r="AA49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:27" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -7152,8 +7182,11 @@
       <c r="Z50" s="30">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="4:26" ht="17.25">
+      <c r="AA50" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="4:27" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -7223,8 +7256,11 @@
       <c r="Z51" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="4:26" ht="17.25">
+      <c r="AA51" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:27" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7295,7 +7331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:26" ht="17.25">
+    <row r="53" spans="4:27" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -7366,7 +7402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:26" ht="18" thickBot="1">
+    <row r="54" spans="4:27" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -7437,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:26" ht="17.25">
+    <row r="55" spans="4:27" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -7508,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:26" ht="18" thickBot="1">
+    <row r="56" spans="4:27" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -7579,7 +7615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="4:26" ht="18" thickBot="1">
+    <row r="57" spans="4:27" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -7650,7 +7686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:26">
+    <row r="58" spans="4:27">
       <c r="L58" s="27"/>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>

</xml_diff>

<commit_message>
updated by Alpna date:21-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4593,8 +4593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M31" workbookViewId="0">
-      <selection activeCell="AA46" sqref="AA46:AA51"/>
+    <sheetView tabSelected="1" topLeftCell="M19" workbookViewId="0">
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5341,6 +5341,7 @@
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
     </row>
     <row r="23" spans="4:27" ht="17.25">
       <c r="D23" s="18" t="s">

</xml_diff>

<commit_message>
updated by sravvani date 24/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -758,26 +757,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -792,7 +791,7 @@
       </c>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -806,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -820,7 +819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -832,7 +831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -844,7 +843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -856,7 +855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -868,7 +867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -880,7 +879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -908,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -930,7 +929,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1204,7 +1203,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1329,7 +1328,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1454,7 +1453,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1515,7 +1514,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1639,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1725,7 +1724,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1810,7 +1809,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1895,7 +1894,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -1980,7 +1979,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2087,7 +2086,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2194,7 +2193,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2303,7 +2302,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2412,7 +2411,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2539,7 +2538,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2665,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2793,7 +2792,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -2920,7 +2919,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3047,7 +3046,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3174,7 +3173,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3301,7 +3300,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3362,7 +3361,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3489,7 +3488,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3618,7 +3617,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3747,7 +3746,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3876,7 +3875,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3937,7 +3936,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4066,7 +4065,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4193,7 +4192,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4320,7 +4319,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4447,7 +4446,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4592,36 +4591,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC58"/>
+  <dimension ref="A1:AD58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S49" workbookViewId="0">
-      <selection activeCell="AD56" sqref="AD56"/>
+    <sheetView tabSelected="1" topLeftCell="P13" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:29" ht="18">
+    <row r="2" spans="1:30" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="18">
+    <row r="3" spans="1:30" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="27.6">
+    <row r="4" spans="1:30" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="69">
+    <row r="5" spans="1:30" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="18">
+    <row r="6" spans="1:30" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="18">
+    <row r="7" spans="1:30" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="18">
+    <row r="8" spans="1:30" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="18">
+    <row r="9" spans="1:30" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:30">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:30">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="27.6">
+    <row r="12" spans="1:30" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4757,21 +4757,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:30">
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:30">
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:29" ht="28.2">
+    <row r="15" spans="1:30" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4850,8 +4850,11 @@
       <c r="AC15" s="25">
         <v>40991</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" ht="18">
+      <c r="AD15" s="25">
+        <v>40992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -4930,8 +4933,11 @@
       <c r="AC16" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="4:29" ht="18">
+      <c r="AD16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:30" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5010,8 +5016,11 @@
       <c r="AC17" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="4:29" ht="18">
+      <c r="AD17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:30" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5090,8 +5099,11 @@
       <c r="AC18" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="4:29" ht="18">
+      <c r="AD18" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:30" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5170,8 +5182,11 @@
       <c r="AC19" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="4:29" ht="18">
+      <c r="AD19" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:30" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5246,8 +5261,11 @@
       <c r="AC20" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="4:29" ht="18">
+      <c r="AD20" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:30" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5322,8 +5340,11 @@
       <c r="AC21" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="4:29" ht="18">
+      <c r="AD21" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="4:30" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5389,7 +5410,7 @@
       <c r="AB22" s="26"/>
       <c r="AC22" s="26"/>
     </row>
-    <row r="23" spans="4:29" ht="18">
+    <row r="23" spans="4:30" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5451,7 +5472,7 @@
       <c r="X23" s="26"/>
       <c r="Y23" s="22"/>
     </row>
-    <row r="24" spans="4:29" ht="18">
+    <row r="24" spans="4:30" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5513,7 +5534,7 @@
       <c r="X24" s="26"/>
       <c r="Y24" s="22"/>
     </row>
-    <row r="25" spans="4:29" ht="18">
+    <row r="25" spans="4:30" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5575,7 +5596,7 @@
       <c r="X25" s="26"/>
       <c r="Y25" s="22"/>
     </row>
-    <row r="26" spans="4:29" ht="18">
+    <row r="26" spans="4:30" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5637,7 +5658,7 @@
       <c r="X26" s="26"/>
       <c r="Y26" s="22"/>
     </row>
-    <row r="27" spans="4:29" ht="18">
+    <row r="27" spans="4:30" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -5699,7 +5720,7 @@
       <c r="X27" s="26"/>
       <c r="Y27" s="22"/>
     </row>
-    <row r="28" spans="4:29" ht="18">
+    <row r="28" spans="4:30" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -5754,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:29" ht="18">
+    <row r="29" spans="4:30" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -5809,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:29" ht="18">
+    <row r="30" spans="4:30" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -5864,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:29" ht="18">
+    <row r="31" spans="4:30" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -5919,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:29" ht="18">
+    <row r="32" spans="4:30" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -5971,7 +5992,7 @@
       <c r="X32" s="26"/>
       <c r="Y32" s="22"/>
     </row>
-    <row r="33" spans="4:29" ht="18">
+    <row r="33" spans="4:30" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6023,7 +6044,7 @@
       <c r="X33" s="26"/>
       <c r="Y33" s="22"/>
     </row>
-    <row r="34" spans="4:29" ht="18">
+    <row r="34" spans="4:30" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6091,7 +6112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:29" ht="18">
+    <row r="35" spans="4:30" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6159,7 +6180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="4:29" ht="18">
+    <row r="36" spans="4:30" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6227,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:29" ht="18">
+    <row r="37" spans="4:30" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6295,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:29" ht="18">
+    <row r="38" spans="4:30" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6363,7 +6384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:29" ht="18">
+    <row r="39" spans="4:30" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6431,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:29" ht="18">
+    <row r="40" spans="4:30" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6510,8 +6531,11 @@
       <c r="AC40" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="4:29" ht="18">
+      <c r="AD40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:30" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6590,8 +6614,11 @@
       <c r="AC41" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="4:29" ht="18">
+      <c r="AD41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:30" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -6670,8 +6697,11 @@
       <c r="AC42" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="4:29" ht="18">
+      <c r="AD42" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="4:30" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -6750,8 +6780,11 @@
       <c r="AC43" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="4:29" ht="18">
+      <c r="AD43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:30" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -6830,8 +6863,11 @@
       <c r="AC44" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="4:29" ht="18">
+      <c r="AD44" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:30" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -6910,8 +6946,11 @@
       <c r="AC45" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="4:29" ht="18">
+      <c r="AD45" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:30" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -6990,8 +7029,11 @@
       <c r="AC46" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="4:29" ht="18">
+      <c r="AD46" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:30" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -7070,8 +7112,11 @@
       <c r="AC47" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="4:29" ht="18">
+      <c r="AD47" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:30" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -7150,8 +7195,11 @@
       <c r="AC48" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:29" ht="18">
+      <c r="AD48" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="4:30" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -7230,8 +7278,11 @@
       <c r="AC49" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="4:29" ht="18">
+      <c r="AD49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:30" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -7310,8 +7361,11 @@
       <c r="AC50" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="4:29" ht="18">
+      <c r="AD50" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:30" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -7390,8 +7444,11 @@
       <c r="AC51" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="4:29" ht="18">
+      <c r="AD51" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:30" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7471,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:29" ht="18">
+    <row r="53" spans="4:30" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -7551,7 +7608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:29" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:30" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -7631,7 +7688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:29" ht="18">
+    <row r="55" spans="4:30" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -7711,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:29" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:30" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -7791,7 +7848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:29" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:30" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -7871,7 +7928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="4:29">
+    <row r="58" spans="4:30">
       <c r="L58" s="27"/>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>
@@ -7893,7 +7950,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravvani date 25/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -471,10 +470,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,26 +782,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -812,12 +811,12 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:52" ht="18">
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -831,7 +830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -845,7 +844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -857,7 +856,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -869,7 +868,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -881,7 +880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -893,7 +892,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -905,7 +904,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -933,7 +932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -955,7 +954,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1104,7 +1103,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1229,7 +1228,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1354,7 +1353,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1479,7 +1478,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1540,7 +1539,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1665,7 +1664,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1750,7 +1749,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1835,7 +1834,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1920,7 +1919,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -2005,7 +2004,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2112,7 +2111,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2219,7 +2218,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2328,7 +2327,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2437,7 +2436,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2564,7 +2563,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2691,7 +2690,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2818,7 +2817,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -2945,7 +2944,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3072,7 +3071,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3199,7 +3198,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3326,7 +3325,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3387,7 +3386,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3514,7 +3513,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3643,7 +3642,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3772,7 +3771,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3901,7 +3900,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3962,7 +3961,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4091,7 +4090,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4218,7 +4217,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4345,7 +4344,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4472,7 +4471,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4619,36 +4618,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y49" workbookViewId="0">
-      <selection activeCell="AJ53" sqref="AJ53"/>
+    <sheetView tabSelected="1" topLeftCell="Y40" workbookViewId="0">
+      <selection activeCell="AE40" sqref="AE40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" customWidth="1"/>
-    <col min="31" max="31" width="11.21875" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="33" width="11.21875" customWidth="1"/>
-    <col min="34" max="34" width="11.33203125" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -4658,12 +4655,12 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:34" ht="18">
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:34" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4677,7 +4674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18">
+    <row r="3" spans="1:34" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4691,7 +4688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="27.6">
+    <row r="4" spans="1:34" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4703,7 +4700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="69">
+    <row r="5" spans="1:34" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4715,7 +4712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="18">
+    <row r="6" spans="1:34" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4727,7 +4724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18">
+    <row r="7" spans="1:34" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4739,7 +4736,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="18">
+    <row r="8" spans="1:34" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4751,7 +4748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18">
+    <row r="9" spans="1:34" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4779,7 +4776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="27.6">
+    <row r="12" spans="1:34" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4801,7 +4798,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:34" ht="28.2">
+    <row r="15" spans="1:34" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4896,7 +4893,7 @@
         <v>40996</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="18">
+    <row r="16" spans="1:34" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -4975,7 +4972,7 @@
       <c r="AC16" s="26">
         <v>0</v>
       </c>
-      <c r="AD16" s="32">
+      <c r="AD16" s="31">
         <v>0</v>
       </c>
       <c r="AE16" s="22"/>
@@ -4983,7 +4980,7 @@
       <c r="AG16" s="22"/>
       <c r="AH16" s="22"/>
     </row>
-    <row r="17" spans="4:34" ht="18">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5062,7 +5059,7 @@
       <c r="AC17" s="26">
         <v>0</v>
       </c>
-      <c r="AD17" s="32">
+      <c r="AD17" s="31">
         <v>0</v>
       </c>
       <c r="AE17" s="22"/>
@@ -5070,7 +5067,7 @@
       <c r="AG17" s="22"/>
       <c r="AH17" s="22"/>
     </row>
-    <row r="18" spans="4:34" ht="18">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5149,7 +5146,7 @@
       <c r="AC18" s="26">
         <v>0</v>
       </c>
-      <c r="AD18" s="32">
+      <c r="AD18" s="31">
         <v>3</v>
       </c>
       <c r="AE18" s="22"/>
@@ -5157,7 +5154,7 @@
       <c r="AG18" s="22"/>
       <c r="AH18" s="22"/>
     </row>
-    <row r="19" spans="4:34" ht="18">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5236,7 +5233,7 @@
       <c r="AC19" s="26">
         <v>0</v>
       </c>
-      <c r="AD19" s="32">
+      <c r="AD19" s="31">
         <v>0</v>
       </c>
       <c r="AE19" s="22"/>
@@ -5244,7 +5241,7 @@
       <c r="AG19" s="22"/>
       <c r="AH19" s="22"/>
     </row>
-    <row r="20" spans="4:34" ht="18">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5319,7 +5316,7 @@
       <c r="AC20" s="30">
         <v>0</v>
       </c>
-      <c r="AD20" s="33">
+      <c r="AD20" s="32">
         <v>2</v>
       </c>
       <c r="AE20" s="22"/>
@@ -5327,7 +5324,7 @@
       <c r="AG20" s="22"/>
       <c r="AH20" s="22"/>
     </row>
-    <row r="21" spans="4:34" ht="18">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5402,7 +5399,7 @@
       <c r="AC21" s="26">
         <v>1</v>
       </c>
-      <c r="AD21" s="32">
+      <c r="AD21" s="31">
         <v>1</v>
       </c>
       <c r="AE21" s="22"/>
@@ -5410,7 +5407,7 @@
       <c r="AG21" s="22"/>
       <c r="AH21" s="22"/>
     </row>
-    <row r="22" spans="4:34" ht="18">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5489,7 +5486,7 @@
       <c r="AC22" s="26">
         <v>0</v>
       </c>
-      <c r="AD22" s="32">
+      <c r="AD22" s="31">
         <v>0</v>
       </c>
       <c r="AE22" s="22"/>
@@ -5497,7 +5494,7 @@
       <c r="AG22" s="22"/>
       <c r="AH22" s="22"/>
     </row>
-    <row r="23" spans="4:34" ht="18">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5576,7 +5573,7 @@
       <c r="AC23" s="26">
         <v>0</v>
       </c>
-      <c r="AD23" s="32">
+      <c r="AD23" s="31">
         <v>3</v>
       </c>
       <c r="AE23" s="22"/>
@@ -5584,7 +5581,7 @@
       <c r="AG23" s="22"/>
       <c r="AH23" s="22"/>
     </row>
-    <row r="24" spans="4:34" ht="18">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5663,7 +5660,7 @@
       <c r="AC24" s="26">
         <v>0</v>
       </c>
-      <c r="AD24" s="32">
+      <c r="AD24" s="31">
         <v>0</v>
       </c>
       <c r="AE24" s="22"/>
@@ -5671,7 +5668,7 @@
       <c r="AG24" s="22"/>
       <c r="AH24" s="22"/>
     </row>
-    <row r="25" spans="4:34" ht="18">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5750,7 +5747,7 @@
       <c r="AC25" s="30">
         <v>0</v>
       </c>
-      <c r="AD25" s="33">
+      <c r="AD25" s="32">
         <v>2</v>
       </c>
       <c r="AE25" s="22"/>
@@ -5758,7 +5755,7 @@
       <c r="AG25" s="22"/>
       <c r="AH25" s="22"/>
     </row>
-    <row r="26" spans="4:34" ht="18">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5837,7 +5834,7 @@
       <c r="AC26" s="26">
         <v>1</v>
       </c>
-      <c r="AD26" s="32">
+      <c r="AD26" s="31">
         <v>1</v>
       </c>
       <c r="AE26" s="22"/>
@@ -5845,7 +5842,7 @@
       <c r="AG26" s="22"/>
       <c r="AH26" s="22"/>
     </row>
-    <row r="27" spans="4:34" ht="18">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -5911,7 +5908,7 @@
       <c r="AG27" s="22"/>
       <c r="AH27" s="22"/>
     </row>
-    <row r="28" spans="4:34" ht="18">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -5973,7 +5970,7 @@
       <c r="AG28" s="22"/>
       <c r="AH28" s="22"/>
     </row>
-    <row r="29" spans="4:34" ht="18">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -6035,7 +6032,7 @@
       <c r="AG29" s="22"/>
       <c r="AH29" s="22"/>
     </row>
-    <row r="30" spans="4:34" ht="18">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -6097,7 +6094,7 @@
       <c r="AG30" s="22"/>
       <c r="AH30" s="22"/>
     </row>
-    <row r="31" spans="4:34" ht="18">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -6159,7 +6156,7 @@
       <c r="AG31" s="22"/>
       <c r="AH31" s="22"/>
     </row>
-    <row r="32" spans="4:34" ht="18">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6215,7 +6212,7 @@
       <c r="AG32" s="22"/>
       <c r="AH32" s="22"/>
     </row>
-    <row r="33" spans="4:34" ht="18">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6271,7 +6268,7 @@
       <c r="AG33" s="22"/>
       <c r="AH33" s="22"/>
     </row>
-    <row r="34" spans="4:34" ht="18">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6350,7 +6347,7 @@
       <c r="AC34" s="22">
         <v>2</v>
       </c>
-      <c r="AD34" s="34">
+      <c r="AD34" s="33">
         <v>1</v>
       </c>
       <c r="AE34" s="22"/>
@@ -6358,7 +6355,7 @@
       <c r="AG34" s="22"/>
       <c r="AH34" s="22"/>
     </row>
-    <row r="35" spans="4:34" ht="18">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6437,7 +6434,7 @@
       <c r="AC35" s="22">
         <v>0</v>
       </c>
-      <c r="AD35" s="34">
+      <c r="AD35" s="33">
         <v>0</v>
       </c>
       <c r="AE35" s="22"/>
@@ -6445,7 +6442,7 @@
       <c r="AG35" s="22"/>
       <c r="AH35" s="22"/>
     </row>
-    <row r="36" spans="4:34" ht="18">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6524,7 +6521,7 @@
       <c r="AC36" s="22">
         <v>0</v>
       </c>
-      <c r="AD36" s="34">
+      <c r="AD36" s="33">
         <v>0</v>
       </c>
       <c r="AE36" s="22"/>
@@ -6532,7 +6529,7 @@
       <c r="AG36" s="22"/>
       <c r="AH36" s="22"/>
     </row>
-    <row r="37" spans="4:34" ht="18">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6611,7 +6608,7 @@
       <c r="AC37" s="22">
         <v>0</v>
       </c>
-      <c r="AD37" s="34">
+      <c r="AD37" s="33">
         <v>0</v>
       </c>
       <c r="AE37" s="22"/>
@@ -6619,7 +6616,7 @@
       <c r="AG37" s="22"/>
       <c r="AH37" s="22"/>
     </row>
-    <row r="38" spans="4:34" ht="18">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6698,7 +6695,7 @@
       <c r="AC38" s="22">
         <v>7</v>
       </c>
-      <c r="AD38" s="34">
+      <c r="AD38" s="33">
         <v>8</v>
       </c>
       <c r="AE38" s="22"/>
@@ -6706,7 +6703,7 @@
       <c r="AG38" s="22"/>
       <c r="AH38" s="22"/>
     </row>
-    <row r="39" spans="4:34" ht="18">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -6785,7 +6782,7 @@
       <c r="AC39" s="22">
         <v>0</v>
       </c>
-      <c r="AD39" s="34">
+      <c r="AD39" s="33">
         <v>3</v>
       </c>
       <c r="AE39" s="22"/>
@@ -6793,7 +6790,7 @@
       <c r="AG39" s="22"/>
       <c r="AH39" s="22"/>
     </row>
-    <row r="40" spans="4:34" ht="18">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -6872,15 +6869,17 @@
       <c r="AC40" s="26">
         <v>0</v>
       </c>
-      <c r="AD40" s="32">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="22"/>
+      <c r="AD40" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="22">
+        <v>0</v>
+      </c>
       <c r="AF40" s="22"/>
       <c r="AG40" s="22"/>
       <c r="AH40" s="22"/>
     </row>
-    <row r="41" spans="4:34" ht="18">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -6959,7 +6958,7 @@
       <c r="AC41" s="26">
         <v>0</v>
       </c>
-      <c r="AD41" s="32">
+      <c r="AD41" s="31">
         <v>0</v>
       </c>
       <c r="AE41" s="22"/>
@@ -6967,7 +6966,7 @@
       <c r="AG41" s="22"/>
       <c r="AH41" s="22"/>
     </row>
-    <row r="42" spans="4:34" ht="18">
+    <row r="42" spans="4:34" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7046,7 +7045,7 @@
       <c r="AC42" s="26">
         <v>0</v>
       </c>
-      <c r="AD42" s="32">
+      <c r="AD42" s="31">
         <v>3</v>
       </c>
       <c r="AE42" s="22"/>
@@ -7054,7 +7053,7 @@
       <c r="AG42" s="22"/>
       <c r="AH42" s="22"/>
     </row>
-    <row r="43" spans="4:34" ht="18">
+    <row r="43" spans="4:34" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7133,7 +7132,7 @@
       <c r="AC43" s="26">
         <v>0</v>
       </c>
-      <c r="AD43" s="32">
+      <c r="AD43" s="31">
         <v>0</v>
       </c>
       <c r="AE43" s="22"/>
@@ -7141,7 +7140,7 @@
       <c r="AG43" s="22"/>
       <c r="AH43" s="22"/>
     </row>
-    <row r="44" spans="4:34" ht="18">
+    <row r="44" spans="4:34" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7220,7 +7219,7 @@
       <c r="AC44" s="30">
         <v>0</v>
       </c>
-      <c r="AD44" s="33">
+      <c r="AD44" s="32">
         <v>2</v>
       </c>
       <c r="AE44" s="22"/>
@@ -7228,7 +7227,7 @@
       <c r="AG44" s="22"/>
       <c r="AH44" s="22"/>
     </row>
-    <row r="45" spans="4:34" ht="18">
+    <row r="45" spans="4:34" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -7307,7 +7306,7 @@
       <c r="AC45" s="26">
         <v>1</v>
       </c>
-      <c r="AD45" s="32">
+      <c r="AD45" s="31">
         <v>1</v>
       </c>
       <c r="AE45" s="22"/>
@@ -7315,7 +7314,7 @@
       <c r="AG45" s="22"/>
       <c r="AH45" s="22"/>
     </row>
-    <row r="46" spans="4:34" ht="18">
+    <row r="46" spans="4:34" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -7394,7 +7393,7 @@
       <c r="AC46" s="26">
         <v>0</v>
       </c>
-      <c r="AD46" s="32">
+      <c r="AD46" s="31">
         <v>0</v>
       </c>
       <c r="AE46" s="22"/>
@@ -7402,7 +7401,7 @@
       <c r="AG46" s="22"/>
       <c r="AH46" s="22"/>
     </row>
-    <row r="47" spans="4:34" ht="18">
+    <row r="47" spans="4:34" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -7481,7 +7480,7 @@
       <c r="AC47" s="26">
         <v>0</v>
       </c>
-      <c r="AD47" s="32">
+      <c r="AD47" s="31">
         <v>0</v>
       </c>
       <c r="AE47" s="22"/>
@@ -7489,7 +7488,7 @@
       <c r="AG47" s="22"/>
       <c r="AH47" s="22"/>
     </row>
-    <row r="48" spans="4:34" ht="18">
+    <row r="48" spans="4:34" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -7568,7 +7567,7 @@
       <c r="AC48" s="26">
         <v>0</v>
       </c>
-      <c r="AD48" s="32">
+      <c r="AD48" s="31">
         <v>3</v>
       </c>
       <c r="AE48" s="22"/>
@@ -7576,7 +7575,7 @@
       <c r="AG48" s="22"/>
       <c r="AH48" s="22"/>
     </row>
-    <row r="49" spans="4:34" ht="18">
+    <row r="49" spans="4:34" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -7655,7 +7654,7 @@
       <c r="AC49" s="26">
         <v>0</v>
       </c>
-      <c r="AD49" s="32">
+      <c r="AD49" s="31">
         <v>0</v>
       </c>
       <c r="AE49" s="22"/>
@@ -7663,7 +7662,7 @@
       <c r="AG49" s="22"/>
       <c r="AH49" s="22"/>
     </row>
-    <row r="50" spans="4:34" ht="18">
+    <row r="50" spans="4:34" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -7742,7 +7741,7 @@
       <c r="AC50" s="30">
         <v>0</v>
       </c>
-      <c r="AD50" s="33">
+      <c r="AD50" s="32">
         <v>2</v>
       </c>
       <c r="AE50" s="22"/>
@@ -7750,7 +7749,7 @@
       <c r="AG50" s="22"/>
       <c r="AH50" s="22"/>
     </row>
-    <row r="51" spans="4:34" ht="18">
+    <row r="51" spans="4:34" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -7829,7 +7828,7 @@
       <c r="AC51" s="26">
         <v>1</v>
       </c>
-      <c r="AD51" s="32">
+      <c r="AD51" s="31">
         <v>1</v>
       </c>
       <c r="AE51" s="22"/>
@@ -7837,7 +7836,7 @@
       <c r="AG51" s="22"/>
       <c r="AH51" s="22"/>
     </row>
-    <row r="52" spans="4:34" ht="18">
+    <row r="52" spans="4:34" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -7916,7 +7915,7 @@
       <c r="AC52" s="29">
         <v>0</v>
       </c>
-      <c r="AD52" s="32">
+      <c r="AD52" s="31">
         <v>0</v>
       </c>
       <c r="AE52" s="26">
@@ -7926,7 +7925,7 @@
       <c r="AG52" s="22"/>
       <c r="AH52" s="22"/>
     </row>
-    <row r="53" spans="4:34" ht="18">
+    <row r="53" spans="4:34" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8005,7 +8004,7 @@
       <c r="AC53" s="29">
         <v>0</v>
       </c>
-      <c r="AD53" s="32">
+      <c r="AD53" s="31">
         <v>0</v>
       </c>
       <c r="AE53" s="26">
@@ -8015,7 +8014,7 @@
       <c r="AG53" s="22"/>
       <c r="AH53" s="22"/>
     </row>
-    <row r="54" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:34" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -8094,7 +8093,7 @@
       <c r="AC54" s="29">
         <v>0</v>
       </c>
-      <c r="AD54" s="32">
+      <c r="AD54" s="31">
         <v>3</v>
       </c>
       <c r="AE54" s="26">
@@ -8104,7 +8103,7 @@
       <c r="AG54" s="22"/>
       <c r="AH54" s="22"/>
     </row>
-    <row r="55" spans="4:34" ht="18">
+    <row r="55" spans="4:34" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -8183,7 +8182,7 @@
       <c r="AC55" s="29">
         <v>0</v>
       </c>
-      <c r="AD55" s="32">
+      <c r="AD55" s="31">
         <v>0</v>
       </c>
       <c r="AE55" s="26">
@@ -8193,7 +8192,7 @@
       <c r="AG55" s="22"/>
       <c r="AH55" s="22"/>
     </row>
-    <row r="56" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:34" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -8272,7 +8271,7 @@
       <c r="AC56" s="29">
         <v>0</v>
       </c>
-      <c r="AD56" s="32">
+      <c r="AD56" s="31">
         <v>0</v>
       </c>
       <c r="AE56" s="26">
@@ -8282,7 +8281,7 @@
       <c r="AG56" s="22"/>
       <c r="AH56" s="22"/>
     </row>
-    <row r="57" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:34" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -8361,7 +8360,7 @@
       <c r="AC57" s="29">
         <v>1</v>
       </c>
-      <c r="AD57" s="32">
+      <c r="AD57" s="31">
         <v>1</v>
       </c>
       <c r="AE57" s="26">
@@ -8393,7 +8392,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:25-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4618,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y40" workbookViewId="0">
-      <selection activeCell="AE40" sqref="AE40"/>
+    <sheetView tabSelected="1" topLeftCell="V40" workbookViewId="0">
+      <selection activeCell="AE44" sqref="AE44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6872,7 +6872,7 @@
       <c r="AD40" s="31">
         <v>0</v>
       </c>
-      <c r="AE40" s="22">
+      <c r="AE40" s="31">
         <v>0</v>
       </c>
       <c r="AF40" s="22"/>
@@ -6961,7 +6961,9 @@
       <c r="AD41" s="31">
         <v>0</v>
       </c>
-      <c r="AE41" s="22"/>
+      <c r="AE41" s="31">
+        <v>0</v>
+      </c>
       <c r="AF41" s="22"/>
       <c r="AG41" s="22"/>
       <c r="AH41" s="22"/>
@@ -7048,7 +7050,9 @@
       <c r="AD42" s="31">
         <v>3</v>
       </c>
-      <c r="AE42" s="22"/>
+      <c r="AE42" s="31">
+        <v>0</v>
+      </c>
       <c r="AF42" s="22"/>
       <c r="AG42" s="22"/>
       <c r="AH42" s="22"/>
@@ -7135,7 +7139,9 @@
       <c r="AD43" s="31">
         <v>0</v>
       </c>
-      <c r="AE43" s="22"/>
+      <c r="AE43" s="31">
+        <v>0</v>
+      </c>
       <c r="AF43" s="22"/>
       <c r="AG43" s="22"/>
       <c r="AH43" s="22"/>
@@ -7222,7 +7228,9 @@
       <c r="AD44" s="32">
         <v>2</v>
       </c>
-      <c r="AE44" s="22"/>
+      <c r="AE44" s="31">
+        <v>2</v>
+      </c>
       <c r="AF44" s="22"/>
       <c r="AG44" s="22"/>
       <c r="AH44" s="22"/>
@@ -7309,7 +7317,9 @@
       <c r="AD45" s="31">
         <v>1</v>
       </c>
-      <c r="AE45" s="22"/>
+      <c r="AE45" s="31">
+        <v>0</v>
+      </c>
       <c r="AF45" s="22"/>
       <c r="AG45" s="22"/>
       <c r="AH45" s="22"/>
@@ -7396,7 +7406,9 @@
       <c r="AD46" s="31">
         <v>0</v>
       </c>
-      <c r="AE46" s="22"/>
+      <c r="AE46" s="31">
+        <v>0</v>
+      </c>
       <c r="AF46" s="22"/>
       <c r="AG46" s="22"/>
       <c r="AH46" s="22"/>
@@ -7483,7 +7495,9 @@
       <c r="AD47" s="31">
         <v>0</v>
       </c>
-      <c r="AE47" s="22"/>
+      <c r="AE47" s="31">
+        <v>0</v>
+      </c>
       <c r="AF47" s="22"/>
       <c r="AG47" s="22"/>
       <c r="AH47" s="22"/>
@@ -7570,7 +7584,9 @@
       <c r="AD48" s="31">
         <v>3</v>
       </c>
-      <c r="AE48" s="22"/>
+      <c r="AE48" s="31">
+        <v>0</v>
+      </c>
       <c r="AF48" s="22"/>
       <c r="AG48" s="22"/>
       <c r="AH48" s="22"/>
@@ -7657,7 +7673,9 @@
       <c r="AD49" s="31">
         <v>0</v>
       </c>
-      <c r="AE49" s="22"/>
+      <c r="AE49" s="31">
+        <v>0</v>
+      </c>
       <c r="AF49" s="22"/>
       <c r="AG49" s="22"/>
       <c r="AH49" s="22"/>
@@ -7744,7 +7762,9 @@
       <c r="AD50" s="32">
         <v>2</v>
       </c>
-      <c r="AE50" s="22"/>
+      <c r="AE50" s="31">
+        <v>2</v>
+      </c>
       <c r="AF50" s="22"/>
       <c r="AG50" s="22"/>
       <c r="AH50" s="22"/>
@@ -7831,7 +7851,9 @@
       <c r="AD51" s="31">
         <v>1</v>
       </c>
-      <c r="AE51" s="22"/>
+      <c r="AE51" s="31">
+        <v>0</v>
+      </c>
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="22"/>

</xml_diff>

<commit_message>
updated by Alpna date:25-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4618,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V40" workbookViewId="0">
-      <selection activeCell="AE44" sqref="AE44"/>
+    <sheetView tabSelected="1" topLeftCell="R10" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16:AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4975,7 +4975,9 @@
       <c r="AD16" s="31">
         <v>0</v>
       </c>
-      <c r="AE16" s="22"/>
+      <c r="AE16" s="31">
+        <v>0</v>
+      </c>
       <c r="AF16" s="22"/>
       <c r="AG16" s="22"/>
       <c r="AH16" s="22"/>
@@ -5062,7 +5064,9 @@
       <c r="AD17" s="31">
         <v>0</v>
       </c>
-      <c r="AE17" s="22"/>
+      <c r="AE17" s="31">
+        <v>0</v>
+      </c>
       <c r="AF17" s="22"/>
       <c r="AG17" s="22"/>
       <c r="AH17" s="22"/>
@@ -5149,7 +5153,9 @@
       <c r="AD18" s="31">
         <v>3</v>
       </c>
-      <c r="AE18" s="22"/>
+      <c r="AE18" s="31">
+        <v>0</v>
+      </c>
       <c r="AF18" s="22"/>
       <c r="AG18" s="22"/>
       <c r="AH18" s="22"/>
@@ -5236,7 +5242,9 @@
       <c r="AD19" s="31">
         <v>0</v>
       </c>
-      <c r="AE19" s="22"/>
+      <c r="AE19" s="31">
+        <v>0</v>
+      </c>
       <c r="AF19" s="22"/>
       <c r="AG19" s="22"/>
       <c r="AH19" s="22"/>
@@ -5319,7 +5327,9 @@
       <c r="AD20" s="32">
         <v>2</v>
       </c>
-      <c r="AE20" s="22"/>
+      <c r="AE20" s="31">
+        <v>2</v>
+      </c>
       <c r="AF20" s="22"/>
       <c r="AG20" s="22"/>
       <c r="AH20" s="22"/>
@@ -5402,7 +5412,9 @@
       <c r="AD21" s="31">
         <v>1</v>
       </c>
-      <c r="AE21" s="22"/>
+      <c r="AE21" s="31">
+        <v>0</v>
+      </c>
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
       <c r="AH21" s="22"/>

</xml_diff>

<commit_message>
updated by sravvani date:27/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -4619,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X32" workbookViewId="0">
-      <selection activeCell="AH34" sqref="AH34"/>
+    <sheetView tabSelected="1" topLeftCell="X38" workbookViewId="0">
+      <selection activeCell="AG40" sqref="AG40:AG51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6963,7 +6962,9 @@
       <c r="AF40" s="31">
         <v>0</v>
       </c>
-      <c r="AG40" s="22"/>
+      <c r="AG40" s="31">
+        <v>0</v>
+      </c>
       <c r="AH40" s="22"/>
     </row>
     <row r="41" spans="4:34" ht="17.25">
@@ -7054,7 +7055,9 @@
       <c r="AF41" s="31">
         <v>0</v>
       </c>
-      <c r="AG41" s="22"/>
+      <c r="AG41" s="31">
+        <v>0</v>
+      </c>
       <c r="AH41" s="22"/>
     </row>
     <row r="42" spans="4:34" ht="17.25">
@@ -7145,7 +7148,9 @@
       <c r="AF42" s="31">
         <v>0</v>
       </c>
-      <c r="AG42" s="22"/>
+      <c r="AG42" s="31">
+        <v>0</v>
+      </c>
       <c r="AH42" s="22"/>
     </row>
     <row r="43" spans="4:34" ht="17.25">
@@ -7236,7 +7241,9 @@
       <c r="AF43" s="31">
         <v>0</v>
       </c>
-      <c r="AG43" s="22"/>
+      <c r="AG43" s="31">
+        <v>0</v>
+      </c>
       <c r="AH43" s="22"/>
     </row>
     <row r="44" spans="4:34" ht="17.25">
@@ -7327,7 +7334,9 @@
       <c r="AF44" s="31">
         <v>2</v>
       </c>
-      <c r="AG44" s="22"/>
+      <c r="AG44" s="31">
+        <v>2</v>
+      </c>
       <c r="AH44" s="22"/>
     </row>
     <row r="45" spans="4:34" ht="17.25">
@@ -7418,7 +7427,9 @@
       <c r="AF45" s="31">
         <v>0</v>
       </c>
-      <c r="AG45" s="22"/>
+      <c r="AG45" s="31">
+        <v>0</v>
+      </c>
       <c r="AH45" s="22"/>
     </row>
     <row r="46" spans="4:34" ht="17.25">
@@ -7509,7 +7520,9 @@
       <c r="AF46" s="31">
         <v>0</v>
       </c>
-      <c r="AG46" s="22"/>
+      <c r="AG46" s="31">
+        <v>0</v>
+      </c>
       <c r="AH46" s="22"/>
     </row>
     <row r="47" spans="4:34" ht="17.25">
@@ -7600,7 +7613,9 @@
       <c r="AF47" s="31">
         <v>0</v>
       </c>
-      <c r="AG47" s="22"/>
+      <c r="AG47" s="31">
+        <v>0</v>
+      </c>
       <c r="AH47" s="22"/>
     </row>
     <row r="48" spans="4:34" ht="17.25">
@@ -7691,7 +7706,9 @@
       <c r="AF48" s="31">
         <v>0</v>
       </c>
-      <c r="AG48" s="22"/>
+      <c r="AG48" s="31">
+        <v>0</v>
+      </c>
       <c r="AH48" s="22"/>
     </row>
     <row r="49" spans="4:34" ht="17.25">
@@ -7782,7 +7799,9 @@
       <c r="AF49" s="31">
         <v>0</v>
       </c>
-      <c r="AG49" s="22"/>
+      <c r="AG49" s="31">
+        <v>0</v>
+      </c>
       <c r="AH49" s="22"/>
     </row>
     <row r="50" spans="4:34" ht="17.25">
@@ -7873,7 +7892,9 @@
       <c r="AF50" s="31">
         <v>2</v>
       </c>
-      <c r="AG50" s="22"/>
+      <c r="AG50" s="31">
+        <v>2</v>
+      </c>
       <c r="AH50" s="22"/>
     </row>
     <row r="51" spans="4:34" ht="17.25">
@@ -7964,7 +7985,9 @@
       <c r="AF51" s="31">
         <v>0</v>
       </c>
-      <c r="AG51" s="22"/>
+      <c r="AG51" s="31">
+        <v>0</v>
+      </c>
       <c r="AH51" s="22"/>
     </row>
     <row r="52" spans="4:34" ht="17.25">

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:27-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4618,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X38" workbookViewId="0">
-      <selection activeCell="AG40" sqref="AG40:AG51"/>
+    <sheetView tabSelected="1" topLeftCell="X11" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16:AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4981,7 +4981,9 @@
       <c r="AF16" s="31">
         <v>0</v>
       </c>
-      <c r="AG16" s="22"/>
+      <c r="AG16" s="31">
+        <v>0</v>
+      </c>
       <c r="AH16" s="22"/>
     </row>
     <row r="17" spans="4:34" ht="17.25">
@@ -5072,7 +5074,9 @@
       <c r="AF17" s="31">
         <v>0</v>
       </c>
-      <c r="AG17" s="22"/>
+      <c r="AG17" s="31">
+        <v>0</v>
+      </c>
       <c r="AH17" s="22"/>
     </row>
     <row r="18" spans="4:34" ht="17.25">
@@ -5163,7 +5167,9 @@
       <c r="AF18" s="31">
         <v>0</v>
       </c>
-      <c r="AG18" s="22"/>
+      <c r="AG18" s="31">
+        <v>0</v>
+      </c>
       <c r="AH18" s="22"/>
     </row>
     <row r="19" spans="4:34" ht="17.25">
@@ -5254,7 +5260,9 @@
       <c r="AF19" s="31">
         <v>0</v>
       </c>
-      <c r="AG19" s="22"/>
+      <c r="AG19" s="31">
+        <v>0</v>
+      </c>
       <c r="AH19" s="22"/>
     </row>
     <row r="20" spans="4:34" ht="17.25">
@@ -5341,7 +5349,9 @@
       <c r="AF20" s="31">
         <v>2</v>
       </c>
-      <c r="AG20" s="22"/>
+      <c r="AG20" s="31">
+        <v>2</v>
+      </c>
       <c r="AH20" s="22"/>
     </row>
     <row r="21" spans="4:34" ht="17.25">
@@ -5428,7 +5438,9 @@
       <c r="AF21" s="31">
         <v>0</v>
       </c>
-      <c r="AG21" s="22"/>
+      <c r="AG21" s="31">
+        <v>0</v>
+      </c>
       <c r="AH21" s="22"/>
     </row>
     <row r="22" spans="4:34" ht="17.25">

</xml_diff>

<commit_message>
updated by Alpna date:27-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -11,7 +11,7 @@
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -4616,10 +4616,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH58"/>
+  <dimension ref="A1:AI58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X11" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16:AG21"/>
+      <selection activeCell="AI15" sqref="AI15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4646,9 +4646,10 @@
     <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
     <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4660,7 +4661,7 @@
       </c>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:34" ht="17.25">
+    <row r="2" spans="1:35" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4674,7 +4675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25">
+    <row r="3" spans="1:35" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="28.5">
+    <row r="4" spans="1:35" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="71.25">
+    <row r="5" spans="1:35" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17.25">
+    <row r="6" spans="1:35" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4724,7 +4725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17.25">
+    <row r="7" spans="1:35" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4736,7 +4737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17.25">
+    <row r="8" spans="1:35" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4748,7 +4749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17.25">
+    <row r="9" spans="1:35" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4760,7 +4761,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -4776,7 +4777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="42.75">
+    <row r="12" spans="1:35" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4784,21 +4785,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:35">
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:35">
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:34" ht="30">
+    <row r="15" spans="1:35" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4892,8 +4893,11 @@
       <c r="AH15" s="25">
         <v>40996</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" ht="17.25">
+      <c r="AI15" s="25">
+        <v>40997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
updated by Alpna date:30-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="14745" windowHeight="6390" activeTab="1"/>
@@ -11,7 +11,7 @@
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -166,11 +166,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,7 +405,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -483,7 +483,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -577,7 +576,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -612,7 +610,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -788,14 +785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ47"/>
   <sheetViews>
     <sheetView topLeftCell="AN7" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -817,19 +814,19 @@
     <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="36"/>
-    </row>
-    <row r="2" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -843,7 +840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -857,7 +854,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -869,7 +866,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -881,7 +878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -893,7 +890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -905,7 +902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -917,7 +914,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -929,7 +926,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -937,7 +934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -945,7 +942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -953,21 +950,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52">
       <c r="AN13" s="27"/>
       <c r="AO13" s="27"/>
       <c r="AP13" s="27"/>
       <c r="AQ13" s="27"/>
       <c r="AR13" s="27"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52">
       <c r="AN14" s="27"/>
       <c r="AO14" s="27"/>
       <c r="AP14" s="27"/>
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1241,7 +1238,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1366,7 +1363,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1491,7 +1488,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1552,7 +1549,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1677,7 +1674,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1762,7 +1759,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1847,7 +1844,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1932,7 +1929,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -2017,7 +2014,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2124,7 +2121,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2231,7 +2228,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2340,7 +2337,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2449,7 +2446,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2576,7 +2573,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2703,7 +2700,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2830,7 +2827,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -2957,7 +2954,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3084,7 +3081,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3211,7 +3208,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3338,7 +3335,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3399,7 +3396,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3526,7 +3523,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3655,7 +3652,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3784,7 +3781,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3913,7 +3910,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3974,7 +3971,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4103,7 +4100,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4230,7 +4227,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4357,7 +4354,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4484,7 +4481,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4611,7 +4608,7 @@
       <c r="AY46" s="26"/>
       <c r="AZ46" s="26"/>
     </row>
-    <row r="47" spans="4:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:52">
       <c r="AN47" s="27"/>
       <c r="AO47" s="27"/>
       <c r="AP47" s="27"/>
@@ -4628,14 +4625,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y39" workbookViewId="0">
-      <selection activeCell="AI39" sqref="AI39"/>
+    <sheetView tabSelected="1" topLeftCell="Y15" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16:AJ21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -4660,21 +4657,22 @@
     <col min="32" max="32" width="11" customWidth="1"/>
     <col min="33" max="34" width="11.28515625" customWidth="1"/>
     <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="36"/>
-    </row>
-    <row r="2" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4688,7 +4686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4702,7 +4700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4714,7 +4712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4726,7 +4724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4738,7 +4736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4750,7 +4748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4762,7 +4760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4774,7 +4772,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4782,7 +4780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -4790,7 +4788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4798,21 +4796,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36">
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36">
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4909,8 +4907,11 @@
       <c r="AI15" s="25">
         <v>40997</v>
       </c>
-    </row>
-    <row r="16" spans="1:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ15" s="25">
+        <v>40998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5001,14 +5002,17 @@
       <c r="AG16" s="31">
         <v>0</v>
       </c>
-      <c r="AH16" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AH16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:36" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5099,14 +5103,17 @@
       <c r="AG17" s="31">
         <v>0</v>
       </c>
-      <c r="AH17" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AH17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:36" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5197,14 +5204,17 @@
       <c r="AG18" s="31">
         <v>0</v>
       </c>
-      <c r="AH18" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AH18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:36" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5295,14 +5305,17 @@
       <c r="AG19" s="31">
         <v>0</v>
       </c>
-      <c r="AH19" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AH19" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:36" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5389,14 +5402,17 @@
       <c r="AG20" s="31">
         <v>2</v>
       </c>
-      <c r="AH20" s="22">
+      <c r="AH20" s="26">
         <v>2</v>
       </c>
-      <c r="AI20" s="35">
+      <c r="AI20" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AJ20" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:36" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5483,14 +5499,17 @@
       <c r="AG21" s="31">
         <v>0</v>
       </c>
-      <c r="AH21" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI21" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AH21" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:36" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5585,7 +5604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:36" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5680,7 +5699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:36" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5775,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:36" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5870,7 +5889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:36" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -5965,7 +5984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:36" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -6060,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:36" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -6133,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:36" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -6206,7 +6225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:36" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -6279,7 +6298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:36" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -6352,7 +6371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:36" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6419,7 +6438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:35" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6486,7 +6505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:35" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6579,7 +6598,7 @@
       </c>
       <c r="AH34" s="22"/>
     </row>
-    <row r="35" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:35" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6672,7 +6691,7 @@
       </c>
       <c r="AH35" s="22"/>
     </row>
-    <row r="36" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:35" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6765,7 +6784,7 @@
       </c>
       <c r="AH36" s="22"/>
     </row>
-    <row r="37" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:35" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6858,7 +6877,7 @@
       </c>
       <c r="AH37" s="22"/>
     </row>
-    <row r="38" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:35" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6951,7 +6970,7 @@
       </c>
       <c r="AH38" s="22"/>
     </row>
-    <row r="39" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:35" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -7044,7 +7063,7 @@
       </c>
       <c r="AH39" s="22"/>
     </row>
-    <row r="40" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:35" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -7142,7 +7161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:35" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -7240,7 +7259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:35" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7338,7 +7357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:35" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7436,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:35" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7534,7 +7553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:35" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -7632,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:35" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -7730,7 +7749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:35" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -7828,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:35" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -7926,7 +7945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:35" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -8024,7 +8043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:35" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -8122,7 +8141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:35" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -8220,7 +8239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:35" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -8318,7 +8337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:35" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8416,7 +8435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:35" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -8514,7 +8533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:35" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:35" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -8612,7 +8631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:35" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -8710,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:35" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -8808,7 +8827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:35" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:35">
       <c r="L58" s="27"/>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>
@@ -8820,17 +8839,17 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by sravvani date:30/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4628,8 +4628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y15" workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16:AJ21"/>
+    <sheetView tabSelected="1" topLeftCell="V35" workbookViewId="0">
+      <selection activeCell="AH46" sqref="AH46:AH51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7154,10 +7154,10 @@
       <c r="AG40" s="31">
         <v>0</v>
       </c>
-      <c r="AH40" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI40" s="32">
+      <c r="AH40" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="26">
         <v>0</v>
       </c>
     </row>
@@ -7252,10 +7252,10 @@
       <c r="AG41" s="31">
         <v>0</v>
       </c>
-      <c r="AH41" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI41" s="32">
+      <c r="AH41" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI41" s="26">
         <v>0</v>
       </c>
     </row>
@@ -7350,10 +7350,10 @@
       <c r="AG42" s="31">
         <v>0</v>
       </c>
-      <c r="AH42" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI42" s="32">
+      <c r="AH42" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="26">
         <v>0</v>
       </c>
     </row>
@@ -7448,10 +7448,10 @@
       <c r="AG43" s="31">
         <v>0</v>
       </c>
-      <c r="AH43" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI43" s="32">
+      <c r="AH43" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="26">
         <v>0</v>
       </c>
     </row>
@@ -7546,11 +7546,11 @@
       <c r="AG44" s="31">
         <v>2</v>
       </c>
-      <c r="AH44" s="22">
+      <c r="AH44" s="26">
         <v>2</v>
       </c>
-      <c r="AI44" s="32">
-        <v>0</v>
+      <c r="AI44" s="26">
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="4:35" ht="17.25">
@@ -7644,10 +7644,10 @@
       <c r="AG45" s="31">
         <v>0</v>
       </c>
-      <c r="AH45" s="22">
-        <v>0</v>
-      </c>
-      <c r="AI45" s="32">
+      <c r="AH45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI45" s="26">
         <v>0</v>
       </c>
     </row>
@@ -7742,7 +7742,7 @@
       <c r="AG46" s="31">
         <v>0</v>
       </c>
-      <c r="AH46" s="22">
+      <c r="AH46" s="26">
         <v>0</v>
       </c>
       <c r="AI46" s="32">
@@ -7840,7 +7840,7 @@
       <c r="AG47" s="31">
         <v>0</v>
       </c>
-      <c r="AH47" s="22">
+      <c r="AH47" s="26">
         <v>0</v>
       </c>
       <c r="AI47" s="32">
@@ -7938,7 +7938,7 @@
       <c r="AG48" s="31">
         <v>0</v>
       </c>
-      <c r="AH48" s="22">
+      <c r="AH48" s="26">
         <v>0</v>
       </c>
       <c r="AI48" s="32">
@@ -8036,7 +8036,7 @@
       <c r="AG49" s="31">
         <v>0</v>
       </c>
-      <c r="AH49" s="22">
+      <c r="AH49" s="26">
         <v>0</v>
       </c>
       <c r="AI49" s="32">
@@ -8134,7 +8134,7 @@
       <c r="AG50" s="31">
         <v>2</v>
       </c>
-      <c r="AH50" s="22">
+      <c r="AH50" s="26">
         <v>2</v>
       </c>
       <c r="AI50" s="32">
@@ -8232,7 +8232,7 @@
       <c r="AG51" s="31">
         <v>0</v>
       </c>
-      <c r="AH51" s="22">
+      <c r="AH51" s="26">
         <v>0</v>
       </c>
       <c r="AI51" s="32">

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:30-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4628,8 +4628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V35" workbookViewId="0">
-      <selection activeCell="AH46" sqref="AH46:AH51"/>
+    <sheetView tabSelected="1" topLeftCell="V38" workbookViewId="0">
+      <selection activeCell="AJ46" sqref="AJ46:AJ51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6438,7 +6438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:35" ht="17.25">
+    <row r="33" spans="4:36" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:35" ht="17.25">
+    <row r="34" spans="4:36" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="AH34" s="22"/>
     </row>
-    <row r="35" spans="4:35" ht="17.25">
+    <row r="35" spans="4:36" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6691,7 +6691,7 @@
       </c>
       <c r="AH35" s="22"/>
     </row>
-    <row r="36" spans="4:35" ht="17.25">
+    <row r="36" spans="4:36" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6784,7 +6784,7 @@
       </c>
       <c r="AH36" s="22"/>
     </row>
-    <row r="37" spans="4:35" ht="17.25">
+    <row r="37" spans="4:36" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6877,7 +6877,7 @@
       </c>
       <c r="AH37" s="22"/>
     </row>
-    <row r="38" spans="4:35" ht="17.25">
+    <row r="38" spans="4:36" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -6970,7 +6970,7 @@
       </c>
       <c r="AH38" s="22"/>
     </row>
-    <row r="39" spans="4:35" ht="17.25">
+    <row r="39" spans="4:36" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -7063,7 +7063,7 @@
       </c>
       <c r="AH39" s="22"/>
     </row>
-    <row r="40" spans="4:35" ht="17.25">
+    <row r="40" spans="4:36" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -7160,8 +7160,11 @@
       <c r="AI40" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="4:35" ht="17.25">
+      <c r="AJ40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:36" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -7258,8 +7261,11 @@
       <c r="AI41" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="4:35" ht="17.25">
+      <c r="AJ41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:36" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7356,8 +7362,11 @@
       <c r="AI42" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="4:35" ht="17.25">
+      <c r="AJ42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:36" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7454,8 +7463,11 @@
       <c r="AI43" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="4:35" ht="17.25">
+      <c r="AJ43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:36" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7552,8 +7564,11 @@
       <c r="AI44" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="4:35" ht="17.25">
+      <c r="AJ44" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:36" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -7650,8 +7665,11 @@
       <c r="AI45" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="4:35" ht="17.25">
+      <c r="AJ45" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:36" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -7745,11 +7763,14 @@
       <c r="AH46" s="26">
         <v>0</v>
       </c>
-      <c r="AI46" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="4:35" ht="17.25">
+      <c r="AI46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:36" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -7843,11 +7864,14 @@
       <c r="AH47" s="26">
         <v>0</v>
       </c>
-      <c r="AI47" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="4:35" ht="17.25">
+      <c r="AI47" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:36" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -7941,11 +7965,14 @@
       <c r="AH48" s="26">
         <v>0</v>
       </c>
-      <c r="AI48" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:35" ht="17.25">
+      <c r="AI48" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:36" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -8039,11 +8066,14 @@
       <c r="AH49" s="26">
         <v>0</v>
       </c>
-      <c r="AI49" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:35" ht="17.25">
+      <c r="AI49" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:36" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -8137,11 +8167,14 @@
       <c r="AH50" s="26">
         <v>2</v>
       </c>
-      <c r="AI50" s="32">
+      <c r="AI50" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="4:35" ht="17.25">
+      <c r="AJ50" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:36" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -8235,11 +8268,14 @@
       <c r="AH51" s="26">
         <v>0</v>
       </c>
-      <c r="AI51" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="4:35" ht="17.25">
+      <c r="AI51" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:36" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -8337,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:35" ht="17.25">
+    <row r="53" spans="4:36" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8435,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:35" ht="18" thickBot="1">
+    <row r="54" spans="4:36" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -8533,7 +8569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:35" ht="17.25">
+    <row r="55" spans="4:36" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -8631,7 +8667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:35" ht="18" thickBot="1">
+    <row r="56" spans="4:36" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -8729,7 +8765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:35" ht="18" thickBot="1">
+    <row r="57" spans="4:36" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -8827,7 +8863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:35">
+    <row r="58" spans="4:36">
       <c r="L58" s="27"/>
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>

</xml_diff>

<commit_message>
updated by sravvani date:31/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -808,26 +807,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -842,7 +841,7 @@
       </c>
       <c r="E1" s="37"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -856,7 +855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -870,7 +869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -882,7 +881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -894,7 +893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -906,7 +905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -918,7 +917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -930,7 +929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -958,7 +957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -980,7 +979,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1129,7 +1128,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1254,7 +1253,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1379,7 +1378,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1504,7 +1503,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1565,7 +1564,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1690,7 +1689,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1775,7 +1774,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1860,7 +1859,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1945,7 +1944,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -2030,7 +2029,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2137,7 +2136,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2244,7 +2243,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2353,7 +2352,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2462,7 +2461,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2589,7 +2588,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2716,7 +2715,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2843,7 +2842,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -2970,7 +2969,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3097,7 +3096,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3224,7 +3223,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3351,7 +3350,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3412,7 +3411,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3539,7 +3538,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3668,7 +3667,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3797,7 +3796,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3926,7 +3925,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3987,7 +3986,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4116,7 +4115,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4243,7 +4242,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4370,7 +4369,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4497,7 +4496,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4644,37 +4643,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z49" workbookViewId="0">
-      <selection activeCell="AK58" sqref="AK58"/>
+    <sheetView tabSelected="1" topLeftCell="X15" workbookViewId="0">
+      <selection activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
-    <col min="37" max="37" width="11.77734375" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -4689,7 +4688,7 @@
       </c>
       <c r="E1" s="37"/>
     </row>
-    <row r="2" spans="1:37" ht="18">
+    <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4703,7 +4702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="18">
+    <row r="3" spans="1:37" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="27.6">
+    <row r="4" spans="1:37" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4729,7 +4728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="69">
+    <row r="5" spans="1:37" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4741,7 +4740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="18">
+    <row r="6" spans="1:37" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="18">
+    <row r="7" spans="1:37" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4765,7 +4764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="18">
+    <row r="8" spans="1:37" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="18">
+    <row r="9" spans="1:37" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4805,7 +4804,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="27.6">
+    <row r="12" spans="1:37" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4827,7 +4826,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:37" ht="28.2">
+    <row r="15" spans="1:37" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4931,7 +4930,7 @@
         <v>40999</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="18">
+    <row r="16" spans="1:37" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5031,8 +5030,11 @@
       <c r="AJ16" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="4:36" ht="18">
+      <c r="AK16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:37" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5132,8 +5134,11 @@
       <c r="AJ17" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="4:36" ht="18">
+      <c r="AK17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:37" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5233,8 +5238,11 @@
       <c r="AJ18" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="4:36" ht="18">
+      <c r="AK18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:37" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5334,8 +5342,11 @@
       <c r="AJ19" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="4:36" ht="18">
+      <c r="AK19" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:37" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5431,8 +5442,11 @@
       <c r="AJ20" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="4:36" ht="18">
+      <c r="AK20" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:37" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5528,8 +5542,11 @@
       <c r="AJ21" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="4:36" ht="18">
+      <c r="AK21" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:37" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5624,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:36" ht="18">
+    <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5719,7 +5736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:36" ht="18">
+    <row r="24" spans="4:37" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5814,7 +5831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:36" ht="18">
+    <row r="25" spans="4:37" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5909,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:36" ht="18">
+    <row r="26" spans="4:37" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -6004,7 +6021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="4:36" ht="18">
+    <row r="27" spans="4:37" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -6099,7 +6116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:36" ht="18">
+    <row r="28" spans="4:37" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -6172,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:36" ht="18">
+    <row r="29" spans="4:37" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -6245,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:36" ht="18">
+    <row r="30" spans="4:37" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -6318,7 +6335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="4:36" ht="18">
+    <row r="31" spans="4:37" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -6391,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:36" ht="18">
+    <row r="32" spans="4:37" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6458,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:37" ht="18">
+    <row r="33" spans="4:37" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6525,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:37" ht="18">
+    <row r="34" spans="4:37" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6629,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:37" ht="18">
+    <row r="35" spans="4:37" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -6733,7 +6750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:37" ht="18">
+    <row r="36" spans="4:37" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -6837,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:37" ht="18">
+    <row r="37" spans="4:37" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -6941,7 +6958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:37" ht="18">
+    <row r="38" spans="4:37" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -7045,7 +7062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:37" ht="18">
+    <row r="39" spans="4:37" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -7149,7 +7166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:37" ht="18">
+    <row r="40" spans="4:37" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -7249,8 +7266,11 @@
       <c r="AJ40" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="4:37" ht="18">
+      <c r="AK40" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:37" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -7350,8 +7370,11 @@
       <c r="AJ41" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="4:37" ht="18">
+      <c r="AK41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:37" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7451,8 +7474,11 @@
       <c r="AJ42" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="4:37" ht="18">
+      <c r="AK42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:37" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7552,8 +7578,11 @@
       <c r="AJ43" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="4:37" ht="18">
+      <c r="AK43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:37" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7653,8 +7682,11 @@
       <c r="AJ44" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="4:37" ht="18">
+      <c r="AK44" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="4:37" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -7754,8 +7786,11 @@
       <c r="AJ45" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="4:37" ht="18">
+      <c r="AK45" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:37" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -7855,8 +7890,11 @@
       <c r="AJ46" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="4:37" ht="18">
+      <c r="AK46" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:37" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -7956,8 +7994,11 @@
       <c r="AJ47" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="4:37" ht="18">
+      <c r="AK47" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:37" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -8057,8 +8098,11 @@
       <c r="AJ48" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="4:37" ht="18">
+      <c r="AK48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:37" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -8158,8 +8202,11 @@
       <c r="AJ49" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="4:37" ht="18">
+      <c r="AK49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:37" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -8259,8 +8306,11 @@
       <c r="AJ50" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="4:37" ht="18">
+      <c r="AK50" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="4:37" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -8360,8 +8410,11 @@
       <c r="AJ51" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="4:37" ht="18">
+      <c r="AK51" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:37" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -8465,7 +8518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:37" ht="18">
+    <row r="53" spans="4:37" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8569,7 +8622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:37" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -8673,7 +8726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:37" ht="18">
+    <row r="55" spans="4:37" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -8777,7 +8830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:37" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -8881,7 +8934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:37" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -9007,7 +9060,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated by Alpna date 31-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4644,7 +4644,7 @@
   <dimension ref="A1:AK58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X15" workbookViewId="0">
-      <selection activeCell="AK20" sqref="AK20"/>
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5640,6 +5640,9 @@
       <c r="AH22" s="22">
         <v>0</v>
       </c>
+      <c r="AK22" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="18" t="s">

</xml_diff>

<commit_message>
Done by B.S.Deepthi date 31-03-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4643,8 +4643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X15" workbookViewId="0">
-      <selection activeCell="AK22" sqref="AK22"/>
+    <sheetView tabSelected="1" topLeftCell="X38" workbookViewId="0">
+      <selection activeCell="AK51" sqref="AK51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5543,7 +5543,7 @@
         <v>0</v>
       </c>
       <c r="AK21" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="4:37" ht="17.25">
@@ -5736,6 +5736,9 @@
         <v>0</v>
       </c>
       <c r="AH23" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="26">
         <v>0</v>
       </c>
     </row>
@@ -7790,7 +7793,7 @@
         <v>0</v>
       </c>
       <c r="AK45" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="4:37" ht="17.25">
@@ -8414,7 +8417,7 @@
         <v>0</v>
       </c>
       <c r="AK51" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="4:37" ht="17.25">

</xml_diff>

<commit_message>
updated by sravvani date:03/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4896" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A23:G34"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -839,26 +838,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -873,7 +872,7 @@
       </c>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -887,7 +886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -901,7 +900,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -913,7 +912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -925,7 +924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -937,7 +936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -949,7 +948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -961,7 +960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -989,7 +988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -1011,7 +1010,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1160,7 +1159,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1285,7 +1284,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1410,7 +1409,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1535,7 +1534,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1596,7 +1595,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1721,7 +1720,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1806,7 +1805,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1891,7 +1890,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1976,7 +1975,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -2061,7 +2060,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2168,7 +2167,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2275,7 +2274,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2384,7 +2383,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2493,7 +2492,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2620,7 +2619,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2747,7 +2746,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2874,7 +2873,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -3001,7 +3000,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3128,7 +3127,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3255,7 +3254,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3382,7 +3381,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3443,7 +3442,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3570,7 +3569,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3699,7 +3698,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3828,7 +3827,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3957,7 +3956,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -4018,7 +4017,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4147,7 +4146,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4274,7 +4273,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4401,7 +4400,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4528,7 +4527,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4679,33 +4678,33 @@
       <selection activeCell="AK34" sqref="AK34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -4720,7 +4719,7 @@
       </c>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:37" ht="18">
+    <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="18">
+    <row r="3" spans="1:37" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="27.6">
+    <row r="4" spans="1:37" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="69">
+    <row r="5" spans="1:37" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4772,7 +4771,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="18">
+    <row r="6" spans="1:37" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4784,7 +4783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="18">
+    <row r="7" spans="1:37" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4796,7 +4795,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="18">
+    <row r="8" spans="1:37" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="18">
+    <row r="9" spans="1:37" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4836,7 +4835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="27.6">
+    <row r="12" spans="1:37" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4858,7 +4857,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:37" ht="28.2">
+    <row r="15" spans="1:37" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4962,7 +4961,7 @@
         <v>40999</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="18">
+    <row r="16" spans="1:37" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5066,7 +5065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:37" ht="18">
+    <row r="17" spans="4:37" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5170,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:37" ht="18">
+    <row r="18" spans="4:37" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5274,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:37" ht="18">
+    <row r="19" spans="4:37" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5378,7 +5377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:37" ht="18">
+    <row r="20" spans="4:37" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5478,7 +5477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="4:37" ht="18">
+    <row r="21" spans="4:37" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5578,7 +5577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:37" ht="18">
+    <row r="22" spans="4:37" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5682,7 +5681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:37" ht="18">
+    <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5786,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:37" ht="18">
+    <row r="24" spans="4:37" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5890,7 +5889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:37" ht="18">
+    <row r="25" spans="4:37" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5994,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:37" ht="18">
+    <row r="26" spans="4:37" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -6098,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:37" ht="18">
+    <row r="27" spans="4:37" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -6202,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:37" ht="18">
+    <row r="28" spans="4:37" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -6304,7 +6303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:37" ht="18">
+    <row r="29" spans="4:37" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -6406,7 +6405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:37" ht="18">
+    <row r="30" spans="4:37" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -6508,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:37" ht="18">
+    <row r="31" spans="4:37" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -6610,7 +6609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:37" ht="18">
+    <row r="32" spans="4:37" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6712,7 +6711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:37" ht="18">
+    <row r="33" spans="4:37" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6814,7 +6813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:37" ht="18">
+    <row r="34" spans="4:37" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6918,7 +6917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:37" ht="18">
+    <row r="35" spans="4:37" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -7022,7 +7021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:37" ht="18">
+    <row r="36" spans="4:37" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -7126,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:37" ht="18">
+    <row r="37" spans="4:37" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -7230,7 +7229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:37" ht="18">
+    <row r="38" spans="4:37" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -7334,7 +7333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:37" ht="18">
+    <row r="39" spans="4:37" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -7438,7 +7437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:37" ht="18">
+    <row r="40" spans="4:37" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -7542,7 +7541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:37" ht="18">
+    <row r="41" spans="4:37" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -7646,7 +7645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:37" ht="18">
+    <row r="42" spans="4:37" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7750,7 +7749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:37" ht="18">
+    <row r="43" spans="4:37" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7854,7 +7853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:37" ht="18">
+    <row r="44" spans="4:37" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7958,7 +7957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="4:37" ht="18">
+    <row r="45" spans="4:37" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -8062,7 +8061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="4:37" ht="18">
+    <row r="46" spans="4:37" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -8166,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:37" ht="18">
+    <row r="47" spans="4:37" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -8270,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:37" ht="18">
+    <row r="48" spans="4:37" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -8374,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:37" ht="18">
+    <row r="49" spans="4:37" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -8478,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:37" ht="18">
+    <row r="50" spans="4:37" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -8582,7 +8581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="4:37" ht="18">
+    <row r="51" spans="4:37" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:37" ht="18">
+    <row r="52" spans="4:37" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -8790,7 +8789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:37" ht="18">
+    <row r="53" spans="4:37" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8894,7 +8893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:37" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -8998,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:37" ht="18">
+    <row r="55" spans="4:37" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -9102,7 +9101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:37" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -9206,7 +9205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:37" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -9330,36 +9329,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -9374,7 +9373,7 @@
       </c>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:36" ht="18">
+    <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -9388,7 +9387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="18">
+    <row r="3" spans="1:36" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -9402,7 +9401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="27.6">
+    <row r="4" spans="1:36" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -9414,7 +9413,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="69">
+    <row r="5" spans="1:36" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -9426,7 +9425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="18">
+    <row r="6" spans="1:36" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -9438,7 +9437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="18">
+    <row r="7" spans="1:36" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -9450,7 +9449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="18">
+    <row r="8" spans="1:36" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -9462,7 +9461,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="18">
+    <row r="9" spans="1:36" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -9490,7 +9489,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="27.6">
+    <row r="12" spans="1:36" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -9512,7 +9511,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:36" ht="28.2">
+    <row r="15" spans="1:36" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -9613,7 +9612,7 @@
         <v>41029</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="18">
+    <row r="16" spans="1:36" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -9623,11 +9622,15 @@
       <c r="F16" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="26"/>
+      <c r="G16" s="41">
+        <v>0</v>
+      </c>
+      <c r="H16" s="41">
+        <v>0</v>
+      </c>
+      <c r="I16" s="41">
+        <v>0</v>
+      </c>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
@@ -9656,7 +9659,7 @@
       <c r="AI16" s="26"/>
       <c r="AJ16" s="26"/>
     </row>
-    <row r="17" spans="4:36" ht="18">
+    <row r="17" spans="4:36" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -9666,11 +9669,15 @@
       <c r="F17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="26"/>
+      <c r="G17" s="41">
+        <v>0</v>
+      </c>
+      <c r="H17" s="41">
+        <v>0</v>
+      </c>
+      <c r="I17" s="41">
+        <v>0</v>
+      </c>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
@@ -9699,7 +9706,7 @@
       <c r="AI17" s="26"/>
       <c r="AJ17" s="26"/>
     </row>
-    <row r="18" spans="4:36" ht="18">
+    <row r="18" spans="4:36" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -9709,11 +9716,15 @@
       <c r="F18" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="26"/>
+      <c r="G18" s="41">
+        <v>0</v>
+      </c>
+      <c r="H18" s="41">
+        <v>0</v>
+      </c>
+      <c r="I18" s="41">
+        <v>0</v>
+      </c>
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
       <c r="L18" s="26"/>
@@ -9742,7 +9753,7 @@
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
     </row>
-    <row r="19" spans="4:36" ht="18">
+    <row r="19" spans="4:36" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -9752,11 +9763,15 @@
       <c r="F19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="26"/>
+      <c r="G19" s="41">
+        <v>0</v>
+      </c>
+      <c r="H19" s="41">
+        <v>0</v>
+      </c>
+      <c r="I19" s="41">
+        <v>0</v>
+      </c>
       <c r="J19" s="26"/>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
@@ -9785,7 +9800,7 @@
       <c r="AI19" s="26"/>
       <c r="AJ19" s="26"/>
     </row>
-    <row r="20" spans="4:36" ht="18">
+    <row r="20" spans="4:36" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -9795,11 +9810,15 @@
       <c r="F20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="19">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="26"/>
+      <c r="G20" s="41">
+        <v>3</v>
+      </c>
+      <c r="H20" s="41">
+        <v>3</v>
+      </c>
+      <c r="I20" s="41">
+        <v>6</v>
+      </c>
       <c r="J20" s="26"/>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
@@ -9828,7 +9847,7 @@
       <c r="AI20" s="26"/>
       <c r="AJ20" s="26"/>
     </row>
-    <row r="21" spans="4:36" ht="18">
+    <row r="21" spans="4:36" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -9838,11 +9857,15 @@
       <c r="F21" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="19">
-        <v>0</v>
-      </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="26"/>
+      <c r="G21" s="41">
+        <v>0</v>
+      </c>
+      <c r="H21" s="41">
+        <v>0</v>
+      </c>
+      <c r="I21" s="41">
+        <v>0</v>
+      </c>
       <c r="J21" s="26"/>
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
@@ -9871,7 +9894,7 @@
       <c r="AI21" s="26"/>
       <c r="AJ21" s="26"/>
     </row>
-    <row r="22" spans="4:36" ht="18">
+    <row r="22" spans="4:36" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -9910,7 +9933,7 @@
       <c r="AG22" s="31"/>
       <c r="AH22" s="22"/>
     </row>
-    <row r="23" spans="4:36" ht="18">
+    <row r="23" spans="4:36" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -9949,7 +9972,7 @@
       <c r="AG23" s="31"/>
       <c r="AH23" s="22"/>
     </row>
-    <row r="24" spans="4:36" ht="18">
+    <row r="24" spans="4:36" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -9988,7 +10011,7 @@
       <c r="AG24" s="31"/>
       <c r="AH24" s="22"/>
     </row>
-    <row r="25" spans="4:36" ht="18">
+    <row r="25" spans="4:36" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -10027,7 +10050,7 @@
       <c r="AG25" s="31"/>
       <c r="AH25" s="22"/>
     </row>
-    <row r="26" spans="4:36" ht="18">
+    <row r="26" spans="4:36" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -10066,7 +10089,7 @@
       <c r="AG26" s="31"/>
       <c r="AH26" s="22"/>
     </row>
-    <row r="27" spans="4:36" ht="18">
+    <row r="27" spans="4:36" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -10105,7 +10128,7 @@
       <c r="AG27" s="31"/>
       <c r="AH27" s="22"/>
     </row>
-    <row r="28" spans="4:36" ht="18">
+    <row r="28" spans="4:36" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -10145,7 +10168,7 @@
       <c r="AI28" s="34"/>
       <c r="AJ28" s="34"/>
     </row>
-    <row r="29" spans="4:36" ht="18">
+    <row r="29" spans="4:36" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -10185,7 +10208,7 @@
       <c r="AI29" s="34"/>
       <c r="AJ29" s="34"/>
     </row>
-    <row r="30" spans="4:36" ht="18">
+    <row r="30" spans="4:36" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -10225,7 +10248,7 @@
       <c r="AI30" s="34"/>
       <c r="AJ30" s="34"/>
     </row>
-    <row r="31" spans="4:36" ht="18">
+    <row r="31" spans="4:36" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -10265,7 +10288,7 @@
       <c r="AI31" s="34"/>
       <c r="AJ31" s="34"/>
     </row>
-    <row r="32" spans="4:36" ht="18">
+    <row r="32" spans="4:36" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -10305,7 +10328,7 @@
       <c r="AI32" s="34"/>
       <c r="AJ32" s="34"/>
     </row>
-    <row r="33" spans="4:36" ht="18">
+    <row r="33" spans="4:36" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -10345,7 +10368,7 @@
       <c r="AI33" s="34"/>
       <c r="AJ33" s="34"/>
     </row>
-    <row r="34" spans="4:36" ht="18">
+    <row r="34" spans="4:36" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -10392,7 +10415,7 @@
       <c r="AI34" s="36"/>
       <c r="AJ34" s="22"/>
     </row>
-    <row r="35" spans="4:36" ht="18">
+    <row r="35" spans="4:36" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -10439,7 +10462,7 @@
       <c r="AI35" s="36"/>
       <c r="AJ35" s="22"/>
     </row>
-    <row r="36" spans="4:36" ht="18">
+    <row r="36" spans="4:36" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -10486,7 +10509,7 @@
       <c r="AI36" s="36"/>
       <c r="AJ36" s="22"/>
     </row>
-    <row r="37" spans="4:36" ht="18">
+    <row r="37" spans="4:36" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -10533,7 +10556,7 @@
       <c r="AI37" s="36"/>
       <c r="AJ37" s="22"/>
     </row>
-    <row r="38" spans="4:36" ht="18">
+    <row r="38" spans="4:36" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -10580,7 +10603,7 @@
       <c r="AI38" s="36"/>
       <c r="AJ38" s="22"/>
     </row>
-    <row r="39" spans="4:36" ht="18">
+    <row r="39" spans="4:36" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -10627,7 +10650,7 @@
       <c r="AI39" s="36"/>
       <c r="AJ39" s="22"/>
     </row>
-    <row r="40" spans="4:36" ht="18">
+    <row r="40" spans="4:36" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -10637,11 +10660,15 @@
       <c r="F40" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="20">
-        <v>0</v>
-      </c>
-      <c r="H40" s="20"/>
-      <c r="I40" s="26"/>
+      <c r="G40" s="41">
+        <v>0</v>
+      </c>
+      <c r="H40" s="41">
+        <v>0</v>
+      </c>
+      <c r="I40" s="41">
+        <v>0</v>
+      </c>
       <c r="J40" s="26"/>
       <c r="K40" s="26"/>
       <c r="L40" s="26"/>
@@ -10670,7 +10697,7 @@
       <c r="AI40" s="35"/>
       <c r="AJ40" s="35"/>
     </row>
-    <row r="41" spans="4:36" ht="18">
+    <row r="41" spans="4:36" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -10680,11 +10707,15 @@
       <c r="F41" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="20">
-        <v>0</v>
-      </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="26"/>
+      <c r="G41" s="41">
+        <v>0</v>
+      </c>
+      <c r="H41" s="41">
+        <v>0</v>
+      </c>
+      <c r="I41" s="41">
+        <v>0</v>
+      </c>
       <c r="J41" s="26"/>
       <c r="K41" s="26"/>
       <c r="L41" s="26"/>
@@ -10713,7 +10744,7 @@
       <c r="AI41" s="26"/>
       <c r="AJ41" s="26"/>
     </row>
-    <row r="42" spans="4:36" ht="18">
+    <row r="42" spans="4:36" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -10723,11 +10754,15 @@
       <c r="F42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="20">
-        <v>0</v>
-      </c>
-      <c r="H42" s="20"/>
-      <c r="I42" s="26"/>
+      <c r="G42" s="41">
+        <v>0</v>
+      </c>
+      <c r="H42" s="41">
+        <v>0</v>
+      </c>
+      <c r="I42" s="41">
+        <v>0</v>
+      </c>
       <c r="J42" s="26"/>
       <c r="K42" s="26"/>
       <c r="L42" s="26"/>
@@ -10756,7 +10791,7 @@
       <c r="AI42" s="26"/>
       <c r="AJ42" s="26"/>
     </row>
-    <row r="43" spans="4:36" ht="18">
+    <row r="43" spans="4:36" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -10766,11 +10801,15 @@
       <c r="F43" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="20">
-        <v>0</v>
-      </c>
-      <c r="H43" s="20"/>
-      <c r="I43" s="26"/>
+      <c r="G43" s="41">
+        <v>0</v>
+      </c>
+      <c r="H43" s="41">
+        <v>0</v>
+      </c>
+      <c r="I43" s="41">
+        <v>0</v>
+      </c>
       <c r="J43" s="26"/>
       <c r="K43" s="26"/>
       <c r="L43" s="26"/>
@@ -10799,7 +10838,7 @@
       <c r="AI43" s="26"/>
       <c r="AJ43" s="26"/>
     </row>
-    <row r="44" spans="4:36" ht="18">
+    <row r="44" spans="4:36" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -10809,11 +10848,15 @@
       <c r="F44" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="20">
+      <c r="G44" s="41">
         <v>3</v>
       </c>
-      <c r="H44" s="20"/>
-      <c r="I44" s="26"/>
+      <c r="H44" s="41">
+        <v>3</v>
+      </c>
+      <c r="I44" s="41">
+        <v>6</v>
+      </c>
       <c r="J44" s="26"/>
       <c r="K44" s="26"/>
       <c r="L44" s="26"/>
@@ -10842,7 +10885,7 @@
       <c r="AI44" s="26"/>
       <c r="AJ44" s="26"/>
     </row>
-    <row r="45" spans="4:36" ht="18">
+    <row r="45" spans="4:36" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -10852,11 +10895,15 @@
       <c r="F45" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="20">
-        <v>0</v>
-      </c>
-      <c r="H45" s="20"/>
-      <c r="I45" s="26"/>
+      <c r="G45" s="41">
+        <v>0</v>
+      </c>
+      <c r="H45" s="41">
+        <v>0</v>
+      </c>
+      <c r="I45" s="41">
+        <v>0</v>
+      </c>
       <c r="J45" s="26"/>
       <c r="K45" s="26"/>
       <c r="L45" s="26"/>
@@ -10885,7 +10932,7 @@
       <c r="AI45" s="26"/>
       <c r="AJ45" s="26"/>
     </row>
-    <row r="46" spans="4:36" ht="18">
+    <row r="46" spans="4:36" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -10895,11 +10942,15 @@
       <c r="F46" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="20">
-        <v>0</v>
-      </c>
-      <c r="H46" s="20"/>
-      <c r="I46" s="26"/>
+      <c r="G46" s="41">
+        <v>0</v>
+      </c>
+      <c r="H46" s="41">
+        <v>0</v>
+      </c>
+      <c r="I46" s="41">
+        <v>0</v>
+      </c>
       <c r="J46" s="26"/>
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
@@ -10928,7 +10979,7 @@
       <c r="AI46" s="26"/>
       <c r="AJ46" s="26"/>
     </row>
-    <row r="47" spans="4:36" ht="18">
+    <row r="47" spans="4:36" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -10938,11 +10989,15 @@
       <c r="F47" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="20">
-        <v>0</v>
-      </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="26"/>
+      <c r="G47" s="41">
+        <v>0</v>
+      </c>
+      <c r="H47" s="41">
+        <v>0</v>
+      </c>
+      <c r="I47" s="41">
+        <v>0</v>
+      </c>
       <c r="J47" s="26"/>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
@@ -10971,7 +11026,7 @@
       <c r="AI47" s="26"/>
       <c r="AJ47" s="26"/>
     </row>
-    <row r="48" spans="4:36" ht="18">
+    <row r="48" spans="4:36" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -10981,11 +11036,15 @@
       <c r="F48" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="20">
-        <v>0</v>
-      </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="26"/>
+      <c r="G48" s="41">
+        <v>0</v>
+      </c>
+      <c r="H48" s="41">
+        <v>0</v>
+      </c>
+      <c r="I48" s="41">
+        <v>0</v>
+      </c>
       <c r="J48" s="26"/>
       <c r="K48" s="26"/>
       <c r="L48" s="26"/>
@@ -11014,7 +11073,7 @@
       <c r="AI48" s="26"/>
       <c r="AJ48" s="26"/>
     </row>
-    <row r="49" spans="4:36" ht="18">
+    <row r="49" spans="4:36" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -11024,11 +11083,15 @@
       <c r="F49" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="20">
-        <v>0</v>
-      </c>
-      <c r="H49" s="20"/>
-      <c r="I49" s="26"/>
+      <c r="G49" s="41">
+        <v>0</v>
+      </c>
+      <c r="H49" s="41">
+        <v>0</v>
+      </c>
+      <c r="I49" s="41">
+        <v>0</v>
+      </c>
       <c r="J49" s="26"/>
       <c r="K49" s="26"/>
       <c r="L49" s="26"/>
@@ -11057,7 +11120,7 @@
       <c r="AI49" s="26"/>
       <c r="AJ49" s="26"/>
     </row>
-    <row r="50" spans="4:36" ht="18">
+    <row r="50" spans="4:36" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -11067,11 +11130,15 @@
       <c r="F50" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G50" s="20">
-        <v>2</v>
-      </c>
-      <c r="H50" s="20"/>
-      <c r="I50" s="26"/>
+      <c r="G50" s="41">
+        <v>3</v>
+      </c>
+      <c r="H50" s="41">
+        <v>3</v>
+      </c>
+      <c r="I50" s="41">
+        <v>6</v>
+      </c>
       <c r="J50" s="26"/>
       <c r="K50" s="26"/>
       <c r="L50" s="26"/>
@@ -11100,7 +11167,7 @@
       <c r="AI50" s="26"/>
       <c r="AJ50" s="26"/>
     </row>
-    <row r="51" spans="4:36" ht="18">
+    <row r="51" spans="4:36" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -11110,11 +11177,15 @@
       <c r="F51" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="20">
-        <v>0</v>
-      </c>
-      <c r="H51" s="20"/>
-      <c r="I51" s="26"/>
+      <c r="G51" s="41">
+        <v>0</v>
+      </c>
+      <c r="H51" s="41">
+        <v>0</v>
+      </c>
+      <c r="I51" s="41">
+        <v>0</v>
+      </c>
       <c r="J51" s="26"/>
       <c r="K51" s="26"/>
       <c r="L51" s="26"/>
@@ -11143,7 +11214,7 @@
       <c r="AI51" s="26"/>
       <c r="AJ51" s="26"/>
     </row>
-    <row r="52" spans="4:36" ht="18">
+    <row r="52" spans="4:36" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -11190,7 +11261,7 @@
       <c r="AI52" s="26"/>
       <c r="AJ52" s="29"/>
     </row>
-    <row r="53" spans="4:36" ht="18">
+    <row r="53" spans="4:36" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -11237,7 +11308,7 @@
       <c r="AI53" s="26"/>
       <c r="AJ53" s="29"/>
     </row>
-    <row r="54" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:36" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -11284,7 +11355,7 @@
       <c r="AI54" s="26"/>
       <c r="AJ54" s="29"/>
     </row>
-    <row r="55" spans="4:36" ht="18">
+    <row r="55" spans="4:36" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -11331,7 +11402,7 @@
       <c r="AI55" s="26"/>
       <c r="AJ55" s="29"/>
     </row>
-    <row r="56" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:36" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -11378,7 +11449,7 @@
       <c r="AI56" s="26"/>
       <c r="AJ56" s="29"/>
     </row>
-    <row r="57" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:36" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date: 03-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9330,7 +9330,7 @@
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9904,10 +9904,10 @@
       <c r="F22" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
       <c r="M22" s="20"/>
@@ -9943,10 +9943,10 @@
       <c r="F23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
       <c r="K23" s="26"/>
       <c r="L23" s="26"/>
       <c r="M23" s="20"/>
@@ -9982,10 +9982,10 @@
       <c r="F24" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
       <c r="M24" s="20"/>
@@ -10021,10 +10021,10 @@
       <c r="F25" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
       <c r="K25" s="26"/>
       <c r="L25" s="26"/>
       <c r="M25" s="20"/>
@@ -10060,10 +10060,10 @@
       <c r="F26" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
       <c r="K26" s="26"/>
       <c r="L26" s="26"/>
       <c r="M26" s="20"/>
@@ -10099,10 +10099,10 @@
       <c r="F27" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
       <c r="M27" s="20"/>

</xml_diff>

<commit_message>
updated by Alpna date: 03-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9329,8 +9329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9910,12 +9910,12 @@
       <c r="J22" s="41"/>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
       <c r="S22" s="28"/>
       <c r="T22" s="26"/>
       <c r="U22" s="26"/>
@@ -9949,12 +9949,12 @@
       <c r="J23" s="41"/>
       <c r="K23" s="26"/>
       <c r="L23" s="26"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
       <c r="S23" s="28"/>
       <c r="T23" s="26"/>
       <c r="U23" s="26"/>
@@ -9988,12 +9988,12 @@
       <c r="J24" s="41"/>
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
       <c r="S24" s="28"/>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
@@ -10027,12 +10027,12 @@
       <c r="J25" s="41"/>
       <c r="K25" s="26"/>
       <c r="L25" s="26"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
       <c r="S25" s="28"/>
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
@@ -10066,12 +10066,12 @@
       <c r="J26" s="41"/>
       <c r="K26" s="26"/>
       <c r="L26" s="26"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
       <c r="S26" s="28"/>
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
@@ -10105,12 +10105,12 @@
       <c r="J27" s="41"/>
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
       <c r="S27" s="28"/>
       <c r="T27" s="26"/>
       <c r="U27" s="26"/>

</xml_diff>

<commit_message>
updated by sravvani date 9/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4836" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -842,26 +841,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -876,7 +875,7 @@
       </c>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -890,7 +889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -904,7 +903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -916,7 +915,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -928,7 +927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -940,7 +939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -952,7 +951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -964,7 +963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -992,7 +991,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +1013,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1288,7 +1287,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1413,7 +1412,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1538,7 +1537,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1599,7 +1598,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1723,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1809,7 +1808,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1894,7 +1893,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1979,7 +1978,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -2064,7 +2063,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2171,7 +2170,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2278,7 +2277,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2387,7 +2386,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2496,7 +2495,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2623,7 +2622,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2750,7 +2749,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2877,7 +2876,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -3004,7 +3003,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3131,7 +3130,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3258,7 +3257,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3385,7 +3384,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3446,7 +3445,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3573,7 +3572,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3702,7 +3701,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3831,7 +3830,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3960,7 +3959,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -4021,7 +4020,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4150,7 +4149,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4277,7 +4276,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4404,7 +4403,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4531,7 +4530,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4682,33 +4681,33 @@
       <selection activeCell="AK34" sqref="AK34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -4723,7 +4722,7 @@
       </c>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:37" ht="18">
+    <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="18">
+    <row r="3" spans="1:37" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="27.6">
+    <row r="4" spans="1:37" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4763,7 +4762,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="69">
+    <row r="5" spans="1:37" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="18">
+    <row r="6" spans="1:37" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4787,7 +4786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="18">
+    <row r="7" spans="1:37" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="18">
+    <row r="8" spans="1:37" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4811,7 +4810,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="18">
+    <row r="9" spans="1:37" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4839,7 +4838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="27.6">
+    <row r="12" spans="1:37" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4861,7 +4860,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:37" ht="28.2">
+    <row r="15" spans="1:37" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4965,7 +4964,7 @@
         <v>40999</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="18">
+    <row r="16" spans="1:37" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5069,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:37" ht="18">
+    <row r="17" spans="4:37" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:37" ht="18">
+    <row r="18" spans="4:37" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5277,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:37" ht="18">
+    <row r="19" spans="4:37" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5381,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:37" ht="18">
+    <row r="20" spans="4:37" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5481,7 +5480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="4:37" ht="18">
+    <row r="21" spans="4:37" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5581,7 +5580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:37" ht="18">
+    <row r="22" spans="4:37" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5685,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:37" ht="18">
+    <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5789,7 +5788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:37" ht="18">
+    <row r="24" spans="4:37" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5893,7 +5892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:37" ht="18">
+    <row r="25" spans="4:37" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5997,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:37" ht="18">
+    <row r="26" spans="4:37" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -6101,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:37" ht="18">
+    <row r="27" spans="4:37" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -6205,7 +6204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:37" ht="18">
+    <row r="28" spans="4:37" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -6307,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:37" ht="18">
+    <row r="29" spans="4:37" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -6409,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:37" ht="18">
+    <row r="30" spans="4:37" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -6511,7 +6510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:37" ht="18">
+    <row r="31" spans="4:37" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:37" ht="18">
+    <row r="32" spans="4:37" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:37" ht="18">
+    <row r="33" spans="4:37" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6817,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:37" ht="18">
+    <row r="34" spans="4:37" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6921,7 +6920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:37" ht="18">
+    <row r="35" spans="4:37" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -7025,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:37" ht="18">
+    <row r="36" spans="4:37" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -7129,7 +7128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:37" ht="18">
+    <row r="37" spans="4:37" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -7233,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:37" ht="18">
+    <row r="38" spans="4:37" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -7337,7 +7336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:37" ht="18">
+    <row r="39" spans="4:37" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -7441,7 +7440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:37" ht="18">
+    <row r="40" spans="4:37" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -7545,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:37" ht="18">
+    <row r="41" spans="4:37" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -7649,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:37" ht="18">
+    <row r="42" spans="4:37" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7753,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:37" ht="18">
+    <row r="43" spans="4:37" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7857,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:37" ht="18">
+    <row r="44" spans="4:37" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7961,7 +7960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="4:37" ht="18">
+    <row r="45" spans="4:37" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -8065,7 +8064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="4:37" ht="18">
+    <row r="46" spans="4:37" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -8169,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:37" ht="18">
+    <row r="47" spans="4:37" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -8273,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:37" ht="18">
+    <row r="48" spans="4:37" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -8377,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:37" ht="18">
+    <row r="49" spans="4:37" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:37" ht="18">
+    <row r="50" spans="4:37" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -8585,7 +8584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="4:37" ht="18">
+    <row r="51" spans="4:37" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -8689,7 +8688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:37" ht="18">
+    <row r="52" spans="4:37" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -8793,7 +8792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:37" ht="18">
+    <row r="53" spans="4:37" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8897,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:37" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -9001,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:37" ht="18">
+    <row r="55" spans="4:37" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -9105,7 +9104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:37" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -9209,7 +9208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:37" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -9333,36 +9332,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46:O51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -9377,7 +9376,7 @@
       </c>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:36" ht="18">
+    <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -9391,7 +9390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="18">
+    <row r="3" spans="1:36" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -9405,7 +9404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="27.6">
+    <row r="4" spans="1:36" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -9417,7 +9416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="69">
+    <row r="5" spans="1:36" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -9429,7 +9428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="18">
+    <row r="6" spans="1:36" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -9441,7 +9440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="18">
+    <row r="7" spans="1:36" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -9453,7 +9452,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="18">
+    <row r="8" spans="1:36" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -9465,7 +9464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="18">
+    <row r="9" spans="1:36" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -9493,7 +9492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="27.6">
+    <row r="12" spans="1:36" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -9515,7 +9514,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:36" ht="28.2">
+    <row r="15" spans="1:36" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -9616,7 +9615,7 @@
         <v>41029</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="18">
+    <row r="16" spans="1:36" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -9644,9 +9643,15 @@
       <c r="L16" s="26">
         <v>0</v>
       </c>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
+      <c r="M16" s="41">
+        <v>0</v>
+      </c>
+      <c r="N16" s="41">
+        <v>0</v>
+      </c>
+      <c r="O16" s="41">
+        <v>0</v>
+      </c>
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26"/>
@@ -9669,7 +9674,7 @@
       <c r="AI16" s="26"/>
       <c r="AJ16" s="26"/>
     </row>
-    <row r="17" spans="4:36" ht="18">
+    <row r="17" spans="4:36" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -9697,9 +9702,15 @@
       <c r="L17" s="26">
         <v>0</v>
       </c>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
+      <c r="M17" s="41">
+        <v>0</v>
+      </c>
+      <c r="N17" s="41">
+        <v>0</v>
+      </c>
+      <c r="O17" s="41">
+        <v>0</v>
+      </c>
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
@@ -9722,7 +9733,7 @@
       <c r="AI17" s="26"/>
       <c r="AJ17" s="26"/>
     </row>
-    <row r="18" spans="4:36" ht="18">
+    <row r="18" spans="4:36" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -9750,9 +9761,15 @@
       <c r="L18" s="26">
         <v>0</v>
       </c>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
+      <c r="M18" s="41">
+        <v>0</v>
+      </c>
+      <c r="N18" s="41">
+        <v>0</v>
+      </c>
+      <c r="O18" s="41">
+        <v>0</v>
+      </c>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
@@ -9775,7 +9792,7 @@
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
     </row>
-    <row r="19" spans="4:36" ht="18">
+    <row r="19" spans="4:36" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -9803,9 +9820,15 @@
       <c r="L19" s="19">
         <v>0</v>
       </c>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="19"/>
+      <c r="M19" s="37">
+        <v>0</v>
+      </c>
+      <c r="N19" s="37">
+        <v>0</v>
+      </c>
+      <c r="O19" s="37">
+        <v>0</v>
+      </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="26"/>
       <c r="R19" s="26"/>
@@ -9828,7 +9851,7 @@
       <c r="AI19" s="26"/>
       <c r="AJ19" s="26"/>
     </row>
-    <row r="20" spans="4:36" ht="18">
+    <row r="20" spans="4:36" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -9856,9 +9879,15 @@
       <c r="L20" s="19">
         <v>4</v>
       </c>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="19"/>
+      <c r="M20" s="37">
+        <v>4</v>
+      </c>
+      <c r="N20" s="37">
+        <v>4</v>
+      </c>
+      <c r="O20" s="37">
+        <v>4</v>
+      </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="26"/>
       <c r="R20" s="26"/>
@@ -9881,7 +9910,7 @@
       <c r="AI20" s="26"/>
       <c r="AJ20" s="26"/>
     </row>
-    <row r="21" spans="4:36" ht="18">
+    <row r="21" spans="4:36" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -9909,9 +9938,15 @@
       <c r="L21" s="26">
         <v>0</v>
       </c>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
+      <c r="M21" s="41">
+        <v>0</v>
+      </c>
+      <c r="N21" s="41">
+        <v>0</v>
+      </c>
+      <c r="O21" s="41">
+        <v>0</v>
+      </c>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
@@ -9934,7 +9969,7 @@
       <c r="AI21" s="26"/>
       <c r="AJ21" s="26"/>
     </row>
-    <row r="22" spans="4:36" ht="18">
+    <row r="22" spans="4:36" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -9979,7 +10014,7 @@
       <c r="AG22" s="31"/>
       <c r="AH22" s="22"/>
     </row>
-    <row r="23" spans="4:36" ht="18">
+    <row r="23" spans="4:36" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -10024,7 +10059,7 @@
       <c r="AG23" s="31"/>
       <c r="AH23" s="22"/>
     </row>
-    <row r="24" spans="4:36" ht="18">
+    <row r="24" spans="4:36" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -10069,7 +10104,7 @@
       <c r="AG24" s="31"/>
       <c r="AH24" s="22"/>
     </row>
-    <row r="25" spans="4:36" ht="18">
+    <row r="25" spans="4:36" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -10114,7 +10149,7 @@
       <c r="AG25" s="31"/>
       <c r="AH25" s="22"/>
     </row>
-    <row r="26" spans="4:36" ht="18">
+    <row r="26" spans="4:36" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -10159,7 +10194,7 @@
       <c r="AG26" s="31"/>
       <c r="AH26" s="22"/>
     </row>
-    <row r="27" spans="4:36" ht="18">
+    <row r="27" spans="4:36" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -10204,7 +10239,7 @@
       <c r="AG27" s="31"/>
       <c r="AH27" s="22"/>
     </row>
-    <row r="28" spans="4:36" ht="18">
+    <row r="28" spans="4:36" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -10252,7 +10287,7 @@
       <c r="AI28" s="34"/>
       <c r="AJ28" s="34"/>
     </row>
-    <row r="29" spans="4:36" ht="18">
+    <row r="29" spans="4:36" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -10300,7 +10335,7 @@
       <c r="AI29" s="34"/>
       <c r="AJ29" s="34"/>
     </row>
-    <row r="30" spans="4:36" ht="18">
+    <row r="30" spans="4:36" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -10348,7 +10383,7 @@
       <c r="AI30" s="34"/>
       <c r="AJ30" s="34"/>
     </row>
-    <row r="31" spans="4:36" ht="18">
+    <row r="31" spans="4:36" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -10396,7 +10431,7 @@
       <c r="AI31" s="34"/>
       <c r="AJ31" s="34"/>
     </row>
-    <row r="32" spans="4:36" ht="18">
+    <row r="32" spans="4:36" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -10444,7 +10479,7 @@
       <c r="AI32" s="34"/>
       <c r="AJ32" s="34"/>
     </row>
-    <row r="33" spans="4:36" ht="18">
+    <row r="33" spans="4:36" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -10492,7 +10527,7 @@
       <c r="AI33" s="34"/>
       <c r="AJ33" s="34"/>
     </row>
-    <row r="34" spans="4:36" ht="18">
+    <row r="34" spans="4:36" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -10549,7 +10584,7 @@
       <c r="AI34" s="36"/>
       <c r="AJ34" s="22"/>
     </row>
-    <row r="35" spans="4:36" ht="18">
+    <row r="35" spans="4:36" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -10606,7 +10641,7 @@
       <c r="AI35" s="36"/>
       <c r="AJ35" s="22"/>
     </row>
-    <row r="36" spans="4:36" ht="18">
+    <row r="36" spans="4:36" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -10663,7 +10698,7 @@
       <c r="AI36" s="36"/>
       <c r="AJ36" s="22"/>
     </row>
-    <row r="37" spans="4:36" ht="18">
+    <row r="37" spans="4:36" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -10720,7 +10755,7 @@
       <c r="AI37" s="36"/>
       <c r="AJ37" s="22"/>
     </row>
-    <row r="38" spans="4:36" ht="18">
+    <row r="38" spans="4:36" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -10777,7 +10812,7 @@
       <c r="AI38" s="36"/>
       <c r="AJ38" s="22"/>
     </row>
-    <row r="39" spans="4:36" ht="18">
+    <row r="39" spans="4:36" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -10834,7 +10869,7 @@
       <c r="AI39" s="36"/>
       <c r="AJ39" s="22"/>
     </row>
-    <row r="40" spans="4:36" ht="18">
+    <row r="40" spans="4:36" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -10862,9 +10897,15 @@
       <c r="L40" s="26">
         <v>0</v>
       </c>
-      <c r="M40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
+      <c r="M40" s="41">
+        <v>0</v>
+      </c>
+      <c r="N40" s="41">
+        <v>0</v>
+      </c>
+      <c r="O40" s="41">
+        <v>0</v>
+      </c>
       <c r="P40" s="26"/>
       <c r="Q40" s="26"/>
       <c r="R40" s="26"/>
@@ -10887,7 +10928,7 @@
       <c r="AI40" s="35"/>
       <c r="AJ40" s="35"/>
     </row>
-    <row r="41" spans="4:36" ht="18">
+    <row r="41" spans="4:36" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -10915,9 +10956,15 @@
       <c r="L41" s="26">
         <v>0</v>
       </c>
-      <c r="M41" s="26"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
+      <c r="M41" s="41">
+        <v>0</v>
+      </c>
+      <c r="N41" s="41">
+        <v>0</v>
+      </c>
+      <c r="O41" s="41">
+        <v>0</v>
+      </c>
       <c r="P41" s="26"/>
       <c r="Q41" s="26"/>
       <c r="R41" s="26"/>
@@ -10940,7 +10987,7 @@
       <c r="AI41" s="26"/>
       <c r="AJ41" s="26"/>
     </row>
-    <row r="42" spans="4:36" ht="18">
+    <row r="42" spans="4:36" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -10968,9 +11015,15 @@
       <c r="L42" s="26">
         <v>0</v>
       </c>
-      <c r="M42" s="26"/>
-      <c r="N42" s="26"/>
-      <c r="O42" s="26"/>
+      <c r="M42" s="41">
+        <v>0</v>
+      </c>
+      <c r="N42" s="41">
+        <v>0</v>
+      </c>
+      <c r="O42" s="41">
+        <v>0</v>
+      </c>
       <c r="P42" s="26"/>
       <c r="Q42" s="26"/>
       <c r="R42" s="26"/>
@@ -10993,7 +11046,7 @@
       <c r="AI42" s="26"/>
       <c r="AJ42" s="26"/>
     </row>
-    <row r="43" spans="4:36" ht="18">
+    <row r="43" spans="4:36" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -11021,9 +11074,15 @@
       <c r="L43" s="26">
         <v>0</v>
       </c>
-      <c r="M43" s="26"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
+      <c r="M43" s="41">
+        <v>0</v>
+      </c>
+      <c r="N43" s="41">
+        <v>0</v>
+      </c>
+      <c r="O43" s="41">
+        <v>0</v>
+      </c>
       <c r="P43" s="26"/>
       <c r="Q43" s="26"/>
       <c r="R43" s="26"/>
@@ -11046,7 +11105,7 @@
       <c r="AI43" s="26"/>
       <c r="AJ43" s="26"/>
     </row>
-    <row r="44" spans="4:36" ht="18">
+    <row r="44" spans="4:36" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -11074,9 +11133,15 @@
       <c r="L44" s="26">
         <v>3</v>
       </c>
-      <c r="M44" s="26"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
+      <c r="M44" s="37">
+        <v>4</v>
+      </c>
+      <c r="N44" s="37">
+        <v>4</v>
+      </c>
+      <c r="O44" s="37">
+        <v>4</v>
+      </c>
       <c r="P44" s="26"/>
       <c r="Q44" s="26"/>
       <c r="R44" s="26"/>
@@ -11099,7 +11164,7 @@
       <c r="AI44" s="26"/>
       <c r="AJ44" s="26"/>
     </row>
-    <row r="45" spans="4:36" ht="18">
+    <row r="45" spans="4:36" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -11127,9 +11192,15 @@
       <c r="L45" s="26">
         <v>0</v>
       </c>
-      <c r="M45" s="26"/>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
+      <c r="M45" s="41">
+        <v>0</v>
+      </c>
+      <c r="N45" s="41">
+        <v>0</v>
+      </c>
+      <c r="O45" s="41">
+        <v>0</v>
+      </c>
       <c r="P45" s="26"/>
       <c r="Q45" s="26"/>
       <c r="R45" s="26"/>
@@ -11152,7 +11223,7 @@
       <c r="AI45" s="26"/>
       <c r="AJ45" s="26"/>
     </row>
-    <row r="46" spans="4:36" ht="18">
+    <row r="46" spans="4:36" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -11180,9 +11251,15 @@
       <c r="L46" s="26">
         <v>0</v>
       </c>
-      <c r="M46" s="26"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="26"/>
+      <c r="M46" s="41">
+        <v>0</v>
+      </c>
+      <c r="N46" s="41">
+        <v>0</v>
+      </c>
+      <c r="O46" s="41">
+        <v>0</v>
+      </c>
       <c r="P46" s="26"/>
       <c r="Q46" s="26"/>
       <c r="R46" s="26"/>
@@ -11205,7 +11282,7 @@
       <c r="AI46" s="26"/>
       <c r="AJ46" s="26"/>
     </row>
-    <row r="47" spans="4:36" ht="18">
+    <row r="47" spans="4:36" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -11233,9 +11310,15 @@
       <c r="L47" s="26">
         <v>0</v>
       </c>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="26"/>
+      <c r="M47" s="41">
+        <v>0</v>
+      </c>
+      <c r="N47" s="41">
+        <v>0</v>
+      </c>
+      <c r="O47" s="41">
+        <v>0</v>
+      </c>
       <c r="P47" s="26"/>
       <c r="Q47" s="26"/>
       <c r="R47" s="26"/>
@@ -11258,7 +11341,7 @@
       <c r="AI47" s="26"/>
       <c r="AJ47" s="26"/>
     </row>
-    <row r="48" spans="4:36" ht="18">
+    <row r="48" spans="4:36" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -11286,9 +11369,15 @@
       <c r="L48" s="26">
         <v>0</v>
       </c>
-      <c r="M48" s="26"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="26"/>
+      <c r="M48" s="41">
+        <v>0</v>
+      </c>
+      <c r="N48" s="41">
+        <v>0</v>
+      </c>
+      <c r="O48" s="41">
+        <v>0</v>
+      </c>
       <c r="P48" s="26"/>
       <c r="Q48" s="26"/>
       <c r="R48" s="26"/>
@@ -11311,7 +11400,7 @@
       <c r="AI48" s="26"/>
       <c r="AJ48" s="26"/>
     </row>
-    <row r="49" spans="4:36" ht="18">
+    <row r="49" spans="4:36" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -11339,9 +11428,15 @@
       <c r="L49" s="26">
         <v>0</v>
       </c>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="26"/>
+      <c r="M49" s="41">
+        <v>0</v>
+      </c>
+      <c r="N49" s="41">
+        <v>0</v>
+      </c>
+      <c r="O49" s="41">
+        <v>0</v>
+      </c>
       <c r="P49" s="26"/>
       <c r="Q49" s="26"/>
       <c r="R49" s="26"/>
@@ -11364,7 +11459,7 @@
       <c r="AI49" s="26"/>
       <c r="AJ49" s="26"/>
     </row>
-    <row r="50" spans="4:36" ht="18">
+    <row r="50" spans="4:36" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -11392,9 +11487,15 @@
       <c r="L50" s="26">
         <v>3</v>
       </c>
-      <c r="M50" s="26"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="26"/>
+      <c r="M50" s="37">
+        <v>4</v>
+      </c>
+      <c r="N50" s="37">
+        <v>4</v>
+      </c>
+      <c r="O50" s="37">
+        <v>4</v>
+      </c>
       <c r="P50" s="26"/>
       <c r="Q50" s="26"/>
       <c r="R50" s="26"/>
@@ -11417,7 +11518,7 @@
       <c r="AI50" s="26"/>
       <c r="AJ50" s="26"/>
     </row>
-    <row r="51" spans="4:36" ht="18">
+    <row r="51" spans="4:36" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -11445,9 +11546,15 @@
       <c r="L51" s="26">
         <v>0</v>
       </c>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="26"/>
+      <c r="M51" s="41">
+        <v>0</v>
+      </c>
+      <c r="N51" s="41">
+        <v>0</v>
+      </c>
+      <c r="O51" s="41">
+        <v>0</v>
+      </c>
       <c r="P51" s="26"/>
       <c r="Q51" s="26"/>
       <c r="R51" s="26"/>
@@ -11470,7 +11577,7 @@
       <c r="AI51" s="26"/>
       <c r="AJ51" s="26"/>
     </row>
-    <row r="52" spans="4:36" ht="18">
+    <row r="52" spans="4:36" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -11527,7 +11634,7 @@
       <c r="AI52" s="26"/>
       <c r="AJ52" s="29"/>
     </row>
-    <row r="53" spans="4:36" ht="18">
+    <row r="53" spans="4:36" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -11584,7 +11691,7 @@
       <c r="AI53" s="26"/>
       <c r="AJ53" s="29"/>
     </row>
-    <row r="54" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:36" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -11641,7 +11748,7 @@
       <c r="AI54" s="26"/>
       <c r="AJ54" s="29"/>
     </row>
-    <row r="55" spans="4:36" ht="18">
+    <row r="55" spans="4:36" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -11698,7 +11805,7 @@
       <c r="AI55" s="26"/>
       <c r="AJ55" s="29"/>
     </row>
-    <row r="56" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:36" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -11755,7 +11862,7 @@
       <c r="AI56" s="26"/>
       <c r="AJ56" s="29"/>
     </row>
-    <row r="57" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:36" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:09-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9332,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46:O51"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10558,7 +10558,7 @@
       <c r="M34" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="N34" s="53">
+      <c r="N34" s="41">
         <v>5</v>
       </c>
       <c r="O34" s="53"/>
@@ -10615,7 +10615,7 @@
       <c r="M35" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="N35" s="53">
+      <c r="N35" s="41">
         <v>0</v>
       </c>
       <c r="O35" s="53"/>
@@ -10672,7 +10672,7 @@
       <c r="M36" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="N36" s="53">
+      <c r="N36" s="41">
         <v>0</v>
       </c>
       <c r="O36" s="53"/>
@@ -10729,7 +10729,7 @@
       <c r="M37" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="N37" s="53">
+      <c r="N37" s="41">
         <v>0</v>
       </c>
       <c r="O37" s="53"/>
@@ -10786,7 +10786,7 @@
       <c r="M38" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="N38" s="53">
+      <c r="N38" s="41">
         <v>5</v>
       </c>
       <c r="O38" s="53"/>
@@ -10843,7 +10843,7 @@
       <c r="M39" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="N39" s="53">
+      <c r="N39" s="41">
         <v>0</v>
       </c>
       <c r="O39" s="53"/>

</xml_diff>

<commit_message>
updated by Alpna date:09-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -11,7 +11,7 @@
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -9332,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9652,7 +9652,9 @@
       <c r="O16" s="41">
         <v>0</v>
       </c>
-      <c r="P16" s="26"/>
+      <c r="P16" s="26">
+        <v>0</v>
+      </c>
       <c r="Q16" s="26"/>
       <c r="R16" s="26"/>
       <c r="S16" s="26"/>

</xml_diff>

<commit_message>
updated by sravvani date:10/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15840" windowHeight="7215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="7215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -9333,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22:O27"/>
+    <sheetView tabSelected="1" topLeftCell="G38" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9653,7 +9652,7 @@
       <c r="O16" s="41">
         <v>0</v>
       </c>
-      <c r="P16" s="26">
+      <c r="P16" s="41">
         <v>0</v>
       </c>
       <c r="Q16" s="26"/>
@@ -9714,7 +9713,9 @@
       <c r="O17" s="41">
         <v>0</v>
       </c>
-      <c r="P17" s="26"/>
+      <c r="P17" s="41">
+        <v>0</v>
+      </c>
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26"/>
@@ -9773,7 +9774,9 @@
       <c r="O18" s="41">
         <v>0</v>
       </c>
-      <c r="P18" s="26"/>
+      <c r="P18" s="41">
+        <v>0</v>
+      </c>
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
@@ -9832,7 +9835,9 @@
       <c r="O19" s="37">
         <v>0</v>
       </c>
-      <c r="P19" s="19"/>
+      <c r="P19" s="37">
+        <v>0</v>
+      </c>
       <c r="Q19" s="26"/>
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
@@ -9889,9 +9894,11 @@
         <v>4</v>
       </c>
       <c r="O20" s="37">
-        <v>4</v>
-      </c>
-      <c r="P20" s="19"/>
+        <v>2</v>
+      </c>
+      <c r="P20" s="37">
+        <v>2</v>
+      </c>
       <c r="Q20" s="26"/>
       <c r="R20" s="26"/>
       <c r="S20" s="26"/>
@@ -9950,7 +9957,9 @@
       <c r="O21" s="41">
         <v>0</v>
       </c>
-      <c r="P21" s="26"/>
+      <c r="P21" s="41">
+        <v>0.1</v>
+      </c>
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
@@ -10981,7 +10990,9 @@
       <c r="O40" s="41">
         <v>0</v>
       </c>
-      <c r="P40" s="26"/>
+      <c r="P40" s="41">
+        <v>0</v>
+      </c>
       <c r="Q40" s="26"/>
       <c r="R40" s="26"/>
       <c r="S40" s="26"/>
@@ -11040,7 +11051,9 @@
       <c r="O41" s="41">
         <v>0</v>
       </c>
-      <c r="P41" s="26"/>
+      <c r="P41" s="41">
+        <v>0</v>
+      </c>
       <c r="Q41" s="26"/>
       <c r="R41" s="26"/>
       <c r="S41" s="26"/>
@@ -11099,7 +11112,9 @@
       <c r="O42" s="41">
         <v>0</v>
       </c>
-      <c r="P42" s="26"/>
+      <c r="P42" s="41">
+        <v>0</v>
+      </c>
       <c r="Q42" s="26"/>
       <c r="R42" s="26"/>
       <c r="S42" s="26"/>
@@ -11158,7 +11173,9 @@
       <c r="O43" s="41">
         <v>0</v>
       </c>
-      <c r="P43" s="26"/>
+      <c r="P43" s="37">
+        <v>0</v>
+      </c>
       <c r="Q43" s="26"/>
       <c r="R43" s="26"/>
       <c r="S43" s="26"/>
@@ -11215,9 +11232,11 @@
         <v>4</v>
       </c>
       <c r="O44" s="37">
-        <v>4</v>
-      </c>
-      <c r="P44" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="P44" s="37">
+        <v>2</v>
+      </c>
       <c r="Q44" s="26"/>
       <c r="R44" s="26"/>
       <c r="S44" s="26"/>
@@ -11276,7 +11295,9 @@
       <c r="O45" s="41">
         <v>0</v>
       </c>
-      <c r="P45" s="26"/>
+      <c r="P45" s="41">
+        <v>0.1</v>
+      </c>
       <c r="Q45" s="26"/>
       <c r="R45" s="26"/>
       <c r="S45" s="26"/>
@@ -11335,7 +11356,9 @@
       <c r="O46" s="41">
         <v>0</v>
       </c>
-      <c r="P46" s="26"/>
+      <c r="P46" s="41">
+        <v>0</v>
+      </c>
       <c r="Q46" s="26"/>
       <c r="R46" s="26"/>
       <c r="S46" s="26"/>
@@ -11394,7 +11417,9 @@
       <c r="O47" s="41">
         <v>0</v>
       </c>
-      <c r="P47" s="26"/>
+      <c r="P47" s="41">
+        <v>0</v>
+      </c>
       <c r="Q47" s="26"/>
       <c r="R47" s="26"/>
       <c r="S47" s="26"/>
@@ -11453,7 +11478,9 @@
       <c r="O48" s="41">
         <v>0</v>
       </c>
-      <c r="P48" s="26"/>
+      <c r="P48" s="41">
+        <v>0</v>
+      </c>
       <c r="Q48" s="26"/>
       <c r="R48" s="26"/>
       <c r="S48" s="26"/>
@@ -11512,7 +11539,9 @@
       <c r="O49" s="41">
         <v>0</v>
       </c>
-      <c r="P49" s="26"/>
+      <c r="P49" s="37">
+        <v>0</v>
+      </c>
       <c r="Q49" s="26"/>
       <c r="R49" s="26"/>
       <c r="S49" s="26"/>
@@ -11569,9 +11598,11 @@
         <v>4</v>
       </c>
       <c r="O50" s="37">
-        <v>4</v>
-      </c>
-      <c r="P50" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="P50" s="37">
+        <v>2</v>
+      </c>
       <c r="Q50" s="26"/>
       <c r="R50" s="26"/>
       <c r="S50" s="26"/>
@@ -11630,7 +11661,9 @@
       <c r="O51" s="41">
         <v>0</v>
       </c>
-      <c r="P51" s="26"/>
+      <c r="P51" s="41">
+        <v>0.1</v>
+      </c>
       <c r="Q51" s="26"/>
       <c r="R51" s="26"/>
       <c r="S51" s="26"/>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:10-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9332,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G38" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="G14" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9820,22 +9820,22 @@
       <c r="J19" s="26">
         <v>0</v>
       </c>
-      <c r="K19" s="19">
-        <v>0</v>
-      </c>
-      <c r="L19" s="19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="37">
-        <v>0</v>
-      </c>
-      <c r="N19" s="37">
-        <v>0</v>
-      </c>
-      <c r="O19" s="37">
-        <v>0</v>
-      </c>
-      <c r="P19" s="37">
+      <c r="K19" s="41">
+        <v>0</v>
+      </c>
+      <c r="L19" s="41">
+        <v>0</v>
+      </c>
+      <c r="M19" s="41">
+        <v>0</v>
+      </c>
+      <c r="N19" s="41">
+        <v>0</v>
+      </c>
+      <c r="O19" s="41">
+        <v>0</v>
+      </c>
+      <c r="P19" s="41">
         <v>0</v>
       </c>
       <c r="Q19" s="26"/>

</xml_diff>

<commit_message>
Updated by Alpna date:10-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9333,7 +9333,7 @@
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G14" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10174,19 +10174,19 @@
       <c r="J25" s="41">
         <v>0</v>
       </c>
-      <c r="K25" s="37">
-        <v>0</v>
-      </c>
-      <c r="L25" s="37">
-        <v>0</v>
-      </c>
-      <c r="M25" s="37">
-        <v>0</v>
-      </c>
-      <c r="N25" s="37">
-        <v>0</v>
-      </c>
-      <c r="O25" s="37">
+      <c r="K25" s="41">
+        <v>0</v>
+      </c>
+      <c r="L25" s="41">
+        <v>0</v>
+      </c>
+      <c r="M25" s="41">
+        <v>0</v>
+      </c>
+      <c r="N25" s="41">
+        <v>0</v>
+      </c>
+      <c r="O25" s="41">
         <v>0</v>
       </c>
       <c r="P25" s="41"/>
@@ -10231,19 +10231,19 @@
       <c r="J26" s="41">
         <v>3</v>
       </c>
-      <c r="K26" s="37">
+      <c r="K26" s="41">
         <v>3</v>
       </c>
-      <c r="L26" s="37">
+      <c r="L26" s="41">
         <v>4</v>
       </c>
-      <c r="M26" s="37">
+      <c r="M26" s="41">
         <v>4</v>
       </c>
-      <c r="N26" s="37">
+      <c r="N26" s="41">
         <v>4</v>
       </c>
-      <c r="O26" s="37">
+      <c r="O26" s="41">
         <v>4</v>
       </c>
       <c r="P26" s="41"/>

</xml_diff>

<commit_message>
updated by sravvani date:13/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4836" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -842,26 +841,26 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -876,7 +875,7 @@
       </c>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -890,7 +889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:52" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -904,7 +903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:52" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -916,7 +915,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:52" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -928,7 +927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18">
+    <row r="6" spans="1:52" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -940,7 +939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:52" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -952,7 +951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:52" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -964,7 +963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:52" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -992,7 +991,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="27.6">
+    <row r="12" spans="1:52" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +1013,7 @@
       <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:52" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>40986</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:52" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -1288,7 +1287,7 @@
       <c r="AY16" s="26"/>
       <c r="AZ16" s="26"/>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:52" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -1413,7 +1412,7 @@
       <c r="AY17" s="26"/>
       <c r="AZ17" s="26"/>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:52" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -1538,7 +1537,7 @@
       <c r="AY18" s="26"/>
       <c r="AZ18" s="26"/>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:52" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -1599,7 +1598,7 @@
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:52" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1723,7 @@
       <c r="AY20" s="26"/>
       <c r="AZ20" s="26"/>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:52" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -1809,7 +1808,7 @@
       <c r="AY21" s="26"/>
       <c r="AZ21" s="26"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:52" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -1894,7 +1893,7 @@
       <c r="AY22" s="26"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:52" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -1979,7 +1978,7 @@
       <c r="AY23" s="26"/>
       <c r="AZ23" s="26"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:52" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -2064,7 +2063,7 @@
       <c r="AY24" s="26"/>
       <c r="AZ24" s="26"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:52" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -2171,7 +2170,7 @@
       <c r="AY25" s="26"/>
       <c r="AZ25" s="26"/>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:52" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -2278,7 +2277,7 @@
       <c r="AY26" s="26"/>
       <c r="AZ26" s="26"/>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:52" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -2387,7 +2386,7 @@
       <c r="AY27" s="26"/>
       <c r="AZ27" s="26"/>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:52" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -2496,7 +2495,7 @@
       <c r="AY28" s="26"/>
       <c r="AZ28" s="26"/>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:52" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -2623,7 +2622,7 @@
       <c r="AY29" s="26"/>
       <c r="AZ29" s="26"/>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:52" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -2750,7 +2749,7 @@
       <c r="AY30" s="26"/>
       <c r="AZ30" s="26"/>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:52" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -2877,7 +2876,7 @@
       <c r="AY31" s="26"/>
       <c r="AZ31" s="26"/>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:52" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -3004,7 +3003,7 @@
       <c r="AY32" s="26"/>
       <c r="AZ32" s="26"/>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:52" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -3131,7 +3130,7 @@
       <c r="AY33" s="26"/>
       <c r="AZ33" s="26"/>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:52" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -3258,7 +3257,7 @@
       <c r="AY34" s="26"/>
       <c r="AZ34" s="26"/>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:52" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3385,7 +3384,7 @@
       <c r="AY35" s="26"/>
       <c r="AZ35" s="26"/>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:52" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -3446,7 +3445,7 @@
       <c r="AY36" s="26"/>
       <c r="AZ36" s="26"/>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:52" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -3573,7 +3572,7 @@
       <c r="AY37" s="26"/>
       <c r="AZ37" s="26"/>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:52" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -3702,7 +3701,7 @@
       <c r="AY38" s="26"/>
       <c r="AZ38" s="26"/>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:52" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -3831,7 +3830,7 @@
       <c r="AY39" s="26"/>
       <c r="AZ39" s="26"/>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:52" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3960,7 +3959,7 @@
       <c r="AY40" s="26"/>
       <c r="AZ40" s="26"/>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:52" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -4021,7 +4020,7 @@
       <c r="AY41" s="26"/>
       <c r="AZ41" s="26"/>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:52" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -4150,7 +4149,7 @@
       <c r="AY42" s="26"/>
       <c r="AZ42" s="26"/>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:52" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -4277,7 +4276,7 @@
       <c r="AY43" s="26"/>
       <c r="AZ43" s="26"/>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:52" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -4404,7 +4403,7 @@
       <c r="AY44" s="26"/>
       <c r="AZ44" s="26"/>
     </row>
-    <row r="45" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:52" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -4531,7 +4530,7 @@
       <c r="AY45" s="26"/>
       <c r="AZ45" s="26"/>
     </row>
-    <row r="46" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:52" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -4682,33 +4681,33 @@
       <selection activeCell="AK34" sqref="AK34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -4723,7 +4722,7 @@
       </c>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:37" ht="18">
+    <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="18">
+    <row r="3" spans="1:37" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="27.6">
+    <row r="4" spans="1:37" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -4763,7 +4762,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="69">
+    <row r="5" spans="1:37" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="18">
+    <row r="6" spans="1:37" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -4787,7 +4786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="18">
+    <row r="7" spans="1:37" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="18">
+    <row r="8" spans="1:37" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -4811,7 +4810,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="18">
+    <row r="9" spans="1:37" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -4839,7 +4838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="27.6">
+    <row r="12" spans="1:37" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -4861,7 +4860,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:37" ht="28.2">
+    <row r="15" spans="1:37" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -4965,7 +4964,7 @@
         <v>40999</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="18">
+    <row r="16" spans="1:37" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5069,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:37" ht="18">
+    <row r="17" spans="4:37" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:37" ht="18">
+    <row r="18" spans="4:37" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5277,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:37" ht="18">
+    <row r="19" spans="4:37" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5381,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:37" ht="18">
+    <row r="20" spans="4:37" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5481,7 +5480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="4:37" ht="18">
+    <row r="21" spans="4:37" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -5581,7 +5580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:37" ht="18">
+    <row r="22" spans="4:37" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5685,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:37" ht="18">
+    <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5789,7 +5788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:37" ht="18">
+    <row r="24" spans="4:37" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5893,7 +5892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:37" ht="18">
+    <row r="25" spans="4:37" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -5997,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:37" ht="18">
+    <row r="26" spans="4:37" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -6101,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:37" ht="18">
+    <row r="27" spans="4:37" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -6205,7 +6204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:37" ht="18">
+    <row r="28" spans="4:37" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -6307,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:37" ht="18">
+    <row r="29" spans="4:37" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -6409,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:37" ht="18">
+    <row r="30" spans="4:37" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -6511,7 +6510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:37" ht="18">
+    <row r="31" spans="4:37" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:37" ht="18">
+    <row r="32" spans="4:37" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:37" ht="18">
+    <row r="33" spans="4:37" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -6817,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:37" ht="18">
+    <row r="34" spans="4:37" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -6921,7 +6920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:37" ht="18">
+    <row r="35" spans="4:37" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -7025,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:37" ht="18">
+    <row r="36" spans="4:37" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -7129,7 +7128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:37" ht="18">
+    <row r="37" spans="4:37" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -7233,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:37" ht="18">
+    <row r="38" spans="4:37" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -7337,7 +7336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:37" ht="18">
+    <row r="39" spans="4:37" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -7441,7 +7440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:37" ht="18">
+    <row r="40" spans="4:37" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -7545,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:37" ht="18">
+    <row r="41" spans="4:37" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -7649,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:37" ht="18">
+    <row r="42" spans="4:37" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -7753,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:37" ht="18">
+    <row r="43" spans="4:37" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -7857,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:37" ht="18">
+    <row r="44" spans="4:37" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -7961,7 +7960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="4:37" ht="18">
+    <row r="45" spans="4:37" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -8065,7 +8064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="4:37" ht="18">
+    <row r="46" spans="4:37" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -8169,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:37" ht="18">
+    <row r="47" spans="4:37" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -8273,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:37" ht="18">
+    <row r="48" spans="4:37" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -8377,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:37" ht="18">
+    <row r="49" spans="4:37" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:37" ht="18">
+    <row r="50" spans="4:37" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -8585,7 +8584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="4:37" ht="18">
+    <row r="51" spans="4:37" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -8689,7 +8688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:37" ht="18">
+    <row r="52" spans="4:37" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -8793,7 +8792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:37" ht="18">
+    <row r="53" spans="4:37" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -8897,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:37" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -9001,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:37" ht="18">
+    <row r="55" spans="4:37" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -9105,7 +9104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:37" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -9209,7 +9208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:37" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -9333,36 +9332,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J11" workbookViewId="0">
-      <selection activeCell="S52" sqref="S52:S57"/>
+    <sheetView tabSelected="1" topLeftCell="J38" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46:S51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -9377,7 +9376,7 @@
       </c>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:36" ht="18">
+    <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -9391,7 +9390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="18">
+    <row r="3" spans="1:36" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -9405,7 +9404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="27.6">
+    <row r="4" spans="1:36" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -9417,7 +9416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="69">
+    <row r="5" spans="1:36" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -9429,7 +9428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="18">
+    <row r="6" spans="1:36" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -9441,7 +9440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="18">
+    <row r="7" spans="1:36" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -9453,7 +9452,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="18">
+    <row r="8" spans="1:36" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -9465,7 +9464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="18">
+    <row r="9" spans="1:36" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -9493,7 +9492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="27.6">
+    <row r="12" spans="1:36" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -9515,7 +9514,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:36" ht="28.2">
+    <row r="15" spans="1:36" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -9616,7 +9615,7 @@
         <v>41029</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="18">
+    <row r="16" spans="1:36" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -9662,7 +9661,9 @@
       <c r="R16" s="26">
         <v>0</v>
       </c>
-      <c r="S16" s="26"/>
+      <c r="S16" s="41">
+        <v>0</v>
+      </c>
       <c r="T16" s="26"/>
       <c r="U16" s="26"/>
       <c r="V16" s="26"/>
@@ -9681,7 +9682,7 @@
       <c r="AI16" s="26"/>
       <c r="AJ16" s="26"/>
     </row>
-    <row r="17" spans="4:36" ht="18">
+    <row r="17" spans="4:36" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -9727,7 +9728,9 @@
       <c r="R17" s="26">
         <v>0</v>
       </c>
-      <c r="S17" s="26"/>
+      <c r="S17" s="41">
+        <v>0</v>
+      </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
       <c r="V17" s="26"/>
@@ -9746,7 +9749,7 @@
       <c r="AI17" s="26"/>
       <c r="AJ17" s="26"/>
     </row>
-    <row r="18" spans="4:36" ht="18">
+    <row r="18" spans="4:36" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -9792,7 +9795,9 @@
       <c r="R18" s="26">
         <v>0</v>
       </c>
-      <c r="S18" s="26"/>
+      <c r="S18" s="41">
+        <v>0</v>
+      </c>
       <c r="T18" s="26"/>
       <c r="U18" s="26"/>
       <c r="V18" s="26"/>
@@ -9811,7 +9816,7 @@
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
     </row>
-    <row r="19" spans="4:36" ht="18">
+    <row r="19" spans="4:36" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -9857,7 +9862,9 @@
       <c r="R19" s="26">
         <v>0</v>
       </c>
-      <c r="S19" s="26"/>
+      <c r="S19" s="41">
+        <v>0</v>
+      </c>
       <c r="T19" s="26"/>
       <c r="U19" s="26"/>
       <c r="V19" s="26"/>
@@ -9876,7 +9883,7 @@
       <c r="AI19" s="26"/>
       <c r="AJ19" s="26"/>
     </row>
-    <row r="20" spans="4:36" ht="18">
+    <row r="20" spans="4:36" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -9922,7 +9929,9 @@
       <c r="R20" s="26">
         <v>4</v>
       </c>
-      <c r="S20" s="26"/>
+      <c r="S20" s="41">
+        <v>4</v>
+      </c>
       <c r="T20" s="26"/>
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
@@ -9941,7 +9950,7 @@
       <c r="AI20" s="26"/>
       <c r="AJ20" s="26"/>
     </row>
-    <row r="21" spans="4:36" ht="18">
+    <row r="21" spans="4:36" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -9987,7 +9996,9 @@
       <c r="R21" s="26">
         <v>0</v>
       </c>
-      <c r="S21" s="26"/>
+      <c r="S21" s="41">
+        <v>0</v>
+      </c>
       <c r="T21" s="26"/>
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
@@ -10006,7 +10017,7 @@
       <c r="AI21" s="26"/>
       <c r="AJ21" s="26"/>
     </row>
-    <row r="22" spans="4:36" ht="18">
+    <row r="22" spans="4:36" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -10063,7 +10074,7 @@
       <c r="AG22" s="31"/>
       <c r="AH22" s="22"/>
     </row>
-    <row r="23" spans="4:36" ht="18">
+    <row r="23" spans="4:36" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -10120,7 +10131,7 @@
       <c r="AG23" s="31"/>
       <c r="AH23" s="22"/>
     </row>
-    <row r="24" spans="4:36" ht="18">
+    <row r="24" spans="4:36" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -10177,7 +10188,7 @@
       <c r="AG24" s="31"/>
       <c r="AH24" s="22"/>
     </row>
-    <row r="25" spans="4:36" ht="18">
+    <row r="25" spans="4:36" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -10234,7 +10245,7 @@
       <c r="AG25" s="31"/>
       <c r="AH25" s="22"/>
     </row>
-    <row r="26" spans="4:36" ht="18">
+    <row r="26" spans="4:36" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -10291,7 +10302,7 @@
       <c r="AG26" s="31"/>
       <c r="AH26" s="22"/>
     </row>
-    <row r="27" spans="4:36" ht="18">
+    <row r="27" spans="4:36" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -10348,7 +10359,7 @@
       <c r="AG27" s="31"/>
       <c r="AH27" s="22"/>
     </row>
-    <row r="28" spans="4:36" ht="18">
+    <row r="28" spans="4:36" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -10408,7 +10419,7 @@
       <c r="AI28" s="34"/>
       <c r="AJ28" s="34"/>
     </row>
-    <row r="29" spans="4:36" ht="18">
+    <row r="29" spans="4:36" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -10468,7 +10479,7 @@
       <c r="AI29" s="34"/>
       <c r="AJ29" s="34"/>
     </row>
-    <row r="30" spans="4:36" ht="18">
+    <row r="30" spans="4:36" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -10528,7 +10539,7 @@
       <c r="AI30" s="34"/>
       <c r="AJ30" s="34"/>
     </row>
-    <row r="31" spans="4:36" ht="18">
+    <row r="31" spans="4:36" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -10588,7 +10599,7 @@
       <c r="AI31" s="34"/>
       <c r="AJ31" s="34"/>
     </row>
-    <row r="32" spans="4:36" ht="18">
+    <row r="32" spans="4:36" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -10648,7 +10659,7 @@
       <c r="AI32" s="34"/>
       <c r="AJ32" s="34"/>
     </row>
-    <row r="33" spans="4:36" ht="18">
+    <row r="33" spans="4:36" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -10708,7 +10719,7 @@
       <c r="AI33" s="34"/>
       <c r="AJ33" s="34"/>
     </row>
-    <row r="34" spans="4:36" ht="18">
+    <row r="34" spans="4:36" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -10773,7 +10784,7 @@
       <c r="AI34" s="36"/>
       <c r="AJ34" s="22"/>
     </row>
-    <row r="35" spans="4:36" ht="18">
+    <row r="35" spans="4:36" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -10838,7 +10849,7 @@
       <c r="AI35" s="36"/>
       <c r="AJ35" s="22"/>
     </row>
-    <row r="36" spans="4:36" ht="18">
+    <row r="36" spans="4:36" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -10903,7 +10914,7 @@
       <c r="AI36" s="36"/>
       <c r="AJ36" s="22"/>
     </row>
-    <row r="37" spans="4:36" ht="18">
+    <row r="37" spans="4:36" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -10968,7 +10979,7 @@
       <c r="AI37" s="36"/>
       <c r="AJ37" s="22"/>
     </row>
-    <row r="38" spans="4:36" ht="18">
+    <row r="38" spans="4:36" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -11033,7 +11044,7 @@
       <c r="AI38" s="36"/>
       <c r="AJ38" s="22"/>
     </row>
-    <row r="39" spans="4:36" ht="18">
+    <row r="39" spans="4:36" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -11098,7 +11109,7 @@
       <c r="AI39" s="36"/>
       <c r="AJ39" s="22"/>
     </row>
-    <row r="40" spans="4:36" ht="18">
+    <row r="40" spans="4:36" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -11144,7 +11155,9 @@
       <c r="R40" s="26">
         <v>0</v>
       </c>
-      <c r="S40" s="26"/>
+      <c r="S40" s="41">
+        <v>0</v>
+      </c>
       <c r="T40" s="26"/>
       <c r="U40" s="26"/>
       <c r="V40" s="26"/>
@@ -11163,7 +11176,7 @@
       <c r="AI40" s="35"/>
       <c r="AJ40" s="35"/>
     </row>
-    <row r="41" spans="4:36" ht="18">
+    <row r="41" spans="4:36" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -11209,7 +11222,9 @@
       <c r="R41" s="26">
         <v>0</v>
       </c>
-      <c r="S41" s="26"/>
+      <c r="S41" s="41">
+        <v>0</v>
+      </c>
       <c r="T41" s="26"/>
       <c r="U41" s="26"/>
       <c r="V41" s="26"/>
@@ -11228,7 +11243,7 @@
       <c r="AI41" s="26"/>
       <c r="AJ41" s="26"/>
     </row>
-    <row r="42" spans="4:36" ht="18">
+    <row r="42" spans="4:36" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -11274,7 +11289,9 @@
       <c r="R42" s="26">
         <v>0</v>
       </c>
-      <c r="S42" s="26"/>
+      <c r="S42" s="41">
+        <v>0</v>
+      </c>
       <c r="T42" s="26"/>
       <c r="U42" s="26"/>
       <c r="V42" s="26"/>
@@ -11293,7 +11310,7 @@
       <c r="AI42" s="26"/>
       <c r="AJ42" s="26"/>
     </row>
-    <row r="43" spans="4:36" ht="18">
+    <row r="43" spans="4:36" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -11339,7 +11356,9 @@
       <c r="R43" s="26">
         <v>0</v>
       </c>
-      <c r="S43" s="26"/>
+      <c r="S43" s="41">
+        <v>0</v>
+      </c>
       <c r="T43" s="26"/>
       <c r="U43" s="26"/>
       <c r="V43" s="26"/>
@@ -11358,7 +11377,7 @@
       <c r="AI43" s="26"/>
       <c r="AJ43" s="26"/>
     </row>
-    <row r="44" spans="4:36" ht="18">
+    <row r="44" spans="4:36" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -11404,7 +11423,9 @@
       <c r="R44" s="26">
         <v>2</v>
       </c>
-      <c r="S44" s="26"/>
+      <c r="S44" s="41">
+        <v>4</v>
+      </c>
       <c r="T44" s="26"/>
       <c r="U44" s="26"/>
       <c r="V44" s="26"/>
@@ -11423,7 +11444,7 @@
       <c r="AI44" s="26"/>
       <c r="AJ44" s="26"/>
     </row>
-    <row r="45" spans="4:36" ht="18">
+    <row r="45" spans="4:36" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -11469,7 +11490,9 @@
       <c r="R45" s="26">
         <v>0</v>
       </c>
-      <c r="S45" s="26"/>
+      <c r="S45" s="41">
+        <v>0</v>
+      </c>
       <c r="T45" s="26"/>
       <c r="U45" s="26"/>
       <c r="V45" s="26"/>
@@ -11488,7 +11511,7 @@
       <c r="AI45" s="26"/>
       <c r="AJ45" s="26"/>
     </row>
-    <row r="46" spans="4:36" ht="18">
+    <row r="46" spans="4:36" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -11534,7 +11557,9 @@
       <c r="R46" s="26">
         <v>0</v>
       </c>
-      <c r="S46" s="26"/>
+      <c r="S46" s="41">
+        <v>0</v>
+      </c>
       <c r="T46" s="26"/>
       <c r="U46" s="26"/>
       <c r="V46" s="26"/>
@@ -11553,7 +11578,7 @@
       <c r="AI46" s="26"/>
       <c r="AJ46" s="26"/>
     </row>
-    <row r="47" spans="4:36" ht="18">
+    <row r="47" spans="4:36" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -11599,7 +11624,9 @@
       <c r="R47" s="26">
         <v>0</v>
       </c>
-      <c r="S47" s="26"/>
+      <c r="S47" s="41">
+        <v>0</v>
+      </c>
       <c r="T47" s="26"/>
       <c r="U47" s="26"/>
       <c r="V47" s="26"/>
@@ -11618,7 +11645,7 @@
       <c r="AI47" s="26"/>
       <c r="AJ47" s="26"/>
     </row>
-    <row r="48" spans="4:36" ht="18">
+    <row r="48" spans="4:36" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -11664,7 +11691,9 @@
       <c r="R48" s="26">
         <v>0</v>
       </c>
-      <c r="S48" s="26"/>
+      <c r="S48" s="41">
+        <v>0</v>
+      </c>
       <c r="T48" s="26"/>
       <c r="U48" s="26"/>
       <c r="V48" s="26"/>
@@ -11683,7 +11712,7 @@
       <c r="AI48" s="26"/>
       <c r="AJ48" s="26"/>
     </row>
-    <row r="49" spans="4:36" ht="18">
+    <row r="49" spans="4:36" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -11729,7 +11758,9 @@
       <c r="R49" s="26">
         <v>0</v>
       </c>
-      <c r="S49" s="26"/>
+      <c r="S49" s="41">
+        <v>0</v>
+      </c>
       <c r="T49" s="26"/>
       <c r="U49" s="26"/>
       <c r="V49" s="26"/>
@@ -11748,7 +11779,7 @@
       <c r="AI49" s="26"/>
       <c r="AJ49" s="26"/>
     </row>
-    <row r="50" spans="4:36" ht="18">
+    <row r="50" spans="4:36" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -11794,7 +11825,9 @@
       <c r="R50" s="26">
         <v>2</v>
       </c>
-      <c r="S50" s="26"/>
+      <c r="S50" s="41">
+        <v>4</v>
+      </c>
       <c r="T50" s="26"/>
       <c r="U50" s="26"/>
       <c r="V50" s="26"/>
@@ -11813,7 +11846,7 @@
       <c r="AI50" s="26"/>
       <c r="AJ50" s="26"/>
     </row>
-    <row r="51" spans="4:36" ht="18">
+    <row r="51" spans="4:36" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -11859,7 +11892,9 @@
       <c r="R51" s="26">
         <v>0</v>
       </c>
-      <c r="S51" s="26"/>
+      <c r="S51" s="41">
+        <v>0</v>
+      </c>
       <c r="T51" s="26"/>
       <c r="U51" s="26"/>
       <c r="V51" s="26"/>
@@ -11878,7 +11913,7 @@
       <c r="AI51" s="26"/>
       <c r="AJ51" s="26"/>
     </row>
-    <row r="52" spans="4:36" ht="18">
+    <row r="52" spans="4:36" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -11945,7 +11980,7 @@
       <c r="AI52" s="26"/>
       <c r="AJ52" s="29"/>
     </row>
-    <row r="53" spans="4:36" ht="18">
+    <row r="53" spans="4:36" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -12012,7 +12047,7 @@
       <c r="AI53" s="26"/>
       <c r="AJ53" s="29"/>
     </row>
-    <row r="54" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:36" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -12079,7 +12114,7 @@
       <c r="AI54" s="26"/>
       <c r="AJ54" s="29"/>
     </row>
-    <row r="55" spans="4:36" ht="18">
+    <row r="55" spans="4:36" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -12146,7 +12181,7 @@
       <c r="AI55" s="26"/>
       <c r="AJ55" s="29"/>
     </row>
-    <row r="56" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:36" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -12213,7 +12248,7 @@
       <c r="AI56" s="26"/>
       <c r="AJ56" s="29"/>
     </row>
-    <row r="57" spans="4:36" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:36" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Done by B.S.Deepthi date:13-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9333,7 +9333,7 @@
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J38" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46:S51"/>
+      <selection activeCell="J41" sqref="J41:M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11198,10 +11198,10 @@
       <c r="J41" s="41">
         <v>0</v>
       </c>
-      <c r="K41" s="26">
-        <v>0</v>
-      </c>
-      <c r="L41" s="26">
+      <c r="K41" s="41">
+        <v>0</v>
+      </c>
+      <c r="L41" s="41">
         <v>0</v>
       </c>
       <c r="M41" s="41">
@@ -11265,10 +11265,10 @@
       <c r="J42" s="41">
         <v>0</v>
       </c>
-      <c r="K42" s="26">
-        <v>0</v>
-      </c>
-      <c r="L42" s="26">
+      <c r="K42" s="41">
+        <v>0</v>
+      </c>
+      <c r="L42" s="41">
         <v>0</v>
       </c>
       <c r="M42" s="41">
@@ -11332,10 +11332,10 @@
       <c r="J43" s="41">
         <v>0</v>
       </c>
-      <c r="K43" s="26">
-        <v>0</v>
-      </c>
-      <c r="L43" s="26">
+      <c r="K43" s="41">
+        <v>0</v>
+      </c>
+      <c r="L43" s="41">
         <v>0</v>
       </c>
       <c r="M43" s="41">
@@ -11347,7 +11347,7 @@
       <c r="O43" s="41">
         <v>0</v>
       </c>
-      <c r="P43" s="37">
+      <c r="P43" s="41">
         <v>0</v>
       </c>
       <c r="Q43" s="37">
@@ -11399,22 +11399,22 @@
       <c r="J44" s="41">
         <v>3</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K44" s="41">
         <v>2</v>
       </c>
-      <c r="L44" s="26">
+      <c r="L44" s="41">
         <v>3</v>
       </c>
-      <c r="M44" s="37">
+      <c r="M44" s="41">
         <v>4</v>
       </c>
-      <c r="N44" s="37">
+      <c r="N44" s="41">
         <v>4</v>
       </c>
-      <c r="O44" s="37">
+      <c r="O44" s="41">
         <v>2</v>
       </c>
-      <c r="P44" s="37">
+      <c r="P44" s="41">
         <v>2</v>
       </c>
       <c r="Q44" s="37">
@@ -11466,10 +11466,10 @@
       <c r="J45" s="41">
         <v>0.1</v>
       </c>
-      <c r="K45" s="26">
-        <v>0</v>
-      </c>
-      <c r="L45" s="26">
+      <c r="K45" s="41">
+        <v>0</v>
+      </c>
+      <c r="L45" s="41">
         <v>0</v>
       </c>
       <c r="M45" s="41">
@@ -11533,10 +11533,10 @@
       <c r="J46" s="41">
         <v>0</v>
       </c>
-      <c r="K46" s="26">
-        <v>0</v>
-      </c>
-      <c r="L46" s="26">
+      <c r="K46" s="41">
+        <v>0</v>
+      </c>
+      <c r="L46" s="41">
         <v>0</v>
       </c>
       <c r="M46" s="41">
@@ -11600,10 +11600,10 @@
       <c r="J47" s="41">
         <v>0</v>
       </c>
-      <c r="K47" s="26">
-        <v>0</v>
-      </c>
-      <c r="L47" s="26">
+      <c r="K47" s="41">
+        <v>0</v>
+      </c>
+      <c r="L47" s="41">
         <v>0</v>
       </c>
       <c r="M47" s="41">

</xml_diff>

<commit_message>
updated by Alpna date:13/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9332,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J38" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41:M47"/>
+    <sheetView tabSelected="1" topLeftCell="J32" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11670,7 +11670,7 @@
       <c r="K48" s="26">
         <v>0</v>
       </c>
-      <c r="L48" s="26">
+      <c r="L48" s="41">
         <v>0</v>
       </c>
       <c r="M48" s="41">
@@ -11688,7 +11688,7 @@
       <c r="Q48" s="41">
         <v>0</v>
       </c>
-      <c r="R48" s="26">
+      <c r="R48" s="41">
         <v>0</v>
       </c>
       <c r="S48" s="41">
@@ -11737,7 +11737,7 @@
       <c r="K49" s="26">
         <v>0</v>
       </c>
-      <c r="L49" s="26">
+      <c r="L49" s="41">
         <v>0</v>
       </c>
       <c r="M49" s="41">
@@ -11749,13 +11749,13 @@
       <c r="O49" s="41">
         <v>0</v>
       </c>
-      <c r="P49" s="37">
+      <c r="P49" s="41">
         <v>0</v>
       </c>
       <c r="Q49" s="41">
         <v>0</v>
       </c>
-      <c r="R49" s="26">
+      <c r="R49" s="41">
         <v>0</v>
       </c>
       <c r="S49" s="41">
@@ -11804,25 +11804,25 @@
       <c r="K50" s="26">
         <v>2</v>
       </c>
-      <c r="L50" s="26">
+      <c r="L50" s="41">
         <v>3</v>
       </c>
-      <c r="M50" s="37">
+      <c r="M50" s="41">
         <v>4</v>
       </c>
-      <c r="N50" s="37">
+      <c r="N50" s="41">
         <v>4</v>
       </c>
-      <c r="O50" s="37">
+      <c r="O50" s="41">
         <v>2</v>
       </c>
-      <c r="P50" s="37">
+      <c r="P50" s="41">
         <v>2</v>
       </c>
       <c r="Q50" s="41">
         <v>0</v>
       </c>
-      <c r="R50" s="26">
+      <c r="R50" s="41">
         <v>2</v>
       </c>
       <c r="S50" s="41">

</xml_diff>

<commit_message>
updated by sravvani date:15/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13920" windowHeight="6645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="6645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="February 2013" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -9333,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L31" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="L37" workbookViewId="0">
+      <selection activeCell="U46" sqref="U46:U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9665,8 +9664,12 @@
       <c r="S16" s="41">
         <v>0</v>
       </c>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
+      <c r="T16" s="41">
+        <v>0</v>
+      </c>
+      <c r="U16" s="41">
+        <v>0</v>
+      </c>
       <c r="V16" s="26"/>
       <c r="W16" s="26"/>
       <c r="X16" s="26"/>
@@ -9732,8 +9735,12 @@
       <c r="S17" s="41">
         <v>0</v>
       </c>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
+      <c r="T17" s="41">
+        <v>0</v>
+      </c>
+      <c r="U17" s="41">
+        <v>0</v>
+      </c>
       <c r="V17" s="26"/>
       <c r="W17" s="26"/>
       <c r="X17" s="26"/>
@@ -9799,8 +9806,12 @@
       <c r="S18" s="41">
         <v>0</v>
       </c>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
+      <c r="T18" s="41">
+        <v>0</v>
+      </c>
+      <c r="U18" s="41">
+        <v>0</v>
+      </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
@@ -9866,8 +9877,12 @@
       <c r="S19" s="41">
         <v>0</v>
       </c>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
+      <c r="T19" s="41">
+        <v>0</v>
+      </c>
+      <c r="U19" s="41">
+        <v>0</v>
+      </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
       <c r="X19" s="26"/>
@@ -9933,8 +9948,12 @@
       <c r="S20" s="41">
         <v>4</v>
       </c>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
+      <c r="T20" s="41">
+        <v>4</v>
+      </c>
+      <c r="U20" s="41">
+        <v>4</v>
+      </c>
       <c r="V20" s="26"/>
       <c r="W20" s="26"/>
       <c r="X20" s="26"/>
@@ -10000,8 +10019,12 @@
       <c r="S21" s="41">
         <v>0</v>
       </c>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
+      <c r="T21" s="41">
+        <v>0</v>
+      </c>
+      <c r="U21" s="41">
+        <v>0</v>
+      </c>
       <c r="V21" s="26"/>
       <c r="W21" s="26"/>
       <c r="X21" s="26"/>
@@ -11207,8 +11230,12 @@
       <c r="S40" s="41">
         <v>0</v>
       </c>
-      <c r="T40" s="26"/>
-      <c r="U40" s="26"/>
+      <c r="T40" s="41">
+        <v>0</v>
+      </c>
+      <c r="U40" s="41">
+        <v>0</v>
+      </c>
       <c r="V40" s="26"/>
       <c r="W40" s="26"/>
       <c r="X40" s="26"/>
@@ -11274,8 +11301,12 @@
       <c r="S41" s="41">
         <v>0</v>
       </c>
-      <c r="T41" s="26"/>
-      <c r="U41" s="26"/>
+      <c r="T41" s="41">
+        <v>0</v>
+      </c>
+      <c r="U41" s="41">
+        <v>0</v>
+      </c>
       <c r="V41" s="26"/>
       <c r="W41" s="26"/>
       <c r="X41" s="26"/>
@@ -11341,8 +11372,12 @@
       <c r="S42" s="41">
         <v>0</v>
       </c>
-      <c r="T42" s="26"/>
-      <c r="U42" s="26"/>
+      <c r="T42" s="41">
+        <v>0</v>
+      </c>
+      <c r="U42" s="41">
+        <v>0</v>
+      </c>
       <c r="V42" s="26"/>
       <c r="W42" s="26"/>
       <c r="X42" s="26"/>
@@ -11408,8 +11443,12 @@
       <c r="S43" s="41">
         <v>0</v>
       </c>
-      <c r="T43" s="26"/>
-      <c r="U43" s="26"/>
+      <c r="T43" s="41">
+        <v>0</v>
+      </c>
+      <c r="U43" s="41">
+        <v>0</v>
+      </c>
       <c r="V43" s="26"/>
       <c r="W43" s="26"/>
       <c r="X43" s="26"/>
@@ -11475,8 +11514,12 @@
       <c r="S44" s="41">
         <v>4</v>
       </c>
-      <c r="T44" s="26"/>
-      <c r="U44" s="26"/>
+      <c r="T44" s="41">
+        <v>4</v>
+      </c>
+      <c r="U44" s="41">
+        <v>4</v>
+      </c>
       <c r="V44" s="26"/>
       <c r="W44" s="26"/>
       <c r="X44" s="26"/>
@@ -11542,8 +11585,12 @@
       <c r="S45" s="41">
         <v>0</v>
       </c>
-      <c r="T45" s="26"/>
-      <c r="U45" s="26"/>
+      <c r="T45" s="41">
+        <v>0</v>
+      </c>
+      <c r="U45" s="41">
+        <v>0</v>
+      </c>
       <c r="V45" s="26"/>
       <c r="W45" s="26"/>
       <c r="X45" s="26"/>
@@ -11609,8 +11656,12 @@
       <c r="S46" s="41">
         <v>0</v>
       </c>
-      <c r="T46" s="26"/>
-      <c r="U46" s="26"/>
+      <c r="T46" s="41">
+        <v>0</v>
+      </c>
+      <c r="U46" s="41">
+        <v>0</v>
+      </c>
       <c r="V46" s="26"/>
       <c r="W46" s="26"/>
       <c r="X46" s="26"/>
@@ -11676,8 +11727,12 @@
       <c r="S47" s="41">
         <v>0</v>
       </c>
-      <c r="T47" s="26"/>
-      <c r="U47" s="26"/>
+      <c r="T47" s="41">
+        <v>0</v>
+      </c>
+      <c r="U47" s="41">
+        <v>0</v>
+      </c>
       <c r="V47" s="26"/>
       <c r="W47" s="26"/>
       <c r="X47" s="26"/>
@@ -11743,8 +11798,12 @@
       <c r="S48" s="41">
         <v>0</v>
       </c>
-      <c r="T48" s="26"/>
-      <c r="U48" s="26"/>
+      <c r="T48" s="41">
+        <v>0</v>
+      </c>
+      <c r="U48" s="41">
+        <v>0</v>
+      </c>
       <c r="V48" s="26"/>
       <c r="W48" s="26"/>
       <c r="X48" s="26"/>
@@ -11810,8 +11869,12 @@
       <c r="S49" s="41">
         <v>0</v>
       </c>
-      <c r="T49" s="26"/>
-      <c r="U49" s="26"/>
+      <c r="T49" s="41">
+        <v>0</v>
+      </c>
+      <c r="U49" s="41">
+        <v>0</v>
+      </c>
       <c r="V49" s="26"/>
       <c r="W49" s="26"/>
       <c r="X49" s="26"/>
@@ -11877,8 +11940,12 @@
       <c r="S50" s="41">
         <v>4</v>
       </c>
-      <c r="T50" s="26"/>
-      <c r="U50" s="26"/>
+      <c r="T50" s="41">
+        <v>4</v>
+      </c>
+      <c r="U50" s="41">
+        <v>4</v>
+      </c>
       <c r="V50" s="26"/>
       <c r="W50" s="26"/>
       <c r="X50" s="26"/>
@@ -11944,8 +12011,12 @@
       <c r="S51" s="41">
         <v>0</v>
       </c>
-      <c r="T51" s="26"/>
-      <c r="U51" s="26"/>
+      <c r="T51" s="41">
+        <v>0</v>
+      </c>
+      <c r="U51" s="41">
+        <v>0</v>
+      </c>
       <c r="V51" s="26"/>
       <c r="W51" s="26"/>
       <c r="X51" s="26"/>

</xml_diff>

<commit_message>
updated by deepthi date:15-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -11,7 +11,7 @@
     <sheet name="March 2013" sheetId="2" r:id="rId2"/>
     <sheet name="April 2013 " sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -9332,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L37" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46:U51"/>
+    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10020,7 +10020,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" s="41">
         <v>0</v>

</xml_diff>

<commit_message>
updated by Alpna date:14-04-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -9332,8 +9332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="L34" workbookViewId="0">
+      <selection activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11586,7 +11586,7 @@
         <v>0</v>
       </c>
       <c r="T45" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45" s="41">
         <v>0</v>
@@ -12012,7 +12012,7 @@
         <v>0</v>
       </c>
       <c r="T51" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51" s="41">
         <v>0</v>

</xml_diff>

<commit_message>
updated by sravvani date:25/04/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="11088" windowHeight="4836" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="January 2013" sheetId="5" r:id="rId1"/>
@@ -12,8 +12,7 @@
     <sheet name="March 2013" sheetId="2" r:id="rId3"/>
     <sheet name="April 2013 " sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A47:H57"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -923,26 +922,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ51"/>
+  <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView topLeftCell="AB42" workbookViewId="0">
-      <selection activeCell="AD48" sqref="AD48"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41:U45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:37">
       <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
@@ -987,7 +986,7 @@
       <c r="AJ1" s="51"/>
       <c r="AK1" s="51"/>
     </row>
-    <row r="2" spans="1:52" ht="18">
+    <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="55" t="s">
         <v>2</v>
       </c>
@@ -1034,7 +1033,7 @@
       <c r="AJ2" s="51"/>
       <c r="AK2" s="51"/>
     </row>
-    <row r="3" spans="1:52" ht="18">
+    <row r="3" spans="1:37" ht="17.25">
       <c r="A3" s="57" t="s">
         <v>4</v>
       </c>
@@ -1081,7 +1080,7 @@
       <c r="AJ3" s="51"/>
       <c r="AK3" s="51"/>
     </row>
-    <row r="4" spans="1:52" ht="27.6">
+    <row r="4" spans="1:37" ht="28.5">
       <c r="A4" s="57" t="s">
         <v>6</v>
       </c>
@@ -1126,7 +1125,7 @@
       <c r="AJ4" s="51"/>
       <c r="AK4" s="51"/>
     </row>
-    <row r="5" spans="1:52" ht="69">
+    <row r="5" spans="1:37" ht="71.25">
       <c r="A5" s="57" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1170,7 @@
       <c r="AJ5" s="51"/>
       <c r="AK5" s="51"/>
     </row>
-    <row r="6" spans="1:52" ht="27.6">
+    <row r="6" spans="1:37" ht="42.75">
       <c r="A6" s="59" t="s">
         <v>20</v>
       </c>
@@ -1216,7 +1215,7 @@
       <c r="AJ6" s="51"/>
       <c r="AK6" s="51"/>
     </row>
-    <row r="7" spans="1:52" ht="18">
+    <row r="7" spans="1:37" ht="17.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -1257,7 +1256,7 @@
       <c r="AJ7" s="51"/>
       <c r="AK7" s="51"/>
     </row>
-    <row r="8" spans="1:52" ht="18">
+    <row r="8" spans="1:37" ht="17.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -1298,7 +1297,7 @@
       <c r="AJ8" s="51"/>
       <c r="AK8" s="51"/>
     </row>
-    <row r="9" spans="1:52" ht="18">
+    <row r="9" spans="1:37" ht="17.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -1339,19 +1338,19 @@
       <c r="AJ9" s="51"/>
       <c r="AK9" s="51"/>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:37">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:37">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:37">
       <c r="A12" s="9"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:37">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
@@ -1390,7 +1389,7 @@
       <c r="AJ13" s="51"/>
       <c r="AK13" s="51"/>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:37">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -1429,7 +1428,7 @@
       <c r="AJ14" s="51"/>
       <c r="AK14" s="51"/>
     </row>
-    <row r="15" spans="1:52" ht="28.2">
+    <row r="15" spans="1:37" ht="30">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
@@ -1536,7 +1535,7 @@
         <v>40939</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18">
+    <row r="16" spans="1:37" ht="17.25">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -1559,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="67">
         <v>0</v>
@@ -1568,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="67">
         <v>0</v>
@@ -1643,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:52" ht="18">
+    <row r="17" spans="4:37" ht="17.25">
       <c r="D17" s="66" t="s">
         <v>37</v>
       </c>
@@ -1687,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S17" s="67">
         <v>0</v>
@@ -1696,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V17" s="67">
         <v>0</v>
@@ -1747,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:52" ht="18">
+    <row r="18" spans="4:37" ht="17.25">
       <c r="D18" s="66" t="s">
         <v>37</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:52" ht="18">
+    <row r="19" spans="4:37" ht="17.25">
       <c r="D19" s="66" t="s">
         <v>37</v>
       </c>
@@ -1951,7 +1950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="4:52" ht="18">
+    <row r="20" spans="4:37" ht="17.25">
       <c r="D20" s="66" t="s">
         <v>37</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O20" s="67">
         <v>0</v>
@@ -2055,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:52" ht="18">
+    <row r="21" spans="4:37" ht="17.25">
       <c r="D21" s="66" t="s">
         <v>38</v>
       </c>
@@ -2125,7 +2124,7 @@
       <c r="AJ21" s="69"/>
       <c r="AK21" s="72"/>
     </row>
-    <row r="22" spans="4:52" ht="18">
+    <row r="22" spans="4:37" ht="17.25">
       <c r="D22" s="66" t="s">
         <v>38</v>
       </c>
@@ -2195,7 +2194,7 @@
       <c r="AJ22" s="69"/>
       <c r="AK22" s="72"/>
     </row>
-    <row r="23" spans="4:52" ht="18">
+    <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="66" t="s">
         <v>38</v>
       </c>
@@ -2265,7 +2264,7 @@
       <c r="AJ23" s="69"/>
       <c r="AK23" s="72"/>
     </row>
-    <row r="24" spans="4:52" ht="18">
+    <row r="24" spans="4:37" ht="17.25">
       <c r="D24" s="66" t="s">
         <v>38</v>
       </c>
@@ -2335,7 +2334,7 @@
       <c r="AJ24" s="69"/>
       <c r="AK24" s="72"/>
     </row>
-    <row r="25" spans="4:52" ht="18">
+    <row r="25" spans="4:37" ht="17.25">
       <c r="D25" s="66" t="s">
         <v>38</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:52" ht="18">
+    <row r="26" spans="4:37" ht="17.25">
       <c r="D26" s="66" t="s">
         <v>39</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="89">
         <v>0</v>
@@ -2468,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="89">
         <v>0</v>
@@ -2543,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:52" ht="18">
+    <row r="27" spans="4:37" ht="17.25">
       <c r="D27" s="66" t="s">
         <v>39</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="R27" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S27" s="89">
         <v>0</v>
@@ -2596,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="U27" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V27" s="89">
         <v>0</v>
@@ -2647,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:52" ht="18">
+    <row r="28" spans="4:37" ht="17.25">
       <c r="D28" s="66" t="s">
         <v>39</v>
       </c>
@@ -2751,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:52" ht="18">
+    <row r="29" spans="4:37" ht="17.25">
       <c r="D29" s="66" t="s">
         <v>39</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="4:52" ht="18">
+    <row r="30" spans="4:37" ht="17.25">
       <c r="D30" s="66" t="s">
         <v>39</v>
       </c>
@@ -2883,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O30" s="89">
         <v>0</v>
@@ -2955,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:52" ht="18">
+    <row r="31" spans="4:37" ht="17.25">
       <c r="D31" s="66" t="s">
         <v>40</v>
       </c>
@@ -3029,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:52" ht="18">
+    <row r="32" spans="4:37" ht="17.25">
       <c r="D32" s="66" t="s">
         <v>40</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:52" ht="18">
+    <row r="33" spans="4:37" ht="17.25">
       <c r="D33" s="66" t="s">
         <v>40</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:52" ht="18">
+    <row r="34" spans="4:37" ht="17.25">
       <c r="D34" s="66" t="s">
         <v>40</v>
       </c>
@@ -3273,7 +3272,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="4:52" ht="18">
+    <row r="35" spans="4:37" ht="17.25">
       <c r="D35" s="66" t="s">
         <v>40</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:52" ht="18">
+    <row r="36" spans="4:37" ht="17.25">
       <c r="D36" s="66" t="s">
         <v>41</v>
       </c>
@@ -3397,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="89">
         <v>0</v>
@@ -3406,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" s="89">
         <v>0</v>
@@ -3481,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:52" ht="18">
+    <row r="37" spans="4:37" ht="17.25">
       <c r="D37" s="66" t="s">
         <v>41</v>
       </c>
@@ -3525,7 +3524,7 @@
         <v>0</v>
       </c>
       <c r="R37" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S37" s="89">
         <v>0</v>
@@ -3534,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="U37" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V37" s="89">
         <v>0</v>
@@ -3585,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:52" ht="18">
+    <row r="38" spans="4:37" ht="17.25">
       <c r="D38" s="66" t="s">
         <v>41</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:52" ht="18">
+    <row r="39" spans="4:37" ht="17.25">
       <c r="D39" s="66" t="s">
         <v>41</v>
       </c>
@@ -3789,7 +3788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="4:52" ht="18">
+    <row r="40" spans="4:37" ht="17.25">
       <c r="D40" s="66" t="s">
         <v>41</v>
       </c>
@@ -3821,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="N40" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O40" s="89">
         <v>0</v>
@@ -3893,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:52" ht="18">
+    <row r="41" spans="4:37" ht="17.25">
       <c r="D41" s="66" t="s">
         <v>42</v>
       </c>
@@ -3913,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="89">
         <v>0</v>
@@ -3922,7 +3921,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N41" s="89">
         <v>0</v>
@@ -3997,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:52" ht="18">
+    <row r="42" spans="4:37" ht="17.25">
       <c r="D42" s="66" t="s">
         <v>42</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S42" s="89">
         <v>0</v>
@@ -4050,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="U42" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V42" s="89">
         <v>0</v>
@@ -4101,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:52" ht="18">
+    <row r="43" spans="4:37" ht="17.25">
       <c r="D43" s="66" t="s">
         <v>42</v>
       </c>
@@ -4205,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:52" ht="18">
+    <row r="44" spans="4:37" ht="17.25">
       <c r="D44" s="66" t="s">
         <v>42</v>
       </c>
@@ -4305,7 +4304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="4:52" ht="18">
+    <row r="45" spans="4:37" ht="17.25">
       <c r="D45" s="66" t="s">
         <v>42</v>
       </c>
@@ -4337,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="N45" s="89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O45" s="89">
         <v>0</v>
@@ -4409,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:52" ht="18">
+    <row r="46" spans="4:37" ht="17.25">
       <c r="D46" s="66" t="s">
         <v>44</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:52" ht="18">
+    <row r="47" spans="4:37" ht="17.25">
       <c r="D47" s="66" t="s">
         <v>44</v>
       </c>
@@ -4617,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:52" ht="18">
+    <row r="48" spans="4:37" ht="17.25">
       <c r="D48" s="66" t="s">
         <v>44</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:52" ht="18">
+    <row r="49" spans="4:37" ht="17.25">
       <c r="D49" s="66" t="s">
         <v>44</v>
       </c>
@@ -4825,7 +4824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="4:52" ht="18.600000000000001" thickBot="1">
+    <row r="50" spans="4:37" ht="18" thickBot="1">
       <c r="D50" s="62" t="s">
         <v>44</v>
       </c>
@@ -4929,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:52">
+    <row r="51" spans="4:37">
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
       <c r="F51" s="51"/>
@@ -4982,26 +4981,26 @@
       <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.5546875" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="39" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.28515625" customWidth="1"/>
     <col min="40" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
-    <col min="43" max="45" width="11.33203125" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="48" width="11.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="43" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="48" width="11.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
     <col min="50" max="50" width="11" customWidth="1"/>
-    <col min="51" max="51" width="11.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
@@ -5016,7 +5015,7 @@
       </c>
       <c r="E1" s="94"/>
     </row>
-    <row r="2" spans="1:44" ht="18">
+    <row r="2" spans="1:44" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="18">
+    <row r="3" spans="1:44" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -5044,7 +5043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:44" ht="27.6">
+    <row r="4" spans="1:44" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -5056,7 +5055,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:44" ht="69">
+    <row r="5" spans="1:44" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -5068,7 +5067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:44" ht="18">
+    <row r="6" spans="1:44" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -5080,7 +5079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:44" ht="18">
+    <row r="7" spans="1:44" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -5092,7 +5091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:44" ht="18">
+    <row r="8" spans="1:44" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -5104,7 +5103,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:44" ht="18">
+    <row r="9" spans="1:44" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -5132,7 +5131,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:44" ht="27.6">
+    <row r="12" spans="1:44" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -5154,7 +5153,7 @@
       <c r="AQ14" s="26"/>
       <c r="AR14" s="26"/>
     </row>
-    <row r="15" spans="1:44" ht="28.2">
+    <row r="15" spans="1:44" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -5249,7 +5248,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="18">
+    <row r="16" spans="1:44" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -5328,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:34" ht="18">
+    <row r="17" spans="4:34" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -5407,7 +5406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:34" ht="18">
+    <row r="18" spans="4:34" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -5486,7 +5485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:34" ht="18">
+    <row r="19" spans="4:34" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -5525,7 +5524,7 @@
       <c r="AG19" s="19"/>
       <c r="AH19" s="19"/>
     </row>
-    <row r="20" spans="4:34" ht="18">
+    <row r="20" spans="4:34" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:34" ht="18">
+    <row r="21" spans="4:34" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>38</v>
       </c>
@@ -5671,7 +5670,7 @@
       <c r="AG21" s="19"/>
       <c r="AH21" s="19"/>
     </row>
-    <row r="22" spans="4:34" ht="18">
+    <row r="22" spans="4:34" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -5738,7 +5737,7 @@
       <c r="AG22" s="19"/>
       <c r="AH22" s="19"/>
     </row>
-    <row r="23" spans="4:34" ht="18">
+    <row r="23" spans="4:34" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -5805,7 +5804,7 @@
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
     </row>
-    <row r="24" spans="4:34" ht="18">
+    <row r="24" spans="4:34" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -5872,7 +5871,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
     </row>
-    <row r="25" spans="4:34" ht="18">
+    <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -5939,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:34" ht="18">
+    <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
@@ -6006,7 +6005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:34" ht="18">
+    <row r="27" spans="4:34" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>39</v>
       </c>
@@ -6075,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:34" ht="18">
+    <row r="28" spans="4:34" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -6144,7 +6143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:34" ht="18">
+    <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>40</v>
       </c>
@@ -6227,7 +6226,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:34" ht="18">
+    <row r="30" spans="4:34" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>40</v>
       </c>
@@ -6310,7 +6309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="4:34" ht="18">
+    <row r="31" spans="4:34" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
@@ -6393,7 +6392,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="4:34" ht="18">
+    <row r="32" spans="4:34" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>40</v>
       </c>
@@ -6476,7 +6475,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="4:34" ht="18">
+    <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>41</v>
       </c>
@@ -6557,7 +6556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="4:34" ht="18">
+    <row r="34" spans="4:34" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
@@ -6638,7 +6637,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="4:34" ht="18">
+    <row r="35" spans="4:34" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
@@ -6719,7 +6718,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="4:34" ht="18">
+    <row r="36" spans="4:34" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>41</v>
       </c>
@@ -6758,7 +6757,7 @@
       <c r="AG36" s="20"/>
       <c r="AH36" s="20"/>
     </row>
-    <row r="37" spans="4:34" ht="18">
+    <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>41</v>
       </c>
@@ -6839,7 +6838,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="4:34" ht="18">
+    <row r="38" spans="4:34" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>42</v>
       </c>
@@ -6922,7 +6921,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="4:34" ht="18">
+    <row r="39" spans="4:34" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>42</v>
       </c>
@@ -7005,7 +7004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:34" ht="18">
+    <row r="40" spans="4:34" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>42</v>
       </c>
@@ -7088,7 +7087,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="4:34" ht="18">
+    <row r="41" spans="4:34" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>42</v>
       </c>
@@ -7127,7 +7126,7 @@
       <c r="AG41" s="20"/>
       <c r="AH41" s="20"/>
     </row>
-    <row r="42" spans="4:34" ht="18">
+    <row r="42" spans="4:34" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>42</v>
       </c>
@@ -7210,7 +7209,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:34" ht="18">
+    <row r="43" spans="4:34" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>44</v>
       </c>
@@ -7291,7 +7290,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="4:34" ht="18">
+    <row r="44" spans="4:34" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>44</v>
       </c>
@@ -7372,7 +7371,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="45" spans="4:34" ht="18" thickBot="1">
       <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
@@ -7453,7 +7452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:34" ht="18.600000000000001" thickBot="1">
+    <row r="46" spans="4:34" ht="18" thickBot="1">
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
@@ -7551,33 +7550,33 @@
       <selection activeCell="AK34" sqref="AK34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -7592,7 +7591,7 @@
       </c>
       <c r="E1" s="94"/>
     </row>
-    <row r="2" spans="1:37" ht="18">
+    <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -7606,7 +7605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="18">
+    <row r="3" spans="1:37" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -7620,7 +7619,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="27.6">
+    <row r="4" spans="1:37" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -7632,7 +7631,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="69">
+    <row r="5" spans="1:37" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -7644,7 +7643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="18">
+    <row r="6" spans="1:37" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -7656,7 +7655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="18">
+    <row r="7" spans="1:37" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -7668,7 +7667,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="18">
+    <row r="8" spans="1:37" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -7680,7 +7679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="18">
+    <row r="9" spans="1:37" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -7708,7 +7707,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="27.6">
+    <row r="12" spans="1:37" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -7730,7 +7729,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
     </row>
-    <row r="15" spans="1:37" ht="28.2">
+    <row r="15" spans="1:37" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -7834,7 +7833,7 @@
         <v>40999</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="18">
+    <row r="16" spans="1:37" ht="17.25">
       <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
@@ -7938,7 +7937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:37" ht="18">
+    <row r="17" spans="4:37" ht="17.25">
       <c r="D17" s="18" t="s">
         <v>37</v>
       </c>
@@ -8042,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:37" ht="18">
+    <row r="18" spans="4:37" ht="17.25">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -8146,7 +8145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:37" ht="18">
+    <row r="19" spans="4:37" ht="17.25">
       <c r="D19" s="18" t="s">
         <v>37</v>
       </c>
@@ -8250,7 +8249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:37" ht="18">
+    <row r="20" spans="4:37" ht="17.25">
       <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
@@ -8350,7 +8349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="4:37" ht="18">
+    <row r="21" spans="4:37" ht="17.25">
       <c r="D21" s="18" t="s">
         <v>37</v>
       </c>
@@ -8450,7 +8449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:37" ht="18">
+    <row r="22" spans="4:37" ht="17.25">
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -8554,7 +8553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:37" ht="18">
+    <row r="23" spans="4:37" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -8658,7 +8657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:37" ht="18">
+    <row r="24" spans="4:37" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -8762,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:37" ht="18">
+    <row r="25" spans="4:37" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -8866,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:37" ht="18">
+    <row r="26" spans="4:37" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -8970,7 +8969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:37" ht="18">
+    <row r="27" spans="4:37" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -9074,7 +9073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:37" ht="18">
+    <row r="28" spans="4:37" ht="17.25">
       <c r="D28" s="18" t="s">
         <v>39</v>
       </c>
@@ -9176,7 +9175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:37" ht="18">
+    <row r="29" spans="4:37" ht="17.25">
       <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
@@ -9278,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:37" ht="18">
+    <row r="30" spans="4:37" ht="17.25">
       <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
@@ -9380,7 +9379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:37" ht="18">
+    <row r="31" spans="4:37" ht="17.25">
       <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
@@ -9482,7 +9481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:37" ht="18">
+    <row r="32" spans="4:37" ht="17.25">
       <c r="D32" s="18" t="s">
         <v>39</v>
       </c>
@@ -9584,7 +9583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:37" ht="18">
+    <row r="33" spans="4:37" ht="17.25">
       <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
@@ -9686,7 +9685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:37" ht="18">
+    <row r="34" spans="4:37" ht="17.25">
       <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
@@ -9790,7 +9789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:37" ht="18">
+    <row r="35" spans="4:37" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -9894,7 +9893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:37" ht="18">
+    <row r="36" spans="4:37" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -9998,7 +9997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:37" ht="18">
+    <row r="37" spans="4:37" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -10102,7 +10101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:37" ht="18">
+    <row r="38" spans="4:37" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -10206,7 +10205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:37" ht="18">
+    <row r="39" spans="4:37" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -10310,7 +10309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:37" ht="18">
+    <row r="40" spans="4:37" ht="17.25">
       <c r="D40" s="18" t="s">
         <v>41</v>
       </c>
@@ -10414,7 +10413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:37" ht="18">
+    <row r="41" spans="4:37" ht="17.25">
       <c r="D41" s="18" t="s">
         <v>41</v>
       </c>
@@ -10518,7 +10517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:37" ht="18">
+    <row r="42" spans="4:37" ht="17.25">
       <c r="D42" s="18" t="s">
         <v>41</v>
       </c>
@@ -10622,7 +10621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:37" ht="18">
+    <row r="43" spans="4:37" ht="17.25">
       <c r="D43" s="18" t="s">
         <v>41</v>
       </c>
@@ -10726,7 +10725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:37" ht="18">
+    <row r="44" spans="4:37" ht="17.25">
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
@@ -10830,7 +10829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="4:37" ht="18">
+    <row r="45" spans="4:37" ht="17.25">
       <c r="D45" s="18" t="s">
         <v>41</v>
       </c>
@@ -10934,7 +10933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="4:37" ht="18">
+    <row r="46" spans="4:37" ht="17.25">
       <c r="D46" s="18" t="s">
         <v>42</v>
       </c>
@@ -11038,7 +11037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:37" ht="18">
+    <row r="47" spans="4:37" ht="17.25">
       <c r="D47" s="18" t="s">
         <v>42</v>
       </c>
@@ -11142,7 +11141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:37" ht="18">
+    <row r="48" spans="4:37" ht="17.25">
       <c r="D48" s="18" t="s">
         <v>42</v>
       </c>
@@ -11246,7 +11245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:37" ht="18">
+    <row r="49" spans="4:37" ht="17.25">
       <c r="D49" s="18" t="s">
         <v>42</v>
       </c>
@@ -11350,7 +11349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:37" ht="18">
+    <row r="50" spans="4:37" ht="17.25">
       <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
@@ -11454,7 +11453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="4:37" ht="18">
+    <row r="51" spans="4:37" ht="17.25">
       <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
@@ -11558,7 +11557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:37" ht="18">
+    <row r="52" spans="4:37" ht="17.25">
       <c r="D52" s="18" t="s">
         <v>44</v>
       </c>
@@ -11662,7 +11661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:37" ht="18">
+    <row r="53" spans="4:37" ht="17.25">
       <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
@@ -11766,7 +11765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="4:37" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -11870,7 +11869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:37" ht="18">
+    <row r="55" spans="4:37" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -11974,7 +11973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="4:37" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -12078,7 +12077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="4:37" ht="18.600000000000001" thickBot="1">
+    <row r="57" spans="4:37" ht="18" thickBot="1">
       <c r="D57" s="12" t="s">
         <v>44</v>
       </c>
@@ -12202,36 +12201,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y11" workbookViewId="0">
-      <selection activeCell="AJ55" sqref="AJ55"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
+    <col min="28" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.28515625" customWidth="1"/>
     <col min="32" max="32" width="11" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" customWidth="1"/>
-    <col min="35" max="35" width="12.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" customWidth="1"/>
+    <col min="33" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -12246,7 +12245,7 @@
       </c>
       <c r="E1" s="94"/>
     </row>
-    <row r="2" spans="1:36" ht="18">
+    <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -12260,7 +12259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="18">
+    <row r="3" spans="1:36" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -12274,7 +12273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="27.6">
+    <row r="4" spans="1:36" ht="28.5">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -12286,7 +12285,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="69">
+    <row r="5" spans="1:36" ht="71.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -12298,7 +12297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="18">
+    <row r="6" spans="1:36" ht="17.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -12310,7 +12309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="18">
+    <row r="7" spans="1:36" ht="17.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -12322,7 +12321,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="18">
+    <row r="8" spans="1:36" ht="17.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -12334,7 +12333,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="18">
+    <row r="9" spans="1:36" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -12362,7 +12361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="27.6">
+    <row r="12" spans="1:36" ht="42.75">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -12384,7 +12383,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
     </row>
-    <row r="15" spans="1:36" ht="28.2">
+    <row r="15" spans="1:36" ht="30">
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
@@ -12485,7 +12484,7 @@
         <v>41029</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="18">
+    <row r="16" spans="1:36" ht="17.25">
       <c r="A16" s="74"/>
       <c r="B16" s="74"/>
       <c r="C16" s="74"/>
@@ -12589,7 +12588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="18">
+    <row r="17" spans="1:36" ht="17.25">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
@@ -12693,7 +12692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="18">
+    <row r="18" spans="1:36" ht="17.25">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
@@ -12797,7 +12796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="18">
+    <row r="19" spans="1:36" ht="17.25">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
@@ -12901,7 +12900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="18">
+    <row r="20" spans="1:36" ht="17.25">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
@@ -13005,7 +13004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="18">
+    <row r="21" spans="1:36" ht="17.25">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
@@ -13109,7 +13108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="18">
+    <row r="22" spans="1:36" ht="17.25">
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
@@ -13193,7 +13192,7 @@
       <c r="AI22" s="77"/>
       <c r="AJ22" s="77"/>
     </row>
-    <row r="23" spans="1:36" ht="18">
+    <row r="23" spans="1:36" ht="17.25">
       <c r="D23" s="18" t="s">
         <v>38</v>
       </c>
@@ -13272,7 +13271,7 @@
       <c r="AG23" s="30"/>
       <c r="AH23" s="22"/>
     </row>
-    <row r="24" spans="1:36" ht="18">
+    <row r="24" spans="1:36" ht="17.25">
       <c r="D24" s="18" t="s">
         <v>38</v>
       </c>
@@ -13351,7 +13350,7 @@
       <c r="AG24" s="30"/>
       <c r="AH24" s="22"/>
     </row>
-    <row r="25" spans="1:36" ht="18">
+    <row r="25" spans="1:36" ht="17.25">
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
@@ -13430,7 +13429,7 @@
       <c r="AG25" s="30"/>
       <c r="AH25" s="22"/>
     </row>
-    <row r="26" spans="1:36" ht="18">
+    <row r="26" spans="1:36" ht="17.25">
       <c r="D26" s="18" t="s">
         <v>38</v>
       </c>
@@ -13509,7 +13508,7 @@
       <c r="AG26" s="30"/>
       <c r="AH26" s="22"/>
     </row>
-    <row r="27" spans="1:36" ht="18">
+    <row r="27" spans="1:36" ht="17.25">
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
@@ -13588,7 +13587,7 @@
       <c r="AG27" s="30"/>
       <c r="AH27" s="22"/>
     </row>
-    <row r="28" spans="1:36" ht="18">
+    <row r="28" spans="1:36" ht="17.25">
       <c r="A28" s="74"/>
       <c r="B28" s="74"/>
       <c r="C28" s="74"/>
@@ -13692,7 +13691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="18">
+    <row r="29" spans="1:36" ht="17.25">
       <c r="A29" s="74"/>
       <c r="B29" s="74"/>
       <c r="C29" s="74"/>
@@ -13796,7 +13795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="18">
+    <row r="30" spans="1:36" ht="17.25">
       <c r="A30" s="74"/>
       <c r="B30" s="74"/>
       <c r="C30" s="74"/>
@@ -13900,7 +13899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="18">
+    <row r="31" spans="1:36" ht="17.25">
       <c r="A31" s="74"/>
       <c r="B31" s="74"/>
       <c r="C31" s="74"/>
@@ -14004,7 +14003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="18">
+    <row r="32" spans="1:36" ht="17.25">
       <c r="A32" s="74"/>
       <c r="B32" s="74"/>
       <c r="C32" s="74"/>
@@ -14108,7 +14107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="18">
+    <row r="33" spans="1:36" ht="17.25">
       <c r="A33" s="74"/>
       <c r="B33" s="74"/>
       <c r="C33" s="74"/>
@@ -14212,7 +14211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="18">
+    <row r="34" spans="1:36" ht="17.25">
       <c r="A34" s="74"/>
       <c r="B34" s="74"/>
       <c r="C34" s="74"/>
@@ -14316,7 +14315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="18">
+    <row r="35" spans="1:36" ht="17.25">
       <c r="D35" s="18" t="s">
         <v>40</v>
       </c>
@@ -14407,7 +14406,7 @@
       <c r="AI35" s="33"/>
       <c r="AJ35" s="22"/>
     </row>
-    <row r="36" spans="1:36" ht="18">
+    <row r="36" spans="1:36" ht="17.25">
       <c r="D36" s="18" t="s">
         <v>40</v>
       </c>
@@ -14498,7 +14497,7 @@
       <c r="AI36" s="33"/>
       <c r="AJ36" s="22"/>
     </row>
-    <row r="37" spans="1:36" ht="18">
+    <row r="37" spans="1:36" ht="17.25">
       <c r="D37" s="18" t="s">
         <v>40</v>
       </c>
@@ -14589,7 +14588,7 @@
       <c r="AI37" s="33"/>
       <c r="AJ37" s="22"/>
     </row>
-    <row r="38" spans="1:36" ht="18">
+    <row r="38" spans="1:36" ht="17.25">
       <c r="D38" s="18" t="s">
         <v>40</v>
       </c>
@@ -14680,7 +14679,7 @@
       <c r="AI38" s="33"/>
       <c r="AJ38" s="22"/>
     </row>
-    <row r="39" spans="1:36" ht="18">
+    <row r="39" spans="1:36" ht="17.25">
       <c r="D39" s="18" t="s">
         <v>40</v>
       </c>
@@ -14771,7 +14770,7 @@
       <c r="AI39" s="33"/>
       <c r="AJ39" s="22"/>
     </row>
-    <row r="40" spans="1:36" ht="18">
+    <row r="40" spans="1:36" ht="17.25">
       <c r="A40" s="80"/>
       <c r="B40" s="80"/>
       <c r="C40" s="80"/>
@@ -14875,7 +14874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="18">
+    <row r="41" spans="1:36" ht="17.25">
       <c r="A41" s="80"/>
       <c r="B41" s="80"/>
       <c r="C41" s="80"/>
@@ -14979,7 +14978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="18">
+    <row r="42" spans="1:36" ht="17.25">
       <c r="A42" s="80"/>
       <c r="B42" s="80"/>
       <c r="C42" s="80"/>
@@ -15083,7 +15082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="18">
+    <row r="43" spans="1:36" ht="17.25">
       <c r="A43" s="80"/>
       <c r="B43" s="80"/>
       <c r="C43" s="80"/>
@@ -15187,7 +15186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="18">
+    <row r="44" spans="1:36" ht="17.25">
       <c r="A44" s="80"/>
       <c r="B44" s="80"/>
       <c r="C44" s="80"/>
@@ -15291,7 +15290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="18">
+    <row r="45" spans="1:36" ht="17.25">
       <c r="A45" s="80"/>
       <c r="B45" s="80"/>
       <c r="C45" s="80"/>
@@ -15395,7 +15394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="18">
+    <row r="46" spans="1:36" ht="17.25">
       <c r="A46" s="80"/>
       <c r="B46" s="80"/>
       <c r="C46" s="80"/>
@@ -15499,7 +15498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="18">
+    <row r="47" spans="1:36" ht="17.25">
       <c r="A47" s="80"/>
       <c r="B47" s="80"/>
       <c r="C47" s="80"/>
@@ -15603,7 +15602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="18">
+    <row r="48" spans="1:36" ht="17.25">
       <c r="A48" s="80"/>
       <c r="B48" s="80"/>
       <c r="C48" s="80"/>
@@ -15707,7 +15706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="18">
+    <row r="49" spans="1:36" ht="17.25">
       <c r="A49" s="80"/>
       <c r="B49" s="80"/>
       <c r="C49" s="80"/>
@@ -15811,7 +15810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="18">
+    <row r="50" spans="1:36" ht="17.25">
       <c r="A50" s="80"/>
       <c r="B50" s="80"/>
       <c r="C50" s="80"/>
@@ -15915,7 +15914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="18">
+    <row r="51" spans="1:36" ht="17.25">
       <c r="A51" s="80"/>
       <c r="B51" s="80"/>
       <c r="C51" s="80"/>
@@ -16019,7 +16018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="18">
+    <row r="52" spans="1:36" ht="17.25">
       <c r="A52" s="80"/>
       <c r="B52" s="80"/>
       <c r="C52" s="80"/>
@@ -16123,7 +16122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="18">
+    <row r="53" spans="1:36" ht="17.25">
       <c r="A53" s="80"/>
       <c r="B53" s="80"/>
       <c r="C53" s="80"/>
@@ -16227,7 +16226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="18.600000000000001" thickBot="1">
+    <row r="54" spans="1:36" ht="18" thickBot="1">
       <c r="D54" s="12" t="s">
         <v>44</v>
       </c>
@@ -16328,7 +16327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="18">
+    <row r="55" spans="1:36" ht="17.25">
       <c r="D55" s="18" t="s">
         <v>44</v>
       </c>
@@ -16429,7 +16428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="18.600000000000001" thickBot="1">
+    <row r="56" spans="1:36" ht="18" thickBot="1">
       <c r="D56" s="12" t="s">
         <v>44</v>
       </c>
@@ -16530,7 +16529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="18">
+    <row r="57" spans="1:36" ht="17.25">
       <c r="D57" s="88" t="s">
         <v>44</v>
       </c>
@@ -16631,7 +16630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="18.600000000000001" thickBot="1">
+    <row r="58" spans="1:36" ht="18" thickBot="1">
       <c r="D58" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Done By: B S Deepthi Date: 25-4-2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="January 2013" sheetId="5" r:id="rId1"/>
@@ -13,12 +13,11 @@
     <sheet name="April 2013 " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="AD8:AQ24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="49">
   <si>
     <t>Activity Code</t>
   </si>
@@ -168,6 +167,9 @@
     <t>Documentation(includes usecases, 
 Interaction Stories, test transactions, Flow of events,
  Screen navigation diagrams,other project documentation)</t>
+  </si>
+  <si>
+    <t>Time Sheet for th month of January</t>
   </si>
 </sst>
 </file>
@@ -421,7 +423,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -621,6 +623,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:N25"/>
+    <sheetView topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -951,7 +957,7 @@
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="94" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E1" s="94"/>
       <c r="F1" s="51"/>
@@ -4056,518 +4062,518 @@
       </c>
     </row>
     <row r="41" spans="4:37" ht="17.25">
-      <c r="D41" s="66" t="s">
+      <c r="D41" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="66" t="s">
+      <c r="E41" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="G41" s="89">
-        <v>0</v>
-      </c>
-      <c r="H41" s="89">
-        <v>0</v>
-      </c>
-      <c r="I41" s="89">
-        <v>0</v>
-      </c>
-      <c r="J41" s="89">
+      <c r="F41" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="48">
+        <v>0</v>
+      </c>
+      <c r="H41" s="48">
+        <v>0</v>
+      </c>
+      <c r="I41" s="48">
+        <v>0</v>
+      </c>
+      <c r="J41" s="48">
         <v>1</v>
       </c>
-      <c r="K41" s="89">
-        <v>0</v>
-      </c>
-      <c r="L41" s="89">
-        <v>0</v>
-      </c>
-      <c r="M41" s="89">
+      <c r="K41" s="48">
+        <v>2</v>
+      </c>
+      <c r="L41" s="48">
+        <v>0</v>
+      </c>
+      <c r="M41" s="48">
         <v>1</v>
       </c>
-      <c r="N41" s="89">
-        <v>0</v>
-      </c>
-      <c r="O41" s="89">
-        <v>0</v>
-      </c>
-      <c r="P41" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="89">
-        <v>0</v>
-      </c>
-      <c r="R41" s="89">
-        <v>0</v>
-      </c>
-      <c r="S41" s="89">
-        <v>0</v>
-      </c>
-      <c r="T41" s="89">
-        <v>0</v>
-      </c>
-      <c r="U41" s="89">
-        <v>0</v>
-      </c>
-      <c r="V41" s="89">
-        <v>2</v>
-      </c>
-      <c r="W41" s="89">
+      <c r="N41" s="48">
+        <v>2</v>
+      </c>
+      <c r="O41" s="48">
+        <v>0</v>
+      </c>
+      <c r="P41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="48">
+        <v>0</v>
+      </c>
+      <c r="R41" s="48">
+        <v>2</v>
+      </c>
+      <c r="S41" s="48">
+        <v>0</v>
+      </c>
+      <c r="T41" s="48">
+        <v>0</v>
+      </c>
+      <c r="U41" s="48">
+        <v>0</v>
+      </c>
+      <c r="V41" s="48">
+        <v>2</v>
+      </c>
+      <c r="W41" s="48">
+        <v>3</v>
+      </c>
+      <c r="X41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="48">
+        <v>4</v>
+      </c>
+      <c r="AE41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="48">
+        <v>3</v>
+      </c>
+      <c r="AI41" s="48">
+        <v>3</v>
+      </c>
+      <c r="AJ41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AK41" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:37" ht="17.25">
+      <c r="D42" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="48">
+        <v>0</v>
+      </c>
+      <c r="H42" s="48">
+        <v>0</v>
+      </c>
+      <c r="I42" s="48">
+        <v>0</v>
+      </c>
+      <c r="J42" s="48">
+        <v>0</v>
+      </c>
+      <c r="K42" s="48">
+        <v>0</v>
+      </c>
+      <c r="L42" s="48">
+        <v>0</v>
+      </c>
+      <c r="M42" s="48">
+        <v>0</v>
+      </c>
+      <c r="N42" s="48">
+        <v>0</v>
+      </c>
+      <c r="O42" s="48">
+        <v>0</v>
+      </c>
+      <c r="P42" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="48">
+        <v>0</v>
+      </c>
+      <c r="R42" s="48">
+        <v>0</v>
+      </c>
+      <c r="S42" s="48">
+        <v>0</v>
+      </c>
+      <c r="T42" s="48">
+        <v>0</v>
+      </c>
+      <c r="U42" s="48">
+        <v>0</v>
+      </c>
+      <c r="V42" s="48">
+        <v>0</v>
+      </c>
+      <c r="W42" s="48">
+        <v>0</v>
+      </c>
+      <c r="X42" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="48">
+        <v>2</v>
+      </c>
+      <c r="Z42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="48">
+        <v>3</v>
+      </c>
+      <c r="AC42" s="48">
+        <v>2</v>
+      </c>
+      <c r="AD42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:37" ht="17.25">
+      <c r="D43" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="48">
+        <v>0</v>
+      </c>
+      <c r="H43" s="48">
+        <v>0</v>
+      </c>
+      <c r="I43" s="48">
+        <v>0</v>
+      </c>
+      <c r="J43" s="48">
+        <v>0</v>
+      </c>
+      <c r="K43" s="48">
+        <v>0</v>
+      </c>
+      <c r="L43" s="48">
+        <v>0</v>
+      </c>
+      <c r="M43" s="48">
+        <v>0</v>
+      </c>
+      <c r="N43" s="48">
+        <v>0</v>
+      </c>
+      <c r="O43" s="48">
+        <v>0</v>
+      </c>
+      <c r="P43" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="48">
+        <v>0</v>
+      </c>
+      <c r="R43" s="48">
+        <v>0</v>
+      </c>
+      <c r="S43" s="48">
+        <v>0</v>
+      </c>
+      <c r="T43" s="48">
+        <v>0</v>
+      </c>
+      <c r="U43" s="48">
+        <v>0</v>
+      </c>
+      <c r="V43" s="48">
+        <v>0</v>
+      </c>
+      <c r="W43" s="48">
+        <v>0</v>
+      </c>
+      <c r="X43" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AK43" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:37" ht="17.25">
+      <c r="D44" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="F44" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="48">
+        <v>0</v>
+      </c>
+      <c r="H44" s="48">
+        <v>0</v>
+      </c>
+      <c r="I44" s="48">
+        <v>0</v>
+      </c>
+      <c r="J44" s="48">
+        <v>0</v>
+      </c>
+      <c r="K44" s="48">
+        <v>0</v>
+      </c>
+      <c r="L44" s="48">
+        <v>0</v>
+      </c>
+      <c r="M44" s="48">
+        <v>0</v>
+      </c>
+      <c r="N44" s="48">
+        <v>0</v>
+      </c>
+      <c r="O44" s="48">
+        <v>0</v>
+      </c>
+      <c r="P44" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="48">
+        <v>0</v>
+      </c>
+      <c r="R44" s="48">
+        <v>0</v>
+      </c>
+      <c r="S44" s="48">
+        <v>0</v>
+      </c>
+      <c r="T44" s="48">
+        <v>0</v>
+      </c>
+      <c r="U44" s="48">
+        <v>0</v>
+      </c>
+      <c r="V44" s="48">
+        <v>0</v>
+      </c>
+      <c r="W44" s="48">
+        <v>0</v>
+      </c>
+      <c r="X44" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="48"/>
+      <c r="AA44" s="48"/>
+      <c r="AB44" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="48">
+        <v>3</v>
+      </c>
+      <c r="AD44" s="48">
         <v>1</v>
       </c>
-      <c r="X41" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="89">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="68">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AE41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AF41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AG41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AH41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AI41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AJ41" s="89">
-        <v>0</v>
-      </c>
-      <c r="AK41" s="90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="4:37" ht="17.25">
-      <c r="D42" s="66" t="s">
+      <c r="AE44" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF44" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH44" s="48">
+        <v>0</v>
+      </c>
+      <c r="AI44" s="48">
+        <v>4</v>
+      </c>
+      <c r="AJ44" s="48">
+        <v>3</v>
+      </c>
+      <c r="AK44" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:37" ht="17.25">
+      <c r="D45" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="66" t="s">
+      <c r="E45" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" s="89">
-        <v>0</v>
-      </c>
-      <c r="H42" s="89">
-        <v>0</v>
-      </c>
-      <c r="I42" s="89">
-        <v>0</v>
-      </c>
-      <c r="J42" s="89">
-        <v>0</v>
-      </c>
-      <c r="K42" s="89">
-        <v>0</v>
-      </c>
-      <c r="L42" s="89">
-        <v>0</v>
-      </c>
-      <c r="M42" s="89">
-        <v>0</v>
-      </c>
-      <c r="N42" s="89">
-        <v>0</v>
-      </c>
-      <c r="O42" s="89">
-        <v>0</v>
-      </c>
-      <c r="P42" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="89">
-        <v>0</v>
-      </c>
-      <c r="R42" s="89">
-        <v>2</v>
-      </c>
-      <c r="S42" s="89">
-        <v>0</v>
-      </c>
-      <c r="T42" s="89">
-        <v>0</v>
-      </c>
-      <c r="U42" s="89">
-        <v>2</v>
-      </c>
-      <c r="V42" s="89">
-        <v>0</v>
-      </c>
-      <c r="W42" s="89">
-        <v>0</v>
-      </c>
-      <c r="X42" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="89">
-        <v>2</v>
-      </c>
-      <c r="Z42" s="68">
-        <v>0</v>
-      </c>
-      <c r="AA42" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB42" s="89">
-        <v>3</v>
-      </c>
-      <c r="AC42" s="89">
-        <v>2</v>
-      </c>
-      <c r="AD42" s="89">
-        <v>1</v>
-      </c>
-      <c r="AE42" s="89">
-        <v>0</v>
-      </c>
-      <c r="AF42" s="89">
-        <v>0</v>
-      </c>
-      <c r="AG42" s="89">
-        <v>0</v>
-      </c>
-      <c r="AH42" s="89">
-        <v>2</v>
-      </c>
-      <c r="AI42" s="89">
-        <v>0</v>
-      </c>
-      <c r="AJ42" s="89">
-        <v>0</v>
-      </c>
-      <c r="AK42" s="90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="4:37" ht="17.25">
-      <c r="D43" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="G43" s="89">
-        <v>0</v>
-      </c>
-      <c r="H43" s="89">
-        <v>0</v>
-      </c>
-      <c r="I43" s="89">
-        <v>0</v>
-      </c>
-      <c r="J43" s="89">
-        <v>0</v>
-      </c>
-      <c r="K43" s="89">
-        <v>0</v>
-      </c>
-      <c r="L43" s="89">
-        <v>0</v>
-      </c>
-      <c r="M43" s="89">
-        <v>0</v>
-      </c>
-      <c r="N43" s="89">
-        <v>0</v>
-      </c>
-      <c r="O43" s="89">
-        <v>0</v>
-      </c>
-      <c r="P43" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="89">
-        <v>0</v>
-      </c>
-      <c r="R43" s="89">
-        <v>0</v>
-      </c>
-      <c r="S43" s="89">
-        <v>0</v>
-      </c>
-      <c r="T43" s="89">
-        <v>0</v>
-      </c>
-      <c r="U43" s="89">
-        <v>0</v>
-      </c>
-      <c r="V43" s="89">
-        <v>0</v>
-      </c>
-      <c r="W43" s="89">
-        <v>0</v>
-      </c>
-      <c r="X43" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="89">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="68">
-        <v>0</v>
-      </c>
-      <c r="AA43" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AD43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AE43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AF43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AG43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AH43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AI43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AJ43" s="89">
-        <v>0</v>
-      </c>
-      <c r="AK43" s="90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="4:37" ht="17.25">
-      <c r="D44" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="F44" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="89">
-        <v>0</v>
-      </c>
-      <c r="H44" s="89">
-        <v>0</v>
-      </c>
-      <c r="I44" s="89">
-        <v>0</v>
-      </c>
-      <c r="J44" s="89">
-        <v>0</v>
-      </c>
-      <c r="K44" s="89">
-        <v>0</v>
-      </c>
-      <c r="L44" s="89">
-        <v>0</v>
-      </c>
-      <c r="M44" s="89">
-        <v>0</v>
-      </c>
-      <c r="N44" s="89">
-        <v>0</v>
-      </c>
-      <c r="O44" s="89">
-        <v>0</v>
-      </c>
-      <c r="P44" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="89">
-        <v>0</v>
-      </c>
-      <c r="R44" s="89">
-        <v>0</v>
-      </c>
-      <c r="S44" s="89">
-        <v>0</v>
-      </c>
-      <c r="T44" s="89">
-        <v>0</v>
-      </c>
-      <c r="U44" s="89">
-        <v>0</v>
-      </c>
-      <c r="V44" s="89">
-        <v>0</v>
-      </c>
-      <c r="W44" s="89">
-        <v>0</v>
-      </c>
-      <c r="X44" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="89">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="68"/>
-      <c r="AA44" s="68"/>
-      <c r="AB44" s="89">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="89">
-        <v>3</v>
-      </c>
-      <c r="AD44" s="89">
-        <v>1</v>
-      </c>
-      <c r="AE44" s="89">
-        <v>0</v>
-      </c>
-      <c r="AF44" s="89">
-        <v>0</v>
-      </c>
-      <c r="AG44" s="89">
-        <v>0</v>
-      </c>
-      <c r="AH44" s="89">
-        <v>0</v>
-      </c>
-      <c r="AI44" s="89">
-        <v>4</v>
-      </c>
-      <c r="AJ44" s="89">
-        <v>3</v>
-      </c>
-      <c r="AK44" s="90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="4:37" ht="17.25">
-      <c r="D45" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="67" t="s">
+      <c r="F45" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="89">
-        <v>0</v>
-      </c>
-      <c r="H45" s="89">
-        <v>0</v>
-      </c>
-      <c r="I45" s="89">
-        <v>0</v>
-      </c>
-      <c r="J45" s="89">
-        <v>0</v>
-      </c>
-      <c r="K45" s="89">
-        <v>0</v>
-      </c>
-      <c r="L45" s="89">
-        <v>0</v>
-      </c>
-      <c r="M45" s="89">
-        <v>0</v>
-      </c>
-      <c r="N45" s="89">
-        <v>2</v>
-      </c>
-      <c r="O45" s="89">
-        <v>0</v>
-      </c>
-      <c r="P45" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="89">
-        <v>0</v>
-      </c>
-      <c r="R45" s="89">
-        <v>0</v>
-      </c>
-      <c r="S45" s="89">
-        <v>0</v>
-      </c>
-      <c r="T45" s="89">
-        <v>0</v>
-      </c>
-      <c r="U45" s="89">
-        <v>0</v>
-      </c>
-      <c r="V45" s="89">
-        <v>0</v>
-      </c>
-      <c r="W45" s="89">
-        <v>0</v>
-      </c>
-      <c r="X45" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="89">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="68">
-        <v>0</v>
-      </c>
-      <c r="AA45" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="89">
+      <c r="G45" s="48">
+        <v>0</v>
+      </c>
+      <c r="H45" s="48">
+        <v>0</v>
+      </c>
+      <c r="I45" s="48">
+        <v>0</v>
+      </c>
+      <c r="J45" s="48">
+        <v>0</v>
+      </c>
+      <c r="K45" s="48">
+        <v>0</v>
+      </c>
+      <c r="L45" s="48">
+        <v>0</v>
+      </c>
+      <c r="M45" s="48">
+        <v>0</v>
+      </c>
+      <c r="N45" s="48">
+        <v>0</v>
+      </c>
+      <c r="O45" s="48">
+        <v>0</v>
+      </c>
+      <c r="P45" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="48">
+        <v>0</v>
+      </c>
+      <c r="R45" s="48">
+        <v>0</v>
+      </c>
+      <c r="S45" s="48">
+        <v>0</v>
+      </c>
+      <c r="T45" s="48">
+        <v>0</v>
+      </c>
+      <c r="U45" s="48">
+        <v>0</v>
+      </c>
+      <c r="V45" s="48">
+        <v>0</v>
+      </c>
+      <c r="W45" s="48">
+        <v>0</v>
+      </c>
+      <c r="X45" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="48">
         <v>2.5</v>
       </c>
-      <c r="AC45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AD45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AE45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AF45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AG45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AH45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AI45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AJ45" s="89">
-        <v>0</v>
-      </c>
-      <c r="AK45" s="90">
+      <c r="AC45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AI45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AJ45" s="48">
+        <v>0</v>
+      </c>
+      <c r="AK45" s="40">
         <v>0</v>
       </c>
     </row>
@@ -5140,8 +5146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AR46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="X21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:AH42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7088,374 +7094,478 @@
       </c>
     </row>
     <row r="38" spans="4:34" ht="17.25">
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N38" s="19">
-        <v>0</v>
-      </c>
-      <c r="O38" s="19">
-        <v>0</v>
-      </c>
-      <c r="P38" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R38" s="19">
-        <v>0</v>
-      </c>
-      <c r="S38" s="19">
-        <v>0</v>
-      </c>
-      <c r="T38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U38" s="19">
-        <v>0</v>
-      </c>
-      <c r="V38" s="19">
-        <v>0</v>
-      </c>
-      <c r="W38" s="19">
-        <v>0</v>
-      </c>
-      <c r="X38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y38" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA38" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH38" s="20" t="s">
-        <v>43</v>
+      <c r="G38" s="48">
+        <v>0</v>
+      </c>
+      <c r="H38" s="48">
+        <v>0</v>
+      </c>
+      <c r="I38" s="48">
+        <v>0</v>
+      </c>
+      <c r="J38" s="48">
+        <v>0</v>
+      </c>
+      <c r="K38" s="48">
+        <v>0</v>
+      </c>
+      <c r="L38" s="48">
+        <v>0</v>
+      </c>
+      <c r="M38" s="48">
+        <v>0</v>
+      </c>
+      <c r="N38" s="48">
+        <v>0</v>
+      </c>
+      <c r="O38" s="48">
+        <v>0</v>
+      </c>
+      <c r="P38" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="48">
+        <v>0</v>
+      </c>
+      <c r="R38" s="48">
+        <v>0</v>
+      </c>
+      <c r="S38" s="48">
+        <v>0</v>
+      </c>
+      <c r="T38" s="48">
+        <v>0</v>
+      </c>
+      <c r="U38" s="48">
+        <v>0</v>
+      </c>
+      <c r="V38" s="48">
+        <v>0</v>
+      </c>
+      <c r="W38" s="48">
+        <v>0</v>
+      </c>
+      <c r="X38" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="4:34" ht="17.25">
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N39" s="19">
+      <c r="G39" s="48">
+        <v>0</v>
+      </c>
+      <c r="H39" s="48">
+        <v>3</v>
+      </c>
+      <c r="I39" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="J39" s="48">
+        <v>3</v>
+      </c>
+      <c r="K39" s="48">
+        <v>3</v>
+      </c>
+      <c r="L39" s="48">
+        <v>6</v>
+      </c>
+      <c r="M39" s="48">
+        <v>0</v>
+      </c>
+      <c r="N39" s="48">
         <v>0.5</v>
       </c>
-      <c r="O39" s="19">
+      <c r="O39" s="48">
         <v>9</v>
       </c>
-      <c r="P39" s="19">
+      <c r="P39" s="48">
         <v>7</v>
       </c>
-      <c r="Q39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R39" s="19">
-        <v>0</v>
-      </c>
-      <c r="S39" s="19">
-        <v>0</v>
-      </c>
-      <c r="T39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U39" s="19">
-        <v>0</v>
-      </c>
-      <c r="V39" s="19">
-        <v>0</v>
-      </c>
-      <c r="W39" s="19">
-        <v>0</v>
-      </c>
-      <c r="X39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y39" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA39" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH39" s="20" t="s">
-        <v>43</v>
+      <c r="Q39" s="48">
+        <v>0</v>
+      </c>
+      <c r="R39" s="48">
+        <v>0</v>
+      </c>
+      <c r="S39" s="48">
+        <v>0</v>
+      </c>
+      <c r="T39" s="48">
+        <v>0</v>
+      </c>
+      <c r="U39" s="48">
+        <v>0</v>
+      </c>
+      <c r="V39" s="48">
+        <v>0</v>
+      </c>
+      <c r="W39" s="48">
+        <v>0</v>
+      </c>
+      <c r="X39" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="4:34" ht="17.25">
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N40" s="19">
+      <c r="G40" s="48">
+        <v>0</v>
+      </c>
+      <c r="H40" s="48">
+        <v>0</v>
+      </c>
+      <c r="I40" s="48">
+        <v>0</v>
+      </c>
+      <c r="J40" s="48">
+        <v>0</v>
+      </c>
+      <c r="K40" s="48">
+        <v>0</v>
+      </c>
+      <c r="L40" s="48">
+        <v>0</v>
+      </c>
+      <c r="M40" s="48">
+        <v>0</v>
+      </c>
+      <c r="N40" s="48">
         <v>4</v>
       </c>
-      <c r="O40" s="19">
-        <v>0</v>
-      </c>
-      <c r="P40" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R40" s="19">
-        <v>2</v>
-      </c>
-      <c r="S40" s="19">
+      <c r="O40" s="48">
+        <v>0</v>
+      </c>
+      <c r="P40" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="48">
+        <v>0</v>
+      </c>
+      <c r="R40" s="48">
+        <v>2</v>
+      </c>
+      <c r="S40" s="48">
         <v>0.5</v>
       </c>
-      <c r="T40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U40" s="19">
+      <c r="T40" s="48">
+        <v>0</v>
+      </c>
+      <c r="U40" s="48">
         <v>5</v>
       </c>
-      <c r="V40" s="19">
-        <v>2</v>
-      </c>
-      <c r="W40" s="19">
+      <c r="V40" s="48">
+        <v>2</v>
+      </c>
+      <c r="W40" s="48">
         <v>0.5</v>
       </c>
-      <c r="X40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y40" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA40" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH40" s="20" t="s">
-        <v>43</v>
+      <c r="X40" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="4:34" ht="17.25">
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="20"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="20"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="20"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="20"/>
-      <c r="AA41" s="19"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="20"/>
-      <c r="AD41" s="20"/>
-      <c r="AE41" s="20"/>
-      <c r="AF41" s="20"/>
-      <c r="AG41" s="20"/>
-      <c r="AH41" s="20"/>
+      <c r="G41" s="48">
+        <v>2</v>
+      </c>
+      <c r="H41" s="48">
+        <v>0</v>
+      </c>
+      <c r="I41" s="48">
+        <v>0</v>
+      </c>
+      <c r="J41" s="48">
+        <v>0</v>
+      </c>
+      <c r="K41" s="48">
+        <v>0</v>
+      </c>
+      <c r="L41" s="48">
+        <v>0</v>
+      </c>
+      <c r="M41" s="48">
+        <v>0</v>
+      </c>
+      <c r="N41" s="48">
+        <v>0</v>
+      </c>
+      <c r="O41" s="48">
+        <v>0</v>
+      </c>
+      <c r="P41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="48">
+        <v>0</v>
+      </c>
+      <c r="R41" s="48">
+        <v>0</v>
+      </c>
+      <c r="S41" s="48">
+        <v>0</v>
+      </c>
+      <c r="T41" s="48">
+        <v>0</v>
+      </c>
+      <c r="U41" s="48">
+        <v>0</v>
+      </c>
+      <c r="V41" s="48">
+        <v>0</v>
+      </c>
+      <c r="W41" s="48">
+        <v>0</v>
+      </c>
+      <c r="X41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="4:34" ht="17.25">
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F42" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N42" s="19">
+      <c r="G42" s="48">
+        <v>0</v>
+      </c>
+      <c r="H42" s="48">
+        <v>0</v>
+      </c>
+      <c r="I42" s="48">
+        <v>0</v>
+      </c>
+      <c r="J42" s="48">
+        <v>0</v>
+      </c>
+      <c r="K42" s="48">
+        <v>0</v>
+      </c>
+      <c r="L42" s="48">
+        <v>0</v>
+      </c>
+      <c r="M42" s="48">
+        <v>0</v>
+      </c>
+      <c r="N42" s="48">
         <v>0.25</v>
       </c>
-      <c r="O42" s="19">
+      <c r="O42" s="48">
         <v>1</v>
       </c>
-      <c r="P42" s="19">
+      <c r="P42" s="48">
         <v>1</v>
       </c>
-      <c r="Q42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R42" s="19">
+      <c r="Q42" s="48">
+        <v>0</v>
+      </c>
+      <c r="R42" s="48">
         <v>1.5</v>
       </c>
-      <c r="S42" s="19">
-        <v>0</v>
-      </c>
-      <c r="T42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U42" s="19">
-        <v>0</v>
-      </c>
-      <c r="V42" s="19">
-        <v>0</v>
-      </c>
-      <c r="W42" s="19">
+      <c r="S42" s="48">
+        <v>0</v>
+      </c>
+      <c r="T42" s="48">
+        <v>0</v>
+      </c>
+      <c r="U42" s="48">
+        <v>0</v>
+      </c>
+      <c r="V42" s="48">
+        <v>0</v>
+      </c>
+      <c r="W42" s="48">
         <v>0.5</v>
       </c>
-      <c r="X42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y42" s="19">
+      <c r="X42" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="48">
         <v>1</v>
       </c>
-      <c r="Z42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA42" s="19">
+      <c r="Z42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="48">
         <v>1.5</v>
       </c>
-      <c r="AB42" s="19">
+      <c r="AB42" s="48">
         <v>1.5</v>
       </c>
-      <c r="AC42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH42" s="20" t="s">
-        <v>43</v>
+      <c r="AC42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="4:34" ht="17.25">
@@ -7795,8 +7905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK58"/>
   <sheetViews>
-    <sheetView topLeftCell="AA28" workbookViewId="0">
-      <selection activeCell="AK34" sqref="AK34"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11183,626 +11293,626 @@
       </c>
     </row>
     <row r="46" spans="4:37" ht="17.25">
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F46" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H46" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="K46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="M46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="N46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="O46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="S46" s="38">
-        <v>0</v>
-      </c>
-      <c r="T46" s="38">
-        <v>0</v>
-      </c>
-      <c r="U46" s="38">
-        <v>0</v>
-      </c>
-      <c r="V46" s="38">
-        <v>0</v>
-      </c>
-      <c r="W46" s="38">
-        <v>0</v>
-      </c>
-      <c r="X46" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD46" s="42">
-        <v>0</v>
-      </c>
-      <c r="AE46" s="42">
-        <v>0</v>
-      </c>
-      <c r="AF46" s="42">
-        <v>0</v>
-      </c>
-      <c r="AG46" s="42">
-        <v>0</v>
-      </c>
-      <c r="AH46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AJ46" s="38">
-        <v>0</v>
-      </c>
-      <c r="AK46" s="38">
+      <c r="G46" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="N46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R46" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="S46" s="40">
+        <v>0</v>
+      </c>
+      <c r="T46" s="40">
+        <v>0</v>
+      </c>
+      <c r="U46" s="40">
+        <v>0</v>
+      </c>
+      <c r="V46" s="40">
+        <v>0</v>
+      </c>
+      <c r="W46" s="40">
+        <v>0</v>
+      </c>
+      <c r="X46" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="96">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="96">
+        <v>0</v>
+      </c>
+      <c r="AF46" s="96">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="96">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="4:37" ht="17.25">
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E47" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H47" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="K47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="M47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="N47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="O47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="S47" s="38">
-        <v>0</v>
-      </c>
-      <c r="T47" s="38">
-        <v>0</v>
-      </c>
-      <c r="U47" s="38">
-        <v>0</v>
-      </c>
-      <c r="V47" s="38">
-        <v>0</v>
-      </c>
-      <c r="W47" s="38">
-        <v>0</v>
-      </c>
-      <c r="X47" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="38">
+      <c r="G47" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H47" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="N47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R47" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="S47" s="40">
+        <v>0</v>
+      </c>
+      <c r="T47" s="40">
+        <v>0</v>
+      </c>
+      <c r="U47" s="40">
+        <v>0</v>
+      </c>
+      <c r="V47" s="40">
+        <v>0</v>
+      </c>
+      <c r="W47" s="40">
+        <v>0</v>
+      </c>
+      <c r="X47" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="40">
         <v>5</v>
       </c>
-      <c r="Z47" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB47" s="38">
+      <c r="Z47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="40">
         <v>1</v>
       </c>
-      <c r="AC47" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD47" s="42">
-        <v>0</v>
-      </c>
-      <c r="AE47" s="42">
-        <v>0</v>
-      </c>
-      <c r="AF47" s="42">
-        <v>0</v>
-      </c>
-      <c r="AG47" s="42">
-        <v>0</v>
-      </c>
-      <c r="AH47" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI47" s="38">
-        <v>0</v>
-      </c>
-      <c r="AJ47" s="38">
-        <v>0</v>
-      </c>
-      <c r="AK47" s="38">
+      <c r="AC47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="96">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="96">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="96">
+        <v>0</v>
+      </c>
+      <c r="AG47" s="96">
+        <v>0</v>
+      </c>
+      <c r="AH47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="4:37" ht="17.25">
-      <c r="D48" s="18" t="s">
+      <c r="D48" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="E48" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H48" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="K48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="M48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="N48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="O48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="S48" s="38">
-        <v>0</v>
-      </c>
-      <c r="T48" s="38">
-        <v>0</v>
-      </c>
-      <c r="U48" s="38">
-        <v>0</v>
-      </c>
-      <c r="V48" s="38">
-        <v>0</v>
-      </c>
-      <c r="W48" s="38">
-        <v>0</v>
-      </c>
-      <c r="X48" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD48" s="42">
+      <c r="G48" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="N48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R48" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="S48" s="40">
+        <v>0</v>
+      </c>
+      <c r="T48" s="40">
+        <v>0</v>
+      </c>
+      <c r="U48" s="40">
+        <v>0</v>
+      </c>
+      <c r="V48" s="40">
+        <v>0</v>
+      </c>
+      <c r="W48" s="40">
+        <v>0</v>
+      </c>
+      <c r="X48" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="96">
         <v>3</v>
       </c>
-      <c r="AE48" s="42">
-        <v>0</v>
-      </c>
-      <c r="AF48" s="42">
-        <v>0</v>
-      </c>
-      <c r="AG48" s="42">
-        <v>0</v>
-      </c>
-      <c r="AH48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AJ48" s="38">
-        <v>0</v>
-      </c>
-      <c r="AK48" s="38">
+      <c r="AE48" s="96">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="96">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="96">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK48" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="4:37" ht="17.25">
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="F49" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H49" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="K49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="M49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="N49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="O49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R49" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="S49" s="38">
+      <c r="G49" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="N49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R49" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="S49" s="40">
         <v>1</v>
       </c>
-      <c r="T49" s="38">
-        <v>2</v>
-      </c>
-      <c r="U49" s="38">
-        <v>2</v>
-      </c>
-      <c r="V49" s="38">
-        <v>0</v>
-      </c>
-      <c r="W49" s="38">
-        <v>0</v>
-      </c>
-      <c r="X49" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD49" s="42">
-        <v>0</v>
-      </c>
-      <c r="AE49" s="42">
-        <v>0</v>
-      </c>
-      <c r="AF49" s="42">
-        <v>0</v>
-      </c>
-      <c r="AG49" s="42">
-        <v>0</v>
-      </c>
-      <c r="AH49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AJ49" s="38">
-        <v>0</v>
-      </c>
-      <c r="AK49" s="38">
+      <c r="T49" s="40">
+        <v>2</v>
+      </c>
+      <c r="U49" s="40">
+        <v>2</v>
+      </c>
+      <c r="V49" s="40">
+        <v>0</v>
+      </c>
+      <c r="W49" s="40">
+        <v>0</v>
+      </c>
+      <c r="X49" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="96">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="96">
+        <v>0</v>
+      </c>
+      <c r="AF49" s="96">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="96">
+        <v>0</v>
+      </c>
+      <c r="AH49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK49" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="4:37" ht="17.25">
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E50" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F50" s="19" t="s">
+      <c r="F50" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G50" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H50" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="K50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="M50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="N50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="O50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R50" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="S50" s="38">
-        <v>0</v>
-      </c>
-      <c r="T50" s="38">
-        <v>0</v>
-      </c>
-      <c r="U50" s="38">
-        <v>0</v>
-      </c>
-      <c r="V50" s="38">
+      <c r="G50" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="N50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R50" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="S50" s="40">
+        <v>0</v>
+      </c>
+      <c r="T50" s="40">
+        <v>0</v>
+      </c>
+      <c r="U50" s="40">
+        <v>0</v>
+      </c>
+      <c r="V50" s="40">
         <v>4</v>
       </c>
-      <c r="W50" s="38">
+      <c r="W50" s="40">
         <v>4</v>
       </c>
-      <c r="X50" s="38">
+      <c r="X50" s="40">
         <v>5</v>
       </c>
-      <c r="Y50" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="41">
+      <c r="Y50" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="91">
         <v>4</v>
       </c>
-      <c r="AA50" s="41">
+      <c r="AA50" s="91">
         <v>5</v>
       </c>
-      <c r="AB50" s="41">
-        <v>0</v>
-      </c>
-      <c r="AC50" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD50" s="43">
-        <v>2</v>
-      </c>
-      <c r="AE50" s="42">
-        <v>2</v>
-      </c>
-      <c r="AF50" s="42">
-        <v>2</v>
-      </c>
-      <c r="AG50" s="42">
-        <v>2</v>
-      </c>
-      <c r="AH50" s="38">
-        <v>2</v>
-      </c>
-      <c r="AI50" s="38">
-        <v>2</v>
-      </c>
-      <c r="AJ50" s="38">
-        <v>2</v>
-      </c>
-      <c r="AK50" s="38">
+      <c r="AB50" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="93">
+        <v>2</v>
+      </c>
+      <c r="AE50" s="96">
+        <v>2</v>
+      </c>
+      <c r="AF50" s="96">
+        <v>2</v>
+      </c>
+      <c r="AG50" s="96">
+        <v>2</v>
+      </c>
+      <c r="AH50" s="40">
+        <v>2</v>
+      </c>
+      <c r="AI50" s="40">
+        <v>2</v>
+      </c>
+      <c r="AJ50" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK50" s="40">
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="4:37" ht="17.25">
-      <c r="D51" s="18" t="s">
+      <c r="D51" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H51" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="K51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="M51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="N51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="O51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="R51" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="S51" s="38">
-        <v>0</v>
-      </c>
-      <c r="T51" s="38">
+      <c r="G51" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="N51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R51" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="S51" s="40">
+        <v>0</v>
+      </c>
+      <c r="T51" s="40">
         <v>1</v>
       </c>
-      <c r="U51" s="38">
-        <v>0</v>
-      </c>
-      <c r="V51" s="38">
-        <v>0</v>
-      </c>
-      <c r="W51" s="38">
-        <v>0</v>
-      </c>
-      <c r="X51" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA51" s="38">
+      <c r="U51" s="40">
+        <v>0</v>
+      </c>
+      <c r="V51" s="40">
+        <v>0</v>
+      </c>
+      <c r="W51" s="40">
+        <v>0</v>
+      </c>
+      <c r="X51" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="40">
         <v>1</v>
       </c>
-      <c r="AB51" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC51" s="38">
+      <c r="AB51" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="40">
         <v>1</v>
       </c>
-      <c r="AD51" s="42">
+      <c r="AD51" s="96">
         <v>1</v>
       </c>
-      <c r="AE51" s="42">
-        <v>0</v>
-      </c>
-      <c r="AF51" s="42">
-        <v>0</v>
-      </c>
-      <c r="AG51" s="42">
-        <v>0</v>
-      </c>
-      <c r="AH51" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI51" s="38">
-        <v>0</v>
-      </c>
-      <c r="AJ51" s="38">
-        <v>0</v>
-      </c>
-      <c r="AK51" s="38">
+      <c r="AE51" s="96">
+        <v>0</v>
+      </c>
+      <c r="AF51" s="96">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="96">
+        <v>0</v>
+      </c>
+      <c r="AH51" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI51" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK51" s="40">
         <v>1</v>
       </c>
     </row>
@@ -12450,8 +12560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="W46" workbookViewId="0">
+      <selection activeCell="AL51" sqref="AL51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated by sravvani date:26/03/2013
</commit_message>
<xml_diff>
--- a/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
+++ b/Ebay2013/WebContent/TimeSheet/Timesheet_Group5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6060" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="January 2013" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="49">
   <si>
     <t>Activity Code</t>
   </si>
@@ -622,11 +622,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="51"/>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="94"/>
+      <c r="E1" s="96"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
       <c r="H1" s="51"/>
@@ -4062,10 +4062,10 @@
       </c>
     </row>
     <row r="41" spans="4:37" ht="17.25">
-      <c r="D41" s="95" t="s">
+      <c r="D41" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="95" t="s">
+      <c r="E41" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F41" s="48" t="s">
@@ -4166,10 +4166,10 @@
       </c>
     </row>
     <row r="42" spans="4:37" ht="17.25">
-      <c r="D42" s="95" t="s">
+      <c r="D42" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="95" t="s">
+      <c r="E42" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F42" s="48" t="s">
@@ -4270,10 +4270,10 @@
       </c>
     </row>
     <row r="43" spans="4:37" ht="17.25">
-      <c r="D43" s="95" t="s">
+      <c r="D43" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="95" t="s">
+      <c r="E43" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F43" s="48" t="s">
@@ -4374,10 +4374,10 @@
       </c>
     </row>
     <row r="44" spans="4:37" ht="17.25">
-      <c r="D44" s="95" t="s">
+      <c r="D44" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="95" t="s">
+      <c r="E44" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F44" s="48" t="s">
@@ -4474,10 +4474,10 @@
       </c>
     </row>
     <row r="45" spans="4:37" ht="17.25">
-      <c r="D45" s="95" t="s">
+      <c r="D45" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="95" t="s">
+      <c r="E45" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F45" s="48" t="s">
@@ -5144,10 +5144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR46"/>
+  <dimension ref="A1:AR48"/>
   <sheetViews>
-    <sheetView topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38:AH42"/>
+    <sheetView tabSelected="1" topLeftCell="S29" workbookViewId="0">
+      <selection activeCell="AH37" sqref="AH37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5179,10 +5179,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="94"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:44" ht="17.25">
       <c r="A2" s="4" t="s">
@@ -5427,15 +5427,31 @@
       <c r="F16" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19">
+      <c r="G16" s="48">
+        <v>0</v>
+      </c>
+      <c r="H16" s="48">
+        <v>0</v>
+      </c>
+      <c r="I16" s="48">
+        <v>0</v>
+      </c>
+      <c r="J16" s="48">
+        <v>0</v>
+      </c>
+      <c r="K16" s="48">
+        <v>0</v>
+      </c>
+      <c r="L16" s="48">
+        <v>0</v>
+      </c>
+      <c r="M16" s="48">
+        <v>0</v>
+      </c>
+      <c r="N16" s="89">
+        <v>0</v>
+      </c>
+      <c r="O16" s="89">
         <v>0</v>
       </c>
       <c r="P16" s="19">
@@ -5506,16 +5522,32 @@
       <c r="F17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19">
+      <c r="G17" s="48">
+        <v>0</v>
+      </c>
+      <c r="H17" s="48">
+        <v>3</v>
+      </c>
+      <c r="I17" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="J17" s="48">
+        <v>3</v>
+      </c>
+      <c r="K17" s="48">
+        <v>3</v>
+      </c>
+      <c r="L17" s="48">
         <v>6</v>
+      </c>
+      <c r="M17" s="48">
+        <v>0</v>
+      </c>
+      <c r="N17" s="89">
+        <v>2</v>
+      </c>
+      <c r="O17" s="89">
+        <v>8</v>
       </c>
       <c r="P17" s="19">
         <v>8</v>
@@ -5585,15 +5617,31 @@
       <c r="F18" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19">
+      <c r="G18" s="48">
+        <v>0</v>
+      </c>
+      <c r="H18" s="48">
+        <v>0</v>
+      </c>
+      <c r="I18" s="48">
+        <v>0</v>
+      </c>
+      <c r="J18" s="48">
+        <v>0</v>
+      </c>
+      <c r="K18" s="48">
+        <v>0</v>
+      </c>
+      <c r="L18" s="48">
+        <v>0</v>
+      </c>
+      <c r="M18" s="48">
+        <v>0</v>
+      </c>
+      <c r="N18" s="89">
+        <v>4</v>
+      </c>
+      <c r="O18" s="89">
         <v>0</v>
       </c>
       <c r="P18" s="19">
@@ -5664,15 +5712,33 @@
       <c r="F19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
+      <c r="G19" s="48">
+        <v>2</v>
+      </c>
+      <c r="H19" s="48">
+        <v>0</v>
+      </c>
+      <c r="I19" s="48">
+        <v>0</v>
+      </c>
+      <c r="J19" s="48">
+        <v>0</v>
+      </c>
+      <c r="K19" s="48">
+        <v>0</v>
+      </c>
+      <c r="L19" s="48">
+        <v>0</v>
+      </c>
+      <c r="M19" s="48">
+        <v>0</v>
+      </c>
+      <c r="N19" s="89">
+        <v>0</v>
+      </c>
+      <c r="O19" s="89">
+        <v>0</v>
+      </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
       <c r="R19" s="19"/>
@@ -5703,15 +5769,31 @@
       <c r="F20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19">
+      <c r="G20" s="48">
+        <v>0</v>
+      </c>
+      <c r="H20" s="48">
+        <v>0</v>
+      </c>
+      <c r="I20" s="48">
+        <v>0</v>
+      </c>
+      <c r="J20" s="48">
+        <v>0</v>
+      </c>
+      <c r="K20" s="48">
+        <v>0</v>
+      </c>
+      <c r="L20" s="48">
+        <v>0</v>
+      </c>
+      <c r="M20" s="48">
+        <v>0</v>
+      </c>
+      <c r="N20" s="89">
+        <v>0.25</v>
+      </c>
+      <c r="O20" s="89">
         <v>1</v>
       </c>
       <c r="P20" s="19">
@@ -5782,14 +5864,30 @@
       <c r="F21" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="G21" s="48">
+        <v>0</v>
+      </c>
+      <c r="H21" s="48">
+        <v>0</v>
+      </c>
+      <c r="I21" s="48">
+        <v>0</v>
+      </c>
+      <c r="J21" s="48">
+        <v>0</v>
+      </c>
+      <c r="K21" s="48">
+        <v>0</v>
+      </c>
+      <c r="L21" s="48">
+        <v>0</v>
+      </c>
+      <c r="M21" s="48">
+        <v>0</v>
+      </c>
+      <c r="N21" s="89">
+        <v>0</v>
+      </c>
       <c r="O21" s="19">
         <v>0</v>
       </c>
@@ -5861,14 +5959,30 @@
       <c r="F22" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
+      <c r="G22" s="48">
+        <v>0</v>
+      </c>
+      <c r="H22" s="48">
+        <v>3</v>
+      </c>
+      <c r="I22" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="J22" s="48">
+        <v>3</v>
+      </c>
+      <c r="K22" s="48">
+        <v>3</v>
+      </c>
+      <c r="L22" s="48">
+        <v>6</v>
+      </c>
+      <c r="M22" s="48">
+        <v>0</v>
+      </c>
+      <c r="N22" s="89">
+        <v>2</v>
+      </c>
       <c r="O22" s="19">
         <v>10</v>
       </c>
@@ -5940,14 +6054,30 @@
       <c r="F23" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
+      <c r="G23" s="48">
+        <v>0</v>
+      </c>
+      <c r="H23" s="48">
+        <v>0</v>
+      </c>
+      <c r="I23" s="48">
+        <v>0</v>
+      </c>
+      <c r="J23" s="48">
+        <v>0</v>
+      </c>
+      <c r="K23" s="48">
+        <v>0</v>
+      </c>
+      <c r="L23" s="48">
+        <v>0</v>
+      </c>
+      <c r="M23" s="48">
+        <v>0</v>
+      </c>
+      <c r="N23" s="89">
+        <v>4</v>
+      </c>
       <c r="O23" s="19">
         <v>0</v>
       </c>
@@ -6009,66 +6139,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:34" ht="17.25">
-      <c r="D24" s="18" t="s">
+    <row r="24" spans="4:34" s="80" customFormat="1" ht="17.25">
+      <c r="D24" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="22">
-        <v>1</v>
-      </c>
-      <c r="P24" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="22">
-        <v>1</v>
-      </c>
-      <c r="R24" s="22">
-        <v>0</v>
-      </c>
-      <c r="S24" s="22">
-        <v>3</v>
-      </c>
-      <c r="T24" s="22">
-        <v>0</v>
-      </c>
-      <c r="U24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="V24" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="W24" s="22">
-        <v>1</v>
-      </c>
-      <c r="X24" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA24" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="AB24" s="19">
-        <v>1</v>
-      </c>
+      <c r="F24" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="48">
+        <v>2</v>
+      </c>
+      <c r="H24" s="48">
+        <v>0</v>
+      </c>
+      <c r="I24" s="48">
+        <v>0</v>
+      </c>
+      <c r="J24" s="48">
+        <v>0</v>
+      </c>
+      <c r="K24" s="48">
+        <v>0</v>
+      </c>
+      <c r="L24" s="48">
+        <v>0</v>
+      </c>
+      <c r="M24" s="48">
+        <v>0</v>
+      </c>
+      <c r="N24" s="89">
+        <v>0</v>
+      </c>
+      <c r="O24" s="89"/>
+      <c r="P24" s="89"/>
+      <c r="Q24" s="89"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="89"/>
+      <c r="T24" s="89"/>
+      <c r="U24" s="68"/>
+      <c r="V24" s="89"/>
+      <c r="W24" s="89"/>
+      <c r="X24" s="89"/>
+      <c r="Y24" s="89"/>
+      <c r="Z24" s="89"/>
+      <c r="AA24" s="89"/>
+      <c r="AB24" s="89"/>
       <c r="AC24" s="89"/>
       <c r="AD24" s="89"/>
       <c r="AE24" s="89"/>
@@ -6078,40 +6196,64 @@
     </row>
     <row r="25" spans="4:34" ht="17.25">
       <c r="D25" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19">
-        <v>0</v>
-      </c>
-      <c r="T25" s="19">
-        <v>0</v>
-      </c>
-      <c r="U25" s="19">
-        <v>0</v>
-      </c>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G25" s="48">
+        <v>0</v>
+      </c>
+      <c r="H25" s="48">
+        <v>0</v>
+      </c>
+      <c r="I25" s="48">
+        <v>0</v>
+      </c>
+      <c r="J25" s="48">
+        <v>0</v>
+      </c>
+      <c r="K25" s="48">
+        <v>0</v>
+      </c>
+      <c r="L25" s="48">
+        <v>0</v>
+      </c>
+      <c r="M25" s="48">
+        <v>0</v>
+      </c>
+      <c r="N25" s="89">
+        <v>0.25</v>
+      </c>
+      <c r="O25" s="22">
+        <v>1</v>
+      </c>
+      <c r="P25" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="22">
+        <v>1</v>
+      </c>
+      <c r="R25" s="22">
+        <v>0</v>
+      </c>
+      <c r="S25" s="22">
+        <v>3</v>
+      </c>
+      <c r="T25" s="22">
+        <v>0</v>
+      </c>
+      <c r="U25" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="V25" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="W25" s="22">
+        <v>1</v>
       </c>
       <c r="X25" s="19">
         <v>0</v>
@@ -6123,27 +6265,17 @@
         <v>0</v>
       </c>
       <c r="AA25" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="89">
-        <v>0</v>
-      </c>
-      <c r="AD25" s="89">
-        <v>0</v>
-      </c>
-      <c r="AE25" s="89">
-        <v>0</v>
-      </c>
-      <c r="AF25" s="89">
-        <v>0</v>
-      </c>
-      <c r="AG25" s="89">
-        <v>0</v>
-      </c>
-      <c r="AH25" s="89">
-        <v>0</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="AB25" s="19">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="89"/>
+      <c r="AD25" s="89"/>
+      <c r="AE25" s="89"/>
+      <c r="AF25" s="89"/>
+      <c r="AG25" s="89"/>
+      <c r="AH25" s="89"/>
     </row>
     <row r="26" spans="4:34" ht="17.25">
       <c r="D26" s="18" t="s">
@@ -6153,27 +6285,45 @@
         <v>29</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
+        <v>4</v>
+      </c>
+      <c r="G26" s="48">
+        <v>0</v>
+      </c>
+      <c r="H26" s="48">
+        <v>0</v>
+      </c>
+      <c r="I26" s="48">
+        <v>0</v>
+      </c>
+      <c r="J26" s="48">
+        <v>0</v>
+      </c>
+      <c r="K26" s="48">
+        <v>0</v>
+      </c>
+      <c r="L26" s="48">
+        <v>0</v>
+      </c>
+      <c r="M26" s="48">
+        <v>0</v>
+      </c>
+      <c r="N26" s="89">
+        <v>0</v>
+      </c>
+      <c r="O26" s="89">
+        <v>0</v>
+      </c>
       <c r="P26" s="19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
       <c r="S26" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T26" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="19">
         <v>0</v>
@@ -6195,20 +6345,22 @@
         <v>0</v>
       </c>
       <c r="AB26" s="19"/>
-      <c r="AC26" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="19">
-        <v>0</v>
-      </c>
-      <c r="AE26" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF26" s="19">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="19"/>
-      <c r="AH26" s="19">
+      <c r="AC26" s="89">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="89">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="89">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="89">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="89">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="89">
         <v>0</v>
       </c>
     </row>
@@ -6220,42 +6372,58 @@
         <v>29</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="G27" s="48">
+        <v>0</v>
+      </c>
+      <c r="H27" s="48">
+        <v>3</v>
+      </c>
+      <c r="I27" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="J27" s="48">
+        <v>3</v>
+      </c>
+      <c r="K27" s="48">
+        <v>3</v>
+      </c>
+      <c r="L27" s="48">
+        <v>6</v>
+      </c>
+      <c r="M27" s="48">
+        <v>0</v>
+      </c>
+      <c r="N27" s="89">
+        <v>2</v>
+      </c>
+      <c r="O27" s="89">
+        <v>8</v>
+      </c>
       <c r="P27" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q27" s="19"/>
-      <c r="R27" s="19">
-        <v>2</v>
-      </c>
+      <c r="R27" s="19"/>
       <c r="S27" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T27" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U27" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" s="19"/>
       <c r="W27" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="19">
         <v>0</v>
@@ -6289,48 +6457,66 @@
         <v>29</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="G28" s="48">
+        <v>0</v>
+      </c>
+      <c r="H28" s="48">
+        <v>0</v>
+      </c>
+      <c r="I28" s="48">
+        <v>0</v>
+      </c>
+      <c r="J28" s="48">
+        <v>0</v>
+      </c>
+      <c r="K28" s="48">
+        <v>0</v>
+      </c>
+      <c r="L28" s="48">
+        <v>0</v>
+      </c>
+      <c r="M28" s="48">
+        <v>0</v>
+      </c>
+      <c r="N28" s="89">
+        <v>4</v>
+      </c>
+      <c r="O28" s="89">
+        <v>0</v>
+      </c>
       <c r="P28" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19">
+        <v>2</v>
+      </c>
+      <c r="S28" s="19">
+        <v>0</v>
+      </c>
+      <c r="T28" s="19">
+        <v>0</v>
+      </c>
+      <c r="U28" s="19">
         <v>1</v>
-      </c>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="23">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S28" s="19">
-        <v>0</v>
-      </c>
-      <c r="T28" s="19">
-        <v>0</v>
-      </c>
-      <c r="U28" s="19">
-        <v>2</v>
       </c>
       <c r="V28" s="19"/>
       <c r="W28" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X28" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y28" s="19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z28" s="19">
         <v>0</v>
       </c>
-      <c r="AA28" s="23">
-        <v>4.8611111111111112E-2</v>
+      <c r="AA28" s="19">
+        <v>0</v>
       </c>
       <c r="AB28" s="19"/>
       <c r="AC28" s="19">
@@ -6352,49 +6538,47 @@
     </row>
     <row r="29" spans="4:34" ht="17.25">
       <c r="D29" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="19">
-        <v>0</v>
-      </c>
-      <c r="H29" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="I29" s="19">
-        <v>0</v>
-      </c>
-      <c r="J29" s="19">
+        <v>20</v>
+      </c>
+      <c r="G29" s="48">
+        <v>2</v>
+      </c>
+      <c r="H29" s="48">
+        <v>0</v>
+      </c>
+      <c r="I29" s="48">
+        <v>0</v>
+      </c>
+      <c r="J29" s="48">
+        <v>0</v>
+      </c>
+      <c r="K29" s="48">
+        <v>0</v>
+      </c>
+      <c r="L29" s="48">
+        <v>0</v>
+      </c>
+      <c r="M29" s="48">
+        <v>0</v>
+      </c>
+      <c r="N29" s="89">
+        <v>0</v>
+      </c>
+      <c r="O29" s="89">
+        <v>0</v>
+      </c>
+      <c r="P29" s="19">
         <v>1</v>
       </c>
-      <c r="K29" s="19">
-        <v>0</v>
-      </c>
-      <c r="L29" s="19">
-        <v>0</v>
-      </c>
-      <c r="M29" s="19">
-        <v>2</v>
-      </c>
-      <c r="N29" s="19">
-        <v>0</v>
-      </c>
-      <c r="O29" s="19">
-        <v>0</v>
-      </c>
-      <c r="P29" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="19">
-        <v>0</v>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="23">
+        <v>6.25E-2</v>
       </c>
       <c r="S29" s="19">
         <v>0</v>
@@ -6403,46 +6587,40 @@
         <v>0</v>
       </c>
       <c r="U29" s="19">
-        <v>0</v>
-      </c>
-      <c r="V29" s="22">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="V29" s="19"/>
       <c r="W29" s="19">
-        <v>0</v>
-      </c>
-      <c r="X29" s="20" t="s">
-        <v>43</v>
+        <v>0.5</v>
+      </c>
+      <c r="X29" s="19">
+        <v>0</v>
       </c>
       <c r="Y29" s="19">
         <v>0</v>
       </c>
-      <c r="Z29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA29" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH29" s="20" t="s">
-        <v>43</v>
+      <c r="Z29" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="23">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="4:34" ht="17.25">
@@ -6453,37 +6631,37 @@
         <v>30</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="H30" s="19">
-        <v>0</v>
-      </c>
-      <c r="I30" s="19">
-        <v>5</v>
-      </c>
-      <c r="J30" s="19">
+        <v>4</v>
+      </c>
+      <c r="G30" s="48">
+        <v>0</v>
+      </c>
+      <c r="H30" s="48">
+        <v>0</v>
+      </c>
+      <c r="I30" s="48">
+        <v>0</v>
+      </c>
+      <c r="J30" s="48">
+        <v>0</v>
+      </c>
+      <c r="K30" s="48">
+        <v>0</v>
+      </c>
+      <c r="L30" s="48">
+        <v>0</v>
+      </c>
+      <c r="M30" s="48">
+        <v>0</v>
+      </c>
+      <c r="N30" s="89">
+        <v>0.25</v>
+      </c>
+      <c r="O30" s="89">
         <v>1</v>
       </c>
-      <c r="K30" s="19">
-        <v>2</v>
-      </c>
-      <c r="L30" s="19">
-        <v>0</v>
-      </c>
-      <c r="M30" s="19">
-        <v>7</v>
-      </c>
-      <c r="N30" s="19">
-        <v>2</v>
-      </c>
-      <c r="O30" s="19">
-        <v>2</v>
-      </c>
       <c r="P30" s="19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="20" t="s">
         <v>43</v>
@@ -6492,7 +6670,7 @@
         <v>0</v>
       </c>
       <c r="S30" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T30" s="19">
         <v>0</v>
@@ -6548,64 +6726,64 @@
         <v>30</v>
       </c>
       <c r="F31" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="H31" s="19">
+        <v>0</v>
+      </c>
+      <c r="I31" s="19">
+        <v>5</v>
+      </c>
+      <c r="J31" s="19">
+        <v>1</v>
+      </c>
+      <c r="K31" s="19">
+        <v>2</v>
+      </c>
+      <c r="L31" s="19">
+        <v>0</v>
+      </c>
+      <c r="M31" s="19">
         <v>7</v>
       </c>
-      <c r="G31" s="19">
-        <v>0</v>
-      </c>
-      <c r="H31" s="19">
-        <v>0</v>
-      </c>
-      <c r="I31" s="19">
-        <v>0</v>
-      </c>
-      <c r="J31" s="19">
-        <v>0</v>
-      </c>
-      <c r="K31" s="19">
-        <v>0</v>
-      </c>
-      <c r="L31" s="19">
-        <v>0</v>
-      </c>
-      <c r="M31" s="19">
-        <v>0</v>
-      </c>
       <c r="N31" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O31" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P31" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q31" s="20" t="s">
         <v>43</v>
       </c>
       <c r="R31" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S31" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T31" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U31" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V31" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W31" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X31" s="20" t="s">
         <v>43</v>
       </c>
       <c r="Y31" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="20" t="s">
         <v>43</v>
@@ -6643,10 +6821,10 @@
         <v>30</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G32" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H32" s="19">
         <v>0</v>
@@ -6667,35 +6845,35 @@
         <v>0</v>
       </c>
       <c r="N32" s="19">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="O32" s="19">
+        <v>0</v>
+      </c>
+      <c r="P32" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R32" s="19">
+        <v>2</v>
+      </c>
+      <c r="S32" s="19">
+        <v>0</v>
+      </c>
+      <c r="T32" s="19">
+        <v>3</v>
+      </c>
+      <c r="U32" s="19">
+        <v>3</v>
+      </c>
+      <c r="V32" s="22">
+        <v>2</v>
+      </c>
+      <c r="W32" s="19">
         <v>1</v>
       </c>
-      <c r="P32" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R32" s="19">
-        <v>1.3</v>
-      </c>
-      <c r="S32" s="19">
-        <v>0</v>
-      </c>
-      <c r="T32" s="19">
-        <v>1.4</v>
-      </c>
-      <c r="U32" s="19">
-        <v>2</v>
-      </c>
-      <c r="V32" s="22">
-        <v>0</v>
-      </c>
-      <c r="W32" s="19">
-        <v>0.5</v>
-      </c>
       <c r="X32" s="20" t="s">
         <v>43</v>
       </c>
@@ -6706,10 +6884,10 @@
         <v>43</v>
       </c>
       <c r="AA32" s="19">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AB32" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC32" s="20" t="s">
         <v>43</v>
@@ -6732,65 +6910,79 @@
     </row>
     <row r="33" spans="4:34" ht="17.25">
       <c r="D33" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="G33" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="19">
+        <v>0</v>
+      </c>
+      <c r="I33" s="19">
+        <v>0</v>
+      </c>
+      <c r="J33" s="19">
+        <v>0</v>
+      </c>
+      <c r="K33" s="19">
+        <v>0</v>
+      </c>
+      <c r="L33" s="19">
+        <v>0</v>
+      </c>
+      <c r="M33" s="19">
+        <v>0</v>
+      </c>
       <c r="N33" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O33" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="R33" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="S33" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T33" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="U33" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="V33" s="20" t="s">
-        <v>46</v>
+      <c r="R33" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="S33" s="19">
+        <v>0</v>
+      </c>
+      <c r="T33" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="U33" s="19">
+        <v>2</v>
+      </c>
+      <c r="V33" s="22">
+        <v>0</v>
       </c>
       <c r="W33" s="19">
-        <v>0</v>
-      </c>
-      <c r="X33" s="19">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="X33" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="Y33" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z33" s="20" t="s">
         <v>43</v>
       </c>
       <c r="AA33" s="19">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AB33" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC33" s="20" t="s">
         <v>43</v>
@@ -6819,23 +7011,37 @@
         <v>31</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
+        <v>4</v>
+      </c>
+      <c r="G34" s="48">
+        <v>0</v>
+      </c>
+      <c r="H34" s="48">
+        <v>0</v>
+      </c>
+      <c r="I34" s="48">
+        <v>0</v>
+      </c>
+      <c r="J34" s="48">
+        <v>0</v>
+      </c>
+      <c r="K34" s="48">
+        <v>0</v>
+      </c>
+      <c r="L34" s="48">
+        <v>0</v>
+      </c>
+      <c r="M34" s="48">
+        <v>0</v>
+      </c>
       <c r="N34" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O34" s="19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P34" s="19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="20" t="s">
         <v>43</v>
@@ -6900,23 +7106,37 @@
         <v>31</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="G35" s="48">
+        <v>0</v>
+      </c>
+      <c r="H35" s="48">
+        <v>3</v>
+      </c>
+      <c r="I35" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="J35" s="48">
+        <v>3</v>
+      </c>
+      <c r="K35" s="48">
+        <v>3</v>
+      </c>
+      <c r="L35" s="48">
+        <v>6</v>
+      </c>
+      <c r="M35" s="48">
+        <v>0</v>
+      </c>
       <c r="N35" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O35" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P35" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q35" s="20" t="s">
         <v>43</v>
@@ -6937,10 +7157,10 @@
         <v>46</v>
       </c>
       <c r="W35" s="19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="X35" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y35" s="19">
         <v>0</v>
@@ -6981,36 +7201,92 @@
         <v>31</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="19"/>
-      <c r="Y36" s="19"/>
-      <c r="Z36" s="20"/>
-      <c r="AA36" s="19"/>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="20"/>
-      <c r="AD36" s="20"/>
-      <c r="AE36" s="20"/>
-      <c r="AF36" s="20"/>
-      <c r="AG36" s="20"/>
-      <c r="AH36" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="G36" s="48">
+        <v>0</v>
+      </c>
+      <c r="H36" s="48">
+        <v>0</v>
+      </c>
+      <c r="I36" s="48">
+        <v>0</v>
+      </c>
+      <c r="J36" s="48">
+        <v>0</v>
+      </c>
+      <c r="K36" s="48">
+        <v>0</v>
+      </c>
+      <c r="L36" s="48">
+        <v>0</v>
+      </c>
+      <c r="M36" s="48">
+        <v>0</v>
+      </c>
+      <c r="N36" s="19">
+        <v>4</v>
+      </c>
+      <c r="O36" s="19">
+        <v>0</v>
+      </c>
+      <c r="P36" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R36" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S36" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T36" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U36" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="V36" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="W36" s="19">
+        <v>7</v>
+      </c>
+      <c r="X36" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y36" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA36" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH36" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="4:34" ht="17.25">
       <c r="D37" s="18" t="s">
@@ -7020,633 +7296,661 @@
         <v>31</v>
       </c>
       <c r="F37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="48">
+        <v>2</v>
+      </c>
+      <c r="H37" s="48">
+        <v>0</v>
+      </c>
+      <c r="I37" s="48">
+        <v>0</v>
+      </c>
+      <c r="J37" s="48">
+        <v>0</v>
+      </c>
+      <c r="K37" s="48">
+        <v>0</v>
+      </c>
+      <c r="L37" s="48">
+        <v>0</v>
+      </c>
+      <c r="M37" s="48">
+        <v>0</v>
+      </c>
+      <c r="N37" s="19">
+        <v>0</v>
+      </c>
+      <c r="O37" s="19">
+        <v>0</v>
+      </c>
+      <c r="P37" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="R37" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="S37" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="T37" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="U37" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="V37" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="W37" s="19">
+        <v>0</v>
+      </c>
+      <c r="X37" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA37" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG37" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH37" s="68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="4:34" ht="17.25">
+      <c r="D38" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19">
+      <c r="G38" s="48">
+        <v>0</v>
+      </c>
+      <c r="H38" s="48">
+        <v>0</v>
+      </c>
+      <c r="I38" s="48">
+        <v>0</v>
+      </c>
+      <c r="J38" s="48">
+        <v>0</v>
+      </c>
+      <c r="K38" s="48">
+        <v>0</v>
+      </c>
+      <c r="L38" s="48">
+        <v>0</v>
+      </c>
+      <c r="M38" s="48">
+        <v>0</v>
+      </c>
+      <c r="N38" s="19">
         <v>0.25</v>
       </c>
-      <c r="O37" s="19">
+      <c r="O38" s="19">
         <v>1</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P38" s="19">
         <v>1</v>
       </c>
-      <c r="Q37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R37" s="20" t="s">
+      <c r="Q38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="R38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="S37" s="20" t="s">
+      <c r="S38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="T37" s="20" t="s">
+      <c r="T38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="U37" s="20" t="s">
+      <c r="U38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="V37" s="20" t="s">
+      <c r="V38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="W37" s="19">
+      <c r="W38" s="19">
         <v>0.5</v>
       </c>
-      <c r="X37" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="19">
-        <v>2</v>
-      </c>
-      <c r="Z37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA37" s="19">
+      <c r="X38" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="19">
+        <v>2</v>
+      </c>
+      <c r="Z38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA38" s="19">
         <v>1.5</v>
       </c>
-      <c r="AB37" s="19">
+      <c r="AB38" s="19">
         <v>1</v>
       </c>
-      <c r="AC37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG37" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH37" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="4:34" ht="17.25">
-      <c r="D38" s="95" t="s">
+      <c r="AC38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG38" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH38" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="4:34" ht="17.25">
+      <c r="D39" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="95" t="s">
+      <c r="E39" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="48" t="s">
+      <c r="F39" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="48">
-        <v>0</v>
-      </c>
-      <c r="H38" s="48">
-        <v>0</v>
-      </c>
-      <c r="I38" s="48">
-        <v>0</v>
-      </c>
-      <c r="J38" s="48">
-        <v>0</v>
-      </c>
-      <c r="K38" s="48">
-        <v>0</v>
-      </c>
-      <c r="L38" s="48">
-        <v>0</v>
-      </c>
-      <c r="M38" s="48">
-        <v>0</v>
-      </c>
-      <c r="N38" s="48">
-        <v>0</v>
-      </c>
-      <c r="O38" s="48">
-        <v>0</v>
-      </c>
-      <c r="P38" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="48">
-        <v>0</v>
-      </c>
-      <c r="R38" s="48">
-        <v>0</v>
-      </c>
-      <c r="S38" s="48">
-        <v>0</v>
-      </c>
-      <c r="T38" s="48">
-        <v>0</v>
-      </c>
-      <c r="U38" s="48">
-        <v>0</v>
-      </c>
-      <c r="V38" s="48">
-        <v>0</v>
-      </c>
-      <c r="W38" s="48">
-        <v>0</v>
-      </c>
-      <c r="X38" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AE38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AF38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AG38" s="48">
-        <v>0</v>
-      </c>
-      <c r="AH38" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="4:34" ht="17.25">
-      <c r="D39" s="95" t="s">
+      <c r="G39" s="48">
+        <v>0</v>
+      </c>
+      <c r="H39" s="48">
+        <v>0</v>
+      </c>
+      <c r="I39" s="48">
+        <v>0</v>
+      </c>
+      <c r="J39" s="48">
+        <v>0</v>
+      </c>
+      <c r="K39" s="48">
+        <v>0</v>
+      </c>
+      <c r="L39" s="48">
+        <v>0</v>
+      </c>
+      <c r="M39" s="48">
+        <v>0</v>
+      </c>
+      <c r="N39" s="48">
+        <v>0</v>
+      </c>
+      <c r="O39" s="48">
+        <v>0</v>
+      </c>
+      <c r="P39" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="48">
+        <v>0</v>
+      </c>
+      <c r="R39" s="48">
+        <v>0</v>
+      </c>
+      <c r="S39" s="48">
+        <v>0</v>
+      </c>
+      <c r="T39" s="48">
+        <v>0</v>
+      </c>
+      <c r="U39" s="48">
+        <v>0</v>
+      </c>
+      <c r="V39" s="48">
+        <v>0</v>
+      </c>
+      <c r="W39" s="48">
+        <v>0</v>
+      </c>
+      <c r="X39" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:34" ht="17.25">
+      <c r="D40" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="95" t="s">
+      <c r="E40" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="48" t="s">
+      <c r="F40" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="48">
-        <v>0</v>
-      </c>
-      <c r="H39" s="48">
+      <c r="G40" s="48">
+        <v>0</v>
+      </c>
+      <c r="H40" s="48">
         <v>3</v>
       </c>
-      <c r="I39" s="48">
+      <c r="I40" s="48">
         <v>1.5</v>
       </c>
-      <c r="J39" s="48">
+      <c r="J40" s="48">
         <v>3</v>
       </c>
-      <c r="K39" s="48">
+      <c r="K40" s="48">
         <v>3</v>
       </c>
-      <c r="L39" s="48">
+      <c r="L40" s="48">
         <v>6</v>
       </c>
-      <c r="M39" s="48">
-        <v>0</v>
-      </c>
-      <c r="N39" s="48">
+      <c r="M40" s="48">
+        <v>0</v>
+      </c>
+      <c r="N40" s="48">
         <v>0.5</v>
       </c>
-      <c r="O39" s="48">
+      <c r="O40" s="48">
         <v>9</v>
       </c>
-      <c r="P39" s="48">
+      <c r="P40" s="48">
         <v>7</v>
       </c>
-      <c r="Q39" s="48">
-        <v>0</v>
-      </c>
-      <c r="R39" s="48">
-        <v>0</v>
-      </c>
-      <c r="S39" s="48">
-        <v>0</v>
-      </c>
-      <c r="T39" s="48">
-        <v>0</v>
-      </c>
-      <c r="U39" s="48">
-        <v>0</v>
-      </c>
-      <c r="V39" s="48">
-        <v>0</v>
-      </c>
-      <c r="W39" s="48">
-        <v>0</v>
-      </c>
-      <c r="X39" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AE39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AF39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AG39" s="48">
-        <v>0</v>
-      </c>
-      <c r="AH39" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="4:34" ht="17.25">
-      <c r="D40" s="95" t="s">
+      <c r="Q40" s="48">
+        <v>0</v>
+      </c>
+      <c r="R40" s="48">
+        <v>0</v>
+      </c>
+      <c r="S40" s="48">
+        <v>0</v>
+      </c>
+      <c r="T40" s="48">
+        <v>0</v>
+      </c>
+      <c r="U40" s="48">
+        <v>0</v>
+      </c>
+      <c r="V40" s="48">
+        <v>0</v>
+      </c>
+      <c r="W40" s="48">
+        <v>0</v>
+      </c>
+      <c r="X40" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:34" ht="17.25">
+      <c r="D41" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="95" t="s">
+      <c r="E41" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="48" t="s">
+      <c r="F41" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="48">
-        <v>0</v>
-      </c>
-      <c r="H40" s="48">
-        <v>0</v>
-      </c>
-      <c r="I40" s="48">
-        <v>0</v>
-      </c>
-      <c r="J40" s="48">
-        <v>0</v>
-      </c>
-      <c r="K40" s="48">
-        <v>0</v>
-      </c>
-      <c r="L40" s="48">
-        <v>0</v>
-      </c>
-      <c r="M40" s="48">
-        <v>0</v>
-      </c>
-      <c r="N40" s="48">
+      <c r="G41" s="48">
+        <v>0</v>
+      </c>
+      <c r="H41" s="48">
+        <v>0</v>
+      </c>
+      <c r="I41" s="48">
+        <v>0</v>
+      </c>
+      <c r="J41" s="48">
+        <v>0</v>
+      </c>
+      <c r="K41" s="48">
+        <v>0</v>
+      </c>
+      <c r="L41" s="48">
+        <v>0</v>
+      </c>
+      <c r="M41" s="48">
+        <v>0</v>
+      </c>
+      <c r="N41" s="48">
         <v>4</v>
       </c>
-      <c r="O40" s="48">
-        <v>0</v>
-      </c>
-      <c r="P40" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="48">
-        <v>0</v>
-      </c>
-      <c r="R40" s="48">
-        <v>2</v>
-      </c>
-      <c r="S40" s="48">
+      <c r="O41" s="48">
+        <v>0</v>
+      </c>
+      <c r="P41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="48">
+        <v>0</v>
+      </c>
+      <c r="R41" s="48">
+        <v>2</v>
+      </c>
+      <c r="S41" s="48">
         <v>0.5</v>
       </c>
-      <c r="T40" s="48">
-        <v>0</v>
-      </c>
-      <c r="U40" s="48">
+      <c r="T41" s="48">
+        <v>0</v>
+      </c>
+      <c r="U41" s="48">
         <v>5</v>
       </c>
-      <c r="V40" s="48">
-        <v>2</v>
-      </c>
-      <c r="W40" s="48">
+      <c r="V41" s="48">
+        <v>2</v>
+      </c>
+      <c r="W41" s="48">
         <v>0.5</v>
       </c>
-      <c r="X40" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AF40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AG40" s="48">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="4:34" ht="17.25">
-      <c r="D41" s="95" t="s">
+      <c r="X41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG41" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:34" ht="17.25">
+      <c r="D42" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="95" t="s">
+      <c r="E42" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="48" t="s">
+      <c r="F42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="48">
-        <v>2</v>
-      </c>
-      <c r="H41" s="48">
-        <v>0</v>
-      </c>
-      <c r="I41" s="48">
-        <v>0</v>
-      </c>
-      <c r="J41" s="48">
-        <v>0</v>
-      </c>
-      <c r="K41" s="48">
-        <v>0</v>
-      </c>
-      <c r="L41" s="48">
-        <v>0</v>
-      </c>
-      <c r="M41" s="48">
-        <v>0</v>
-      </c>
-      <c r="N41" s="48">
-        <v>0</v>
-      </c>
-      <c r="O41" s="48">
-        <v>0</v>
-      </c>
-      <c r="P41" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="48">
-        <v>0</v>
-      </c>
-      <c r="R41" s="48">
-        <v>0</v>
-      </c>
-      <c r="S41" s="48">
-        <v>0</v>
-      </c>
-      <c r="T41" s="48">
-        <v>0</v>
-      </c>
-      <c r="U41" s="48">
-        <v>0</v>
-      </c>
-      <c r="V41" s="48">
-        <v>0</v>
-      </c>
-      <c r="W41" s="48">
-        <v>0</v>
-      </c>
-      <c r="X41" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AE41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AF41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AG41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AH41" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="4:34" ht="17.25">
-      <c r="D42" s="95" t="s">
+      <c r="G42" s="48">
+        <v>2</v>
+      </c>
+      <c r="H42" s="48">
+        <v>0</v>
+      </c>
+      <c r="I42" s="48">
+        <v>0</v>
+      </c>
+      <c r="J42" s="48">
+        <v>0</v>
+      </c>
+      <c r="K42" s="48">
+        <v>0</v>
+      </c>
+      <c r="L42" s="48">
+        <v>0</v>
+      </c>
+      <c r="M42" s="48">
+        <v>0</v>
+      </c>
+      <c r="N42" s="48">
+        <v>0</v>
+      </c>
+      <c r="O42" s="48">
+        <v>0</v>
+      </c>
+      <c r="P42" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="48">
+        <v>0</v>
+      </c>
+      <c r="R42" s="48">
+        <v>0</v>
+      </c>
+      <c r="S42" s="48">
+        <v>0</v>
+      </c>
+      <c r="T42" s="48">
+        <v>0</v>
+      </c>
+      <c r="U42" s="48">
+        <v>0</v>
+      </c>
+      <c r="V42" s="48">
+        <v>0</v>
+      </c>
+      <c r="W42" s="48">
+        <v>0</v>
+      </c>
+      <c r="X42" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:34" ht="17.25">
+      <c r="D43" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="95" t="s">
+      <c r="E43" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="48" t="s">
+      <c r="F43" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="48">
-        <v>0</v>
-      </c>
-      <c r="H42" s="48">
-        <v>0</v>
-      </c>
-      <c r="I42" s="48">
-        <v>0</v>
-      </c>
-      <c r="J42" s="48">
-        <v>0</v>
-      </c>
-      <c r="K42" s="48">
-        <v>0</v>
-      </c>
-      <c r="L42" s="48">
-        <v>0</v>
-      </c>
-      <c r="M42" s="48">
-        <v>0</v>
-      </c>
-      <c r="N42" s="48">
+      <c r="G43" s="48">
+        <v>0</v>
+      </c>
+      <c r="H43" s="48">
+        <v>0</v>
+      </c>
+      <c r="I43" s="48">
+        <v>0</v>
+      </c>
+      <c r="J43" s="48">
+        <v>0</v>
+      </c>
+      <c r="K43" s="48">
+        <v>0</v>
+      </c>
+      <c r="L43" s="48">
+        <v>0</v>
+      </c>
+      <c r="M43" s="48">
+        <v>0</v>
+      </c>
+      <c r="N43" s="48">
         <v>0.25</v>
       </c>
-      <c r="O42" s="48">
+      <c r="O43" s="48">
         <v>1</v>
       </c>
-      <c r="P42" s="48">
+      <c r="P43" s="48">
         <v>1</v>
       </c>
-      <c r="Q42" s="48">
-        <v>0</v>
-      </c>
-      <c r="R42" s="48">
+      <c r="Q43" s="48">
+        <v>0</v>
+      </c>
+      <c r="R43" s="48">
         <v>1.5</v>
       </c>
-      <c r="S42" s="48">
-        <v>0</v>
-      </c>
-      <c r="T42" s="48">
-        <v>0</v>
-      </c>
-      <c r="U42" s="48">
-        <v>0</v>
-      </c>
-      <c r="V42" s="48">
-        <v>0</v>
-      </c>
-      <c r="W42" s="48">
+      <c r="S43" s="48">
+        <v>0</v>
+      </c>
+      <c r="T43" s="48">
+        <v>0</v>
+      </c>
+      <c r="U43" s="48">
+        <v>0</v>
+      </c>
+      <c r="V43" s="48">
+        <v>0</v>
+      </c>
+      <c r="W43" s="48">
         <v>0.5</v>
       </c>
-      <c r="X42" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="48">
+      <c r="X43" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="48">
         <v>1</v>
       </c>
-      <c r="Z42" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA42" s="48">
+      <c r="Z43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="48">
         <v>1.5</v>
       </c>
-      <c r="AB42" s="48">
+      <c r="AB43" s="48">
         <v>1.5</v>
       </c>
-      <c r="AC42" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD42" s="48">
-        <v>0</v>
-      </c>
-      <c r="AE42" s="48">
-        <v>0</v>
-      </c>
-      <c r="AF42" s="48">
-        <v>0</v>
-      </c>
-      <c r="AG42" s="48">
-        <v>0</v>
-      </c>
-      <c r="AH42" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="4:34" ht="17.25">
-      <c r="D43" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19">
-        <v>0</v>
-      </c>
-      <c r="O43" s="19">
-        <v>0</v>
-      </c>
-      <c r="P43" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="19">
-        <v>0</v>
-      </c>
-      <c r="R43" s="19">
-        <v>0</v>
-      </c>
-      <c r="S43" s="19">
-        <v>0</v>
-      </c>
-      <c r="T43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U43" s="19">
-        <v>0</v>
-      </c>
-      <c r="V43" s="19">
-        <v>0</v>
-      </c>
-      <c r="W43" s="19">
-        <v>0</v>
-      </c>
-      <c r="X43" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB43" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH43" s="20" t="s">
-        <v>43</v>
+      <c r="AC43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="48">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="4:34" ht="17.25">
@@ -7657,105 +7961,133 @@
         <v>33</v>
       </c>
       <c r="F44" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="48">
+        <v>0</v>
+      </c>
+      <c r="H44" s="48">
+        <v>0</v>
+      </c>
+      <c r="I44" s="48">
+        <v>0</v>
+      </c>
+      <c r="J44" s="48">
+        <v>0</v>
+      </c>
+      <c r="K44" s="48">
+        <v>0</v>
+      </c>
+      <c r="L44" s="48">
+        <v>0</v>
+      </c>
+      <c r="M44" s="48">
+        <v>0</v>
+      </c>
+      <c r="N44" s="19">
+        <v>0</v>
+      </c>
+      <c r="O44" s="19">
+        <v>0</v>
+      </c>
+      <c r="P44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="19">
+        <v>0</v>
+      </c>
+      <c r="R44" s="19">
+        <v>0</v>
+      </c>
+      <c r="S44" s="19">
+        <v>0</v>
+      </c>
+      <c r="T44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U44" s="19">
+        <v>0</v>
+      </c>
+      <c r="V44" s="19">
+        <v>0</v>
+      </c>
+      <c r="W44" s="19">
+        <v>0</v>
+      </c>
+      <c r="X44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB44" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG44" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH44" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="4:34" ht="17.25">
+      <c r="D45" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19">
+      <c r="G45" s="48">
+        <v>0</v>
+      </c>
+      <c r="H45" s="48">
+        <v>3</v>
+      </c>
+      <c r="I45" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="J45" s="48">
+        <v>3</v>
+      </c>
+      <c r="K45" s="48">
+        <v>3</v>
+      </c>
+      <c r="L45" s="48">
+        <v>6</v>
+      </c>
+      <c r="M45" s="48">
+        <v>0</v>
+      </c>
+      <c r="N45" s="19">
         <v>10</v>
       </c>
-      <c r="O44" s="19">
+      <c r="O45" s="19">
         <v>6</v>
       </c>
-      <c r="P44" s="19">
+      <c r="P45" s="19">
         <v>7</v>
       </c>
-      <c r="Q44" s="19">
-        <v>0</v>
-      </c>
-      <c r="R44" s="19">
-        <v>0</v>
-      </c>
-      <c r="S44" s="19">
-        <v>0</v>
-      </c>
-      <c r="T44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U44" s="19">
-        <v>0</v>
-      </c>
-      <c r="V44" s="19">
-        <v>0</v>
-      </c>
-      <c r="W44" s="19">
-        <v>0</v>
-      </c>
-      <c r="X44" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB44" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH44" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="4:34" ht="18" thickBot="1">
-      <c r="D45" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19">
-        <v>0</v>
-      </c>
-      <c r="O45" s="19">
-        <v>0</v>
-      </c>
-      <c r="P45" s="19">
-        <v>0</v>
-      </c>
       <c r="Q45" s="19">
         <v>0</v>
       </c>
@@ -7769,19 +8101,19 @@
         <v>43</v>
       </c>
       <c r="U45" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V45" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W45" s="19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="X45" s="19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Y45" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z45" s="20" t="s">
         <v>43</v>
@@ -7815,80 +8147,284 @@
       <c r="D46" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="12" t="s">
         <v>33</v>
       </c>
       <c r="F46" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="48">
+        <v>0</v>
+      </c>
+      <c r="H46" s="48">
+        <v>0</v>
+      </c>
+      <c r="I46" s="48">
+        <v>0</v>
+      </c>
+      <c r="J46" s="48">
+        <v>0</v>
+      </c>
+      <c r="K46" s="48">
+        <v>0</v>
+      </c>
+      <c r="L46" s="48">
+        <v>0</v>
+      </c>
+      <c r="M46" s="48">
+        <v>0</v>
+      </c>
+      <c r="N46" s="19">
+        <v>0</v>
+      </c>
+      <c r="O46" s="19">
+        <v>0</v>
+      </c>
+      <c r="P46" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="19">
+        <v>0</v>
+      </c>
+      <c r="R46" s="19">
+        <v>0</v>
+      </c>
+      <c r="S46" s="19">
+        <v>0</v>
+      </c>
+      <c r="T46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U46" s="19">
+        <v>1</v>
+      </c>
+      <c r="V46" s="19">
+        <v>2</v>
+      </c>
+      <c r="W46" s="19">
+        <v>7</v>
+      </c>
+      <c r="X46" s="19">
+        <v>7</v>
+      </c>
+      <c r="Y46" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB46" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG46" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH46" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="4:34" s="80" customFormat="1" ht="18" thickBot="1">
+      <c r="D47" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="48">
+        <v>2</v>
+      </c>
+      <c r="H47" s="48">
+        <v>0</v>
+      </c>
+      <c r="I47" s="48">
+        <v>0</v>
+      </c>
+      <c r="J47" s="48">
+        <v>0</v>
+      </c>
+      <c r="K47" s="48">
+        <v>0</v>
+      </c>
+      <c r="L47" s="48">
+        <v>0</v>
+      </c>
+      <c r="M47" s="48">
+        <v>0</v>
+      </c>
+      <c r="N47" s="89">
+        <v>0</v>
+      </c>
+      <c r="O47" s="89">
+        <v>0</v>
+      </c>
+      <c r="P47" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="89">
+        <v>0</v>
+      </c>
+      <c r="R47" s="89">
+        <v>0</v>
+      </c>
+      <c r="S47" s="89">
+        <v>0</v>
+      </c>
+      <c r="T47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="U47" s="89">
+        <v>0</v>
+      </c>
+      <c r="V47" s="89">
+        <v>0</v>
+      </c>
+      <c r="W47" s="89">
+        <v>0</v>
+      </c>
+      <c r="X47" s="89">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="89">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB47" s="89">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH47" s="68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="4:34" ht="18" thickBot="1">
+      <c r="D48" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22">
+      <c r="G48" s="48">
+        <v>0</v>
+      </c>
+      <c r="H48" s="48">
+        <v>0</v>
+      </c>
+      <c r="I48" s="48">
+        <v>0</v>
+      </c>
+      <c r="J48" s="48">
+        <v>0</v>
+      </c>
+      <c r="K48" s="48">
+        <v>0</v>
+      </c>
+      <c r="L48" s="48">
+        <v>0</v>
+      </c>
+      <c r="M48" s="48">
+        <v>0</v>
+      </c>
+      <c r="N48" s="22">
         <v>1</v>
       </c>
-      <c r="O46" s="22">
+      <c r="O48" s="22">
         <v>1</v>
       </c>
-      <c r="P46" s="22">
+      <c r="P48" s="22">
         <v>1</v>
       </c>
-      <c r="Q46" s="22">
-        <v>0</v>
-      </c>
-      <c r="R46" s="22">
+      <c r="Q48" s="22">
+        <v>0</v>
+      </c>
+      <c r="R48" s="22">
         <v>3</v>
       </c>
-      <c r="S46" s="22">
-        <v>0</v>
-      </c>
-      <c r="T46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="U46" s="22">
+      <c r="S48" s="22">
+        <v>0</v>
+      </c>
+      <c r="T48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U48" s="22">
         <v>1.5</v>
       </c>
-      <c r="V46" s="22">
+      <c r="V48" s="22">
         <v>1</v>
       </c>
-      <c r="W46" s="22">
+      <c r="W48" s="22">
         <v>0.5</v>
       </c>
-      <c r="X46" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="22">
+      <c r="X48" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="22">
         <v>1</v>
       </c>
-      <c r="Z46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB46" s="22">
-        <v>2</v>
-      </c>
-      <c r="AC46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH46" s="20" t="s">
+      <c r="Z48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB48" s="22">
+        <v>2</v>
+      </c>
+      <c r="AC48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG48" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH48" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -7945,10 +8481,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="94"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:37" ht="17.25">
       <c r="A2" s="4" t="s">
@@ -11293,10 +11829,10 @@
       </c>
     </row>
     <row r="46" spans="4:37" ht="17.25">
-      <c r="D46" s="95" t="s">
+      <c r="D46" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="95" t="s">
+      <c r="E46" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F46" s="48" t="s">
@@ -11371,16 +11907,16 @@
       <c r="AC46" s="40">
         <v>0</v>
       </c>
-      <c r="AD46" s="96">
-        <v>0</v>
-      </c>
-      <c r="AE46" s="96">
-        <v>0</v>
-      </c>
-      <c r="AF46" s="96">
-        <v>0</v>
-      </c>
-      <c r="AG46" s="96">
+      <c r="AD46" s="95">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="95">
+        <v>0</v>
+      </c>
+      <c r="AF46" s="95">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="95">
         <v>0</v>
       </c>
       <c r="AH46" s="40">
@@ -11397,10 +11933,10 @@
       </c>
     </row>
     <row r="47" spans="4:37" ht="17.25">
-      <c r="D47" s="95" t="s">
+      <c r="D47" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="95" t="s">
+      <c r="E47" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F47" s="48" t="s">
@@ -11475,16 +12011,16 @@
       <c r="AC47" s="40">
         <v>0</v>
       </c>
-      <c r="AD47" s="96">
-        <v>0</v>
-      </c>
-      <c r="AE47" s="96">
-        <v>0</v>
-      </c>
-      <c r="AF47" s="96">
-        <v>0</v>
-      </c>
-      <c r="AG47" s="96">
+      <c r="AD47" s="95">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="95">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="95">
+        <v>0</v>
+      </c>
+      <c r="AG47" s="95">
         <v>0</v>
       </c>
       <c r="AH47" s="40">
@@ -11501,10 +12037,10 @@
       </c>
     </row>
     <row r="48" spans="4:37" ht="17.25">
-      <c r="D48" s="95" t="s">
+      <c r="D48" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="95" t="s">
+      <c r="E48" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F48" s="48" t="s">
@@ -11579,16 +12115,16 @@
       <c r="AC48" s="40">
         <v>0</v>
       </c>
-      <c r="AD48" s="96">
+      <c r="AD48" s="95">
         <v>3</v>
       </c>
-      <c r="AE48" s="96">
-        <v>0</v>
-      </c>
-      <c r="AF48" s="96">
-        <v>0</v>
-      </c>
-      <c r="AG48" s="96">
+      <c r="AE48" s="95">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="95">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="95">
         <v>0</v>
       </c>
       <c r="AH48" s="40">
@@ -11605,10 +12141,10 @@
       </c>
     </row>
     <row r="49" spans="4:37" ht="17.25">
-      <c r="D49" s="95" t="s">
+      <c r="D49" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="95" t="s">
+      <c r="E49" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F49" s="48" t="s">
@@ -11683,16 +12219,16 @@
       <c r="AC49" s="40">
         <v>0</v>
       </c>
-      <c r="AD49" s="96">
-        <v>0</v>
-      </c>
-      <c r="AE49" s="96">
-        <v>0</v>
-      </c>
-      <c r="AF49" s="96">
-        <v>0</v>
-      </c>
-      <c r="AG49" s="96">
+      <c r="AD49" s="95">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="95">
+        <v>0</v>
+      </c>
+      <c r="AF49" s="95">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="95">
         <v>0</v>
       </c>
       <c r="AH49" s="40">
@@ -11709,10 +12245,10 @@
       </c>
     </row>
     <row r="50" spans="4:37" ht="17.25">
-      <c r="D50" s="95" t="s">
+      <c r="D50" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="95" t="s">
+      <c r="E50" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F50" s="48" t="s">
@@ -11790,13 +12326,13 @@
       <c r="AD50" s="93">
         <v>2</v>
       </c>
-      <c r="AE50" s="96">
-        <v>2</v>
-      </c>
-      <c r="AF50" s="96">
-        <v>2</v>
-      </c>
-      <c r="AG50" s="96">
+      <c r="AE50" s="95">
+        <v>2</v>
+      </c>
+      <c r="AF50" s="95">
+        <v>2</v>
+      </c>
+      <c r="AG50" s="95">
         <v>2</v>
       </c>
       <c r="AH50" s="40">
@@ -11813,10 +12349,10 @@
       </c>
     </row>
     <row r="51" spans="4:37" ht="17.25">
-      <c r="D51" s="95" t="s">
+      <c r="D51" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="95" t="s">
+      <c r="E51" s="94" t="s">
         <v>32</v>
       </c>
       <c r="F51" s="48" t="s">
@@ -11891,16 +12427,16 @@
       <c r="AC51" s="40">
         <v>1</v>
       </c>
-      <c r="AD51" s="96">
+      <c r="AD51" s="95">
         <v>1</v>
       </c>
-      <c r="AE51" s="96">
-        <v>0</v>
-      </c>
-      <c r="AF51" s="96">
-        <v>0</v>
-      </c>
-      <c r="AG51" s="96">
+      <c r="AE51" s="95">
+        <v>0</v>
+      </c>
+      <c r="AF51" s="95">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="95">
         <v>0</v>
       </c>
       <c r="AH51" s="40">
@@ -12560,7 +13096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="AL51" sqref="AL51"/>
     </sheetView>
   </sheetViews>
@@ -12599,10 +13135,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="94"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:36" ht="17.25">
       <c r="A2" s="4" t="s">

</xml_diff>